<commit_message>
add one ifop poll and one opinionway poll (previously missed)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Documents/Perso/Divers/Polling2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCAAE07-00BB-5342-9F4B-68E2BCF4EE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4C0D58-A7F1-584E-8A84-07BFD3700F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="18340" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="4420" yWindow="18080" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="41">
   <si>
     <t>year</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>week</t>
+  </si>
+  <si>
+    <t>opinionway</t>
   </si>
 </sst>
 </file>
@@ -511,11 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB43"/>
+  <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="Z43" sqref="Z43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1412,7 +1415,7 @@
         <v>28</v>
       </c>
       <c r="I14">
-        <v>1048</v>
+        <v>891</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1483,7 +1486,7 @@
         <v>28</v>
       </c>
       <c r="I15">
-        <v>1048</v>
+        <v>880</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1554,7 +1557,7 @@
         <v>28</v>
       </c>
       <c r="I16">
-        <v>1048</v>
+        <v>859</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1613,7 +1616,7 @@
         <v>9</v>
       </c>
       <c r="E17">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
         <v>26</v>
@@ -1625,7 +1628,7 @@
         <v>28</v>
       </c>
       <c r="I17">
-        <v>1022</v>
+        <v>869</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -1687,7 +1690,7 @@
         <v>9</v>
       </c>
       <c r="E18">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" t="s">
         <v>26</v>
@@ -1699,7 +1702,7 @@
         <v>28</v>
       </c>
       <c r="I18">
-        <v>1022</v>
+        <v>838</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -1773,7 +1776,7 @@
         <v>28</v>
       </c>
       <c r="I19">
-        <v>1063</v>
+        <v>872</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -1841,7 +1844,7 @@
         <v>28</v>
       </c>
       <c r="I20">
-        <v>1063</v>
+        <v>861</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -1909,7 +1912,7 @@
         <v>28</v>
       </c>
       <c r="I21">
-        <v>1063</v>
+        <v>850</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -1977,7 +1980,7 @@
         <v>28</v>
       </c>
       <c r="I22">
-        <v>1063</v>
+        <v>893</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -2048,7 +2051,7 @@
         <v>28</v>
       </c>
       <c r="I23">
-        <v>1076</v>
+        <v>904</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2116,7 +2119,7 @@
         <v>28</v>
       </c>
       <c r="I24">
-        <v>1076</v>
+        <v>915</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -2184,7 +2187,7 @@
         <v>28</v>
       </c>
       <c r="I25">
-        <v>1076</v>
+        <v>872</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -2252,7 +2255,7 @@
         <v>28</v>
       </c>
       <c r="I26">
-        <v>1076</v>
+        <v>904</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -2323,7 +2326,7 @@
         <v>28</v>
       </c>
       <c r="I27">
-        <v>1076</v>
+        <v>904</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -2456,7 +2459,7 @@
         <v>27</v>
       </c>
       <c r="I29">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="J29">
         <v>1.5</v>
@@ -2521,7 +2524,7 @@
         <v>28</v>
       </c>
       <c r="I30">
-        <v>893</v>
+        <v>642</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -2586,7 +2589,7 @@
         <v>27</v>
       </c>
       <c r="I31">
-        <v>950</v>
+        <v>825</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -2660,7 +2663,7 @@
         <v>27</v>
       </c>
       <c r="I32">
-        <v>950</v>
+        <v>806</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -2734,7 +2737,7 @@
         <v>27</v>
       </c>
       <c r="I33">
-        <v>950</v>
+        <v>815</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -2811,7 +2814,7 @@
         <v>27</v>
       </c>
       <c r="I34">
-        <v>950</v>
+        <v>815</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -2888,7 +2891,7 @@
         <v>28</v>
       </c>
       <c r="I35">
-        <v>1334</v>
+        <v>956</v>
       </c>
       <c r="J35">
         <v>1.5</v>
@@ -2953,7 +2956,7 @@
         <v>28</v>
       </c>
       <c r="I36">
-        <v>1334</v>
+        <v>931</v>
       </c>
       <c r="J36">
         <v>1.5</v>
@@ -3018,7 +3021,7 @@
         <v>28</v>
       </c>
       <c r="I37">
-        <v>1334</v>
+        <v>920</v>
       </c>
       <c r="J37">
         <v>1.5</v>
@@ -3083,7 +3086,7 @@
         <v>27</v>
       </c>
       <c r="I38">
-        <v>950</v>
+        <v>807</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -3163,7 +3166,7 @@
         <v>27</v>
       </c>
       <c r="I39">
-        <v>950</v>
+        <v>788</v>
       </c>
       <c r="J39">
         <v>1</v>
@@ -3243,7 +3246,7 @@
         <v>27</v>
       </c>
       <c r="I40">
-        <v>950</v>
+        <v>779</v>
       </c>
       <c r="J40">
         <v>1</v>
@@ -3323,7 +3326,7 @@
         <v>28</v>
       </c>
       <c r="I41">
-        <v>1062</v>
+        <v>892</v>
       </c>
       <c r="J41">
         <v>1</v>
@@ -3403,7 +3406,7 @@
         <v>28</v>
       </c>
       <c r="I42">
-        <v>1062</v>
+        <v>903</v>
       </c>
       <c r="J42">
         <v>1</v>
@@ -3483,7 +3486,7 @@
         <v>28</v>
       </c>
       <c r="I43">
-        <v>1062</v>
+        <v>892</v>
       </c>
       <c r="J43">
         <v>1</v>
@@ -3535,6 +3538,594 @@
       </c>
       <c r="AB43" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>13</v>
+      </c>
+      <c r="B44">
+        <v>2021</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>9</v>
+      </c>
+      <c r="E44">
+        <v>23</v>
+      </c>
+      <c r="F44" t="s">
+        <v>40</v>
+      </c>
+      <c r="G44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" t="s">
+        <v>27</v>
+      </c>
+      <c r="I44">
+        <v>709</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>7.5</v>
+      </c>
+      <c r="M44">
+        <v>2</v>
+      </c>
+      <c r="N44">
+        <v>2</v>
+      </c>
+      <c r="O44">
+        <v>9</v>
+      </c>
+      <c r="P44">
+        <v>6</v>
+      </c>
+      <c r="Q44">
+        <v>26.5</v>
+      </c>
+      <c r="T44">
+        <v>12.5</v>
+      </c>
+      <c r="V44">
+        <v>2</v>
+      </c>
+      <c r="W44">
+        <v>20</v>
+      </c>
+      <c r="X44">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>13</v>
+      </c>
+      <c r="B45">
+        <v>2021</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>9</v>
+      </c>
+      <c r="E45">
+        <v>23</v>
+      </c>
+      <c r="F45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G45" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" t="s">
+        <v>27</v>
+      </c>
+      <c r="I45">
+        <v>692</v>
+      </c>
+      <c r="J45">
+        <v>1.5</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>7</v>
+      </c>
+      <c r="M45">
+        <v>2</v>
+      </c>
+      <c r="N45">
+        <v>2</v>
+      </c>
+      <c r="O45">
+        <v>9.5</v>
+      </c>
+      <c r="P45">
+        <v>7</v>
+      </c>
+      <c r="Q45">
+        <v>28</v>
+      </c>
+      <c r="R45">
+        <v>12</v>
+      </c>
+      <c r="V45">
+        <v>4.5</v>
+      </c>
+      <c r="W45">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>13</v>
+      </c>
+      <c r="B46">
+        <v>2021</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>9</v>
+      </c>
+      <c r="E46">
+        <v>23</v>
+      </c>
+      <c r="F46" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" t="s">
+        <v>27</v>
+      </c>
+      <c r="I46">
+        <v>689</v>
+      </c>
+      <c r="J46">
+        <v>1.5</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>8</v>
+      </c>
+      <c r="M46">
+        <v>2.5</v>
+      </c>
+      <c r="N46">
+        <v>2.5</v>
+      </c>
+      <c r="O46">
+        <v>9</v>
+      </c>
+      <c r="P46">
+        <v>7</v>
+      </c>
+      <c r="Q46">
+        <v>29.5</v>
+      </c>
+      <c r="S46">
+        <v>7.5</v>
+      </c>
+      <c r="V46">
+        <v>5.5</v>
+      </c>
+      <c r="W46">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>14</v>
+      </c>
+      <c r="B47">
+        <v>2021</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>9</v>
+      </c>
+      <c r="E47">
+        <v>29</v>
+      </c>
+      <c r="F47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G47" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47">
+        <v>959</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>0.5</v>
+      </c>
+      <c r="L47">
+        <v>7.5</v>
+      </c>
+      <c r="M47">
+        <v>2</v>
+      </c>
+      <c r="N47">
+        <v>4</v>
+      </c>
+      <c r="O47">
+        <v>8.5</v>
+      </c>
+      <c r="P47">
+        <v>6</v>
+      </c>
+      <c r="Q47">
+        <v>26</v>
+      </c>
+      <c r="T47">
+        <v>18</v>
+      </c>
+      <c r="U47">
+        <v>1</v>
+      </c>
+      <c r="V47">
+        <v>2.5</v>
+      </c>
+      <c r="W47">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>14</v>
+      </c>
+      <c r="B48">
+        <v>2021</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>9</v>
+      </c>
+      <c r="E48">
+        <v>29</v>
+      </c>
+      <c r="F48" t="s">
+        <v>35</v>
+      </c>
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48">
+        <v>939</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>0.5</v>
+      </c>
+      <c r="L48">
+        <v>8</v>
+      </c>
+      <c r="M48">
+        <v>2.5</v>
+      </c>
+      <c r="N48">
+        <v>4</v>
+      </c>
+      <c r="O48">
+        <v>8.5</v>
+      </c>
+      <c r="P48">
+        <v>6</v>
+      </c>
+      <c r="Q48">
+        <v>27</v>
+      </c>
+      <c r="R48">
+        <v>13</v>
+      </c>
+      <c r="U48">
+        <v>1</v>
+      </c>
+      <c r="V48">
+        <v>3.5</v>
+      </c>
+      <c r="W48">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>14</v>
+      </c>
+      <c r="B49">
+        <v>2021</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>9</v>
+      </c>
+      <c r="E49">
+        <v>29</v>
+      </c>
+      <c r="F49" t="s">
+        <v>35</v>
+      </c>
+      <c r="G49" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49">
+        <v>934</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>0.5</v>
+      </c>
+      <c r="L49">
+        <v>8</v>
+      </c>
+      <c r="M49">
+        <v>2</v>
+      </c>
+      <c r="N49">
+        <v>3.5</v>
+      </c>
+      <c r="O49">
+        <v>9</v>
+      </c>
+      <c r="P49">
+        <v>6</v>
+      </c>
+      <c r="Q49">
+        <v>27</v>
+      </c>
+      <c r="S49">
+        <v>12</v>
+      </c>
+      <c r="U49">
+        <v>2</v>
+      </c>
+      <c r="V49">
+        <v>4</v>
+      </c>
+      <c r="W49">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>14</v>
+      </c>
+      <c r="B50">
+        <v>2021</v>
+      </c>
+      <c r="C50">
+        <v>5</v>
+      </c>
+      <c r="D50">
+        <v>9</v>
+      </c>
+      <c r="E50">
+        <v>29</v>
+      </c>
+      <c r="F50" t="s">
+        <v>35</v>
+      </c>
+      <c r="G50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" t="s">
+        <v>28</v>
+      </c>
+      <c r="I50">
+        <v>990</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>0.5</v>
+      </c>
+      <c r="L50">
+        <v>7</v>
+      </c>
+      <c r="M50">
+        <v>2</v>
+      </c>
+      <c r="N50">
+        <v>3.5</v>
+      </c>
+      <c r="O50">
+        <v>8</v>
+      </c>
+      <c r="P50">
+        <v>5.5</v>
+      </c>
+      <c r="Q50">
+        <v>24</v>
+      </c>
+      <c r="T50">
+        <v>15</v>
+      </c>
+      <c r="U50">
+        <v>1</v>
+      </c>
+      <c r="V50">
+        <v>2.5</v>
+      </c>
+      <c r="W50">
+        <v>18</v>
+      </c>
+      <c r="X50">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>14</v>
+      </c>
+      <c r="B51">
+        <v>2021</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>9</v>
+      </c>
+      <c r="E51">
+        <v>29</v>
+      </c>
+      <c r="F51" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" t="s">
+        <v>28</v>
+      </c>
+      <c r="I51">
+        <v>976</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>0.5</v>
+      </c>
+      <c r="L51">
+        <v>7</v>
+      </c>
+      <c r="M51">
+        <v>2</v>
+      </c>
+      <c r="N51">
+        <v>3</v>
+      </c>
+      <c r="O51">
+        <v>8</v>
+      </c>
+      <c r="P51">
+        <v>6</v>
+      </c>
+      <c r="Q51">
+        <v>26</v>
+      </c>
+      <c r="R51">
+        <v>11</v>
+      </c>
+      <c r="U51">
+        <v>1</v>
+      </c>
+      <c r="V51">
+        <v>2.5</v>
+      </c>
+      <c r="W51">
+        <v>19</v>
+      </c>
+      <c r="X51">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>14</v>
+      </c>
+      <c r="B52">
+        <v>2021</v>
+      </c>
+      <c r="C52">
+        <v>5</v>
+      </c>
+      <c r="D52">
+        <v>9</v>
+      </c>
+      <c r="E52">
+        <v>29</v>
+      </c>
+      <c r="F52" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" t="s">
+        <v>28</v>
+      </c>
+      <c r="I52">
+        <v>967</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52">
+        <v>0.5</v>
+      </c>
+      <c r="L52">
+        <v>7</v>
+      </c>
+      <c r="M52">
+        <v>1.5</v>
+      </c>
+      <c r="N52">
+        <v>3</v>
+      </c>
+      <c r="O52">
+        <v>8.5</v>
+      </c>
+      <c r="P52">
+        <v>6</v>
+      </c>
+      <c r="Q52">
+        <v>26</v>
+      </c>
+      <c r="S52">
+        <v>9.5</v>
+      </c>
+      <c r="U52">
+        <v>1</v>
+      </c>
+      <c r="V52">
+        <v>2.5</v>
+      </c>
+      <c r="W52">
+        <v>19.5</v>
+      </c>
+      <c r="X52">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 10/11 ifop poll
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4C0D58-A7F1-584E-8A84-07BFD3700F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ADB695-8742-EB49-9279-6A197BFBDE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="18080" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="41">
   <si>
     <t>year</t>
   </si>
@@ -514,11 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB52"/>
+  <dimension ref="A1:AB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="V54" sqref="V54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4128,6 +4128,142 @@
         <v>14</v>
       </c>
     </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>15</v>
+      </c>
+      <c r="B53">
+        <v>2021</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>6</v>
+      </c>
+      <c r="F53" t="s">
+        <v>35</v>
+      </c>
+      <c r="G53" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" t="s">
+        <v>28</v>
+      </c>
+      <c r="I53">
+        <v>921</v>
+      </c>
+      <c r="J53">
+        <v>0.5</v>
+      </c>
+      <c r="K53">
+        <v>0.5</v>
+      </c>
+      <c r="L53">
+        <v>7</v>
+      </c>
+      <c r="M53">
+        <v>2</v>
+      </c>
+      <c r="N53">
+        <v>2</v>
+      </c>
+      <c r="O53">
+        <v>8</v>
+      </c>
+      <c r="P53">
+        <v>6</v>
+      </c>
+      <c r="Q53">
+        <v>25</v>
+      </c>
+      <c r="T53">
+        <v>16</v>
+      </c>
+      <c r="U53">
+        <v>1</v>
+      </c>
+      <c r="V53">
+        <v>2</v>
+      </c>
+      <c r="W53">
+        <v>16</v>
+      </c>
+      <c r="X53">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>15</v>
+      </c>
+      <c r="B54">
+        <v>2021</v>
+      </c>
+      <c r="C54">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <v>10</v>
+      </c>
+      <c r="E54">
+        <v>6</v>
+      </c>
+      <c r="F54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G54" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" t="s">
+        <v>28</v>
+      </c>
+      <c r="I54">
+        <v>921</v>
+      </c>
+      <c r="J54">
+        <v>0.5</v>
+      </c>
+      <c r="K54">
+        <v>0.5</v>
+      </c>
+      <c r="L54">
+        <v>8</v>
+      </c>
+      <c r="M54">
+        <v>1.5</v>
+      </c>
+      <c r="N54">
+        <v>2.5</v>
+      </c>
+      <c r="O54">
+        <v>8</v>
+      </c>
+      <c r="P54">
+        <v>6</v>
+      </c>
+      <c r="Q54">
+        <v>26</v>
+      </c>
+      <c r="R54">
+        <v>11</v>
+      </c>
+      <c r="U54">
+        <v>1</v>
+      </c>
+      <c r="V54">
+        <v>3</v>
+      </c>
+      <c r="W54">
+        <v>18</v>
+      </c>
+      <c r="X54">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update with harris poll, 10/13 (warning: overestimated sample size, to be corrected when true sample size is available)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ADB695-8742-EB49-9279-6A197BFBDE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6E5352-82B0-DC4F-AD73-022D603C4E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="18080" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="41">
   <si>
     <t>year</t>
   </si>
@@ -514,11 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB54"/>
+  <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="V54" sqref="V54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="P55" sqref="P55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3859,7 +3859,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>14</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>14</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>14</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>14</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>15</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>15</v>
       </c>
@@ -4262,6 +4262,246 @@
       </c>
       <c r="X54">
         <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>16</v>
+      </c>
+      <c r="B55">
+        <v>2021</v>
+      </c>
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>10</v>
+      </c>
+      <c r="E55">
+        <v>10</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+      <c r="G55" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" t="s">
+        <v>28</v>
+      </c>
+      <c r="I55">
+        <v>1051</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>11</v>
+      </c>
+      <c r="M55">
+        <v>2</v>
+      </c>
+      <c r="N55">
+        <v>2</v>
+      </c>
+      <c r="O55">
+        <v>7</v>
+      </c>
+      <c r="P55">
+        <v>5</v>
+      </c>
+      <c r="Q55">
+        <v>24</v>
+      </c>
+      <c r="T55">
+        <v>14</v>
+      </c>
+      <c r="U55" t="s">
+        <v>30</v>
+      </c>
+      <c r="V55">
+        <v>1</v>
+      </c>
+      <c r="W55">
+        <v>15</v>
+      </c>
+      <c r="X55">
+        <v>17</v>
+      </c>
+      <c r="Y55" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z55" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA55" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB55" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>16</v>
+      </c>
+      <c r="B56">
+        <v>2021</v>
+      </c>
+      <c r="C56">
+        <v>7</v>
+      </c>
+      <c r="D56">
+        <v>10</v>
+      </c>
+      <c r="E56">
+        <v>10</v>
+      </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
+      <c r="G56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" t="s">
+        <v>28</v>
+      </c>
+      <c r="I56">
+        <v>1051</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>11</v>
+      </c>
+      <c r="M56">
+        <v>2</v>
+      </c>
+      <c r="N56">
+        <v>2</v>
+      </c>
+      <c r="O56">
+        <v>8</v>
+      </c>
+      <c r="P56">
+        <v>5</v>
+      </c>
+      <c r="Q56">
+        <v>25</v>
+      </c>
+      <c r="R56">
+        <v>11</v>
+      </c>
+      <c r="U56" t="s">
+        <v>30</v>
+      </c>
+      <c r="V56">
+        <v>2</v>
+      </c>
+      <c r="W56">
+        <v>15</v>
+      </c>
+      <c r="X56">
+        <v>17</v>
+      </c>
+      <c r="Y56" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z56" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA56" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB56" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>16</v>
+      </c>
+      <c r="B57">
+        <v>2021</v>
+      </c>
+      <c r="C57">
+        <v>7</v>
+      </c>
+      <c r="D57">
+        <v>10</v>
+      </c>
+      <c r="E57">
+        <v>10</v>
+      </c>
+      <c r="F57" t="s">
+        <v>26</v>
+      </c>
+      <c r="G57" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" t="s">
+        <v>28</v>
+      </c>
+      <c r="I57">
+        <v>1051</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>11</v>
+      </c>
+      <c r="M57">
+        <v>2</v>
+      </c>
+      <c r="N57">
+        <v>2</v>
+      </c>
+      <c r="O57">
+        <v>8</v>
+      </c>
+      <c r="P57">
+        <v>5</v>
+      </c>
+      <c r="Q57">
+        <v>27</v>
+      </c>
+      <c r="S57">
+        <v>7</v>
+      </c>
+      <c r="U57" t="s">
+        <v>30</v>
+      </c>
+      <c r="V57">
+        <v>2</v>
+      </c>
+      <c r="W57">
+        <v>16</v>
+      </c>
+      <c r="X57">
+        <v>18</v>
+      </c>
+      <c r="Y57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB57" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update sample size in two harris and ifop polls
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6E5352-82B0-DC4F-AD73-022D603C4E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED9EFC4-7847-7542-B5B4-8B2496172895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="18080" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -517,8 +517,8 @@
   <dimension ref="A1:AB57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="P55" sqref="P55"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4154,7 +4154,7 @@
         <v>28</v>
       </c>
       <c r="I53">
-        <v>921</v>
+        <v>701</v>
       </c>
       <c r="J53">
         <v>0.5</v>
@@ -4222,7 +4222,7 @@
         <v>28</v>
       </c>
       <c r="I54">
-        <v>921</v>
+        <v>685</v>
       </c>
       <c r="J54">
         <v>0.5</v>
@@ -4290,7 +4290,7 @@
         <v>28</v>
       </c>
       <c r="I55">
-        <v>1051</v>
+        <v>904</v>
       </c>
       <c r="J55">
         <v>1</v>
@@ -4370,7 +4370,7 @@
         <v>28</v>
       </c>
       <c r="I56">
-        <v>1051</v>
+        <v>893</v>
       </c>
       <c r="J56">
         <v>1</v>
@@ -4450,7 +4450,7 @@
         <v>28</v>
       </c>
       <c r="I57">
-        <v>1051</v>
+        <v>893</v>
       </c>
       <c r="J57">
         <v>1</v>

</xml_diff>

<commit_message>
update with bva poll (10/15)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED9EFC4-7847-7542-B5B4-8B2496172895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A819FB-74FF-9949-8402-4E40E5B57480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="18080" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>opinionway</t>
+  </si>
+  <si>
+    <t>bva</t>
   </si>
 </sst>
 </file>
@@ -514,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB57"/>
+  <dimension ref="A1:AB60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="J52" sqref="J52"/>
+      <selection pane="bottomLeft" activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4272,7 +4275,7 @@
         <v>2021</v>
       </c>
       <c r="C55">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D55">
         <v>10</v>
@@ -4352,7 +4355,7 @@
         <v>2021</v>
       </c>
       <c r="C56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D56">
         <v>10</v>
@@ -4432,7 +4435,7 @@
         <v>2021</v>
       </c>
       <c r="C57">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D57">
         <v>10</v>
@@ -4502,6 +4505,219 @@
       </c>
       <c r="AB57" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>17</v>
+      </c>
+      <c r="B58">
+        <v>2021</v>
+      </c>
+      <c r="C58">
+        <v>6</v>
+      </c>
+      <c r="D58">
+        <v>10</v>
+      </c>
+      <c r="E58">
+        <v>9</v>
+      </c>
+      <c r="F58" t="s">
+        <v>41</v>
+      </c>
+      <c r="G58" t="s">
+        <v>7</v>
+      </c>
+      <c r="H58" t="s">
+        <v>8</v>
+      </c>
+      <c r="I58">
+        <v>876</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>8</v>
+      </c>
+      <c r="M58">
+        <v>1.5</v>
+      </c>
+      <c r="N58">
+        <v>4</v>
+      </c>
+      <c r="O58">
+        <v>8</v>
+      </c>
+      <c r="P58">
+        <v>4</v>
+      </c>
+      <c r="Q58">
+        <v>27</v>
+      </c>
+      <c r="R58">
+        <v>10</v>
+      </c>
+      <c r="U58">
+        <v>1.5</v>
+      </c>
+      <c r="V58">
+        <v>2.5</v>
+      </c>
+      <c r="W58">
+        <v>17</v>
+      </c>
+      <c r="X58">
+        <v>14</v>
+      </c>
+      <c r="Y58">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>17</v>
+      </c>
+      <c r="B59">
+        <v>2021</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+      <c r="D59">
+        <v>10</v>
+      </c>
+      <c r="E59">
+        <v>9</v>
+      </c>
+      <c r="F59" t="s">
+        <v>41</v>
+      </c>
+      <c r="G59" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" t="s">
+        <v>8</v>
+      </c>
+      <c r="I59">
+        <v>879</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <v>8.5</v>
+      </c>
+      <c r="M59">
+        <v>1.5</v>
+      </c>
+      <c r="N59">
+        <v>4</v>
+      </c>
+      <c r="O59">
+        <v>8</v>
+      </c>
+      <c r="P59">
+        <v>4</v>
+      </c>
+      <c r="Q59">
+        <v>28</v>
+      </c>
+      <c r="S59">
+        <v>8.5</v>
+      </c>
+      <c r="U59">
+        <v>1.5</v>
+      </c>
+      <c r="V59">
+        <v>3</v>
+      </c>
+      <c r="W59">
+        <v>17</v>
+      </c>
+      <c r="X59">
+        <v>13</v>
+      </c>
+      <c r="Y59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>17</v>
+      </c>
+      <c r="B60">
+        <v>2021</v>
+      </c>
+      <c r="C60">
+        <v>6</v>
+      </c>
+      <c r="D60">
+        <v>10</v>
+      </c>
+      <c r="E60">
+        <v>9</v>
+      </c>
+      <c r="F60" t="s">
+        <v>41</v>
+      </c>
+      <c r="G60" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" t="s">
+        <v>8</v>
+      </c>
+      <c r="I60">
+        <v>885</v>
+      </c>
+      <c r="J60">
+        <v>0.5</v>
+      </c>
+      <c r="K60">
+        <v>1.5</v>
+      </c>
+      <c r="L60">
+        <v>8</v>
+      </c>
+      <c r="M60">
+        <v>1.5</v>
+      </c>
+      <c r="N60">
+        <v>4</v>
+      </c>
+      <c r="O60">
+        <v>8</v>
+      </c>
+      <c r="P60">
+        <v>4</v>
+      </c>
+      <c r="Q60">
+        <v>26</v>
+      </c>
+      <c r="T60">
+        <v>12</v>
+      </c>
+      <c r="U60">
+        <v>1</v>
+      </c>
+      <c r="V60">
+        <v>2.5</v>
+      </c>
+      <c r="W60">
+        <v>16</v>
+      </c>
+      <c r="X60">
+        <v>14</v>
+      </c>
+      <c r="Y60">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with odoxa and ifop polls, 10/15
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A819FB-74FF-9949-8402-4E40E5B57480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D06C56-4ABE-FB42-BD2C-6A1B6DFC02AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="18080" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB60"/>
+  <dimension ref="A1:AB66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="Z66" sqref="Z66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4720,6 +4720,399 @@
         <v>1</v>
       </c>
     </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>18</v>
+      </c>
+      <c r="B61">
+        <v>2021</v>
+      </c>
+      <c r="C61">
+        <v>7</v>
+      </c>
+      <c r="D61">
+        <v>10</v>
+      </c>
+      <c r="E61">
+        <v>11</v>
+      </c>
+      <c r="F61" t="s">
+        <v>35</v>
+      </c>
+      <c r="G61" t="s">
+        <v>7</v>
+      </c>
+      <c r="H61" t="s">
+        <v>28</v>
+      </c>
+      <c r="I61">
+        <v>3432</v>
+      </c>
+      <c r="J61">
+        <v>0.5</v>
+      </c>
+      <c r="K61">
+        <v>0.5</v>
+      </c>
+      <c r="L61">
+        <v>8</v>
+      </c>
+      <c r="M61">
+        <v>1.5</v>
+      </c>
+      <c r="N61">
+        <v>1.5</v>
+      </c>
+      <c r="O61">
+        <v>7</v>
+      </c>
+      <c r="P61">
+        <v>5</v>
+      </c>
+      <c r="Q61">
+        <v>25</v>
+      </c>
+      <c r="T61">
+        <v>15</v>
+      </c>
+      <c r="U61">
+        <v>0.5</v>
+      </c>
+      <c r="V61">
+        <v>2.5</v>
+      </c>
+      <c r="W61">
+        <v>17</v>
+      </c>
+      <c r="X61">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>18</v>
+      </c>
+      <c r="B62">
+        <v>2021</v>
+      </c>
+      <c r="C62">
+        <v>7</v>
+      </c>
+      <c r="D62">
+        <v>10</v>
+      </c>
+      <c r="E62">
+        <v>11</v>
+      </c>
+      <c r="F62" t="s">
+        <v>35</v>
+      </c>
+      <c r="G62" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I62">
+        <v>3430</v>
+      </c>
+      <c r="J62">
+        <v>0.5</v>
+      </c>
+      <c r="K62">
+        <v>0.5</v>
+      </c>
+      <c r="L62">
+        <v>8</v>
+      </c>
+      <c r="M62">
+        <v>2</v>
+      </c>
+      <c r="N62">
+        <v>2</v>
+      </c>
+      <c r="O62">
+        <v>7</v>
+      </c>
+      <c r="P62">
+        <v>5.5</v>
+      </c>
+      <c r="Q62">
+        <v>26</v>
+      </c>
+      <c r="R62">
+        <v>10</v>
+      </c>
+      <c r="U62">
+        <v>1</v>
+      </c>
+      <c r="V62">
+        <v>2.5</v>
+      </c>
+      <c r="W62">
+        <v>18</v>
+      </c>
+      <c r="X62">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>18</v>
+      </c>
+      <c r="B63">
+        <v>2021</v>
+      </c>
+      <c r="C63">
+        <v>7</v>
+      </c>
+      <c r="D63">
+        <v>10</v>
+      </c>
+      <c r="E63">
+        <v>11</v>
+      </c>
+      <c r="F63" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" t="s">
+        <v>28</v>
+      </c>
+      <c r="I63">
+        <v>3429</v>
+      </c>
+      <c r="J63">
+        <v>0.5</v>
+      </c>
+      <c r="K63">
+        <v>0.5</v>
+      </c>
+      <c r="L63">
+        <v>8</v>
+      </c>
+      <c r="M63">
+        <v>2</v>
+      </c>
+      <c r="N63">
+        <v>2</v>
+      </c>
+      <c r="O63">
+        <v>7</v>
+      </c>
+      <c r="P63">
+        <v>5.5</v>
+      </c>
+      <c r="Q63">
+        <v>27</v>
+      </c>
+      <c r="S63">
+        <v>8</v>
+      </c>
+      <c r="U63">
+        <v>1</v>
+      </c>
+      <c r="V63">
+        <v>3</v>
+      </c>
+      <c r="W63">
+        <v>18.5</v>
+      </c>
+      <c r="X63">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>19</v>
+      </c>
+      <c r="B64">
+        <v>2021</v>
+      </c>
+      <c r="C64">
+        <v>6</v>
+      </c>
+      <c r="D64">
+        <v>10</v>
+      </c>
+      <c r="E64">
+        <v>8</v>
+      </c>
+      <c r="F64" t="s">
+        <v>34</v>
+      </c>
+      <c r="G64" t="s">
+        <v>7</v>
+      </c>
+      <c r="H64" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64">
+        <v>1856</v>
+      </c>
+      <c r="J64">
+        <v>2</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>8</v>
+      </c>
+      <c r="M64">
+        <v>2</v>
+      </c>
+      <c r="N64">
+        <v>2</v>
+      </c>
+      <c r="O64">
+        <v>6.5</v>
+      </c>
+      <c r="P64">
+        <v>4.5</v>
+      </c>
+      <c r="Q64">
+        <v>25</v>
+      </c>
+      <c r="T64">
+        <v>13</v>
+      </c>
+      <c r="V64">
+        <v>2</v>
+      </c>
+      <c r="W64">
+        <v>18</v>
+      </c>
+      <c r="X64">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>19</v>
+      </c>
+      <c r="B65">
+        <v>2021</v>
+      </c>
+      <c r="C65">
+        <v>6</v>
+      </c>
+      <c r="D65">
+        <v>10</v>
+      </c>
+      <c r="E65">
+        <v>8</v>
+      </c>
+      <c r="F65" t="s">
+        <v>34</v>
+      </c>
+      <c r="G65" t="s">
+        <v>7</v>
+      </c>
+      <c r="H65" t="s">
+        <v>27</v>
+      </c>
+      <c r="I65">
+        <v>1942</v>
+      </c>
+      <c r="J65">
+        <v>2</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>9</v>
+      </c>
+      <c r="M65">
+        <v>2</v>
+      </c>
+      <c r="N65">
+        <v>2.5</v>
+      </c>
+      <c r="O65">
+        <v>7</v>
+      </c>
+      <c r="P65">
+        <v>4</v>
+      </c>
+      <c r="Q65">
+        <v>26.5</v>
+      </c>
+      <c r="R65">
+        <v>6.5</v>
+      </c>
+      <c r="V65">
+        <v>2.5</v>
+      </c>
+      <c r="W65">
+        <v>18.5</v>
+      </c>
+      <c r="X65">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>19</v>
+      </c>
+      <c r="B66">
+        <v>2021</v>
+      </c>
+      <c r="C66">
+        <v>6</v>
+      </c>
+      <c r="D66">
+        <v>10</v>
+      </c>
+      <c r="E66">
+        <v>8</v>
+      </c>
+      <c r="F66" t="s">
+        <v>34</v>
+      </c>
+      <c r="G66" t="s">
+        <v>7</v>
+      </c>
+      <c r="H66" t="s">
+        <v>27</v>
+      </c>
+      <c r="I66">
+        <v>1917</v>
+      </c>
+      <c r="J66">
+        <v>2</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="L66">
+        <v>8.5</v>
+      </c>
+      <c r="M66">
+        <v>2</v>
+      </c>
+      <c r="O66">
+        <v>11</v>
+      </c>
+      <c r="Q66">
+        <v>26</v>
+      </c>
+      <c r="T66">
+        <v>13</v>
+      </c>
+      <c r="V66">
+        <v>2.5</v>
+      </c>
+      <c r="W66">
+        <v>18</v>
+      </c>
+      <c r="X66">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update with harris poll (10/20)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D06C56-4ABE-FB42-BD2C-6A1B6DFC02AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C38D7C-C1D5-A94A-8D95-2C4DA5138BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="18080" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB66"/>
+  <dimension ref="A1:AB69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="Z66" sqref="Z66"/>
+      <selection pane="bottomLeft" activeCell="Z69" sqref="Z69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4989,7 +4989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>19</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>19</v>
       </c>
@@ -5111,6 +5111,228 @@
       </c>
       <c r="X66">
         <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>20</v>
+      </c>
+      <c r="B67">
+        <v>2021</v>
+      </c>
+      <c r="C67">
+        <v>7</v>
+      </c>
+      <c r="D67">
+        <v>10</v>
+      </c>
+      <c r="E67">
+        <v>17</v>
+      </c>
+      <c r="F67" t="s">
+        <v>26</v>
+      </c>
+      <c r="G67" t="s">
+        <v>7</v>
+      </c>
+      <c r="H67" t="s">
+        <v>28</v>
+      </c>
+      <c r="I67">
+        <v>1705</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>10</v>
+      </c>
+      <c r="M67">
+        <v>2</v>
+      </c>
+      <c r="N67">
+        <v>3</v>
+      </c>
+      <c r="O67">
+        <v>8</v>
+      </c>
+      <c r="P67">
+        <v>4</v>
+      </c>
+      <c r="Q67">
+        <v>23</v>
+      </c>
+      <c r="T67">
+        <v>14</v>
+      </c>
+      <c r="U67" t="s">
+        <v>30</v>
+      </c>
+      <c r="V67">
+        <v>1</v>
+      </c>
+      <c r="W67">
+        <v>16</v>
+      </c>
+      <c r="X67">
+        <v>17</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA67" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>20</v>
+      </c>
+      <c r="B68">
+        <v>2021</v>
+      </c>
+      <c r="C68">
+        <v>7</v>
+      </c>
+      <c r="D68">
+        <v>10</v>
+      </c>
+      <c r="E68">
+        <v>17</v>
+      </c>
+      <c r="F68" t="s">
+        <v>26</v>
+      </c>
+      <c r="G68" t="s">
+        <v>7</v>
+      </c>
+      <c r="H68" t="s">
+        <v>28</v>
+      </c>
+      <c r="I68">
+        <v>1685</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>10</v>
+      </c>
+      <c r="M68">
+        <v>2</v>
+      </c>
+      <c r="N68">
+        <v>3</v>
+      </c>
+      <c r="O68">
+        <v>9</v>
+      </c>
+      <c r="P68">
+        <v>4</v>
+      </c>
+      <c r="Q68">
+        <v>25</v>
+      </c>
+      <c r="R68">
+        <v>10</v>
+      </c>
+      <c r="U68" t="s">
+        <v>30</v>
+      </c>
+      <c r="V68">
+        <v>2</v>
+      </c>
+      <c r="W68">
+        <v>16</v>
+      </c>
+      <c r="X68">
+        <v>17</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA68" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>20</v>
+      </c>
+      <c r="B69">
+        <v>2021</v>
+      </c>
+      <c r="C69">
+        <v>7</v>
+      </c>
+      <c r="D69">
+        <v>10</v>
+      </c>
+      <c r="E69">
+        <v>17</v>
+      </c>
+      <c r="F69" t="s">
+        <v>26</v>
+      </c>
+      <c r="G69" t="s">
+        <v>7</v>
+      </c>
+      <c r="H69" t="s">
+        <v>28</v>
+      </c>
+      <c r="I69">
+        <v>1705</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>10</v>
+      </c>
+      <c r="M69">
+        <v>2</v>
+      </c>
+      <c r="N69">
+        <v>3</v>
+      </c>
+      <c r="O69">
+        <v>9</v>
+      </c>
+      <c r="P69">
+        <v>5</v>
+      </c>
+      <c r="Q69">
+        <v>25</v>
+      </c>
+      <c r="S69">
+        <v>8</v>
+      </c>
+      <c r="U69" t="s">
+        <v>30</v>
+      </c>
+      <c r="V69">
+        <v>2</v>
+      </c>
+      <c r="W69">
+        <v>16</v>
+      </c>
+      <c r="X69">
+        <v>18</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA69" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with ipsos and opinion way polls (10/22)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C38D7C-C1D5-A94A-8D95-2C4DA5138BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE504613-08E5-8B40-8E0C-0273B6756B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="18080" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB69"/>
+  <dimension ref="A1:AB82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="Z69" sqref="Z69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="T71" sqref="T71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5335,6 +5335,866 @@
         <v>30</v>
       </c>
     </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>21</v>
+      </c>
+      <c r="B70">
+        <v>2021</v>
+      </c>
+      <c r="C70">
+        <v>7</v>
+      </c>
+      <c r="D70">
+        <v>10</v>
+      </c>
+      <c r="E70">
+        <v>15</v>
+      </c>
+      <c r="F70" t="s">
+        <v>35</v>
+      </c>
+      <c r="G70" t="s">
+        <v>7</v>
+      </c>
+      <c r="H70" t="s">
+        <v>28</v>
+      </c>
+      <c r="I70">
+        <v>1182</v>
+      </c>
+      <c r="J70">
+        <v>0.5</v>
+      </c>
+      <c r="K70">
+        <v>0.5</v>
+      </c>
+      <c r="L70">
+        <v>8</v>
+      </c>
+      <c r="M70">
+        <v>2</v>
+      </c>
+      <c r="N70">
+        <v>1.5</v>
+      </c>
+      <c r="O70">
+        <v>7</v>
+      </c>
+      <c r="P70">
+        <v>6</v>
+      </c>
+      <c r="Q70">
+        <v>24</v>
+      </c>
+      <c r="T70">
+        <v>15</v>
+      </c>
+      <c r="U70">
+        <v>0.5</v>
+      </c>
+      <c r="V70">
+        <v>2</v>
+      </c>
+      <c r="W70">
+        <v>17</v>
+      </c>
+      <c r="X70">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>21</v>
+      </c>
+      <c r="B71">
+        <v>2021</v>
+      </c>
+      <c r="C71">
+        <v>7</v>
+      </c>
+      <c r="D71">
+        <v>10</v>
+      </c>
+      <c r="E71">
+        <v>15</v>
+      </c>
+      <c r="F71" t="s">
+        <v>35</v>
+      </c>
+      <c r="G71" t="s">
+        <v>7</v>
+      </c>
+      <c r="H71" t="s">
+        <v>28</v>
+      </c>
+      <c r="I71">
+        <v>1182</v>
+      </c>
+      <c r="J71">
+        <v>0.5</v>
+      </c>
+      <c r="K71">
+        <v>0.5</v>
+      </c>
+      <c r="L71">
+        <v>8</v>
+      </c>
+      <c r="M71">
+        <v>2</v>
+      </c>
+      <c r="N71">
+        <v>2</v>
+      </c>
+      <c r="O71">
+        <v>7</v>
+      </c>
+      <c r="P71">
+        <v>6</v>
+      </c>
+      <c r="Q71">
+        <v>25</v>
+      </c>
+      <c r="S71">
+        <v>10</v>
+      </c>
+      <c r="U71">
+        <v>1</v>
+      </c>
+      <c r="V71">
+        <v>3</v>
+      </c>
+      <c r="W71">
+        <v>18</v>
+      </c>
+      <c r="X71">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>21</v>
+      </c>
+      <c r="B72">
+        <v>2021</v>
+      </c>
+      <c r="C72">
+        <v>7</v>
+      </c>
+      <c r="D72">
+        <v>10</v>
+      </c>
+      <c r="E72">
+        <v>15</v>
+      </c>
+      <c r="F72" t="s">
+        <v>35</v>
+      </c>
+      <c r="G72" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" t="s">
+        <v>28</v>
+      </c>
+      <c r="I72">
+        <v>1182</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="K72">
+        <v>0.5</v>
+      </c>
+      <c r="L72">
+        <v>8.5</v>
+      </c>
+      <c r="M72">
+        <v>2.5</v>
+      </c>
+      <c r="N72">
+        <v>2</v>
+      </c>
+      <c r="O72">
+        <v>7</v>
+      </c>
+      <c r="P72">
+        <v>6.5</v>
+      </c>
+      <c r="Q72">
+        <v>24</v>
+      </c>
+      <c r="R72">
+        <v>10</v>
+      </c>
+      <c r="U72">
+        <v>1</v>
+      </c>
+      <c r="V72">
+        <v>3</v>
+      </c>
+      <c r="W72">
+        <v>17</v>
+      </c>
+      <c r="X72">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>22</v>
+      </c>
+      <c r="B73">
+        <v>2021</v>
+      </c>
+      <c r="C73">
+        <v>8</v>
+      </c>
+      <c r="D73">
+        <v>10</v>
+      </c>
+      <c r="E73">
+        <v>19</v>
+      </c>
+      <c r="F73" t="s">
+        <v>40</v>
+      </c>
+      <c r="G73" t="s">
+        <v>7</v>
+      </c>
+      <c r="H73" t="s">
+        <v>28</v>
+      </c>
+      <c r="I73">
+        <v>859</v>
+      </c>
+      <c r="J73">
+        <v>2</v>
+      </c>
+      <c r="K73">
+        <v>1</v>
+      </c>
+      <c r="L73">
+        <v>9</v>
+      </c>
+      <c r="M73">
+        <v>2</v>
+      </c>
+      <c r="N73">
+        <v>2</v>
+      </c>
+      <c r="O73">
+        <v>8</v>
+      </c>
+      <c r="P73">
+        <v>5</v>
+      </c>
+      <c r="Q73">
+        <v>26</v>
+      </c>
+      <c r="T73">
+        <v>9</v>
+      </c>
+      <c r="V73">
+        <v>4</v>
+      </c>
+      <c r="W73">
+        <v>19</v>
+      </c>
+      <c r="X73">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>22</v>
+      </c>
+      <c r="B74">
+        <v>2021</v>
+      </c>
+      <c r="C74">
+        <v>8</v>
+      </c>
+      <c r="D74">
+        <v>10</v>
+      </c>
+      <c r="E74">
+        <v>19</v>
+      </c>
+      <c r="F74" t="s">
+        <v>40</v>
+      </c>
+      <c r="G74" t="s">
+        <v>7</v>
+      </c>
+      <c r="H74" t="s">
+        <v>28</v>
+      </c>
+      <c r="I74">
+        <v>838</v>
+      </c>
+      <c r="J74">
+        <v>2</v>
+      </c>
+      <c r="K74" t="s">
+        <v>37</v>
+      </c>
+      <c r="L74">
+        <v>10</v>
+      </c>
+      <c r="M74">
+        <v>2</v>
+      </c>
+      <c r="N74">
+        <v>3</v>
+      </c>
+      <c r="O74">
+        <v>9</v>
+      </c>
+      <c r="P74">
+        <v>5</v>
+      </c>
+      <c r="Q74">
+        <v>26</v>
+      </c>
+      <c r="R74">
+        <v>6</v>
+      </c>
+      <c r="V74">
+        <v>4</v>
+      </c>
+      <c r="W74">
+        <v>19</v>
+      </c>
+      <c r="X74">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>22</v>
+      </c>
+      <c r="B75">
+        <v>2021</v>
+      </c>
+      <c r="C75">
+        <v>8</v>
+      </c>
+      <c r="D75">
+        <v>10</v>
+      </c>
+      <c r="E75">
+        <v>19</v>
+      </c>
+      <c r="F75" t="s">
+        <v>40</v>
+      </c>
+      <c r="G75" t="s">
+        <v>7</v>
+      </c>
+      <c r="H75" t="s">
+        <v>28</v>
+      </c>
+      <c r="I75">
+        <v>859</v>
+      </c>
+      <c r="J75">
+        <v>2</v>
+      </c>
+      <c r="K75">
+        <v>1</v>
+      </c>
+      <c r="L75">
+        <v>9</v>
+      </c>
+      <c r="M75">
+        <v>2</v>
+      </c>
+      <c r="N75">
+        <v>2</v>
+      </c>
+      <c r="O75">
+        <v>8</v>
+      </c>
+      <c r="P75">
+        <v>6</v>
+      </c>
+      <c r="Q75">
+        <v>26</v>
+      </c>
+      <c r="S75">
+        <v>7</v>
+      </c>
+      <c r="V75">
+        <v>4</v>
+      </c>
+      <c r="W75">
+        <v>20</v>
+      </c>
+      <c r="X75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>22</v>
+      </c>
+      <c r="B76">
+        <v>2021</v>
+      </c>
+      <c r="C76">
+        <v>8</v>
+      </c>
+      <c r="D76">
+        <v>10</v>
+      </c>
+      <c r="E76">
+        <v>19</v>
+      </c>
+      <c r="F76" t="s">
+        <v>40</v>
+      </c>
+      <c r="G76" t="s">
+        <v>7</v>
+      </c>
+      <c r="H76" t="s">
+        <v>28</v>
+      </c>
+      <c r="I76">
+        <v>838</v>
+      </c>
+      <c r="J76">
+        <v>2</v>
+      </c>
+      <c r="K76" t="s">
+        <v>37</v>
+      </c>
+      <c r="L76">
+        <v>10</v>
+      </c>
+      <c r="M76">
+        <v>2</v>
+      </c>
+      <c r="N76">
+        <v>3</v>
+      </c>
+      <c r="O76">
+        <v>8</v>
+      </c>
+      <c r="P76">
+        <v>5</v>
+      </c>
+      <c r="Q76">
+        <v>26</v>
+      </c>
+      <c r="T76">
+        <v>10</v>
+      </c>
+      <c r="V76">
+        <v>6</v>
+      </c>
+      <c r="W76">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>23</v>
+      </c>
+      <c r="B77">
+        <v>2021</v>
+      </c>
+      <c r="C77">
+        <v>6</v>
+      </c>
+      <c r="D77">
+        <v>10</v>
+      </c>
+      <c r="E77">
+        <v>10</v>
+      </c>
+      <c r="F77" t="s">
+        <v>6</v>
+      </c>
+      <c r="G77" t="s">
+        <v>7</v>
+      </c>
+      <c r="H77" t="s">
+        <v>8</v>
+      </c>
+      <c r="I77">
+        <v>8888</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77">
+        <v>1</v>
+      </c>
+      <c r="L77">
+        <v>8</v>
+      </c>
+      <c r="M77">
+        <v>2</v>
+      </c>
+      <c r="N77">
+        <v>2</v>
+      </c>
+      <c r="O77">
+        <v>9</v>
+      </c>
+      <c r="P77">
+        <v>5</v>
+      </c>
+      <c r="Q77">
+        <v>24</v>
+      </c>
+      <c r="T77">
+        <v>13</v>
+      </c>
+      <c r="U77">
+        <v>1</v>
+      </c>
+      <c r="V77">
+        <v>3</v>
+      </c>
+      <c r="W77">
+        <v>15</v>
+      </c>
+      <c r="X77">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>23</v>
+      </c>
+      <c r="B78">
+        <v>2021</v>
+      </c>
+      <c r="C78">
+        <v>6</v>
+      </c>
+      <c r="D78">
+        <v>10</v>
+      </c>
+      <c r="E78">
+        <v>10</v>
+      </c>
+      <c r="F78" t="s">
+        <v>6</v>
+      </c>
+      <c r="G78" t="s">
+        <v>7</v>
+      </c>
+      <c r="H78" t="s">
+        <v>8</v>
+      </c>
+      <c r="I78">
+        <v>8796</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="K78">
+        <v>1</v>
+      </c>
+      <c r="L78">
+        <v>8</v>
+      </c>
+      <c r="M78">
+        <v>2</v>
+      </c>
+      <c r="N78">
+        <v>2</v>
+      </c>
+      <c r="O78">
+        <v>9.5</v>
+      </c>
+      <c r="P78">
+        <v>5</v>
+      </c>
+      <c r="Q78">
+        <v>25.5</v>
+      </c>
+      <c r="R78">
+        <v>10</v>
+      </c>
+      <c r="U78">
+        <v>1</v>
+      </c>
+      <c r="V78">
+        <v>3</v>
+      </c>
+      <c r="W78">
+        <v>16</v>
+      </c>
+      <c r="X78">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>23</v>
+      </c>
+      <c r="B79">
+        <v>2021</v>
+      </c>
+      <c r="C79">
+        <v>6</v>
+      </c>
+      <c r="D79">
+        <v>10</v>
+      </c>
+      <c r="E79">
+        <v>10</v>
+      </c>
+      <c r="F79" t="s">
+        <v>6</v>
+      </c>
+      <c r="G79" t="s">
+        <v>7</v>
+      </c>
+      <c r="H79" t="s">
+        <v>8</v>
+      </c>
+      <c r="I79">
+        <v>8714</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>8</v>
+      </c>
+      <c r="M79">
+        <v>2</v>
+      </c>
+      <c r="N79">
+        <v>2</v>
+      </c>
+      <c r="O79">
+        <v>9.5</v>
+      </c>
+      <c r="P79">
+        <v>5</v>
+      </c>
+      <c r="Q79">
+        <v>26</v>
+      </c>
+      <c r="S79">
+        <v>9</v>
+      </c>
+      <c r="U79">
+        <v>1</v>
+      </c>
+      <c r="V79">
+        <v>3</v>
+      </c>
+      <c r="W79">
+        <v>16</v>
+      </c>
+      <c r="X79">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>23</v>
+      </c>
+      <c r="B80">
+        <v>2021</v>
+      </c>
+      <c r="C80">
+        <v>6</v>
+      </c>
+      <c r="D80">
+        <v>10</v>
+      </c>
+      <c r="E80">
+        <v>10</v>
+      </c>
+      <c r="F80" t="s">
+        <v>6</v>
+      </c>
+      <c r="G80" t="s">
+        <v>7</v>
+      </c>
+      <c r="H80" t="s">
+        <v>8</v>
+      </c>
+      <c r="I80">
+        <v>8698</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>8</v>
+      </c>
+      <c r="M80">
+        <v>2</v>
+      </c>
+      <c r="N80">
+        <v>2</v>
+      </c>
+      <c r="O80">
+        <v>9.5</v>
+      </c>
+      <c r="P80">
+        <v>5</v>
+      </c>
+      <c r="Q80">
+        <v>26</v>
+      </c>
+      <c r="T80">
+        <v>16</v>
+      </c>
+      <c r="U80">
+        <v>1</v>
+      </c>
+      <c r="V80">
+        <v>4.5</v>
+      </c>
+      <c r="W80">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>23</v>
+      </c>
+      <c r="B81">
+        <v>2021</v>
+      </c>
+      <c r="C81">
+        <v>6</v>
+      </c>
+      <c r="D81">
+        <v>10</v>
+      </c>
+      <c r="E81">
+        <v>10</v>
+      </c>
+      <c r="F81" t="s">
+        <v>6</v>
+      </c>
+      <c r="G81" t="s">
+        <v>7</v>
+      </c>
+      <c r="H81" t="s">
+        <v>8</v>
+      </c>
+      <c r="I81">
+        <v>8541</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>8</v>
+      </c>
+      <c r="M81">
+        <v>2</v>
+      </c>
+      <c r="N81">
+        <v>2</v>
+      </c>
+      <c r="O81">
+        <v>10</v>
+      </c>
+      <c r="P81">
+        <v>5</v>
+      </c>
+      <c r="Q81">
+        <v>27</v>
+      </c>
+      <c r="R81">
+        <v>13</v>
+      </c>
+      <c r="U81">
+        <v>1</v>
+      </c>
+      <c r="V81">
+        <v>5</v>
+      </c>
+      <c r="W81">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>23</v>
+      </c>
+      <c r="B82">
+        <v>2021</v>
+      </c>
+      <c r="C82">
+        <v>6</v>
+      </c>
+      <c r="D82">
+        <v>10</v>
+      </c>
+      <c r="E82">
+        <v>10</v>
+      </c>
+      <c r="F82" t="s">
+        <v>6</v>
+      </c>
+      <c r="G82" t="s">
+        <v>7</v>
+      </c>
+      <c r="H82" t="s">
+        <v>8</v>
+      </c>
+      <c r="I82">
+        <v>8541</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82">
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <v>8</v>
+      </c>
+      <c r="M82">
+        <v>2</v>
+      </c>
+      <c r="N82">
+        <v>2</v>
+      </c>
+      <c r="O82">
+        <v>10</v>
+      </c>
+      <c r="P82">
+        <v>5</v>
+      </c>
+      <c r="Q82">
+        <v>28</v>
+      </c>
+      <c r="S82">
+        <v>12</v>
+      </c>
+      <c r="U82">
+        <v>1</v>
+      </c>
+      <c r="V82">
+        <v>5</v>
+      </c>
+      <c r="W82">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update w/ harris poll (11/3)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B9ACAE-1B93-6B4F-A1DF-40039715404A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF781EF-834B-7244-A3E3-F6195458D5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3080" yWindow="18600" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB92"/>
+  <dimension ref="A1:AB95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AB90" sqref="AB90"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="Q92" sqref="Q92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6923,6 +6923,237 @@
         <v>1</v>
       </c>
     </row>
+    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>27</v>
+      </c>
+      <c r="B93">
+        <v>2021</v>
+      </c>
+      <c r="C93">
+        <v>9</v>
+      </c>
+      <c r="D93">
+        <v>10</v>
+      </c>
+      <c r="E93">
+        <v>29</v>
+      </c>
+      <c r="F93" t="s">
+        <v>26</v>
+      </c>
+      <c r="G93" t="s">
+        <v>7</v>
+      </c>
+      <c r="H93" t="s">
+        <v>28</v>
+      </c>
+      <c r="I93">
+        <v>1762</v>
+      </c>
+      <c r="J93">
+        <v>1</v>
+      </c>
+      <c r="K93">
+        <v>1</v>
+      </c>
+      <c r="L93">
+        <v>10</v>
+      </c>
+      <c r="M93">
+        <v>2</v>
+      </c>
+      <c r="N93">
+        <v>2</v>
+      </c>
+      <c r="O93">
+        <v>8</v>
+      </c>
+      <c r="P93">
+        <v>5</v>
+      </c>
+      <c r="Q93">
+        <v>23</v>
+      </c>
+      <c r="T93">
+        <v>14</v>
+      </c>
+      <c r="U93" t="s">
+        <v>30</v>
+      </c>
+      <c r="V93">
+        <v>1</v>
+      </c>
+      <c r="W93">
+        <v>15</v>
+      </c>
+      <c r="X93">
+        <v>17</v>
+      </c>
+      <c r="Y93" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA93">
+        <v>1</v>
+      </c>
+      <c r="AB93" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>27</v>
+      </c>
+      <c r="B94">
+        <v>2021</v>
+      </c>
+      <c r="C94">
+        <v>9</v>
+      </c>
+      <c r="D94">
+        <v>10</v>
+      </c>
+      <c r="E94">
+        <v>29</v>
+      </c>
+      <c r="F94" t="s">
+        <v>26</v>
+      </c>
+      <c r="G94" t="s">
+        <v>7</v>
+      </c>
+      <c r="H94" t="s">
+        <v>28</v>
+      </c>
+      <c r="I94">
+        <v>1723</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+      <c r="K94">
+        <v>1</v>
+      </c>
+      <c r="L94">
+        <v>10</v>
+      </c>
+      <c r="M94">
+        <v>2</v>
+      </c>
+      <c r="N94">
+        <v>2</v>
+      </c>
+      <c r="O94">
+        <v>9</v>
+      </c>
+      <c r="P94">
+        <v>5</v>
+      </c>
+      <c r="Q94">
+        <v>24</v>
+      </c>
+      <c r="R94">
+        <v>10</v>
+      </c>
+      <c r="U94" t="s">
+        <v>30</v>
+      </c>
+      <c r="V94">
+        <v>2</v>
+      </c>
+      <c r="W94">
+        <v>16</v>
+      </c>
+      <c r="X94">
+        <v>17</v>
+      </c>
+      <c r="Y94" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA94">
+        <v>1</v>
+      </c>
+      <c r="AB94" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>27</v>
+      </c>
+      <c r="B95">
+        <v>2021</v>
+      </c>
+      <c r="C95">
+        <v>9</v>
+      </c>
+      <c r="D95">
+        <v>10</v>
+      </c>
+      <c r="E95">
+        <v>29</v>
+      </c>
+      <c r="F95" t="s">
+        <v>26</v>
+      </c>
+      <c r="G95" t="s">
+        <v>7</v>
+      </c>
+      <c r="H95" t="s">
+        <v>28</v>
+      </c>
+      <c r="I95">
+        <v>1703</v>
+      </c>
+      <c r="J95">
+        <v>1</v>
+      </c>
+      <c r="K95">
+        <v>1</v>
+      </c>
+      <c r="L95">
+        <v>10</v>
+      </c>
+      <c r="M95">
+        <v>2</v>
+      </c>
+      <c r="N95">
+        <v>2</v>
+      </c>
+      <c r="O95">
+        <v>9</v>
+      </c>
+      <c r="P95">
+        <v>5</v>
+      </c>
+      <c r="Q95">
+        <v>24</v>
+      </c>
+      <c r="S95">
+        <v>9</v>
+      </c>
+      <c r="U95" t="s">
+        <v>30</v>
+      </c>
+      <c r="V95">
+        <v>2</v>
+      </c>
+      <c r="W95">
+        <v>16</v>
+      </c>
+      <c r="X95">
+        <v>18</v>
+      </c>
+      <c r="Y95" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA95">
+        <v>1</v>
+      </c>
+      <c r="AB95" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update with ifop poll (11/8)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF781EF-834B-7244-A3E3-F6195458D5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B845CFCB-7D96-1D4A-88A8-7A6369A43B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3080" yWindow="18600" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB95"/>
+  <dimension ref="A1:AB98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="Q92" sqref="Q92"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="U99" sqref="U99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7154,6 +7154,210 @@
         <v>30</v>
       </c>
     </row>
+    <row r="96" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>28</v>
+      </c>
+      <c r="B96">
+        <v>2021</v>
+      </c>
+      <c r="C96">
+        <v>10</v>
+      </c>
+      <c r="D96">
+        <v>11</v>
+      </c>
+      <c r="E96">
+        <v>4</v>
+      </c>
+      <c r="F96" t="s">
+        <v>35</v>
+      </c>
+      <c r="G96" t="s">
+        <v>7</v>
+      </c>
+      <c r="H96" t="s">
+        <v>28</v>
+      </c>
+      <c r="I96">
+        <v>1368</v>
+      </c>
+      <c r="J96">
+        <v>0.5</v>
+      </c>
+      <c r="K96">
+        <v>0.5</v>
+      </c>
+      <c r="L96">
+        <v>8.5</v>
+      </c>
+      <c r="M96">
+        <v>2</v>
+      </c>
+      <c r="N96">
+        <v>2.5</v>
+      </c>
+      <c r="O96">
+        <v>7</v>
+      </c>
+      <c r="P96">
+        <v>5</v>
+      </c>
+      <c r="Q96">
+        <v>25</v>
+      </c>
+      <c r="T96">
+        <v>13</v>
+      </c>
+      <c r="U96">
+        <v>0.5</v>
+      </c>
+      <c r="V96">
+        <v>2.5</v>
+      </c>
+      <c r="W96">
+        <v>16</v>
+      </c>
+      <c r="X96">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>28</v>
+      </c>
+      <c r="B97">
+        <v>2021</v>
+      </c>
+      <c r="C97">
+        <v>10</v>
+      </c>
+      <c r="D97">
+        <v>11</v>
+      </c>
+      <c r="E97">
+        <v>4</v>
+      </c>
+      <c r="F97" t="s">
+        <v>35</v>
+      </c>
+      <c r="G97" t="s">
+        <v>7</v>
+      </c>
+      <c r="H97" t="s">
+        <v>28</v>
+      </c>
+      <c r="I97">
+        <v>1368</v>
+      </c>
+      <c r="J97">
+        <v>1</v>
+      </c>
+      <c r="K97">
+        <v>0.5</v>
+      </c>
+      <c r="L97">
+        <v>8</v>
+      </c>
+      <c r="M97">
+        <v>2.5</v>
+      </c>
+      <c r="N97">
+        <v>3</v>
+      </c>
+      <c r="O97">
+        <v>7</v>
+      </c>
+      <c r="P97">
+        <v>6</v>
+      </c>
+      <c r="Q97">
+        <v>25</v>
+      </c>
+      <c r="S97">
+        <v>10</v>
+      </c>
+      <c r="U97">
+        <v>0.5</v>
+      </c>
+      <c r="V97">
+        <v>3</v>
+      </c>
+      <c r="W97">
+        <v>17</v>
+      </c>
+      <c r="X97">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>28</v>
+      </c>
+      <c r="B98">
+        <v>2021</v>
+      </c>
+      <c r="C98">
+        <v>10</v>
+      </c>
+      <c r="D98">
+        <v>11</v>
+      </c>
+      <c r="E98">
+        <v>4</v>
+      </c>
+      <c r="F98" t="s">
+        <v>35</v>
+      </c>
+      <c r="G98" t="s">
+        <v>7</v>
+      </c>
+      <c r="H98" t="s">
+        <v>28</v>
+      </c>
+      <c r="I98">
+        <v>1368</v>
+      </c>
+      <c r="J98">
+        <v>1</v>
+      </c>
+      <c r="K98">
+        <v>0.5</v>
+      </c>
+      <c r="L98">
+        <v>8</v>
+      </c>
+      <c r="M98">
+        <v>2</v>
+      </c>
+      <c r="N98">
+        <v>3</v>
+      </c>
+      <c r="O98">
+        <v>7</v>
+      </c>
+      <c r="P98">
+        <v>6</v>
+      </c>
+      <c r="Q98">
+        <v>26</v>
+      </c>
+      <c r="R98">
+        <v>9</v>
+      </c>
+      <c r="U98">
+        <v>1</v>
+      </c>
+      <c r="V98">
+        <v>3.5</v>
+      </c>
+      <c r="W98">
+        <v>16.5</v>
+      </c>
+      <c r="X98">
+        <v>16.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add harris poll (11/9)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B845CFCB-7D96-1D4A-88A8-7A6369A43B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC4EBEE-22EF-4547-A529-3CDB88465638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="18600" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="15900" yWindow="19240" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB98"/>
+  <dimension ref="A1:AB101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="U99" sqref="U99"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AB101" sqref="AB101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7222,7 +7222,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>28</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>28</v>
       </c>
@@ -7356,6 +7356,237 @@
       </c>
       <c r="X98">
         <v>16.5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>29</v>
+      </c>
+      <c r="B99">
+        <v>2021</v>
+      </c>
+      <c r="C99">
+        <v>10</v>
+      </c>
+      <c r="D99">
+        <v>11</v>
+      </c>
+      <c r="E99">
+        <v>7</v>
+      </c>
+      <c r="F99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G99" t="s">
+        <v>7</v>
+      </c>
+      <c r="H99" t="s">
+        <v>28</v>
+      </c>
+      <c r="I99">
+        <v>2001</v>
+      </c>
+      <c r="J99">
+        <v>1</v>
+      </c>
+      <c r="K99">
+        <v>1</v>
+      </c>
+      <c r="L99">
+        <v>10</v>
+      </c>
+      <c r="M99">
+        <v>2</v>
+      </c>
+      <c r="N99">
+        <v>2</v>
+      </c>
+      <c r="O99">
+        <v>8</v>
+      </c>
+      <c r="P99">
+        <v>4</v>
+      </c>
+      <c r="Q99">
+        <v>23</v>
+      </c>
+      <c r="T99">
+        <v>14</v>
+      </c>
+      <c r="U99" t="s">
+        <v>30</v>
+      </c>
+      <c r="V99">
+        <v>1</v>
+      </c>
+      <c r="W99">
+        <v>15</v>
+      </c>
+      <c r="X99">
+        <v>18</v>
+      </c>
+      <c r="Y99" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA99">
+        <v>1</v>
+      </c>
+      <c r="AB99" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>29</v>
+      </c>
+      <c r="B100">
+        <v>2021</v>
+      </c>
+      <c r="C100">
+        <v>10</v>
+      </c>
+      <c r="D100">
+        <v>11</v>
+      </c>
+      <c r="E100">
+        <v>7</v>
+      </c>
+      <c r="F100" t="s">
+        <v>26</v>
+      </c>
+      <c r="G100" t="s">
+        <v>7</v>
+      </c>
+      <c r="H100" t="s">
+        <v>28</v>
+      </c>
+      <c r="I100">
+        <v>2001</v>
+      </c>
+      <c r="J100">
+        <v>1</v>
+      </c>
+      <c r="K100">
+        <v>1</v>
+      </c>
+      <c r="L100">
+        <v>10</v>
+      </c>
+      <c r="M100">
+        <v>2</v>
+      </c>
+      <c r="N100">
+        <v>2</v>
+      </c>
+      <c r="O100">
+        <v>9</v>
+      </c>
+      <c r="P100">
+        <v>4</v>
+      </c>
+      <c r="Q100">
+        <v>24</v>
+      </c>
+      <c r="R100">
+        <v>10</v>
+      </c>
+      <c r="U100" t="s">
+        <v>30</v>
+      </c>
+      <c r="V100">
+        <v>2</v>
+      </c>
+      <c r="W100">
+        <v>16</v>
+      </c>
+      <c r="X100">
+        <v>18</v>
+      </c>
+      <c r="Y100" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA100">
+        <v>1</v>
+      </c>
+      <c r="AB100" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>29</v>
+      </c>
+      <c r="B101">
+        <v>2021</v>
+      </c>
+      <c r="C101">
+        <v>10</v>
+      </c>
+      <c r="D101">
+        <v>11</v>
+      </c>
+      <c r="E101">
+        <v>7</v>
+      </c>
+      <c r="F101" t="s">
+        <v>26</v>
+      </c>
+      <c r="G101" t="s">
+        <v>7</v>
+      </c>
+      <c r="H101" t="s">
+        <v>28</v>
+      </c>
+      <c r="I101">
+        <v>2001</v>
+      </c>
+      <c r="J101">
+        <v>1</v>
+      </c>
+      <c r="K101">
+        <v>1</v>
+      </c>
+      <c r="L101">
+        <v>10</v>
+      </c>
+      <c r="M101">
+        <v>2</v>
+      </c>
+      <c r="N101">
+        <v>2</v>
+      </c>
+      <c r="O101">
+        <v>9</v>
+      </c>
+      <c r="P101">
+        <v>4</v>
+      </c>
+      <c r="Q101">
+        <v>24</v>
+      </c>
+      <c r="S101">
+        <v>10</v>
+      </c>
+      <c r="U101" t="s">
+        <v>30</v>
+      </c>
+      <c r="V101">
+        <v>2</v>
+      </c>
+      <c r="W101">
+        <v>15</v>
+      </c>
+      <c r="X101">
+        <v>19</v>
+      </c>
+      <c r="Y101" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA101">
+        <v>1</v>
+      </c>
+      <c r="AB101" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add odoxa poll (11/11)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC4EBEE-22EF-4547-A529-3CDB88465638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFB3B98-5A43-AF42-AB82-F6C452FF7519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15900" yWindow="19240" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="2940" yWindow="17240" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB101"/>
+  <dimension ref="A1:AB104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AB101" sqref="AB101"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="U104" sqref="U104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7589,6 +7589,210 @@
         <v>30</v>
       </c>
     </row>
+    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>30</v>
+      </c>
+      <c r="B102">
+        <v>2021</v>
+      </c>
+      <c r="C102">
+        <v>10</v>
+      </c>
+      <c r="D102">
+        <v>11</v>
+      </c>
+      <c r="E102">
+        <v>7</v>
+      </c>
+      <c r="F102" t="s">
+        <v>34</v>
+      </c>
+      <c r="G102" t="s">
+        <v>7</v>
+      </c>
+      <c r="H102" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102">
+        <v>1917</v>
+      </c>
+      <c r="J102">
+        <v>2</v>
+      </c>
+      <c r="K102">
+        <v>1</v>
+      </c>
+      <c r="L102">
+        <v>8.5</v>
+      </c>
+      <c r="M102">
+        <v>2</v>
+      </c>
+      <c r="N102">
+        <v>2</v>
+      </c>
+      <c r="O102">
+        <v>6.5</v>
+      </c>
+      <c r="P102">
+        <v>4.5</v>
+      </c>
+      <c r="Q102">
+        <v>25</v>
+      </c>
+      <c r="T102">
+        <v>12</v>
+      </c>
+      <c r="U102">
+        <v>1.5</v>
+      </c>
+      <c r="V102">
+        <v>3</v>
+      </c>
+      <c r="W102">
+        <v>18</v>
+      </c>
+      <c r="X102">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>30</v>
+      </c>
+      <c r="B103">
+        <v>2021</v>
+      </c>
+      <c r="C103">
+        <v>10</v>
+      </c>
+      <c r="D103">
+        <v>11</v>
+      </c>
+      <c r="E103">
+        <v>7</v>
+      </c>
+      <c r="F103" t="s">
+        <v>34</v>
+      </c>
+      <c r="G103" t="s">
+        <v>7</v>
+      </c>
+      <c r="H103" t="s">
+        <v>27</v>
+      </c>
+      <c r="I103">
+        <v>1946</v>
+      </c>
+      <c r="J103">
+        <v>2.5</v>
+      </c>
+      <c r="K103">
+        <v>1</v>
+      </c>
+      <c r="L103">
+        <v>8.5</v>
+      </c>
+      <c r="M103">
+        <v>2</v>
+      </c>
+      <c r="N103">
+        <v>2</v>
+      </c>
+      <c r="O103">
+        <v>6.5</v>
+      </c>
+      <c r="P103">
+        <v>5</v>
+      </c>
+      <c r="Q103">
+        <v>25</v>
+      </c>
+      <c r="R103">
+        <v>9</v>
+      </c>
+      <c r="U103">
+        <v>1.5</v>
+      </c>
+      <c r="V103">
+        <v>4</v>
+      </c>
+      <c r="W103">
+        <v>18.5</v>
+      </c>
+      <c r="X103">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>30</v>
+      </c>
+      <c r="B104">
+        <v>2021</v>
+      </c>
+      <c r="C104">
+        <v>10</v>
+      </c>
+      <c r="D104">
+        <v>11</v>
+      </c>
+      <c r="E104">
+        <v>7</v>
+      </c>
+      <c r="F104" t="s">
+        <v>34</v>
+      </c>
+      <c r="G104" t="s">
+        <v>7</v>
+      </c>
+      <c r="H104" t="s">
+        <v>27</v>
+      </c>
+      <c r="I104">
+        <v>1917</v>
+      </c>
+      <c r="J104">
+        <v>2</v>
+      </c>
+      <c r="K104">
+        <v>1</v>
+      </c>
+      <c r="L104">
+        <v>9</v>
+      </c>
+      <c r="M104">
+        <v>2</v>
+      </c>
+      <c r="N104">
+        <v>2.5</v>
+      </c>
+      <c r="O104">
+        <v>7</v>
+      </c>
+      <c r="P104">
+        <v>5</v>
+      </c>
+      <c r="Q104">
+        <v>25</v>
+      </c>
+      <c r="S104">
+        <v>9</v>
+      </c>
+      <c r="U104">
+        <v>1</v>
+      </c>
+      <c r="V104">
+        <v>3</v>
+      </c>
+      <c r="W104">
+        <v>19</v>
+      </c>
+      <c r="X104">
+        <v>14.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add elabe poll (11/11)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFB3B98-5A43-AF42-AB82-F6C452FF7519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9261E743-F4FC-D641-AFD8-C0AC22836301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="17240" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="2840" yWindow="17380" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB104"/>
+  <dimension ref="A1:AB107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="U104" sqref="U104"/>
+      <selection pane="bottomLeft" activeCell="AA108" sqref="AA108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7793,6 +7793,237 @@
         <v>14.5</v>
       </c>
     </row>
+    <row r="105" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>31</v>
+      </c>
+      <c r="B105">
+        <v>2021</v>
+      </c>
+      <c r="C105">
+        <v>11</v>
+      </c>
+      <c r="D105">
+        <v>11</v>
+      </c>
+      <c r="E105">
+        <v>11</v>
+      </c>
+      <c r="F105" t="s">
+        <v>36</v>
+      </c>
+      <c r="G105" t="s">
+        <v>7</v>
+      </c>
+      <c r="H105" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105">
+        <v>933</v>
+      </c>
+      <c r="J105">
+        <v>2</v>
+      </c>
+      <c r="K105">
+        <v>1</v>
+      </c>
+      <c r="L105">
+        <v>8</v>
+      </c>
+      <c r="M105">
+        <v>2</v>
+      </c>
+      <c r="N105">
+        <v>2</v>
+      </c>
+      <c r="O105">
+        <v>7</v>
+      </c>
+      <c r="P105">
+        <v>5</v>
+      </c>
+      <c r="Q105">
+        <v>25</v>
+      </c>
+      <c r="T105">
+        <v>13</v>
+      </c>
+      <c r="U105">
+        <v>1</v>
+      </c>
+      <c r="V105">
+        <v>2</v>
+      </c>
+      <c r="W105">
+        <v>17</v>
+      </c>
+      <c r="X105">
+        <v>14</v>
+      </c>
+      <c r="Y105">
+        <v>0.5</v>
+      </c>
+      <c r="Z105" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA105">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>31</v>
+      </c>
+      <c r="B106">
+        <v>2021</v>
+      </c>
+      <c r="C106">
+        <v>11</v>
+      </c>
+      <c r="D106">
+        <v>11</v>
+      </c>
+      <c r="E106">
+        <v>11</v>
+      </c>
+      <c r="F106" t="s">
+        <v>36</v>
+      </c>
+      <c r="G106" t="s">
+        <v>7</v>
+      </c>
+      <c r="H106" t="s">
+        <v>27</v>
+      </c>
+      <c r="I106">
+        <v>919</v>
+      </c>
+      <c r="J106">
+        <v>2</v>
+      </c>
+      <c r="K106">
+        <v>1</v>
+      </c>
+      <c r="L106">
+        <v>8</v>
+      </c>
+      <c r="M106">
+        <v>2</v>
+      </c>
+      <c r="N106">
+        <v>2</v>
+      </c>
+      <c r="O106">
+        <v>7</v>
+      </c>
+      <c r="P106">
+        <v>5</v>
+      </c>
+      <c r="Q106">
+        <v>27</v>
+      </c>
+      <c r="R106">
+        <v>11</v>
+      </c>
+      <c r="U106">
+        <v>0.5</v>
+      </c>
+      <c r="V106">
+        <v>2</v>
+      </c>
+      <c r="W106">
+        <v>18</v>
+      </c>
+      <c r="X106">
+        <v>14</v>
+      </c>
+      <c r="Y106" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z106" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA106">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>31</v>
+      </c>
+      <c r="B107">
+        <v>2021</v>
+      </c>
+      <c r="C107">
+        <v>11</v>
+      </c>
+      <c r="D107">
+        <v>11</v>
+      </c>
+      <c r="E107">
+        <v>11</v>
+      </c>
+      <c r="F107" t="s">
+        <v>36</v>
+      </c>
+      <c r="G107" t="s">
+        <v>7</v>
+      </c>
+      <c r="H107" t="s">
+        <v>27</v>
+      </c>
+      <c r="I107">
+        <v>933</v>
+      </c>
+      <c r="J107">
+        <v>2</v>
+      </c>
+      <c r="K107">
+        <v>1</v>
+      </c>
+      <c r="L107">
+        <v>8</v>
+      </c>
+      <c r="M107">
+        <v>2</v>
+      </c>
+      <c r="N107">
+        <v>2</v>
+      </c>
+      <c r="O107">
+        <v>8</v>
+      </c>
+      <c r="P107">
+        <v>5</v>
+      </c>
+      <c r="Q107">
+        <v>28</v>
+      </c>
+      <c r="S107">
+        <v>9</v>
+      </c>
+      <c r="U107">
+        <v>1</v>
+      </c>
+      <c r="V107">
+        <v>2</v>
+      </c>
+      <c r="W107">
+        <v>18</v>
+      </c>
+      <c r="X107">
+        <v>13</v>
+      </c>
+      <c r="Y107">
+        <v>0.5</v>
+      </c>
+      <c r="Z107" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA107">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adjust sample size for harris, odoxa, elabe, and ifop latest polls
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9261E743-F4FC-D641-AFD8-C0AC22836301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C39181-6BDC-E349-ABC9-13F6F7953B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="17380" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="3680" yWindow="18240" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -520,8 +520,8 @@
   <dimension ref="A1:AB107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AA108" sqref="AA108"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="I105" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7180,7 +7180,7 @@
         <v>28</v>
       </c>
       <c r="I96">
-        <v>1368</v>
+        <v>988</v>
       </c>
       <c r="J96">
         <v>0.5</v>
@@ -7248,7 +7248,7 @@
         <v>28</v>
       </c>
       <c r="I97">
-        <v>1368</v>
+        <v>978</v>
       </c>
       <c r="J97">
         <v>1</v>
@@ -7316,7 +7316,7 @@
         <v>28</v>
       </c>
       <c r="I98">
-        <v>1368</v>
+        <v>986</v>
       </c>
       <c r="J98">
         <v>1</v>
@@ -7384,7 +7384,7 @@
         <v>28</v>
       </c>
       <c r="I99">
-        <v>2001</v>
+        <v>1721</v>
       </c>
       <c r="J99">
         <v>1</v>
@@ -7461,7 +7461,7 @@
         <v>28</v>
       </c>
       <c r="I100">
-        <v>2001</v>
+        <v>1721</v>
       </c>
       <c r="J100">
         <v>1</v>
@@ -7538,7 +7538,7 @@
         <v>28</v>
       </c>
       <c r="I101">
-        <v>2001</v>
+        <v>1721</v>
       </c>
       <c r="J101">
         <v>1</v>
@@ -7615,7 +7615,7 @@
         <v>27</v>
       </c>
       <c r="I102">
-        <v>1917</v>
+        <v>1946</v>
       </c>
       <c r="J102">
         <v>2</v>
@@ -7683,7 +7683,7 @@
         <v>27</v>
       </c>
       <c r="I103">
-        <v>1946</v>
+        <v>1917</v>
       </c>
       <c r="J103">
         <v>2.5</v>
@@ -7751,7 +7751,7 @@
         <v>27</v>
       </c>
       <c r="I104">
-        <v>1917</v>
+        <v>1946</v>
       </c>
       <c r="J104">
         <v>2</v>

</xml_diff>

<commit_message>
update w/ harris poll (11/17)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C39181-6BDC-E349-ABC9-13F6F7953B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20A12C2-6187-ED40-93C7-7B8B4C3C544C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="18240" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB107"/>
+  <dimension ref="A1:AB110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I105" sqref="I105"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AB110" sqref="AB110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8024,6 +8024,228 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>32</v>
+      </c>
+      <c r="B108">
+        <v>2021</v>
+      </c>
+      <c r="C108">
+        <v>12</v>
+      </c>
+      <c r="D108">
+        <v>11</v>
+      </c>
+      <c r="E108">
+        <v>14</v>
+      </c>
+      <c r="F108" t="s">
+        <v>26</v>
+      </c>
+      <c r="G108" t="s">
+        <v>7</v>
+      </c>
+      <c r="H108" t="s">
+        <v>28</v>
+      </c>
+      <c r="I108">
+        <v>2027</v>
+      </c>
+      <c r="J108">
+        <v>1</v>
+      </c>
+      <c r="K108">
+        <v>1</v>
+      </c>
+      <c r="L108">
+        <v>10</v>
+      </c>
+      <c r="M108">
+        <v>2</v>
+      </c>
+      <c r="N108">
+        <v>2</v>
+      </c>
+      <c r="O108">
+        <v>8</v>
+      </c>
+      <c r="P108">
+        <v>4</v>
+      </c>
+      <c r="Q108">
+        <v>23</v>
+      </c>
+      <c r="T108">
+        <v>14</v>
+      </c>
+      <c r="U108" t="s">
+        <v>30</v>
+      </c>
+      <c r="V108">
+        <v>1</v>
+      </c>
+      <c r="W108">
+        <v>16</v>
+      </c>
+      <c r="X108">
+        <v>17</v>
+      </c>
+      <c r="Y108" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>32</v>
+      </c>
+      <c r="B109">
+        <v>2021</v>
+      </c>
+      <c r="C109">
+        <v>12</v>
+      </c>
+      <c r="D109">
+        <v>11</v>
+      </c>
+      <c r="E109">
+        <v>14</v>
+      </c>
+      <c r="F109" t="s">
+        <v>26</v>
+      </c>
+      <c r="G109" t="s">
+        <v>7</v>
+      </c>
+      <c r="H109" t="s">
+        <v>28</v>
+      </c>
+      <c r="I109">
+        <v>2028</v>
+      </c>
+      <c r="J109">
+        <v>1</v>
+      </c>
+      <c r="K109">
+        <v>1</v>
+      </c>
+      <c r="L109">
+        <v>10</v>
+      </c>
+      <c r="M109">
+        <v>2</v>
+      </c>
+      <c r="N109">
+        <v>2</v>
+      </c>
+      <c r="O109">
+        <v>9</v>
+      </c>
+      <c r="P109">
+        <v>4</v>
+      </c>
+      <c r="Q109">
+        <v>24</v>
+      </c>
+      <c r="R109">
+        <v>10</v>
+      </c>
+      <c r="U109" t="s">
+        <v>30</v>
+      </c>
+      <c r="V109">
+        <v>2</v>
+      </c>
+      <c r="W109">
+        <v>16</v>
+      </c>
+      <c r="X109">
+        <v>17</v>
+      </c>
+      <c r="Y109" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>32</v>
+      </c>
+      <c r="B110">
+        <v>2021</v>
+      </c>
+      <c r="C110">
+        <v>12</v>
+      </c>
+      <c r="D110">
+        <v>11</v>
+      </c>
+      <c r="E110">
+        <v>14</v>
+      </c>
+      <c r="F110" t="s">
+        <v>26</v>
+      </c>
+      <c r="G110" t="s">
+        <v>7</v>
+      </c>
+      <c r="H110" t="s">
+        <v>28</v>
+      </c>
+      <c r="I110">
+        <v>2029</v>
+      </c>
+      <c r="J110">
+        <v>1</v>
+      </c>
+      <c r="K110">
+        <v>1</v>
+      </c>
+      <c r="L110">
+        <v>10</v>
+      </c>
+      <c r="M110">
+        <v>2</v>
+      </c>
+      <c r="N110">
+        <v>2</v>
+      </c>
+      <c r="O110">
+        <v>9</v>
+      </c>
+      <c r="P110">
+        <v>4</v>
+      </c>
+      <c r="Q110">
+        <v>24</v>
+      </c>
+      <c r="S110">
+        <v>10</v>
+      </c>
+      <c r="U110" t="s">
+        <v>30</v>
+      </c>
+      <c r="V110">
+        <v>2</v>
+      </c>
+      <c r="W110">
+        <v>16</v>
+      </c>
+      <c r="X110">
+        <v>18</v>
+      </c>
+      <c r="Y110" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA110">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update sample size harris poll (11/17)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20A12C2-6187-ED40-93C7-7B8B4C3C544C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C22A981-1168-2D43-BEFE-3CAA7C137106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="18240" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -519,9 +519,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
   <dimension ref="A1:AB110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AB110" sqref="AB110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8050,7 +8050,7 @@
         <v>28</v>
       </c>
       <c r="I108">
-        <v>2027</v>
+        <v>1743</v>
       </c>
       <c r="J108">
         <v>1</v>
@@ -8124,7 +8124,7 @@
         <v>28</v>
       </c>
       <c r="I109">
-        <v>2028</v>
+        <v>1743</v>
       </c>
       <c r="J109">
         <v>1</v>
@@ -8198,7 +8198,7 @@
         <v>28</v>
       </c>
       <c r="I110">
-        <v>2029</v>
+        <v>1743</v>
       </c>
       <c r="J110">
         <v>1</v>

</xml_diff>

<commit_message>
update with opinionway poll (11/18)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C22A981-1168-2D43-BEFE-3CAA7C137106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4AB6F0-DBBE-7747-8059-6B758C61A3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="18240" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB110"/>
+  <dimension ref="A1:AB113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I110" sqref="I110"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="J112" sqref="J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8246,6 +8246,201 @@
         <v>1</v>
       </c>
     </row>
+    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>33</v>
+      </c>
+      <c r="B111">
+        <v>2021</v>
+      </c>
+      <c r="C111">
+        <v>12</v>
+      </c>
+      <c r="D111">
+        <v>11</v>
+      </c>
+      <c r="E111">
+        <v>16</v>
+      </c>
+      <c r="F111" t="s">
+        <v>40</v>
+      </c>
+      <c r="G111" t="s">
+        <v>7</v>
+      </c>
+      <c r="H111" t="s">
+        <v>28</v>
+      </c>
+      <c r="I111">
+        <v>1178</v>
+      </c>
+      <c r="J111">
+        <v>1</v>
+      </c>
+      <c r="K111">
+        <v>1</v>
+      </c>
+      <c r="L111">
+        <v>9</v>
+      </c>
+      <c r="M111">
+        <v>2</v>
+      </c>
+      <c r="N111">
+        <v>3</v>
+      </c>
+      <c r="O111">
+        <v>8</v>
+      </c>
+      <c r="P111">
+        <v>5</v>
+      </c>
+      <c r="Q111">
+        <v>24</v>
+      </c>
+      <c r="T111">
+        <v>13</v>
+      </c>
+      <c r="V111">
+        <v>3</v>
+      </c>
+      <c r="W111">
+        <v>19</v>
+      </c>
+      <c r="X111">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>33</v>
+      </c>
+      <c r="B112">
+        <v>2021</v>
+      </c>
+      <c r="C112">
+        <v>12</v>
+      </c>
+      <c r="D112">
+        <v>11</v>
+      </c>
+      <c r="E112">
+        <v>16</v>
+      </c>
+      <c r="F112" t="s">
+        <v>40</v>
+      </c>
+      <c r="G112" t="s">
+        <v>7</v>
+      </c>
+      <c r="H112" t="s">
+        <v>28</v>
+      </c>
+      <c r="I112">
+        <v>1178</v>
+      </c>
+      <c r="J112">
+        <v>1</v>
+      </c>
+      <c r="K112">
+        <v>1</v>
+      </c>
+      <c r="L112">
+        <v>9</v>
+      </c>
+      <c r="M112">
+        <v>2</v>
+      </c>
+      <c r="N112">
+        <v>3</v>
+      </c>
+      <c r="O112">
+        <v>8</v>
+      </c>
+      <c r="P112">
+        <v>6</v>
+      </c>
+      <c r="Q112">
+        <v>25</v>
+      </c>
+      <c r="R112">
+        <v>11</v>
+      </c>
+      <c r="V112">
+        <v>3</v>
+      </c>
+      <c r="W112">
+        <v>19</v>
+      </c>
+      <c r="X112">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>33</v>
+      </c>
+      <c r="B113">
+        <v>2021</v>
+      </c>
+      <c r="C113">
+        <v>12</v>
+      </c>
+      <c r="D113">
+        <v>11</v>
+      </c>
+      <c r="E113">
+        <v>16</v>
+      </c>
+      <c r="F113" t="s">
+        <v>40</v>
+      </c>
+      <c r="G113" t="s">
+        <v>7</v>
+      </c>
+      <c r="H113" t="s">
+        <v>28</v>
+      </c>
+      <c r="I113">
+        <v>1178</v>
+      </c>
+      <c r="J113">
+        <v>1</v>
+      </c>
+      <c r="K113">
+        <v>1</v>
+      </c>
+      <c r="L113">
+        <v>9</v>
+      </c>
+      <c r="M113">
+        <v>2</v>
+      </c>
+      <c r="N113">
+        <v>3</v>
+      </c>
+      <c r="O113">
+        <v>8</v>
+      </c>
+      <c r="P113">
+        <v>6</v>
+      </c>
+      <c r="Q113">
+        <v>25</v>
+      </c>
+      <c r="S113">
+        <v>9</v>
+      </c>
+      <c r="V113">
+        <v>3</v>
+      </c>
+      <c r="W113">
+        <v>21</v>
+      </c>
+      <c r="X113">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update with bva poll (11/19)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4AB6F0-DBBE-7747-8059-6B758C61A3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABD24C4-5F75-3E40-BE64-A80DF9F53BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="18240" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="340" yWindow="18500" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB113"/>
+  <dimension ref="A1:AB120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="J112" sqref="J112"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="Y114" sqref="Y114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8272,7 +8272,7 @@
         <v>28</v>
       </c>
       <c r="I111">
-        <v>1178</v>
+        <v>1163</v>
       </c>
       <c r="J111">
         <v>1</v>
@@ -8337,7 +8337,7 @@
         <v>28</v>
       </c>
       <c r="I112">
-        <v>1178</v>
+        <v>1192</v>
       </c>
       <c r="J112">
         <v>1</v>
@@ -8376,7 +8376,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>33</v>
       </c>
@@ -8439,6 +8439,485 @@
       </c>
       <c r="X113">
         <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>33</v>
+      </c>
+      <c r="B114">
+        <v>2021</v>
+      </c>
+      <c r="C114">
+        <v>12</v>
+      </c>
+      <c r="D114">
+        <v>11</v>
+      </c>
+      <c r="E114">
+        <v>16</v>
+      </c>
+      <c r="F114" t="s">
+        <v>40</v>
+      </c>
+      <c r="G114" t="s">
+        <v>7</v>
+      </c>
+      <c r="H114" t="s">
+        <v>28</v>
+      </c>
+      <c r="I114">
+        <v>1163</v>
+      </c>
+      <c r="J114">
+        <v>2</v>
+      </c>
+      <c r="K114">
+        <v>1</v>
+      </c>
+      <c r="L114">
+        <v>9</v>
+      </c>
+      <c r="M114">
+        <v>2</v>
+      </c>
+      <c r="N114">
+        <v>3</v>
+      </c>
+      <c r="O114">
+        <v>8</v>
+      </c>
+      <c r="P114">
+        <v>6</v>
+      </c>
+      <c r="Q114">
+        <v>25</v>
+      </c>
+      <c r="T114">
+        <v>14</v>
+      </c>
+      <c r="V114">
+        <v>4</v>
+      </c>
+      <c r="W114">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="115" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>34</v>
+      </c>
+      <c r="B115">
+        <v>2021</v>
+      </c>
+      <c r="C115">
+        <v>12</v>
+      </c>
+      <c r="D115">
+        <v>11</v>
+      </c>
+      <c r="E115">
+        <v>14</v>
+      </c>
+      <c r="F115" t="s">
+        <v>41</v>
+      </c>
+      <c r="G115" t="s">
+        <v>7</v>
+      </c>
+      <c r="H115" t="s">
+        <v>8</v>
+      </c>
+      <c r="I115">
+        <v>886</v>
+      </c>
+      <c r="J115">
+        <v>1.5</v>
+      </c>
+      <c r="K115">
+        <v>1</v>
+      </c>
+      <c r="L115">
+        <v>7.5</v>
+      </c>
+      <c r="M115">
+        <v>2.5</v>
+      </c>
+      <c r="N115">
+        <v>2</v>
+      </c>
+      <c r="O115">
+        <v>8</v>
+      </c>
+      <c r="P115">
+        <v>5</v>
+      </c>
+      <c r="Q115">
+        <v>26</v>
+      </c>
+      <c r="R115">
+        <v>9</v>
+      </c>
+      <c r="U115">
+        <v>1</v>
+      </c>
+      <c r="V115">
+        <v>2.5</v>
+      </c>
+      <c r="W115">
+        <v>18</v>
+      </c>
+      <c r="X115">
+        <v>15</v>
+      </c>
+      <c r="Y115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>34</v>
+      </c>
+      <c r="B116">
+        <v>2021</v>
+      </c>
+      <c r="C116">
+        <v>12</v>
+      </c>
+      <c r="D116">
+        <v>11</v>
+      </c>
+      <c r="E116">
+        <v>14</v>
+      </c>
+      <c r="F116" t="s">
+        <v>41</v>
+      </c>
+      <c r="G116" t="s">
+        <v>7</v>
+      </c>
+      <c r="H116" t="s">
+        <v>8</v>
+      </c>
+      <c r="I116">
+        <v>877</v>
+      </c>
+      <c r="J116">
+        <v>1.5</v>
+      </c>
+      <c r="K116">
+        <v>1</v>
+      </c>
+      <c r="L116">
+        <v>7.5</v>
+      </c>
+      <c r="M116">
+        <v>2.5</v>
+      </c>
+      <c r="N116">
+        <v>2</v>
+      </c>
+      <c r="O116">
+        <v>8.5</v>
+      </c>
+      <c r="P116">
+        <v>4</v>
+      </c>
+      <c r="Q116">
+        <v>27</v>
+      </c>
+      <c r="S116">
+        <v>8</v>
+      </c>
+      <c r="U116">
+        <v>1</v>
+      </c>
+      <c r="V116">
+        <v>3</v>
+      </c>
+      <c r="W116">
+        <v>19</v>
+      </c>
+      <c r="X116">
+        <v>15</v>
+      </c>
+      <c r="Y116" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>34</v>
+      </c>
+      <c r="B117">
+        <v>2021</v>
+      </c>
+      <c r="C117">
+        <v>12</v>
+      </c>
+      <c r="D117">
+        <v>11</v>
+      </c>
+      <c r="E117">
+        <v>14</v>
+      </c>
+      <c r="F117" t="s">
+        <v>41</v>
+      </c>
+      <c r="G117" t="s">
+        <v>7</v>
+      </c>
+      <c r="H117" t="s">
+        <v>8</v>
+      </c>
+      <c r="I117">
+        <v>888</v>
+      </c>
+      <c r="J117">
+        <v>1.5</v>
+      </c>
+      <c r="K117">
+        <v>1.5</v>
+      </c>
+      <c r="L117">
+        <v>7</v>
+      </c>
+      <c r="M117">
+        <v>2</v>
+      </c>
+      <c r="N117">
+        <v>2</v>
+      </c>
+      <c r="O117">
+        <v>8</v>
+      </c>
+      <c r="P117">
+        <v>4</v>
+      </c>
+      <c r="Q117">
+        <v>26</v>
+      </c>
+      <c r="T117">
+        <v>12</v>
+      </c>
+      <c r="U117">
+        <v>1</v>
+      </c>
+      <c r="V117">
+        <v>1.5</v>
+      </c>
+      <c r="W117">
+        <v>18</v>
+      </c>
+      <c r="X117">
+        <v>15</v>
+      </c>
+      <c r="Y117">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>34</v>
+      </c>
+      <c r="B118">
+        <v>2021</v>
+      </c>
+      <c r="C118">
+        <v>12</v>
+      </c>
+      <c r="D118">
+        <v>11</v>
+      </c>
+      <c r="E118">
+        <v>14</v>
+      </c>
+      <c r="F118" t="s">
+        <v>41</v>
+      </c>
+      <c r="G118" t="s">
+        <v>7</v>
+      </c>
+      <c r="H118" t="s">
+        <v>8</v>
+      </c>
+      <c r="I118">
+        <v>870</v>
+      </c>
+      <c r="J118">
+        <v>1.5</v>
+      </c>
+      <c r="K118">
+        <v>1.5</v>
+      </c>
+      <c r="L118">
+        <v>8</v>
+      </c>
+      <c r="M118">
+        <v>2</v>
+      </c>
+      <c r="N118">
+        <v>2</v>
+      </c>
+      <c r="O118">
+        <v>9</v>
+      </c>
+      <c r="P118">
+        <v>4</v>
+      </c>
+      <c r="Q118">
+        <v>28</v>
+      </c>
+      <c r="R118">
+        <v>11</v>
+      </c>
+      <c r="U118">
+        <v>1.5</v>
+      </c>
+      <c r="V118">
+        <v>4</v>
+      </c>
+      <c r="W118">
+        <v>27</v>
+      </c>
+      <c r="Y118">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>34</v>
+      </c>
+      <c r="B119">
+        <v>2021</v>
+      </c>
+      <c r="C119">
+        <v>12</v>
+      </c>
+      <c r="D119">
+        <v>11</v>
+      </c>
+      <c r="E119">
+        <v>14</v>
+      </c>
+      <c r="F119" t="s">
+        <v>41</v>
+      </c>
+      <c r="G119" t="s">
+        <v>7</v>
+      </c>
+      <c r="H119" t="s">
+        <v>8</v>
+      </c>
+      <c r="I119">
+        <v>856</v>
+      </c>
+      <c r="J119">
+        <v>1.5</v>
+      </c>
+      <c r="K119">
+        <v>1.5</v>
+      </c>
+      <c r="L119">
+        <v>8</v>
+      </c>
+      <c r="M119">
+        <v>2</v>
+      </c>
+      <c r="N119">
+        <v>2</v>
+      </c>
+      <c r="O119">
+        <v>8</v>
+      </c>
+      <c r="P119">
+        <v>5</v>
+      </c>
+      <c r="Q119">
+        <v>29</v>
+      </c>
+      <c r="S119">
+        <v>9</v>
+      </c>
+      <c r="U119">
+        <v>1.5</v>
+      </c>
+      <c r="V119">
+        <v>4</v>
+      </c>
+      <c r="W119">
+        <v>28</v>
+      </c>
+      <c r="Y119">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>34</v>
+      </c>
+      <c r="B120">
+        <v>2021</v>
+      </c>
+      <c r="C120">
+        <v>12</v>
+      </c>
+      <c r="D120">
+        <v>11</v>
+      </c>
+      <c r="E120">
+        <v>14</v>
+      </c>
+      <c r="F120" t="s">
+        <v>41</v>
+      </c>
+      <c r="G120" t="s">
+        <v>7</v>
+      </c>
+      <c r="H120" t="s">
+        <v>8</v>
+      </c>
+      <c r="I120">
+        <v>873</v>
+      </c>
+      <c r="J120">
+        <v>1</v>
+      </c>
+      <c r="K120">
+        <v>1</v>
+      </c>
+      <c r="L120">
+        <v>7.5</v>
+      </c>
+      <c r="M120">
+        <v>2</v>
+      </c>
+      <c r="N120">
+        <v>2</v>
+      </c>
+      <c r="O120">
+        <v>8.5</v>
+      </c>
+      <c r="P120">
+        <v>5</v>
+      </c>
+      <c r="Q120">
+        <v>27</v>
+      </c>
+      <c r="T120">
+        <v>15</v>
+      </c>
+      <c r="U120">
+        <v>1.5</v>
+      </c>
+      <c r="V120">
+        <v>3</v>
+      </c>
+      <c r="W120">
+        <v>26</v>
+      </c>
+      <c r="Y120">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ harris poll (11/24)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABD24C4-5F75-3E40-BE64-A80DF9F53BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B34B5E1-9DF6-C14B-BCFA-0599D9328C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="18500" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -517,11 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB120"/>
+  <dimension ref="A1:AB123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="Y114" sqref="Y114"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AB123" sqref="AB123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8254,7 +8254,7 @@
         <v>2021</v>
       </c>
       <c r="C111">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D111">
         <v>11</v>
@@ -8319,7 +8319,7 @@
         <v>2021</v>
       </c>
       <c r="C112">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D112">
         <v>11</v>
@@ -8376,7 +8376,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>33</v>
       </c>
@@ -8384,7 +8384,7 @@
         <v>2021</v>
       </c>
       <c r="C113">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D113">
         <v>11</v>
@@ -8441,7 +8441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>33</v>
       </c>
@@ -8449,7 +8449,7 @@
         <v>2021</v>
       </c>
       <c r="C114">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D114">
         <v>11</v>
@@ -8503,7 +8503,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>34</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>34</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>34</v>
       </c>
@@ -8716,7 +8716,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>34</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>34</v>
       </c>
@@ -8852,7 +8852,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>34</v>
       </c>
@@ -8918,6 +8918,228 @@
       </c>
       <c r="Y120">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>34</v>
+      </c>
+      <c r="B121">
+        <v>2021</v>
+      </c>
+      <c r="C121">
+        <v>13</v>
+      </c>
+      <c r="D121">
+        <v>11</v>
+      </c>
+      <c r="E121">
+        <v>21</v>
+      </c>
+      <c r="F121" t="s">
+        <v>26</v>
+      </c>
+      <c r="G121" t="s">
+        <v>7</v>
+      </c>
+      <c r="H121" t="s">
+        <v>28</v>
+      </c>
+      <c r="I121">
+        <v>2120</v>
+      </c>
+      <c r="J121">
+        <v>1</v>
+      </c>
+      <c r="K121">
+        <v>1</v>
+      </c>
+      <c r="L121">
+        <v>10</v>
+      </c>
+      <c r="M121">
+        <v>2</v>
+      </c>
+      <c r="N121">
+        <v>1</v>
+      </c>
+      <c r="O121">
+        <v>8</v>
+      </c>
+      <c r="P121">
+        <v>5</v>
+      </c>
+      <c r="Q121">
+        <v>23</v>
+      </c>
+      <c r="T121">
+        <v>14</v>
+      </c>
+      <c r="U121" t="s">
+        <v>30</v>
+      </c>
+      <c r="V121">
+        <v>2</v>
+      </c>
+      <c r="W121">
+        <v>16</v>
+      </c>
+      <c r="X121">
+        <v>16</v>
+      </c>
+      <c r="Y121" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>34</v>
+      </c>
+      <c r="B122">
+        <v>2021</v>
+      </c>
+      <c r="C122">
+        <v>13</v>
+      </c>
+      <c r="D122">
+        <v>11</v>
+      </c>
+      <c r="E122">
+        <v>21</v>
+      </c>
+      <c r="F122" t="s">
+        <v>26</v>
+      </c>
+      <c r="G122" t="s">
+        <v>7</v>
+      </c>
+      <c r="H122" t="s">
+        <v>28</v>
+      </c>
+      <c r="I122">
+        <v>2121</v>
+      </c>
+      <c r="J122">
+        <v>1</v>
+      </c>
+      <c r="K122">
+        <v>1</v>
+      </c>
+      <c r="L122">
+        <v>10</v>
+      </c>
+      <c r="M122">
+        <v>2</v>
+      </c>
+      <c r="N122">
+        <v>1</v>
+      </c>
+      <c r="O122">
+        <v>9</v>
+      </c>
+      <c r="P122">
+        <v>5</v>
+      </c>
+      <c r="Q122">
+        <v>24</v>
+      </c>
+      <c r="R122">
+        <v>11</v>
+      </c>
+      <c r="U122" t="s">
+        <v>30</v>
+      </c>
+      <c r="V122">
+        <v>2</v>
+      </c>
+      <c r="W122">
+        <v>16</v>
+      </c>
+      <c r="X122">
+        <v>16</v>
+      </c>
+      <c r="Y122" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>34</v>
+      </c>
+      <c r="B123">
+        <v>2021</v>
+      </c>
+      <c r="C123">
+        <v>13</v>
+      </c>
+      <c r="D123">
+        <v>11</v>
+      </c>
+      <c r="E123">
+        <v>21</v>
+      </c>
+      <c r="F123" t="s">
+        <v>26</v>
+      </c>
+      <c r="G123" t="s">
+        <v>7</v>
+      </c>
+      <c r="H123" t="s">
+        <v>28</v>
+      </c>
+      <c r="I123">
+        <v>2122</v>
+      </c>
+      <c r="J123">
+        <v>1</v>
+      </c>
+      <c r="K123">
+        <v>1</v>
+      </c>
+      <c r="L123">
+        <v>10</v>
+      </c>
+      <c r="M123">
+        <v>2</v>
+      </c>
+      <c r="N123">
+        <v>1</v>
+      </c>
+      <c r="O123">
+        <v>9</v>
+      </c>
+      <c r="P123">
+        <v>5</v>
+      </c>
+      <c r="Q123">
+        <v>24</v>
+      </c>
+      <c r="S123">
+        <v>10</v>
+      </c>
+      <c r="U123" t="s">
+        <v>30</v>
+      </c>
+      <c r="V123">
+        <v>2</v>
+      </c>
+      <c r="W123">
+        <v>16</v>
+      </c>
+      <c r="X123">
+        <v>17</v>
+      </c>
+      <c r="Y123" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA123">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with cluster17 polls
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B34B5E1-9DF6-C14B-BCFA-0599D9328C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC338B16-54F2-044A-B4FD-3828A1247D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="18500" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="43">
   <si>
     <t>year</t>
   </si>
@@ -159,12 +159,15 @@
   <si>
     <t>bva</t>
   </si>
+  <si>
+    <t>cluster17</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +178,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -517,11 +526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB123"/>
+  <dimension ref="A1:AB131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AB123" sqref="AB123"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AB131" sqref="AB131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8376,7 +8385,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>33</v>
       </c>
@@ -8441,7 +8450,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>33</v>
       </c>
@@ -8503,7 +8512,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>34</v>
       </c>
@@ -8574,7 +8583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>34</v>
       </c>
@@ -8645,7 +8654,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>34</v>
       </c>
@@ -8716,7 +8725,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>34</v>
       </c>
@@ -8784,7 +8793,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>34</v>
       </c>
@@ -8852,7 +8861,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>34</v>
       </c>
@@ -8920,9 +8929,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B121">
         <v>2021</v>
@@ -8994,9 +9003,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B122">
         <v>2021</v>
@@ -9068,9 +9077,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B123">
         <v>2021</v>
@@ -9142,7 +9151,597 @@
         <v>2</v>
       </c>
     </row>
+    <row r="124" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>36</v>
+      </c>
+      <c r="B124">
+        <v>2021</v>
+      </c>
+      <c r="C124">
+        <v>14</v>
+      </c>
+      <c r="D124">
+        <v>11</v>
+      </c>
+      <c r="E124">
+        <v>24</v>
+      </c>
+      <c r="F124" t="s">
+        <v>36</v>
+      </c>
+      <c r="G124" t="s">
+        <v>7</v>
+      </c>
+      <c r="H124" t="s">
+        <v>27</v>
+      </c>
+      <c r="I124">
+        <v>876</v>
+      </c>
+      <c r="J124">
+        <v>1</v>
+      </c>
+      <c r="K124">
+        <v>1</v>
+      </c>
+      <c r="L124">
+        <v>9</v>
+      </c>
+      <c r="M124">
+        <v>2</v>
+      </c>
+      <c r="N124">
+        <v>1</v>
+      </c>
+      <c r="O124">
+        <v>8</v>
+      </c>
+      <c r="P124">
+        <v>4</v>
+      </c>
+      <c r="Q124">
+        <v>25</v>
+      </c>
+      <c r="T124">
+        <v>13</v>
+      </c>
+      <c r="U124">
+        <v>1</v>
+      </c>
+      <c r="V124">
+        <v>2</v>
+      </c>
+      <c r="W124">
+        <v>20</v>
+      </c>
+      <c r="X124">
+        <v>12</v>
+      </c>
+      <c r="Y124" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z124" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>36</v>
+      </c>
+      <c r="B125">
+        <v>2021</v>
+      </c>
+      <c r="C125">
+        <v>14</v>
+      </c>
+      <c r="D125">
+        <v>11</v>
+      </c>
+      <c r="E125">
+        <v>24</v>
+      </c>
+      <c r="F125" t="s">
+        <v>36</v>
+      </c>
+      <c r="G125" t="s">
+        <v>7</v>
+      </c>
+      <c r="H125" t="s">
+        <v>27</v>
+      </c>
+      <c r="I125">
+        <v>905</v>
+      </c>
+      <c r="J125">
+        <v>2</v>
+      </c>
+      <c r="K125">
+        <v>1</v>
+      </c>
+      <c r="L125">
+        <v>9</v>
+      </c>
+      <c r="M125">
+        <v>2</v>
+      </c>
+      <c r="N125">
+        <v>2</v>
+      </c>
+      <c r="O125">
+        <v>8</v>
+      </c>
+      <c r="P125">
+        <v>4</v>
+      </c>
+      <c r="Q125">
+        <v>25</v>
+      </c>
+      <c r="R125">
+        <v>9</v>
+      </c>
+      <c r="U125">
+        <v>1</v>
+      </c>
+      <c r="V125">
+        <v>3</v>
+      </c>
+      <c r="W125">
+        <v>20</v>
+      </c>
+      <c r="X125">
+        <v>13</v>
+      </c>
+      <c r="Y125">
+        <v>1</v>
+      </c>
+      <c r="Z125" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA125" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="126" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>36</v>
+      </c>
+      <c r="B126">
+        <v>2021</v>
+      </c>
+      <c r="C126">
+        <v>14</v>
+      </c>
+      <c r="D126">
+        <v>11</v>
+      </c>
+      <c r="E126">
+        <v>24</v>
+      </c>
+      <c r="F126" t="s">
+        <v>36</v>
+      </c>
+      <c r="G126" t="s">
+        <v>7</v>
+      </c>
+      <c r="H126" t="s">
+        <v>27</v>
+      </c>
+      <c r="I126">
+        <v>891</v>
+      </c>
+      <c r="J126">
+        <v>1</v>
+      </c>
+      <c r="K126">
+        <v>1</v>
+      </c>
+      <c r="L126">
+        <v>9</v>
+      </c>
+      <c r="M126">
+        <v>2</v>
+      </c>
+      <c r="N126">
+        <v>2</v>
+      </c>
+      <c r="O126">
+        <v>8</v>
+      </c>
+      <c r="P126">
+        <v>4</v>
+      </c>
+      <c r="Q126">
+        <v>25</v>
+      </c>
+      <c r="S126">
+        <v>9</v>
+      </c>
+      <c r="U126">
+        <v>1</v>
+      </c>
+      <c r="V126">
+        <v>3</v>
+      </c>
+      <c r="W126">
+        <v>20</v>
+      </c>
+      <c r="X126">
+        <v>13</v>
+      </c>
+      <c r="Y126">
+        <v>1</v>
+      </c>
+      <c r="Z126" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>37</v>
+      </c>
+      <c r="B127">
+        <v>2021</v>
+      </c>
+      <c r="C127">
+        <v>6</v>
+      </c>
+      <c r="D127">
+        <v>11</v>
+      </c>
+      <c r="E127">
+        <v>11</v>
+      </c>
+      <c r="F127" t="s">
+        <v>42</v>
+      </c>
+      <c r="G127" t="s">
+        <v>7</v>
+      </c>
+      <c r="H127" t="s">
+        <v>27</v>
+      </c>
+      <c r="I127">
+        <v>6656</v>
+      </c>
+      <c r="J127">
+        <v>1</v>
+      </c>
+      <c r="K127">
+        <v>0.5</v>
+      </c>
+      <c r="L127">
+        <v>12</v>
+      </c>
+      <c r="M127">
+        <v>2</v>
+      </c>
+      <c r="N127">
+        <v>3</v>
+      </c>
+      <c r="O127">
+        <v>7</v>
+      </c>
+      <c r="P127">
+        <v>4</v>
+      </c>
+      <c r="Q127">
+        <v>24</v>
+      </c>
+      <c r="T127">
+        <v>10</v>
+      </c>
+      <c r="U127">
+        <v>1</v>
+      </c>
+      <c r="V127">
+        <v>2</v>
+      </c>
+      <c r="W127">
+        <v>13</v>
+      </c>
+      <c r="X127">
+        <v>18.5</v>
+      </c>
+      <c r="AA127">
+        <v>1.5</v>
+      </c>
+      <c r="AB127">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>38</v>
+      </c>
+      <c r="B128">
+        <v>2021</v>
+      </c>
+      <c r="C128">
+        <v>11</v>
+      </c>
+      <c r="D128">
+        <v>11</v>
+      </c>
+      <c r="E128">
+        <v>11</v>
+      </c>
+      <c r="F128" t="s">
+        <v>42</v>
+      </c>
+      <c r="G128" t="s">
+        <v>7</v>
+      </c>
+      <c r="H128" t="s">
+        <v>27</v>
+      </c>
+      <c r="I128">
+        <v>1727</v>
+      </c>
+      <c r="J128">
+        <v>1</v>
+      </c>
+      <c r="K128">
+        <v>0.5</v>
+      </c>
+      <c r="L128">
+        <v>11</v>
+      </c>
+      <c r="M128">
+        <v>1.5</v>
+      </c>
+      <c r="N128">
+        <v>3</v>
+      </c>
+      <c r="O128">
+        <v>6</v>
+      </c>
+      <c r="P128">
+        <v>4</v>
+      </c>
+      <c r="Q128">
+        <v>23</v>
+      </c>
+      <c r="T128">
+        <v>11</v>
+      </c>
+      <c r="U128">
+        <v>1</v>
+      </c>
+      <c r="V128">
+        <v>3</v>
+      </c>
+      <c r="W128">
+        <v>14</v>
+      </c>
+      <c r="X128">
+        <v>19</v>
+      </c>
+      <c r="AA128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>39</v>
+      </c>
+      <c r="B129">
+        <v>2021</v>
+      </c>
+      <c r="C129">
+        <v>13</v>
+      </c>
+      <c r="D129">
+        <v>11</v>
+      </c>
+      <c r="E129">
+        <v>19</v>
+      </c>
+      <c r="F129" t="s">
+        <v>42</v>
+      </c>
+      <c r="G129" t="s">
+        <v>7</v>
+      </c>
+      <c r="H129" t="s">
+        <v>27</v>
+      </c>
+      <c r="I129">
+        <v>1654</v>
+      </c>
+      <c r="J129">
+        <v>2</v>
+      </c>
+      <c r="K129">
+        <v>0.5</v>
+      </c>
+      <c r="L129">
+        <v>12</v>
+      </c>
+      <c r="M129">
+        <v>2.5</v>
+      </c>
+      <c r="N129">
+        <v>2</v>
+      </c>
+      <c r="O129">
+        <v>7</v>
+      </c>
+      <c r="P129">
+        <v>5</v>
+      </c>
+      <c r="Q129">
+        <v>24</v>
+      </c>
+      <c r="T129">
+        <v>10</v>
+      </c>
+      <c r="U129">
+        <v>1</v>
+      </c>
+      <c r="V129">
+        <v>2</v>
+      </c>
+      <c r="W129">
+        <v>14</v>
+      </c>
+      <c r="X129">
+        <v>17</v>
+      </c>
+      <c r="AA129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>39</v>
+      </c>
+      <c r="B130">
+        <v>2021</v>
+      </c>
+      <c r="C130">
+        <v>13</v>
+      </c>
+      <c r="D130">
+        <v>11</v>
+      </c>
+      <c r="E130">
+        <v>19</v>
+      </c>
+      <c r="F130" t="s">
+        <v>42</v>
+      </c>
+      <c r="G130" t="s">
+        <v>7</v>
+      </c>
+      <c r="H130" t="s">
+        <v>27</v>
+      </c>
+      <c r="I130">
+        <v>1630</v>
+      </c>
+      <c r="J130">
+        <v>2</v>
+      </c>
+      <c r="K130">
+        <v>0.5</v>
+      </c>
+      <c r="L130">
+        <v>12</v>
+      </c>
+      <c r="M130">
+        <v>2.5</v>
+      </c>
+      <c r="N130">
+        <v>2</v>
+      </c>
+      <c r="O130">
+        <v>8</v>
+      </c>
+      <c r="P130">
+        <v>4</v>
+      </c>
+      <c r="Q130">
+        <v>24</v>
+      </c>
+      <c r="R130">
+        <v>9</v>
+      </c>
+      <c r="U130">
+        <v>1</v>
+      </c>
+      <c r="V130">
+        <v>3</v>
+      </c>
+      <c r="W130">
+        <v>15</v>
+      </c>
+      <c r="X130">
+        <v>16</v>
+      </c>
+      <c r="AA130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>39</v>
+      </c>
+      <c r="B131">
+        <v>2021</v>
+      </c>
+      <c r="C131">
+        <v>13</v>
+      </c>
+      <c r="D131">
+        <v>11</v>
+      </c>
+      <c r="E131">
+        <v>19</v>
+      </c>
+      <c r="F131" t="s">
+        <v>42</v>
+      </c>
+      <c r="G131" t="s">
+        <v>7</v>
+      </c>
+      <c r="H131" t="s">
+        <v>27</v>
+      </c>
+      <c r="I131">
+        <v>1581</v>
+      </c>
+      <c r="J131">
+        <v>2</v>
+      </c>
+      <c r="K131">
+        <v>0.5</v>
+      </c>
+      <c r="L131">
+        <v>12</v>
+      </c>
+      <c r="M131">
+        <v>2.5</v>
+      </c>
+      <c r="N131">
+        <v>2</v>
+      </c>
+      <c r="O131">
+        <v>7</v>
+      </c>
+      <c r="P131">
+        <v>5</v>
+      </c>
+      <c r="Q131">
+        <v>24</v>
+      </c>
+      <c r="S131">
+        <v>8</v>
+      </c>
+      <c r="U131">
+        <v>1</v>
+      </c>
+      <c r="V131">
+        <v>3</v>
+      </c>
+      <c r="W131">
+        <v>14</v>
+      </c>
+      <c r="X131">
+        <v>17</v>
+      </c>
+      <c r="AA131">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update w/ ipsos poll 11/28
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC338B16-54F2-044A-B4FD-3828A1247D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B5C18F-638C-E345-971D-E75085A85AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="18500" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="43">
   <si>
     <t>year</t>
   </si>
@@ -526,11 +526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB131"/>
+  <dimension ref="A1:AB134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AB131" sqref="AB131"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AB132" sqref="AB132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9740,6 +9740,210 @@
         <v>2</v>
       </c>
     </row>
+    <row r="132" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>40</v>
+      </c>
+      <c r="B132">
+        <v>2021</v>
+      </c>
+      <c r="C132">
+        <v>14</v>
+      </c>
+      <c r="D132">
+        <v>11</v>
+      </c>
+      <c r="E132">
+        <v>24</v>
+      </c>
+      <c r="F132" t="s">
+        <v>35</v>
+      </c>
+      <c r="G132" t="s">
+        <v>7</v>
+      </c>
+      <c r="H132" t="s">
+        <v>28</v>
+      </c>
+      <c r="I132">
+        <v>1351</v>
+      </c>
+      <c r="J132">
+        <v>1</v>
+      </c>
+      <c r="K132" t="s">
+        <v>30</v>
+      </c>
+      <c r="L132">
+        <v>7.5</v>
+      </c>
+      <c r="M132">
+        <v>2</v>
+      </c>
+      <c r="N132">
+        <v>2</v>
+      </c>
+      <c r="O132">
+        <v>7</v>
+      </c>
+      <c r="P132">
+        <v>6</v>
+      </c>
+      <c r="Q132">
+        <v>25</v>
+      </c>
+      <c r="T132">
+        <v>10</v>
+      </c>
+      <c r="U132">
+        <v>0.5</v>
+      </c>
+      <c r="V132">
+        <v>3</v>
+      </c>
+      <c r="W132">
+        <v>19</v>
+      </c>
+      <c r="X132">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>40</v>
+      </c>
+      <c r="B133">
+        <v>2021</v>
+      </c>
+      <c r="C133">
+        <v>14</v>
+      </c>
+      <c r="D133">
+        <v>11</v>
+      </c>
+      <c r="E133">
+        <v>24</v>
+      </c>
+      <c r="F133" t="s">
+        <v>35</v>
+      </c>
+      <c r="G133" t="s">
+        <v>7</v>
+      </c>
+      <c r="H133" t="s">
+        <v>28</v>
+      </c>
+      <c r="I133">
+        <v>1351</v>
+      </c>
+      <c r="J133">
+        <v>1</v>
+      </c>
+      <c r="K133">
+        <v>0.5</v>
+      </c>
+      <c r="L133">
+        <v>8.5</v>
+      </c>
+      <c r="M133">
+        <v>2.5</v>
+      </c>
+      <c r="N133">
+        <v>2</v>
+      </c>
+      <c r="O133">
+        <v>6.5</v>
+      </c>
+      <c r="P133">
+        <v>6</v>
+      </c>
+      <c r="Q133">
+        <v>25</v>
+      </c>
+      <c r="S133">
+        <v>10</v>
+      </c>
+      <c r="U133">
+        <v>0.5</v>
+      </c>
+      <c r="V133">
+        <v>3.5</v>
+      </c>
+      <c r="W133">
+        <v>19</v>
+      </c>
+      <c r="X133">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>40</v>
+      </c>
+      <c r="B134">
+        <v>2021</v>
+      </c>
+      <c r="C134">
+        <v>14</v>
+      </c>
+      <c r="D134">
+        <v>11</v>
+      </c>
+      <c r="E134">
+        <v>24</v>
+      </c>
+      <c r="F134" t="s">
+        <v>35</v>
+      </c>
+      <c r="G134" t="s">
+        <v>7</v>
+      </c>
+      <c r="H134" t="s">
+        <v>28</v>
+      </c>
+      <c r="I134">
+        <v>1351</v>
+      </c>
+      <c r="J134">
+        <v>1</v>
+      </c>
+      <c r="K134">
+        <v>0.5</v>
+      </c>
+      <c r="L134">
+        <v>8.5</v>
+      </c>
+      <c r="M134">
+        <v>2</v>
+      </c>
+      <c r="N134">
+        <v>2</v>
+      </c>
+      <c r="O134">
+        <v>6.5</v>
+      </c>
+      <c r="P134">
+        <v>6</v>
+      </c>
+      <c r="Q134">
+        <v>25</v>
+      </c>
+      <c r="R134">
+        <v>10</v>
+      </c>
+      <c r="U134" t="s">
+        <v>30</v>
+      </c>
+      <c r="V134">
+        <v>4</v>
+      </c>
+      <c r="W134">
+        <v>19.5</v>
+      </c>
+      <c r="X134">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update with harris (12/1) and ifop (11/28) polls
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B5C18F-638C-E345-971D-E75085A85AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1AE6AF-643E-614A-AE7A-3385260956E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="18500" windowWidth="32720" windowHeight="10200" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="43">
   <si>
     <t>year</t>
   </si>
@@ -526,11 +526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB134"/>
+  <dimension ref="A1:AB137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AB132" sqref="AB132"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="I137" sqref="I137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9766,7 +9766,7 @@
         <v>28</v>
       </c>
       <c r="I132">
-        <v>1351</v>
+        <v>1017</v>
       </c>
       <c r="J132">
         <v>1</v>
@@ -9834,7 +9834,7 @@
         <v>28</v>
       </c>
       <c r="I133">
-        <v>1351</v>
+        <v>1007</v>
       </c>
       <c r="J133">
         <v>1</v>
@@ -9902,7 +9902,7 @@
         <v>28</v>
       </c>
       <c r="I134">
-        <v>1351</v>
+        <v>1004</v>
       </c>
       <c r="J134">
         <v>1</v>
@@ -9942,6 +9942,228 @@
       </c>
       <c r="X134">
         <v>15</v>
+      </c>
+    </row>
+    <row r="135" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>41</v>
+      </c>
+      <c r="B135">
+        <v>2021</v>
+      </c>
+      <c r="C135">
+        <v>14</v>
+      </c>
+      <c r="D135">
+        <v>11</v>
+      </c>
+      <c r="E135">
+        <v>28</v>
+      </c>
+      <c r="F135" t="s">
+        <v>26</v>
+      </c>
+      <c r="G135" t="s">
+        <v>7</v>
+      </c>
+      <c r="H135" t="s">
+        <v>28</v>
+      </c>
+      <c r="I135">
+        <v>1801</v>
+      </c>
+      <c r="J135">
+        <v>1</v>
+      </c>
+      <c r="K135">
+        <v>1</v>
+      </c>
+      <c r="L135">
+        <v>10</v>
+      </c>
+      <c r="M135">
+        <v>2</v>
+      </c>
+      <c r="N135">
+        <v>2</v>
+      </c>
+      <c r="O135">
+        <v>7</v>
+      </c>
+      <c r="P135">
+        <v>5</v>
+      </c>
+      <c r="Q135">
+        <v>23</v>
+      </c>
+      <c r="T135">
+        <v>14</v>
+      </c>
+      <c r="U135" t="s">
+        <v>30</v>
+      </c>
+      <c r="V135">
+        <v>2</v>
+      </c>
+      <c r="W135">
+        <v>19</v>
+      </c>
+      <c r="X135">
+        <v>13</v>
+      </c>
+      <c r="Y135" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>41</v>
+      </c>
+      <c r="B136">
+        <v>2021</v>
+      </c>
+      <c r="C136">
+        <v>14</v>
+      </c>
+      <c r="D136">
+        <v>11</v>
+      </c>
+      <c r="E136">
+        <v>28</v>
+      </c>
+      <c r="F136" t="s">
+        <v>26</v>
+      </c>
+      <c r="G136" t="s">
+        <v>7</v>
+      </c>
+      <c r="H136" t="s">
+        <v>28</v>
+      </c>
+      <c r="I136">
+        <v>1781</v>
+      </c>
+      <c r="J136">
+        <v>1</v>
+      </c>
+      <c r="K136">
+        <v>1</v>
+      </c>
+      <c r="L136">
+        <v>10</v>
+      </c>
+      <c r="M136">
+        <v>2</v>
+      </c>
+      <c r="N136">
+        <v>2</v>
+      </c>
+      <c r="O136">
+        <v>8</v>
+      </c>
+      <c r="P136">
+        <v>5</v>
+      </c>
+      <c r="Q136">
+        <v>24</v>
+      </c>
+      <c r="R136">
+        <v>11</v>
+      </c>
+      <c r="U136" t="s">
+        <v>30</v>
+      </c>
+      <c r="V136">
+        <v>2</v>
+      </c>
+      <c r="W136">
+        <v>20</v>
+      </c>
+      <c r="X136">
+        <v>13</v>
+      </c>
+      <c r="Y136" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>41</v>
+      </c>
+      <c r="B137">
+        <v>2021</v>
+      </c>
+      <c r="C137">
+        <v>14</v>
+      </c>
+      <c r="D137">
+        <v>11</v>
+      </c>
+      <c r="E137">
+        <v>28</v>
+      </c>
+      <c r="F137" t="s">
+        <v>26</v>
+      </c>
+      <c r="G137" t="s">
+        <v>7</v>
+      </c>
+      <c r="H137" t="s">
+        <v>28</v>
+      </c>
+      <c r="I137">
+        <v>1781</v>
+      </c>
+      <c r="J137">
+        <v>1</v>
+      </c>
+      <c r="K137">
+        <v>1</v>
+      </c>
+      <c r="L137">
+        <v>10</v>
+      </c>
+      <c r="M137">
+        <v>2</v>
+      </c>
+      <c r="N137">
+        <v>2</v>
+      </c>
+      <c r="O137">
+        <v>8</v>
+      </c>
+      <c r="P137">
+        <v>5</v>
+      </c>
+      <c r="Q137">
+        <v>24</v>
+      </c>
+      <c r="S137">
+        <v>10</v>
+      </c>
+      <c r="U137" t="s">
+        <v>30</v>
+      </c>
+      <c r="V137">
+        <v>2</v>
+      </c>
+      <c r="W137">
+        <v>20</v>
+      </c>
+      <c r="X137">
+        <v>13</v>
+      </c>
+      <c r="Y137" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA137">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with harris and ifop polls (12/6)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14CE4A7-DFCB-C14F-9E62-68859E532155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50D9B04-ECD8-A34F-97F1-AD10A8A3E5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="5200" windowWidth="32720" windowHeight="23500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="340" yWindow="17520" windowWidth="32720" windowHeight="11180" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="43">
   <si>
     <t>year</t>
   </si>
@@ -529,11 +529,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB133"/>
+  <dimension ref="A1:AB135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AB135" sqref="AB135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9883,6 +9883,148 @@
       </c>
       <c r="AA133">
         <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>40</v>
+      </c>
+      <c r="B134">
+        <v>2021</v>
+      </c>
+      <c r="C134">
+        <v>14</v>
+      </c>
+      <c r="D134">
+        <v>12</v>
+      </c>
+      <c r="E134">
+        <v>5</v>
+      </c>
+      <c r="F134" t="s">
+        <v>26</v>
+      </c>
+      <c r="G134" t="s">
+        <v>7</v>
+      </c>
+      <c r="H134" t="s">
+        <v>28</v>
+      </c>
+      <c r="I134">
+        <v>2129</v>
+      </c>
+      <c r="J134">
+        <v>1</v>
+      </c>
+      <c r="K134">
+        <v>1</v>
+      </c>
+      <c r="L134">
+        <v>11</v>
+      </c>
+      <c r="M134">
+        <v>2</v>
+      </c>
+      <c r="N134">
+        <v>1</v>
+      </c>
+      <c r="O134">
+        <v>7</v>
+      </c>
+      <c r="P134">
+        <v>5</v>
+      </c>
+      <c r="Q134">
+        <v>23</v>
+      </c>
+      <c r="R134">
+        <v>14</v>
+      </c>
+      <c r="U134" t="s">
+        <v>30</v>
+      </c>
+      <c r="V134">
+        <v>2</v>
+      </c>
+      <c r="W134">
+        <v>18</v>
+      </c>
+      <c r="X134">
+        <v>14</v>
+      </c>
+      <c r="Y134" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>41</v>
+      </c>
+      <c r="B135">
+        <v>2021</v>
+      </c>
+      <c r="C135">
+        <v>14</v>
+      </c>
+      <c r="D135">
+        <v>12</v>
+      </c>
+      <c r="E135">
+        <v>5</v>
+      </c>
+      <c r="F135" t="s">
+        <v>35</v>
+      </c>
+      <c r="G135" t="s">
+        <v>7</v>
+      </c>
+      <c r="H135" t="s">
+        <v>28</v>
+      </c>
+      <c r="I135">
+        <v>1341</v>
+      </c>
+      <c r="J135">
+        <v>0.5</v>
+      </c>
+      <c r="K135">
+        <v>0.5</v>
+      </c>
+      <c r="L135">
+        <v>9</v>
+      </c>
+      <c r="M135">
+        <v>2.5</v>
+      </c>
+      <c r="N135">
+        <v>1.5</v>
+      </c>
+      <c r="O135">
+        <v>6</v>
+      </c>
+      <c r="P135">
+        <v>5</v>
+      </c>
+      <c r="Q135">
+        <v>25</v>
+      </c>
+      <c r="R135">
+        <v>17</v>
+      </c>
+      <c r="U135">
+        <v>0.5</v>
+      </c>
+      <c r="V135">
+        <v>2.5</v>
+      </c>
+      <c r="W135">
+        <v>17</v>
+      </c>
+      <c r="X135">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with bva, odoxa and cluster17 polls (12/10)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50D9B04-ECD8-A34F-97F1-AD10A8A3E5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0905BE54-52CF-4247-9BA5-5471DE841350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="17520" windowWidth="32720" windowHeight="11180" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="44">
   <si>
     <t>year</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>cluster17</t>
+  </si>
+  <si>
+    <t>c_thouy</t>
   </si>
 </sst>
 </file>
@@ -529,16 +532,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AB135"/>
+  <dimension ref="A1:AC140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AB135" sqref="AB135"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AA140" sqref="AA140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -623,8 +626,11 @@
       <c r="AB1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -689,7 +695,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -754,7 +760,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -819,7 +825,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -884,7 +890,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -949,7 +955,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1200,7 +1206,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1268,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1336,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1404,7 +1410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1475,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1543,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
@@ -9527,7 +9533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>38</v>
       </c>
@@ -9595,7 +9601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>38</v>
       </c>
@@ -9663,7 +9669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>39</v>
       </c>
@@ -9737,7 +9743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>39</v>
       </c>
@@ -9811,7 +9817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>39</v>
       </c>
@@ -9885,7 +9891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>40</v>
       </c>
@@ -9911,7 +9917,7 @@
         <v>28</v>
       </c>
       <c r="I134">
-        <v>2129</v>
+        <v>1830</v>
       </c>
       <c r="J134">
         <v>1</v>
@@ -9959,7 +9965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>41</v>
       </c>
@@ -9985,7 +9991,7 @@
         <v>28</v>
       </c>
       <c r="I135">
-        <v>1341</v>
+        <v>745</v>
       </c>
       <c r="J135">
         <v>0.5</v>
@@ -10025,6 +10031,364 @@
       </c>
       <c r="X135">
         <v>13</v>
+      </c>
+    </row>
+    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>42</v>
+      </c>
+      <c r="B136">
+        <v>2021</v>
+      </c>
+      <c r="C136">
+        <v>15</v>
+      </c>
+      <c r="D136">
+        <v>12</v>
+      </c>
+      <c r="E136">
+        <v>7</v>
+      </c>
+      <c r="F136" t="s">
+        <v>36</v>
+      </c>
+      <c r="G136" t="s">
+        <v>7</v>
+      </c>
+      <c r="H136" t="s">
+        <v>27</v>
+      </c>
+      <c r="I136">
+        <v>934</v>
+      </c>
+      <c r="J136">
+        <v>2</v>
+      </c>
+      <c r="K136">
+        <v>1</v>
+      </c>
+      <c r="L136">
+        <v>8</v>
+      </c>
+      <c r="M136">
+        <v>1</v>
+      </c>
+      <c r="N136">
+        <v>2</v>
+      </c>
+      <c r="O136">
+        <v>7</v>
+      </c>
+      <c r="P136">
+        <v>3</v>
+      </c>
+      <c r="Q136">
+        <v>23</v>
+      </c>
+      <c r="R136">
+        <v>20</v>
+      </c>
+      <c r="U136">
+        <v>2</v>
+      </c>
+      <c r="V136">
+        <v>2</v>
+      </c>
+      <c r="W136">
+        <v>15</v>
+      </c>
+      <c r="X136">
+        <v>13</v>
+      </c>
+      <c r="Y136" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA136" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC136" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>43</v>
+      </c>
+      <c r="B137">
+        <v>2021</v>
+      </c>
+      <c r="C137">
+        <v>15</v>
+      </c>
+      <c r="D137">
+        <v>12</v>
+      </c>
+      <c r="E137">
+        <v>7</v>
+      </c>
+      <c r="F137" t="s">
+        <v>6</v>
+      </c>
+      <c r="G137" t="s">
+        <v>7</v>
+      </c>
+      <c r="H137" t="s">
+        <v>8</v>
+      </c>
+      <c r="I137">
+        <v>747</v>
+      </c>
+      <c r="J137">
+        <v>1.5</v>
+      </c>
+      <c r="K137">
+        <v>0.5</v>
+      </c>
+      <c r="L137">
+        <v>8</v>
+      </c>
+      <c r="M137">
+        <v>2</v>
+      </c>
+      <c r="N137">
+        <v>2.5</v>
+      </c>
+      <c r="O137">
+        <v>7</v>
+      </c>
+      <c r="P137">
+        <v>5</v>
+      </c>
+      <c r="Q137">
+        <v>25</v>
+      </c>
+      <c r="R137">
+        <v>16</v>
+      </c>
+      <c r="U137">
+        <v>1</v>
+      </c>
+      <c r="V137">
+        <v>1.5</v>
+      </c>
+      <c r="W137">
+        <v>16</v>
+      </c>
+      <c r="X137">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>44</v>
+      </c>
+      <c r="B138">
+        <v>2021</v>
+      </c>
+      <c r="C138">
+        <v>15</v>
+      </c>
+      <c r="D138">
+        <v>12</v>
+      </c>
+      <c r="E138">
+        <v>7</v>
+      </c>
+      <c r="F138" t="s">
+        <v>41</v>
+      </c>
+      <c r="G138" t="s">
+        <v>7</v>
+      </c>
+      <c r="H138" t="s">
+        <v>8</v>
+      </c>
+      <c r="I138">
+        <v>894</v>
+      </c>
+      <c r="J138">
+        <v>1.5</v>
+      </c>
+      <c r="K138">
+        <v>0.5</v>
+      </c>
+      <c r="L138">
+        <v>9</v>
+      </c>
+      <c r="M138">
+        <v>2.5</v>
+      </c>
+      <c r="N138">
+        <v>1</v>
+      </c>
+      <c r="O138">
+        <v>7</v>
+      </c>
+      <c r="P138">
+        <v>5</v>
+      </c>
+      <c r="Q138">
+        <v>24</v>
+      </c>
+      <c r="R138">
+        <v>17</v>
+      </c>
+      <c r="U138">
+        <v>1</v>
+      </c>
+      <c r="V138">
+        <v>2.5</v>
+      </c>
+      <c r="W138">
+        <v>16</v>
+      </c>
+      <c r="X138">
+        <v>13</v>
+      </c>
+      <c r="Y138" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>45</v>
+      </c>
+      <c r="B139">
+        <v>2021</v>
+      </c>
+      <c r="C139">
+        <v>15</v>
+      </c>
+      <c r="D139">
+        <v>12</v>
+      </c>
+      <c r="E139">
+        <v>8</v>
+      </c>
+      <c r="F139" t="s">
+        <v>34</v>
+      </c>
+      <c r="G139" t="s">
+        <v>7</v>
+      </c>
+      <c r="H139" t="s">
+        <v>27</v>
+      </c>
+      <c r="I139">
+        <v>1391</v>
+      </c>
+      <c r="J139">
+        <v>1.5</v>
+      </c>
+      <c r="K139">
+        <v>1</v>
+      </c>
+      <c r="L139">
+        <v>10</v>
+      </c>
+      <c r="M139">
+        <v>2</v>
+      </c>
+      <c r="N139">
+        <v>1</v>
+      </c>
+      <c r="O139">
+        <v>6</v>
+      </c>
+      <c r="P139">
+        <v>3</v>
+      </c>
+      <c r="Q139">
+        <v>24</v>
+      </c>
+      <c r="R139">
+        <v>19</v>
+      </c>
+      <c r="U139">
+        <v>1</v>
+      </c>
+      <c r="V139">
+        <v>2.5</v>
+      </c>
+      <c r="W139">
+        <v>17</v>
+      </c>
+      <c r="X139">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>46</v>
+      </c>
+      <c r="B140">
+        <v>2021</v>
+      </c>
+      <c r="C140">
+        <v>15</v>
+      </c>
+      <c r="D140">
+        <v>12</v>
+      </c>
+      <c r="E140">
+        <v>6</v>
+      </c>
+      <c r="F140" t="s">
+        <v>42</v>
+      </c>
+      <c r="G140" t="s">
+        <v>7</v>
+      </c>
+      <c r="H140" t="s">
+        <v>27</v>
+      </c>
+      <c r="I140">
+        <v>1487</v>
+      </c>
+      <c r="J140">
+        <v>1.5</v>
+      </c>
+      <c r="K140">
+        <v>0.5</v>
+      </c>
+      <c r="L140">
+        <v>13</v>
+      </c>
+      <c r="M140">
+        <v>2</v>
+      </c>
+      <c r="N140">
+        <v>1</v>
+      </c>
+      <c r="O140">
+        <v>5</v>
+      </c>
+      <c r="P140">
+        <v>3</v>
+      </c>
+      <c r="Q140">
+        <v>23</v>
+      </c>
+      <c r="R140">
+        <v>16</v>
+      </c>
+      <c r="U140">
+        <v>1</v>
+      </c>
+      <c r="V140">
+        <v>2</v>
+      </c>
+      <c r="W140">
+        <v>16</v>
+      </c>
+      <c r="X140">
+        <v>15</v>
+      </c>
+      <c r="Y140">
+        <v>0.5</v>
+      </c>
+      <c r="AA140">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ opinionway and harris polls (12/15)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0905BE54-52CF-4247-9BA5-5471DE841350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4868D5D-3588-BC47-AC6C-8200B87F450D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="17520" windowWidth="32720" windowHeight="11180" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="45">
   <si>
     <t>year</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>c_thouy</t>
+  </si>
+  <si>
+    <t>c_taubira</t>
   </si>
 </sst>
 </file>
@@ -532,16 +535,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AC140"/>
+  <dimension ref="A1:AD142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AA140" sqref="AA140"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD142" sqref="AD142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -627,10 +630,13 @@
         <v>38</v>
       </c>
       <c r="AC1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -695,7 +701,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -760,7 +766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -825,7 +831,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -890,7 +896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -955,7 +961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1020,7 +1026,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1082,7 +1088,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1144,7 +1150,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1206,7 +1212,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1342,7 +1348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1410,7 +1416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1481,7 +1487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1549,7 +1555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1617,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1685,7 +1691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1753,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1824,7 +1830,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1897,8 +1903,9 @@
       <c r="AB20" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC20" s="1"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>5</v>
       </c>
@@ -1972,7 +1979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2049,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2126,7 +2133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -2191,7 +2198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -2265,7 +2272,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>7</v>
       </c>
@@ -2339,7 +2346,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>8</v>
       </c>
@@ -2404,7 +2411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>8</v>
       </c>
@@ -2469,7 +2476,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>9</v>
       </c>
@@ -2534,7 +2541,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>9</v>
       </c>
@@ -2596,7 +2603,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>9</v>
       </c>
@@ -2658,7 +2665,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>10</v>
       </c>
@@ -2729,7 +2736,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>10</v>
       </c>
@@ -2800,7 +2807,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>10</v>
       </c>
@@ -2871,7 +2878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>11</v>
       </c>
@@ -2936,7 +2943,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>11</v>
       </c>
@@ -3001,7 +3008,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>11</v>
       </c>
@@ -3066,7 +3073,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>11</v>
       </c>
@@ -3134,7 +3141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>11</v>
       </c>
@@ -3202,7 +3209,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>11</v>
       </c>
@@ -3270,7 +3277,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>12</v>
       </c>
@@ -3338,7 +3345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>12</v>
       </c>
@@ -3406,7 +3413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>12</v>
       </c>
@@ -3474,7 +3481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>12</v>
       </c>
@@ -3539,7 +3546,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>12</v>
       </c>
@@ -3604,7 +3611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>12</v>
       </c>
@@ -3669,7 +3676,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>13</v>
       </c>
@@ -3748,8 +3755,9 @@
       <c r="AB47" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC47" s="1"/>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>13</v>
       </c>
@@ -3828,8 +3836,9 @@
       <c r="AB48" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC48" s="1"/>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>13</v>
       </c>
@@ -3908,8 +3917,9 @@
       <c r="AB49" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC49" s="1"/>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>14</v>
       </c>
@@ -3989,7 +3999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>14</v>
       </c>
@@ -4068,8 +4078,9 @@
       <c r="AB51" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC51" s="1"/>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>14</v>
       </c>
@@ -4148,8 +4159,9 @@
       <c r="AB52" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC52" s="1"/>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>15</v>
       </c>
@@ -4217,7 +4229,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>15</v>
       </c>
@@ -4285,7 +4297,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>16</v>
       </c>
@@ -4350,7 +4362,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>16</v>
       </c>
@@ -4415,7 +4427,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>16</v>
       </c>
@@ -4474,7 +4486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>17</v>
       </c>
@@ -4545,7 +4557,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>17</v>
       </c>
@@ -4616,7 +4628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>17</v>
       </c>
@@ -4687,7 +4699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>18</v>
       </c>
@@ -4766,8 +4778,9 @@
       <c r="AB61" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC61" s="1"/>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>18</v>
       </c>
@@ -4846,8 +4859,9 @@
       <c r="AB62" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC62" s="1"/>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>18</v>
       </c>
@@ -4926,8 +4940,9 @@
       <c r="AB63" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC63" s="1"/>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>19</v>
       </c>
@@ -6086,7 +6101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>23</v>
       </c>
@@ -6151,7 +6166,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>23</v>
       </c>
@@ -6213,7 +6228,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>24</v>
       </c>
@@ -6275,7 +6290,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>24</v>
       </c>
@@ -6340,7 +6355,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>24</v>
       </c>
@@ -6405,7 +6420,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>24</v>
       </c>
@@ -6470,7 +6485,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>25</v>
       </c>
@@ -6546,8 +6561,9 @@
       <c r="AB87" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC87" s="1"/>
+    </row>
+    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>25</v>
       </c>
@@ -6623,8 +6639,9 @@
       <c r="AB88" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC88" s="1"/>
+    </row>
+    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>25</v>
       </c>
@@ -6700,8 +6717,9 @@
       <c r="AB89" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC89" s="1"/>
+    </row>
+    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>26</v>
       </c>
@@ -6780,8 +6798,9 @@
       <c r="AB90" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC90" s="1"/>
+    </row>
+    <row r="91" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>26</v>
       </c>
@@ -6860,8 +6879,9 @@
       <c r="AB91" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC91" s="1"/>
+    </row>
+    <row r="92" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>26</v>
       </c>
@@ -6941,7 +6961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>27</v>
       </c>
@@ -7017,8 +7037,9 @@
       <c r="AB93" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC93" s="1"/>
+    </row>
+    <row r="94" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>27</v>
       </c>
@@ -7094,8 +7115,9 @@
       <c r="AB94" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC94" s="1"/>
+    </row>
+    <row r="95" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>27</v>
       </c>
@@ -7171,8 +7193,9 @@
       <c r="AB95" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC95" s="1"/>
+    </row>
+    <row r="96" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>28</v>
       </c>
@@ -7240,7 +7263,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>28</v>
       </c>
@@ -7308,7 +7331,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>28</v>
       </c>
@@ -7376,7 +7399,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>29</v>
       </c>
@@ -7452,8 +7475,9 @@
       <c r="AB99" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC99" s="1"/>
+    </row>
+    <row r="100" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>29</v>
       </c>
@@ -7529,8 +7553,9 @@
       <c r="AB100" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC100" s="1"/>
+    </row>
+    <row r="101" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>29</v>
       </c>
@@ -7606,8 +7631,9 @@
       <c r="AB101" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC101" s="1"/>
+    </row>
+    <row r="102" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>30</v>
       </c>
@@ -7675,7 +7701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>30</v>
       </c>
@@ -7743,7 +7769,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>30</v>
       </c>
@@ -7811,7 +7837,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>31</v>
       </c>
@@ -7888,7 +7914,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>31</v>
       </c>
@@ -7965,7 +7991,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>31</v>
       </c>
@@ -8042,7 +8068,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>32</v>
       </c>
@@ -8116,7 +8142,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>33</v>
       </c>
@@ -8190,7 +8216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>33</v>
       </c>
@@ -8264,7 +8290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>33</v>
       </c>
@@ -8338,7 +8364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>34</v>
       </c>
@@ -9533,7 +9559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>38</v>
       </c>
@@ -9601,7 +9627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>38</v>
       </c>
@@ -9669,7 +9695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>39</v>
       </c>
@@ -9743,7 +9769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>39</v>
       </c>
@@ -9817,7 +9843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>39</v>
       </c>
@@ -9891,7 +9917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>40</v>
       </c>
@@ -9965,7 +9991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>41</v>
       </c>
@@ -10033,7 +10059,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>42</v>
       </c>
@@ -10106,11 +10132,11 @@
       <c r="AA136" t="s">
         <v>37</v>
       </c>
-      <c r="AC136" t="s">
+      <c r="AD136" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>43</v>
       </c>
@@ -10178,7 +10204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>44</v>
       </c>
@@ -10249,7 +10275,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>45</v>
       </c>
@@ -10317,7 +10343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>46</v>
       </c>
@@ -10389,6 +10415,148 @@
       </c>
       <c r="AA140">
         <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>47</v>
+      </c>
+      <c r="B141">
+        <v>2021</v>
+      </c>
+      <c r="C141">
+        <v>16</v>
+      </c>
+      <c r="D141">
+        <v>12</v>
+      </c>
+      <c r="E141">
+        <v>12</v>
+      </c>
+      <c r="F141" t="s">
+        <v>26</v>
+      </c>
+      <c r="G141" t="s">
+        <v>7</v>
+      </c>
+      <c r="H141" t="s">
+        <v>28</v>
+      </c>
+      <c r="I141">
+        <v>1890</v>
+      </c>
+      <c r="J141">
+        <v>1</v>
+      </c>
+      <c r="K141" t="s">
+        <v>30</v>
+      </c>
+      <c r="L141">
+        <v>11</v>
+      </c>
+      <c r="M141">
+        <v>2</v>
+      </c>
+      <c r="N141">
+        <v>1</v>
+      </c>
+      <c r="O141">
+        <v>7</v>
+      </c>
+      <c r="P141">
+        <v>4</v>
+      </c>
+      <c r="Q141">
+        <v>24</v>
+      </c>
+      <c r="R141">
+        <v>17</v>
+      </c>
+      <c r="U141" t="s">
+        <v>30</v>
+      </c>
+      <c r="V141">
+        <v>2</v>
+      </c>
+      <c r="W141">
+        <v>16</v>
+      </c>
+      <c r="X141">
+        <v>15</v>
+      </c>
+      <c r="Y141" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA141" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="142" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>48</v>
+      </c>
+      <c r="B142">
+        <v>2021</v>
+      </c>
+      <c r="C142">
+        <v>15</v>
+      </c>
+      <c r="D142">
+        <v>12</v>
+      </c>
+      <c r="E142">
+        <v>9</v>
+      </c>
+      <c r="F142" t="s">
+        <v>40</v>
+      </c>
+      <c r="G142" t="s">
+        <v>7</v>
+      </c>
+      <c r="H142" t="s">
+        <v>28</v>
+      </c>
+      <c r="I142">
+        <v>798</v>
+      </c>
+      <c r="J142">
+        <v>2</v>
+      </c>
+      <c r="K142" t="s">
+        <v>37</v>
+      </c>
+      <c r="L142">
+        <v>8</v>
+      </c>
+      <c r="M142">
+        <v>2</v>
+      </c>
+      <c r="N142">
+        <v>1</v>
+      </c>
+      <c r="O142">
+        <v>8</v>
+      </c>
+      <c r="P142">
+        <v>5</v>
+      </c>
+      <c r="Q142">
+        <v>25</v>
+      </c>
+      <c r="R142">
+        <v>17</v>
+      </c>
+      <c r="V142">
+        <v>2</v>
+      </c>
+      <c r="W142">
+        <v>16</v>
+      </c>
+      <c r="X142">
+        <v>12</v>
+      </c>
+      <c r="AC142">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ opinionway poll (12/16)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4868D5D-3588-BC47-AC6C-8200B87F450D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C247F37E-E7C7-6741-8E51-64FB77AEC2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="17520" windowWidth="32720" windowHeight="11180" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="45">
   <si>
     <t>year</t>
   </si>
@@ -535,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AD142"/>
+  <dimension ref="A1:AD143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD142" sqref="AD142"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AE143" sqref="AE143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10557,6 +10557,74 @@
       </c>
       <c r="AC142">
         <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>49</v>
+      </c>
+      <c r="B143">
+        <v>2021</v>
+      </c>
+      <c r="C143">
+        <v>16</v>
+      </c>
+      <c r="D143">
+        <v>12</v>
+      </c>
+      <c r="E143">
+        <v>14</v>
+      </c>
+      <c r="F143" t="s">
+        <v>40</v>
+      </c>
+      <c r="G143" t="s">
+        <v>7</v>
+      </c>
+      <c r="H143" t="s">
+        <v>28</v>
+      </c>
+      <c r="I143">
+        <v>1235</v>
+      </c>
+      <c r="J143">
+        <v>1</v>
+      </c>
+      <c r="K143">
+        <v>1</v>
+      </c>
+      <c r="L143">
+        <v>9</v>
+      </c>
+      <c r="M143">
+        <v>3</v>
+      </c>
+      <c r="N143">
+        <v>2</v>
+      </c>
+      <c r="O143">
+        <v>8</v>
+      </c>
+      <c r="P143">
+        <v>4</v>
+      </c>
+      <c r="Q143">
+        <v>24</v>
+      </c>
+      <c r="R143">
+        <v>17</v>
+      </c>
+      <c r="U143">
+        <v>1</v>
+      </c>
+      <c r="V143">
+        <v>2</v>
+      </c>
+      <c r="W143">
+        <v>16</v>
+      </c>
+      <c r="X143">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ cluster17 poll (12/17)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C247F37E-E7C7-6741-8E51-64FB77AEC2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520EA531-4AC8-2349-8933-04EB2503D80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="17520" windowWidth="32720" windowHeight="11180" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="45">
   <si>
     <t>year</t>
   </si>
@@ -535,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AD143"/>
+  <dimension ref="A1:AD144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AE143" sqref="AE143"/>
+      <selection pane="bottomLeft" activeCell="AB144" sqref="AB144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10625,6 +10625,80 @@
       </c>
       <c r="X143">
         <v>12</v>
+      </c>
+    </row>
+    <row r="144" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>50</v>
+      </c>
+      <c r="B144">
+        <v>2021</v>
+      </c>
+      <c r="C144">
+        <v>16</v>
+      </c>
+      <c r="D144">
+        <v>12</v>
+      </c>
+      <c r="E144">
+        <v>14</v>
+      </c>
+      <c r="F144" t="s">
+        <v>42</v>
+      </c>
+      <c r="G144" t="s">
+        <v>7</v>
+      </c>
+      <c r="H144" t="s">
+        <v>27</v>
+      </c>
+      <c r="I144">
+        <v>1446</v>
+      </c>
+      <c r="J144">
+        <v>1</v>
+      </c>
+      <c r="K144">
+        <v>0.5</v>
+      </c>
+      <c r="L144">
+        <v>13</v>
+      </c>
+      <c r="M144">
+        <v>2</v>
+      </c>
+      <c r="N144">
+        <v>1</v>
+      </c>
+      <c r="O144">
+        <v>5</v>
+      </c>
+      <c r="P144">
+        <v>3</v>
+      </c>
+      <c r="Q144">
+        <v>22</v>
+      </c>
+      <c r="R144">
+        <v>18</v>
+      </c>
+      <c r="U144">
+        <v>1</v>
+      </c>
+      <c r="V144">
+        <v>1.5</v>
+      </c>
+      <c r="W144">
+        <v>15</v>
+      </c>
+      <c r="X144">
+        <v>15</v>
+      </c>
+      <c r="Y144">
+        <v>1</v>
+      </c>
+      <c r="AA144">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ ipsos poll (12/18)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520EA531-4AC8-2349-8933-04EB2503D80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A300E1D-33D3-6447-9B30-7BD86A303A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="17520" windowWidth="32720" windowHeight="11180" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="45">
   <si>
     <t>year</t>
   </si>
@@ -535,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AD144"/>
+  <dimension ref="A1:AD145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AB144" sqref="AB144"/>
+      <selection pane="bottomLeft" activeCell="I145" sqref="I145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10699,6 +10699,74 @@
       </c>
       <c r="AA144">
         <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>51</v>
+      </c>
+      <c r="B145">
+        <v>2021</v>
+      </c>
+      <c r="C145">
+        <v>15</v>
+      </c>
+      <c r="D145">
+        <v>12</v>
+      </c>
+      <c r="E145">
+        <v>10</v>
+      </c>
+      <c r="F145" t="s">
+        <v>6</v>
+      </c>
+      <c r="G145" t="s">
+        <v>7</v>
+      </c>
+      <c r="H145" t="s">
+        <v>27</v>
+      </c>
+      <c r="I145">
+        <v>6266</v>
+      </c>
+      <c r="J145">
+        <v>1.5</v>
+      </c>
+      <c r="K145">
+        <v>0.5</v>
+      </c>
+      <c r="L145">
+        <v>8.5</v>
+      </c>
+      <c r="M145">
+        <v>2</v>
+      </c>
+      <c r="N145">
+        <v>1.5</v>
+      </c>
+      <c r="O145">
+        <v>8.5</v>
+      </c>
+      <c r="P145">
+        <v>4.5</v>
+      </c>
+      <c r="Q145">
+        <v>24</v>
+      </c>
+      <c r="R145">
+        <v>17</v>
+      </c>
+      <c r="U145">
+        <v>1</v>
+      </c>
+      <c r="V145">
+        <v>2</v>
+      </c>
+      <c r="W145">
+        <v>14.5</v>
+      </c>
+      <c r="X145">
+        <v>14.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ ifop poll (12/20)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A300E1D-33D3-6447-9B30-7BD86A303A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FAD45D-E50C-FA4E-88C8-8A27EE6168E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="17520" windowWidth="32720" windowHeight="11180" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="45">
   <si>
     <t>year</t>
   </si>
@@ -535,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AD145"/>
+  <dimension ref="A1:AD146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I145" sqref="I145"/>
+      <selection pane="bottomLeft" activeCell="AC146" sqref="AC146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10767,6 +10767,74 @@
       </c>
       <c r="X145">
         <v>14.5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>52</v>
+      </c>
+      <c r="B146">
+        <v>2021</v>
+      </c>
+      <c r="C146">
+        <v>16</v>
+      </c>
+      <c r="D146">
+        <v>12</v>
+      </c>
+      <c r="E146">
+        <v>15</v>
+      </c>
+      <c r="F146" t="s">
+        <v>35</v>
+      </c>
+      <c r="G146" t="s">
+        <v>7</v>
+      </c>
+      <c r="H146" t="s">
+        <v>28</v>
+      </c>
+      <c r="I146">
+        <v>1017</v>
+      </c>
+      <c r="J146">
+        <v>0.5</v>
+      </c>
+      <c r="K146" t="s">
+        <v>30</v>
+      </c>
+      <c r="L146">
+        <v>9.5</v>
+      </c>
+      <c r="M146">
+        <v>3</v>
+      </c>
+      <c r="N146">
+        <v>1</v>
+      </c>
+      <c r="O146">
+        <v>7.5</v>
+      </c>
+      <c r="P146">
+        <v>4.5</v>
+      </c>
+      <c r="Q146">
+        <v>25.5</v>
+      </c>
+      <c r="R146">
+        <v>18</v>
+      </c>
+      <c r="U146">
+        <v>0.5</v>
+      </c>
+      <c r="V146">
+        <v>2</v>
+      </c>
+      <c r="W146">
+        <v>16</v>
+      </c>
+      <c r="X146">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ elabe poll (12/19)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FAD45D-E50C-FA4E-88C8-8A27EE6168E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823916A9-0A6A-2044-9AFB-5675F8631284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="17520" windowWidth="32720" windowHeight="11180" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="160" yWindow="6720" windowWidth="28020" windowHeight="9460" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AB$133</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="45">
   <si>
     <t>year</t>
   </si>
@@ -535,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AD146"/>
+  <dimension ref="A1:AD148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AC146" sqref="AC146"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD148" sqref="AD148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10701,7 +10701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>51</v>
       </c>
@@ -10769,7 +10769,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>52</v>
       </c>
@@ -10835,6 +10835,160 @@
       </c>
       <c r="X146">
         <v>12</v>
+      </c>
+    </row>
+    <row r="147" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>53</v>
+      </c>
+      <c r="B147">
+        <v>2021</v>
+      </c>
+      <c r="C147">
+        <v>16</v>
+      </c>
+      <c r="D147">
+        <v>12</v>
+      </c>
+      <c r="E147">
+        <v>19</v>
+      </c>
+      <c r="F147" t="s">
+        <v>36</v>
+      </c>
+      <c r="G147" t="s">
+        <v>7</v>
+      </c>
+      <c r="H147" t="s">
+        <v>27</v>
+      </c>
+      <c r="I147">
+        <v>919</v>
+      </c>
+      <c r="J147">
+        <v>1</v>
+      </c>
+      <c r="K147">
+        <v>1</v>
+      </c>
+      <c r="L147">
+        <v>11</v>
+      </c>
+      <c r="M147">
+        <v>1</v>
+      </c>
+      <c r="N147">
+        <v>2</v>
+      </c>
+      <c r="O147">
+        <v>5</v>
+      </c>
+      <c r="P147">
+        <v>3</v>
+      </c>
+      <c r="Q147">
+        <v>26</v>
+      </c>
+      <c r="R147">
+        <v>17</v>
+      </c>
+      <c r="U147">
+        <v>1</v>
+      </c>
+      <c r="V147">
+        <v>2</v>
+      </c>
+      <c r="W147">
+        <v>16</v>
+      </c>
+      <c r="X147">
+        <v>13</v>
+      </c>
+      <c r="Y147" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA147">
+        <v>1</v>
+      </c>
+      <c r="AD147" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="148" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>54</v>
+      </c>
+      <c r="B148">
+        <v>2021</v>
+      </c>
+      <c r="C148">
+        <v>17</v>
+      </c>
+      <c r="D148">
+        <v>12</v>
+      </c>
+      <c r="E148">
+        <v>21</v>
+      </c>
+      <c r="F148" t="s">
+        <v>42</v>
+      </c>
+      <c r="G148" t="s">
+        <v>7</v>
+      </c>
+      <c r="H148" t="s">
+        <v>27</v>
+      </c>
+      <c r="I148">
+        <v>1419</v>
+      </c>
+      <c r="J148">
+        <v>1.5</v>
+      </c>
+      <c r="K148">
+        <v>0.5</v>
+      </c>
+      <c r="L148">
+        <v>12</v>
+      </c>
+      <c r="M148">
+        <v>1.5</v>
+      </c>
+      <c r="N148">
+        <v>1.5</v>
+      </c>
+      <c r="O148">
+        <v>5</v>
+      </c>
+      <c r="P148">
+        <v>2</v>
+      </c>
+      <c r="Q148">
+        <v>20</v>
+      </c>
+      <c r="R148">
+        <v>16</v>
+      </c>
+      <c r="U148">
+        <v>1</v>
+      </c>
+      <c r="V148">
+        <v>2</v>
+      </c>
+      <c r="W148">
+        <v>13</v>
+      </c>
+      <c r="X148">
+        <v>14</v>
+      </c>
+      <c r="Y148">
+        <v>1</v>
+      </c>
+      <c r="AA148">
+        <v>1</v>
+      </c>
+      <c r="AC148">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ opinionway polls (12/29 and 1/3) and cluster17 poll (12/29)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823916A9-0A6A-2044-9AFB-5675F8631284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4901F51-8251-8949-A14A-6849A2996FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="6720" windowWidth="28020" windowHeight="9460" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="45">
   <si>
     <t>year</t>
   </si>
@@ -535,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AD148"/>
+  <dimension ref="A1:AD151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD148" sqref="AD148"/>
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD151" sqref="AD151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10989,6 +10989,222 @@
       </c>
       <c r="AC148">
         <v>7</v>
+      </c>
+    </row>
+    <row r="149" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>55</v>
+      </c>
+      <c r="B149">
+        <v>2021</v>
+      </c>
+      <c r="C149">
+        <v>17</v>
+      </c>
+      <c r="D149">
+        <v>12</v>
+      </c>
+      <c r="E149">
+        <v>22</v>
+      </c>
+      <c r="F149" t="s">
+        <v>40</v>
+      </c>
+      <c r="G149" t="s">
+        <v>7</v>
+      </c>
+      <c r="H149" t="s">
+        <v>28</v>
+      </c>
+      <c r="I149">
+        <v>985</v>
+      </c>
+      <c r="J149">
+        <v>1</v>
+      </c>
+      <c r="K149" t="s">
+        <v>37</v>
+      </c>
+      <c r="L149">
+        <v>8</v>
+      </c>
+      <c r="M149">
+        <v>2</v>
+      </c>
+      <c r="N149">
+        <v>1</v>
+      </c>
+      <c r="O149">
+        <v>6</v>
+      </c>
+      <c r="P149">
+        <v>4</v>
+      </c>
+      <c r="Q149">
+        <v>26</v>
+      </c>
+      <c r="R149">
+        <v>18</v>
+      </c>
+      <c r="U149">
+        <v>1</v>
+      </c>
+      <c r="V149">
+        <v>2</v>
+      </c>
+      <c r="W149">
+        <v>16</v>
+      </c>
+      <c r="X149">
+        <v>12</v>
+      </c>
+      <c r="AC149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>56</v>
+      </c>
+      <c r="B150">
+        <v>2022</v>
+      </c>
+      <c r="C150">
+        <v>18</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>2</v>
+      </c>
+      <c r="F150" t="s">
+        <v>40</v>
+      </c>
+      <c r="G150" t="s">
+        <v>7</v>
+      </c>
+      <c r="H150" t="s">
+        <v>28</v>
+      </c>
+      <c r="I150">
+        <v>1059</v>
+      </c>
+      <c r="J150">
+        <v>1</v>
+      </c>
+      <c r="K150">
+        <v>1</v>
+      </c>
+      <c r="L150">
+        <v>9</v>
+      </c>
+      <c r="M150">
+        <v>3</v>
+      </c>
+      <c r="N150">
+        <v>1</v>
+      </c>
+      <c r="O150">
+        <v>7</v>
+      </c>
+      <c r="P150">
+        <v>4</v>
+      </c>
+      <c r="Q150">
+        <v>26</v>
+      </c>
+      <c r="R150">
+        <v>16</v>
+      </c>
+      <c r="U150">
+        <v>1</v>
+      </c>
+      <c r="V150">
+        <v>2</v>
+      </c>
+      <c r="W150">
+        <v>16</v>
+      </c>
+      <c r="X150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="151" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>57</v>
+      </c>
+      <c r="B151">
+        <v>2021</v>
+      </c>
+      <c r="C151">
+        <v>18</v>
+      </c>
+      <c r="D151">
+        <v>12</v>
+      </c>
+      <c r="E151">
+        <v>29</v>
+      </c>
+      <c r="F151" t="s">
+        <v>42</v>
+      </c>
+      <c r="G151" t="s">
+        <v>7</v>
+      </c>
+      <c r="H151" t="s">
+        <v>27</v>
+      </c>
+      <c r="I151">
+        <v>2176</v>
+      </c>
+      <c r="J151">
+        <v>1</v>
+      </c>
+      <c r="K151">
+        <v>0.5</v>
+      </c>
+      <c r="L151">
+        <v>13</v>
+      </c>
+      <c r="M151">
+        <v>1.5</v>
+      </c>
+      <c r="N151">
+        <v>1.5</v>
+      </c>
+      <c r="O151">
+        <v>4</v>
+      </c>
+      <c r="P151">
+        <v>2</v>
+      </c>
+      <c r="Q151">
+        <v>23</v>
+      </c>
+      <c r="R151">
+        <v>15</v>
+      </c>
+      <c r="U151">
+        <v>1</v>
+      </c>
+      <c r="V151">
+        <v>1.5</v>
+      </c>
+      <c r="W151">
+        <v>14.5</v>
+      </c>
+      <c r="X151">
+        <v>15</v>
+      </c>
+      <c r="Y151">
+        <v>1</v>
+      </c>
+      <c r="AA151">
+        <v>1</v>
+      </c>
+      <c r="AC151">
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ harris poll (12/31) and ow rolling poll (1/6)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4901F51-8251-8949-A14A-6849A2996FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529EA915-466F-3645-AB8C-79D2CACE6CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="45">
   <si>
     <t>year</t>
   </si>
@@ -535,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AD151"/>
+  <dimension ref="A1:AD153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD151" sqref="AD151"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="Y154" sqref="Y154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11070,13 +11070,13 @@
         <v>2022</v>
       </c>
       <c r="C150">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D150">
         <v>1</v>
       </c>
       <c r="E150">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F150" t="s">
         <v>40</v>
@@ -11088,7 +11088,7 @@
         <v>28</v>
       </c>
       <c r="I150">
-        <v>1059</v>
+        <v>761</v>
       </c>
       <c r="J150">
         <v>1</v>
@@ -11205,6 +11205,148 @@
       </c>
       <c r="AC151">
         <v>4.5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>58</v>
+      </c>
+      <c r="B152">
+        <v>2022</v>
+      </c>
+      <c r="C152">
+        <v>19</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="E152">
+        <v>5</v>
+      </c>
+      <c r="F152" t="s">
+        <v>40</v>
+      </c>
+      <c r="G152" t="s">
+        <v>7</v>
+      </c>
+      <c r="H152" t="s">
+        <v>27</v>
+      </c>
+      <c r="I152">
+        <v>1534</v>
+      </c>
+      <c r="J152">
+        <v>1</v>
+      </c>
+      <c r="K152">
+        <v>1</v>
+      </c>
+      <c r="L152">
+        <v>9</v>
+      </c>
+      <c r="M152">
+        <v>3</v>
+      </c>
+      <c r="N152">
+        <v>1</v>
+      </c>
+      <c r="O152">
+        <v>7</v>
+      </c>
+      <c r="P152">
+        <v>4</v>
+      </c>
+      <c r="Q152">
+        <v>25</v>
+      </c>
+      <c r="R152">
+        <v>17</v>
+      </c>
+      <c r="U152">
+        <v>1</v>
+      </c>
+      <c r="V152">
+        <v>2</v>
+      </c>
+      <c r="W152">
+        <v>17</v>
+      </c>
+      <c r="X152">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>59</v>
+      </c>
+      <c r="B153">
+        <v>2021</v>
+      </c>
+      <c r="C153">
+        <v>18</v>
+      </c>
+      <c r="D153">
+        <v>12</v>
+      </c>
+      <c r="E153">
+        <v>30</v>
+      </c>
+      <c r="F153" t="s">
+        <v>26</v>
+      </c>
+      <c r="G153" t="s">
+        <v>7</v>
+      </c>
+      <c r="H153" t="s">
+        <v>28</v>
+      </c>
+      <c r="I153">
+        <v>2183</v>
+      </c>
+      <c r="J153">
+        <v>1</v>
+      </c>
+      <c r="K153" t="s">
+        <v>30</v>
+      </c>
+      <c r="L153">
+        <v>10</v>
+      </c>
+      <c r="M153">
+        <v>3</v>
+      </c>
+      <c r="N153">
+        <v>1</v>
+      </c>
+      <c r="O153">
+        <v>7</v>
+      </c>
+      <c r="P153">
+        <v>4</v>
+      </c>
+      <c r="Q153">
+        <v>24</v>
+      </c>
+      <c r="R153">
+        <v>16</v>
+      </c>
+      <c r="U153" t="s">
+        <v>30</v>
+      </c>
+      <c r="V153">
+        <v>2</v>
+      </c>
+      <c r="W153">
+        <v>16</v>
+      </c>
+      <c r="X153">
+        <v>16</v>
+      </c>
+      <c r="Y153" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA153" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ ifop poll (1/6)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529EA915-466F-3645-AB8C-79D2CACE6CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F9A48E-6278-024C-8531-3BE2C58A2415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="28800" yWindow="1440" windowWidth="21600" windowHeight="15700" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="46">
   <si>
     <t>year</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>c_taubira</t>
+  </si>
+  <si>
+    <t>omit</t>
   </si>
 </sst>
 </file>
@@ -535,16 +538,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AD153"/>
+  <dimension ref="A1:AE159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="Y154" sqref="Y154"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="Z148" sqref="Z148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -635,8 +638,11 @@
       <c r="AD1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -701,7 +707,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -766,7 +772,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -831,7 +837,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -896,7 +902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -961,7 +967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1088,7 +1094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1150,7 +1156,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1212,7 +1218,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1280,7 +1286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1348,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1416,7 +1422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1487,7 +1493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1555,7 +1561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
@@ -10701,7 +10707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>51</v>
       </c>
@@ -10769,7 +10775,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="146" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>52</v>
       </c>
@@ -10837,7 +10843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>53</v>
       </c>
@@ -10914,7 +10920,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="148" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>54</v>
       </c>
@@ -10991,7 +10997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>55</v>
       </c>
@@ -11062,7 +11068,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>56</v>
       </c>
@@ -11130,7 +11136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>57</v>
       </c>
@@ -11207,7 +11213,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="152" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>58</v>
       </c>
@@ -11275,7 +11281,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="153" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>59</v>
       </c>
@@ -11347,6 +11353,429 @@
       </c>
       <c r="AA153" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="154" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>59</v>
+      </c>
+      <c r="B154">
+        <v>2021</v>
+      </c>
+      <c r="C154">
+        <v>18</v>
+      </c>
+      <c r="D154">
+        <v>12</v>
+      </c>
+      <c r="E154">
+        <v>30</v>
+      </c>
+      <c r="F154" t="s">
+        <v>26</v>
+      </c>
+      <c r="G154" t="s">
+        <v>7</v>
+      </c>
+      <c r="H154" t="s">
+        <v>28</v>
+      </c>
+      <c r="I154">
+        <v>2183</v>
+      </c>
+      <c r="J154">
+        <v>1</v>
+      </c>
+      <c r="K154">
+        <v>1</v>
+      </c>
+      <c r="L154">
+        <v>10</v>
+      </c>
+      <c r="M154">
+        <v>3</v>
+      </c>
+      <c r="O154">
+        <v>9</v>
+      </c>
+      <c r="Q154">
+        <v>25</v>
+      </c>
+      <c r="R154">
+        <v>17</v>
+      </c>
+      <c r="U154" t="s">
+        <v>30</v>
+      </c>
+      <c r="V154">
+        <v>2</v>
+      </c>
+      <c r="W154">
+        <v>16</v>
+      </c>
+      <c r="X154">
+        <v>16</v>
+      </c>
+      <c r="Y154" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA154" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>59</v>
+      </c>
+      <c r="B155">
+        <v>2021</v>
+      </c>
+      <c r="C155">
+        <v>18</v>
+      </c>
+      <c r="D155">
+        <v>12</v>
+      </c>
+      <c r="E155">
+        <v>30</v>
+      </c>
+      <c r="F155" t="s">
+        <v>26</v>
+      </c>
+      <c r="G155" t="s">
+        <v>7</v>
+      </c>
+      <c r="H155" t="s">
+        <v>28</v>
+      </c>
+      <c r="I155">
+        <v>2183</v>
+      </c>
+      <c r="J155">
+        <v>1</v>
+      </c>
+      <c r="K155">
+        <v>1</v>
+      </c>
+      <c r="L155">
+        <v>11</v>
+      </c>
+      <c r="M155">
+        <v>3</v>
+      </c>
+      <c r="Q155">
+        <v>25</v>
+      </c>
+      <c r="R155">
+        <v>17</v>
+      </c>
+      <c r="U155" t="s">
+        <v>30</v>
+      </c>
+      <c r="V155">
+        <v>2</v>
+      </c>
+      <c r="W155">
+        <v>16</v>
+      </c>
+      <c r="X155">
+        <v>16</v>
+      </c>
+      <c r="Y155" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA155" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC155">
+        <v>8</v>
+      </c>
+      <c r="AE155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>59</v>
+      </c>
+      <c r="B156">
+        <v>2021</v>
+      </c>
+      <c r="C156">
+        <v>18</v>
+      </c>
+      <c r="D156">
+        <v>12</v>
+      </c>
+      <c r="E156">
+        <v>30</v>
+      </c>
+      <c r="F156" t="s">
+        <v>26</v>
+      </c>
+      <c r="G156" t="s">
+        <v>7</v>
+      </c>
+      <c r="H156" t="s">
+        <v>28</v>
+      </c>
+      <c r="I156">
+        <v>2183</v>
+      </c>
+      <c r="J156">
+        <v>1</v>
+      </c>
+      <c r="K156" t="s">
+        <v>30</v>
+      </c>
+      <c r="L156">
+        <v>12</v>
+      </c>
+      <c r="M156">
+        <v>4</v>
+      </c>
+      <c r="P156">
+        <v>7</v>
+      </c>
+      <c r="Q156">
+        <v>26</v>
+      </c>
+      <c r="R156">
+        <v>16</v>
+      </c>
+      <c r="U156" t="s">
+        <v>30</v>
+      </c>
+      <c r="V156">
+        <v>2</v>
+      </c>
+      <c r="W156">
+        <v>16</v>
+      </c>
+      <c r="X156">
+        <v>16</v>
+      </c>
+      <c r="Y156" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA156" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>60</v>
+      </c>
+      <c r="B157">
+        <v>2022</v>
+      </c>
+      <c r="C157">
+        <v>19</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+      <c r="E157">
+        <v>4</v>
+      </c>
+      <c r="F157" t="s">
+        <v>35</v>
+      </c>
+      <c r="G157" t="s">
+        <v>7</v>
+      </c>
+      <c r="H157" t="s">
+        <v>28</v>
+      </c>
+      <c r="I157">
+        <v>1332</v>
+      </c>
+      <c r="J157">
+        <v>1</v>
+      </c>
+      <c r="K157">
+        <v>0.5</v>
+      </c>
+      <c r="L157">
+        <v>8.5</v>
+      </c>
+      <c r="M157">
+        <v>2.5</v>
+      </c>
+      <c r="N157">
+        <v>1</v>
+      </c>
+      <c r="O157">
+        <v>7</v>
+      </c>
+      <c r="P157">
+        <v>3.5</v>
+      </c>
+      <c r="Q157">
+        <v>27</v>
+      </c>
+      <c r="R157">
+        <v>16</v>
+      </c>
+      <c r="U157">
+        <v>1</v>
+      </c>
+      <c r="V157">
+        <v>2.5</v>
+      </c>
+      <c r="W157">
+        <v>16</v>
+      </c>
+      <c r="X157">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>60</v>
+      </c>
+      <c r="B158">
+        <v>2022</v>
+      </c>
+      <c r="C158">
+        <v>19</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+      <c r="E158">
+        <v>4</v>
+      </c>
+      <c r="F158" t="s">
+        <v>35</v>
+      </c>
+      <c r="G158" t="s">
+        <v>7</v>
+      </c>
+      <c r="H158" t="s">
+        <v>28</v>
+      </c>
+      <c r="I158">
+        <v>1332</v>
+      </c>
+      <c r="J158">
+        <v>1</v>
+      </c>
+      <c r="K158">
+        <v>0.5</v>
+      </c>
+      <c r="L158">
+        <v>8.5</v>
+      </c>
+      <c r="M158">
+        <v>2.5</v>
+      </c>
+      <c r="N158">
+        <v>1</v>
+      </c>
+      <c r="O158">
+        <v>6.5</v>
+      </c>
+      <c r="P158">
+        <v>3</v>
+      </c>
+      <c r="Q158">
+        <v>25.5</v>
+      </c>
+      <c r="R158">
+        <v>16</v>
+      </c>
+      <c r="U158">
+        <v>1</v>
+      </c>
+      <c r="V158">
+        <v>2.5</v>
+      </c>
+      <c r="W158">
+        <v>16.5</v>
+      </c>
+      <c r="X158">
+        <v>13</v>
+      </c>
+      <c r="AC158">
+        <v>2.5</v>
+      </c>
+      <c r="AE158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>60</v>
+      </c>
+      <c r="B159">
+        <v>2022</v>
+      </c>
+      <c r="C159">
+        <v>19</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159">
+        <v>4</v>
+      </c>
+      <c r="F159" t="s">
+        <v>35</v>
+      </c>
+      <c r="G159" t="s">
+        <v>7</v>
+      </c>
+      <c r="H159" t="s">
+        <v>28</v>
+      </c>
+      <c r="I159">
+        <v>1332</v>
+      </c>
+      <c r="J159">
+        <v>1</v>
+      </c>
+      <c r="K159">
+        <v>0.5</v>
+      </c>
+      <c r="L159">
+        <v>8.5</v>
+      </c>
+      <c r="M159">
+        <v>2.5</v>
+      </c>
+      <c r="O159">
+        <v>6.5</v>
+      </c>
+      <c r="Q159">
+        <v>26.5</v>
+      </c>
+      <c r="R159">
+        <v>16.5</v>
+      </c>
+      <c r="U159">
+        <v>1</v>
+      </c>
+      <c r="V159">
+        <v>2.5</v>
+      </c>
+      <c r="W159">
+        <v>16.5</v>
+      </c>
+      <c r="X159">
+        <v>13</v>
+      </c>
+      <c r="AC159">
+        <v>5</v>
+      </c>
+      <c r="AE159">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ bva poll (1/7)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F9A48E-6278-024C-8531-3BE2C58A2415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B22D661-8DEF-D047-A00B-FD2E200B40B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="1440" windowWidth="21600" windowHeight="15700" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="46">
   <si>
     <t>year</t>
   </si>
@@ -538,11 +538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AE159"/>
+  <dimension ref="A1:AE160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="Z148" sqref="Z148"/>
+      <selection pane="bottomLeft" activeCell="Y160" sqref="Y160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11776,6 +11776,77 @@
       </c>
       <c r="AE159">
         <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>61</v>
+      </c>
+      <c r="B160">
+        <v>2022</v>
+      </c>
+      <c r="C160">
+        <v>19</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+      <c r="E160">
+        <v>6</v>
+      </c>
+      <c r="F160" t="s">
+        <v>41</v>
+      </c>
+      <c r="G160" t="s">
+        <v>7</v>
+      </c>
+      <c r="H160" t="s">
+        <v>8</v>
+      </c>
+      <c r="I160">
+        <v>892</v>
+      </c>
+      <c r="J160">
+        <v>1</v>
+      </c>
+      <c r="K160">
+        <v>0.5</v>
+      </c>
+      <c r="L160">
+        <v>10</v>
+      </c>
+      <c r="M160">
+        <v>1.5</v>
+      </c>
+      <c r="N160">
+        <v>1.5</v>
+      </c>
+      <c r="O160">
+        <v>8</v>
+      </c>
+      <c r="P160">
+        <v>3.5</v>
+      </c>
+      <c r="Q160">
+        <v>25</v>
+      </c>
+      <c r="R160">
+        <v>16</v>
+      </c>
+      <c r="U160">
+        <v>1.5</v>
+      </c>
+      <c r="V160">
+        <v>2</v>
+      </c>
+      <c r="W160">
+        <v>17</v>
+      </c>
+      <c r="X160">
+        <v>12</v>
+      </c>
+      <c r="Y160">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ ipsos poll (1/7)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B22D661-8DEF-D047-A00B-FD2E200B40B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA45CE1-B803-3445-9C58-5FFC89C7F07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="3600" yWindow="1400" windowWidth="21600" windowHeight="15700" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="46">
   <si>
     <t>year</t>
   </si>
@@ -538,11 +538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AE160"/>
+  <dimension ref="A1:AE162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="Y160" sqref="Y160"/>
+      <selection pane="bottomLeft" activeCell="J162" sqref="J162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11847,6 +11847,148 @@
       </c>
       <c r="Y160">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>62</v>
+      </c>
+      <c r="B161">
+        <v>2022</v>
+      </c>
+      <c r="C161">
+        <v>19</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>6</v>
+      </c>
+      <c r="F161" t="s">
+        <v>6</v>
+      </c>
+      <c r="G161" t="s">
+        <v>7</v>
+      </c>
+      <c r="H161" t="s">
+        <v>8</v>
+      </c>
+      <c r="I161">
+        <v>725</v>
+      </c>
+      <c r="J161">
+        <v>1</v>
+      </c>
+      <c r="K161">
+        <v>1</v>
+      </c>
+      <c r="L161">
+        <v>9</v>
+      </c>
+      <c r="M161">
+        <v>2</v>
+      </c>
+      <c r="N161">
+        <v>1</v>
+      </c>
+      <c r="O161">
+        <v>8</v>
+      </c>
+      <c r="P161">
+        <v>4.5</v>
+      </c>
+      <c r="Q161">
+        <v>26</v>
+      </c>
+      <c r="R161">
+        <v>16</v>
+      </c>
+      <c r="U161">
+        <v>1</v>
+      </c>
+      <c r="V161">
+        <v>1.5</v>
+      </c>
+      <c r="W161">
+        <v>17</v>
+      </c>
+      <c r="X161">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="162" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>62</v>
+      </c>
+      <c r="B162">
+        <v>2022</v>
+      </c>
+      <c r="C162">
+        <v>19</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+      <c r="E162">
+        <v>6</v>
+      </c>
+      <c r="F162" t="s">
+        <v>6</v>
+      </c>
+      <c r="G162" t="s">
+        <v>7</v>
+      </c>
+      <c r="H162" t="s">
+        <v>8</v>
+      </c>
+      <c r="I162">
+        <v>725</v>
+      </c>
+      <c r="J162">
+        <v>1</v>
+      </c>
+      <c r="K162">
+        <v>1</v>
+      </c>
+      <c r="L162">
+        <v>9</v>
+      </c>
+      <c r="M162">
+        <v>2</v>
+      </c>
+      <c r="N162">
+        <v>1</v>
+      </c>
+      <c r="O162">
+        <v>7</v>
+      </c>
+      <c r="P162">
+        <v>3</v>
+      </c>
+      <c r="Q162">
+        <v>25.5</v>
+      </c>
+      <c r="R162">
+        <v>16</v>
+      </c>
+      <c r="U162">
+        <v>1</v>
+      </c>
+      <c r="V162">
+        <v>1.5</v>
+      </c>
+      <c r="W162">
+        <v>17</v>
+      </c>
+      <c r="X162">
+        <v>12</v>
+      </c>
+      <c r="AC162">
+        <v>3</v>
+      </c>
+      <c r="AE162">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ ifop rolling (1/10)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64ED1F4B-2673-854C-880D-8BCEC4544D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F53DD6-DC37-1045-82A0-F3602FBC23EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="11500" windowWidth="21600" windowHeight="15700" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="7300" yWindow="12820" windowWidth="21600" windowHeight="15700" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF162"/>
+  <dimension ref="A1:AF164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="J157" sqref="J157"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="J165" sqref="J165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12477,6 +12477,160 @@
         <v>3</v>
       </c>
       <c r="AF162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>63</v>
+      </c>
+      <c r="B163">
+        <v>2022</v>
+      </c>
+      <c r="C163">
+        <v>19</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="E163">
+        <v>8</v>
+      </c>
+      <c r="F163" t="s">
+        <v>35</v>
+      </c>
+      <c r="G163" t="s">
+        <v>7</v>
+      </c>
+      <c r="H163" t="s">
+        <v>28</v>
+      </c>
+      <c r="I163">
+        <v>1</v>
+      </c>
+      <c r="J163">
+        <v>1034</v>
+      </c>
+      <c r="K163">
+        <v>1</v>
+      </c>
+      <c r="L163">
+        <v>0.5</v>
+      </c>
+      <c r="M163">
+        <v>9.5</v>
+      </c>
+      <c r="N163">
+        <v>2.5</v>
+      </c>
+      <c r="O163">
+        <v>0.5</v>
+      </c>
+      <c r="P163">
+        <v>6</v>
+      </c>
+      <c r="Q163">
+        <v>4</v>
+      </c>
+      <c r="R163">
+        <v>27</v>
+      </c>
+      <c r="S163">
+        <v>15.5</v>
+      </c>
+      <c r="V163">
+        <v>1</v>
+      </c>
+      <c r="W163">
+        <v>2</v>
+      </c>
+      <c r="X163">
+        <v>17.5</v>
+      </c>
+      <c r="Y163">
+        <v>12.5</v>
+      </c>
+      <c r="AE163">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>63</v>
+      </c>
+      <c r="B164">
+        <v>2022</v>
+      </c>
+      <c r="C164">
+        <v>19</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164">
+        <v>8</v>
+      </c>
+      <c r="F164" t="s">
+        <v>35</v>
+      </c>
+      <c r="G164" t="s">
+        <v>7</v>
+      </c>
+      <c r="H164" t="s">
+        <v>28</v>
+      </c>
+      <c r="I164">
+        <v>1</v>
+      </c>
+      <c r="J164">
+        <v>1042</v>
+      </c>
+      <c r="K164">
+        <v>1</v>
+      </c>
+      <c r="L164">
+        <v>0.5</v>
+      </c>
+      <c r="M164">
+        <v>8.5</v>
+      </c>
+      <c r="N164">
+        <v>2.5</v>
+      </c>
+      <c r="O164">
+        <v>0.5</v>
+      </c>
+      <c r="P164">
+        <v>5.5</v>
+      </c>
+      <c r="Q164">
+        <v>3.5</v>
+      </c>
+      <c r="R164">
+        <v>26</v>
+      </c>
+      <c r="S164">
+        <v>16</v>
+      </c>
+      <c r="V164">
+        <v>1</v>
+      </c>
+      <c r="W164">
+        <v>2</v>
+      </c>
+      <c r="X164">
+        <v>17</v>
+      </c>
+      <c r="Y164">
+        <v>12.5</v>
+      </c>
+      <c r="AD164">
+        <v>3.5</v>
+      </c>
+      <c r="AE164">
+        <v>0.5</v>
+      </c>
+      <c r="AF164">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update w/ opinion way and cluster17 polls (1/11)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F53DD6-DC37-1045-82A0-F3602FBC23EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B522D24-5058-7640-8415-BAE5F226ECD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7300" yWindow="12820" windowWidth="21600" windowHeight="15700" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="1160" yWindow="9440" windowWidth="44500" windowHeight="15700" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF164"/>
+  <dimension ref="A1:AF166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="J165" sqref="J165"/>
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="J167" sqref="J167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12109,6 +12109,9 @@
       <c r="Y157">
         <v>13.5</v>
       </c>
+      <c r="AF157">
+        <v>1</v>
+      </c>
     </row>
     <row r="158" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A158">
@@ -12183,9 +12186,6 @@
       <c r="AD158">
         <v>2.5</v>
       </c>
-      <c r="AF158">
-        <v>1</v>
-      </c>
     </row>
     <row r="159" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A159">
@@ -12402,6 +12402,9 @@
       <c r="Y161">
         <v>12</v>
       </c>
+      <c r="AF161">
+        <v>1</v>
+      </c>
     </row>
     <row r="162" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A162">
@@ -12476,9 +12479,6 @@
       <c r="AD162">
         <v>3</v>
       </c>
-      <c r="AF162">
-        <v>1</v>
-      </c>
     </row>
     <row r="163" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A163">
@@ -12553,6 +12553,9 @@
       <c r="AE163">
         <v>0.5</v>
       </c>
+      <c r="AF163">
+        <v>1</v>
+      </c>
     </row>
     <row r="164" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A164">
@@ -12630,8 +12633,156 @@
       <c r="AE164">
         <v>0.5</v>
       </c>
-      <c r="AF164">
-        <v>1</v>
+    </row>
+    <row r="165" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>64</v>
+      </c>
+      <c r="B165">
+        <v>2022</v>
+      </c>
+      <c r="C165">
+        <v>19</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>6</v>
+      </c>
+      <c r="F165" t="s">
+        <v>42</v>
+      </c>
+      <c r="G165" t="s">
+        <v>7</v>
+      </c>
+      <c r="H165" t="s">
+        <v>27</v>
+      </c>
+      <c r="I165">
+        <v>0</v>
+      </c>
+      <c r="J165">
+        <v>2192</v>
+      </c>
+      <c r="K165">
+        <v>1.5</v>
+      </c>
+      <c r="L165">
+        <v>0.5</v>
+      </c>
+      <c r="M165">
+        <v>12.5</v>
+      </c>
+      <c r="N165">
+        <v>2</v>
+      </c>
+      <c r="O165">
+        <v>0.5</v>
+      </c>
+      <c r="P165">
+        <v>4.5</v>
+      </c>
+      <c r="Q165">
+        <v>2</v>
+      </c>
+      <c r="R165">
+        <v>23</v>
+      </c>
+      <c r="S165">
+        <v>14</v>
+      </c>
+      <c r="V165">
+        <v>1</v>
+      </c>
+      <c r="W165">
+        <v>2</v>
+      </c>
+      <c r="X165">
+        <v>15</v>
+      </c>
+      <c r="Y165">
+        <v>13.5</v>
+      </c>
+      <c r="Z165">
+        <v>1</v>
+      </c>
+      <c r="AB165">
+        <v>1.5</v>
+      </c>
+      <c r="AD165">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>65</v>
+      </c>
+      <c r="B166">
+        <v>2022</v>
+      </c>
+      <c r="C166">
+        <v>20</v>
+      </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+      <c r="E166">
+        <v>10</v>
+      </c>
+      <c r="F166" t="s">
+        <v>40</v>
+      </c>
+      <c r="G166" t="s">
+        <v>7</v>
+      </c>
+      <c r="H166" t="s">
+        <v>27</v>
+      </c>
+      <c r="I166">
+        <v>1</v>
+      </c>
+      <c r="J166">
+        <v>997</v>
+      </c>
+      <c r="K166">
+        <v>2</v>
+      </c>
+      <c r="L166">
+        <v>1</v>
+      </c>
+      <c r="M166">
+        <v>9</v>
+      </c>
+      <c r="N166">
+        <v>2</v>
+      </c>
+      <c r="O166">
+        <v>1</v>
+      </c>
+      <c r="P166">
+        <v>8</v>
+      </c>
+      <c r="Q166">
+        <v>4</v>
+      </c>
+      <c r="R166">
+        <v>25</v>
+      </c>
+      <c r="S166">
+        <v>16</v>
+      </c>
+      <c r="V166">
+        <v>2</v>
+      </c>
+      <c r="W166">
+        <v>2</v>
+      </c>
+      <c r="X166">
+        <v>17</v>
+      </c>
+      <c r="Y166">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ elabe poll (1/12)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B522D24-5058-7640-8415-BAE5F226ECD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2CB04C-02E6-5C4D-8822-1DFC6998F2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="9440" windowWidth="44500" windowHeight="15700" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="1160" yWindow="9440" windowWidth="22320" windowHeight="15700" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF166"/>
+  <dimension ref="A1:AF169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="J167" sqref="J167"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AC169" sqref="AC169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12783,6 +12783,249 @@
       </c>
       <c r="Y166">
         <v>12</v>
+      </c>
+    </row>
+    <row r="167" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>66</v>
+      </c>
+      <c r="B167">
+        <v>2022</v>
+      </c>
+      <c r="C167">
+        <v>20</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+      <c r="E167">
+        <v>11</v>
+      </c>
+      <c r="F167" t="s">
+        <v>36</v>
+      </c>
+      <c r="G167" t="s">
+        <v>7</v>
+      </c>
+      <c r="H167" t="s">
+        <v>27</v>
+      </c>
+      <c r="I167">
+        <v>0</v>
+      </c>
+      <c r="J167">
+        <v>943</v>
+      </c>
+      <c r="K167">
+        <v>1.5</v>
+      </c>
+      <c r="L167">
+        <v>1</v>
+      </c>
+      <c r="M167">
+        <v>9.5</v>
+      </c>
+      <c r="N167">
+        <v>1.5</v>
+      </c>
+      <c r="O167">
+        <v>1</v>
+      </c>
+      <c r="P167">
+        <v>7</v>
+      </c>
+      <c r="Q167">
+        <v>3.5</v>
+      </c>
+      <c r="R167">
+        <v>23</v>
+      </c>
+      <c r="S167">
+        <v>17</v>
+      </c>
+      <c r="V167">
+        <v>2</v>
+      </c>
+      <c r="W167">
+        <v>1.5</v>
+      </c>
+      <c r="X167">
+        <v>17</v>
+      </c>
+      <c r="Y167">
+        <v>13</v>
+      </c>
+      <c r="Z167" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB167">
+        <v>1</v>
+      </c>
+      <c r="AE167">
+        <v>0.5</v>
+      </c>
+      <c r="AF167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>66</v>
+      </c>
+      <c r="B168">
+        <v>2022</v>
+      </c>
+      <c r="C168">
+        <v>20</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="E168">
+        <v>11</v>
+      </c>
+      <c r="F168" t="s">
+        <v>36</v>
+      </c>
+      <c r="G168" t="s">
+        <v>7</v>
+      </c>
+      <c r="H168" t="s">
+        <v>27</v>
+      </c>
+      <c r="I168">
+        <v>0</v>
+      </c>
+      <c r="J168">
+        <v>953</v>
+      </c>
+      <c r="K168">
+        <v>1</v>
+      </c>
+      <c r="L168">
+        <v>0.5</v>
+      </c>
+      <c r="M168">
+        <v>10</v>
+      </c>
+      <c r="N168">
+        <v>1.5</v>
+      </c>
+      <c r="O168">
+        <v>1</v>
+      </c>
+      <c r="P168">
+        <v>6</v>
+      </c>
+      <c r="Q168">
+        <v>2.5</v>
+      </c>
+      <c r="R168">
+        <v>22.5</v>
+      </c>
+      <c r="S168">
+        <v>16</v>
+      </c>
+      <c r="V168">
+        <v>2</v>
+      </c>
+      <c r="W168">
+        <v>2</v>
+      </c>
+      <c r="X168">
+        <v>16.5</v>
+      </c>
+      <c r="Y168">
+        <v>12.5</v>
+      </c>
+      <c r="Z168">
+        <v>0.5</v>
+      </c>
+      <c r="AB168">
+        <v>1</v>
+      </c>
+      <c r="AD168">
+        <v>4</v>
+      </c>
+      <c r="AE168">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>67</v>
+      </c>
+      <c r="B169">
+        <v>2022</v>
+      </c>
+      <c r="C169">
+        <v>19</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="E169">
+        <v>9</v>
+      </c>
+      <c r="F169" t="s">
+        <v>26</v>
+      </c>
+      <c r="G169" t="s">
+        <v>7</v>
+      </c>
+      <c r="H169" t="s">
+        <v>28</v>
+      </c>
+      <c r="I169">
+        <v>0</v>
+      </c>
+      <c r="J169">
+        <v>2124</v>
+      </c>
+      <c r="K169">
+        <v>1</v>
+      </c>
+      <c r="L169" t="s">
+        <v>30</v>
+      </c>
+      <c r="M169">
+        <v>11</v>
+      </c>
+      <c r="N169">
+        <v>2</v>
+      </c>
+      <c r="O169">
+        <v>1</v>
+      </c>
+      <c r="P169">
+        <v>7</v>
+      </c>
+      <c r="Q169">
+        <v>4</v>
+      </c>
+      <c r="R169">
+        <v>25</v>
+      </c>
+      <c r="S169">
+        <v>16</v>
+      </c>
+      <c r="V169" t="s">
+        <v>30</v>
+      </c>
+      <c r="W169">
+        <v>2</v>
+      </c>
+      <c r="X169">
+        <v>16</v>
+      </c>
+      <c r="Y169">
+        <v>15</v>
+      </c>
+      <c r="Z169" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB169" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with opinionway and ifop rollings (1/17 and 1/19) and cluster17 poll (1/20)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A2D312-4C68-AF4E-8859-FC2C0F941CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A803244C-F3E0-3346-AAFD-2391E0D4A9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="5160" windowWidth="22320" windowHeight="15700" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="18920" yWindow="9820" windowWidth="31100" windowHeight="18340" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF169"/>
+  <dimension ref="A1:AF174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="K173" sqref="K173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13020,6 +13020,394 @@
       </c>
       <c r="AE169" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="170" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>67</v>
+      </c>
+      <c r="B170">
+        <v>2022</v>
+      </c>
+      <c r="C170">
+        <v>20</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+      <c r="E170">
+        <v>16</v>
+      </c>
+      <c r="F170" t="s">
+        <v>40</v>
+      </c>
+      <c r="G170" t="s">
+        <v>7</v>
+      </c>
+      <c r="H170" t="s">
+        <v>27</v>
+      </c>
+      <c r="I170">
+        <v>1</v>
+      </c>
+      <c r="J170">
+        <v>668</v>
+      </c>
+      <c r="K170">
+        <v>1</v>
+      </c>
+      <c r="L170" t="s">
+        <v>30</v>
+      </c>
+      <c r="M170">
+        <v>10</v>
+      </c>
+      <c r="N170">
+        <v>3</v>
+      </c>
+      <c r="O170">
+        <v>1</v>
+      </c>
+      <c r="P170">
+        <v>5</v>
+      </c>
+      <c r="Q170">
+        <v>3</v>
+      </c>
+      <c r="R170">
+        <v>24</v>
+      </c>
+      <c r="S170">
+        <v>18</v>
+      </c>
+      <c r="V170">
+        <v>1</v>
+      </c>
+      <c r="W170">
+        <v>1</v>
+      </c>
+      <c r="X170">
+        <v>18</v>
+      </c>
+      <c r="Y170">
+        <v>11</v>
+      </c>
+      <c r="AD170">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>68</v>
+      </c>
+      <c r="B171">
+        <v>2022</v>
+      </c>
+      <c r="C171">
+        <v>21</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+      <c r="E171">
+        <v>18</v>
+      </c>
+      <c r="F171" t="s">
+        <v>26</v>
+      </c>
+      <c r="G171" t="s">
+        <v>7</v>
+      </c>
+      <c r="H171" t="s">
+        <v>28</v>
+      </c>
+      <c r="I171">
+        <v>0</v>
+      </c>
+      <c r="J171">
+        <v>1833</v>
+      </c>
+      <c r="K171">
+        <v>1</v>
+      </c>
+      <c r="L171" t="s">
+        <v>30</v>
+      </c>
+      <c r="M171">
+        <v>11</v>
+      </c>
+      <c r="N171">
+        <v>2</v>
+      </c>
+      <c r="O171">
+        <v>1</v>
+      </c>
+      <c r="P171">
+        <v>7</v>
+      </c>
+      <c r="Q171">
+        <v>3</v>
+      </c>
+      <c r="R171">
+        <v>26</v>
+      </c>
+      <c r="S171">
+        <v>16</v>
+      </c>
+      <c r="V171" t="s">
+        <v>30</v>
+      </c>
+      <c r="W171">
+        <v>1</v>
+      </c>
+      <c r="X171">
+        <v>17</v>
+      </c>
+      <c r="Y171">
+        <v>14</v>
+      </c>
+      <c r="Z171" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>68</v>
+      </c>
+      <c r="B172">
+        <v>2022</v>
+      </c>
+      <c r="C172">
+        <v>21</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="E172">
+        <v>18</v>
+      </c>
+      <c r="F172" t="s">
+        <v>26</v>
+      </c>
+      <c r="G172" t="s">
+        <v>7</v>
+      </c>
+      <c r="H172" t="s">
+        <v>28</v>
+      </c>
+      <c r="I172">
+        <v>0</v>
+      </c>
+      <c r="J172">
+        <v>1811</v>
+      </c>
+      <c r="K172" t="s">
+        <v>30</v>
+      </c>
+      <c r="L172" t="s">
+        <v>30</v>
+      </c>
+      <c r="M172">
+        <v>10</v>
+      </c>
+      <c r="N172">
+        <v>2</v>
+      </c>
+      <c r="O172">
+        <v>1</v>
+      </c>
+      <c r="P172">
+        <v>6</v>
+      </c>
+      <c r="Q172">
+        <v>3</v>
+      </c>
+      <c r="R172">
+        <v>25</v>
+      </c>
+      <c r="S172">
+        <v>16</v>
+      </c>
+      <c r="V172" t="s">
+        <v>30</v>
+      </c>
+      <c r="W172">
+        <v>1</v>
+      </c>
+      <c r="X172">
+        <v>17</v>
+      </c>
+      <c r="Y172">
+        <v>14</v>
+      </c>
+      <c r="Z172" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB172">
+        <v>1</v>
+      </c>
+      <c r="AD172">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>69</v>
+      </c>
+      <c r="B173">
+        <v>2022</v>
+      </c>
+      <c r="C173">
+        <v>21</v>
+      </c>
+      <c r="D173">
+        <v>1</v>
+      </c>
+      <c r="E173">
+        <v>17</v>
+      </c>
+      <c r="F173" t="s">
+        <v>35</v>
+      </c>
+      <c r="G173" t="s">
+        <v>7</v>
+      </c>
+      <c r="H173" t="s">
+        <v>28</v>
+      </c>
+      <c r="I173">
+        <v>1</v>
+      </c>
+      <c r="J173">
+        <v>764</v>
+      </c>
+      <c r="K173">
+        <v>1</v>
+      </c>
+      <c r="L173">
+        <v>0.5</v>
+      </c>
+      <c r="M173">
+        <v>10</v>
+      </c>
+      <c r="N173">
+        <v>2</v>
+      </c>
+      <c r="O173">
+        <v>0.5</v>
+      </c>
+      <c r="P173">
+        <v>5.5</v>
+      </c>
+      <c r="Q173">
+        <v>3</v>
+      </c>
+      <c r="R173">
+        <v>15</v>
+      </c>
+      <c r="S173">
+        <v>16</v>
+      </c>
+      <c r="V173">
+        <v>1.5</v>
+      </c>
+      <c r="W173">
+        <v>1.5</v>
+      </c>
+      <c r="X173">
+        <v>18</v>
+      </c>
+      <c r="Y173">
+        <v>11.5</v>
+      </c>
+      <c r="AD173">
+        <v>3.5</v>
+      </c>
+      <c r="AE173">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>70</v>
+      </c>
+      <c r="B174">
+        <v>2022</v>
+      </c>
+      <c r="C174">
+        <v>20</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+      <c r="E174">
+        <v>13</v>
+      </c>
+      <c r="F174" t="s">
+        <v>42</v>
+      </c>
+      <c r="G174" t="s">
+        <v>7</v>
+      </c>
+      <c r="H174" t="s">
+        <v>27</v>
+      </c>
+      <c r="I174">
+        <v>0</v>
+      </c>
+      <c r="J174">
+        <v>2558</v>
+      </c>
+      <c r="K174">
+        <v>1.5</v>
+      </c>
+      <c r="L174">
+        <v>0.5</v>
+      </c>
+      <c r="M174">
+        <v>12.5</v>
+      </c>
+      <c r="N174">
+        <v>2</v>
+      </c>
+      <c r="O174">
+        <v>1</v>
+      </c>
+      <c r="P174">
+        <v>4.5</v>
+      </c>
+      <c r="Q174">
+        <v>2</v>
+      </c>
+      <c r="R174">
+        <v>22.5</v>
+      </c>
+      <c r="S174">
+        <v>13</v>
+      </c>
+      <c r="V174">
+        <v>1</v>
+      </c>
+      <c r="W174">
+        <v>2.5</v>
+      </c>
+      <c r="X174">
+        <v>14.5</v>
+      </c>
+      <c r="Y174">
+        <v>14</v>
+      </c>
+      <c r="Z174">
+        <v>1.5</v>
+      </c>
+      <c r="AB174">
+        <v>1.5</v>
+      </c>
+      <c r="AD174">
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ cluster17 and ipsos polls (1/18 and 1/22), and ifop rolling (1/19)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A803244C-F3E0-3346-AAFD-2391E0D4A9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6D588E-E119-7F40-B901-AC6F4CFEFEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18920" yWindow="9820" windowWidth="31100" windowHeight="18340" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="7940" yWindow="500" windowWidth="31100" windowHeight="14580" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF174"/>
+  <dimension ref="A1:AF176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K173" sqref="K173"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="S174" sqref="S174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13306,7 +13306,7 @@
         <v>3</v>
       </c>
       <c r="R173">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="S173">
         <v>16</v>
@@ -13408,6 +13408,148 @@
       </c>
       <c r="AD174">
         <v>5.5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>71</v>
+      </c>
+      <c r="B175">
+        <v>2022</v>
+      </c>
+      <c r="C175">
+        <v>21</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+      <c r="E175">
+        <v>20</v>
+      </c>
+      <c r="F175" t="s">
+        <v>40</v>
+      </c>
+      <c r="G175" t="s">
+        <v>7</v>
+      </c>
+      <c r="H175" t="s">
+        <v>27</v>
+      </c>
+      <c r="I175">
+        <v>1</v>
+      </c>
+      <c r="J175">
+        <v>1000</v>
+      </c>
+      <c r="K175">
+        <v>1</v>
+      </c>
+      <c r="L175" t="s">
+        <v>30</v>
+      </c>
+      <c r="M175">
+        <v>9</v>
+      </c>
+      <c r="N175">
+        <v>2</v>
+      </c>
+      <c r="P175">
+        <v>5</v>
+      </c>
+      <c r="Q175">
+        <v>2</v>
+      </c>
+      <c r="R175">
+        <v>25</v>
+      </c>
+      <c r="S175">
+        <v>18</v>
+      </c>
+      <c r="V175">
+        <v>1</v>
+      </c>
+      <c r="W175">
+        <v>1</v>
+      </c>
+      <c r="X175">
+        <v>17</v>
+      </c>
+      <c r="Y175">
+        <v>13</v>
+      </c>
+      <c r="AD175">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>72</v>
+      </c>
+      <c r="B176">
+        <v>2022</v>
+      </c>
+      <c r="C176">
+        <v>20</v>
+      </c>
+      <c r="D176">
+        <v>1</v>
+      </c>
+      <c r="E176">
+        <v>16</v>
+      </c>
+      <c r="F176" t="s">
+        <v>6</v>
+      </c>
+      <c r="G176" t="s">
+        <v>7</v>
+      </c>
+      <c r="H176" t="s">
+        <v>8</v>
+      </c>
+      <c r="I176">
+        <v>0</v>
+      </c>
+      <c r="J176">
+        <v>7947</v>
+      </c>
+      <c r="K176">
+        <v>1.5</v>
+      </c>
+      <c r="L176">
+        <v>0.5</v>
+      </c>
+      <c r="M176">
+        <v>8</v>
+      </c>
+      <c r="N176">
+        <v>2.5</v>
+      </c>
+      <c r="P176">
+        <v>7</v>
+      </c>
+      <c r="Q176">
+        <v>3.5</v>
+      </c>
+      <c r="R176">
+        <v>25</v>
+      </c>
+      <c r="S176">
+        <v>15.5</v>
+      </c>
+      <c r="V176">
+        <v>1</v>
+      </c>
+      <c r="W176">
+        <v>2</v>
+      </c>
+      <c r="X176">
+        <v>15.5</v>
+      </c>
+      <c r="Y176">
+        <v>13</v>
+      </c>
+      <c r="AD176">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ ifop rolling (1/24) and opinionway poll (1/20)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6D588E-E119-7F40-B901-AC6F4CFEFEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E48CFA-D529-DE46-AD3E-EA167D60076F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="500" windowWidth="31100" windowHeight="14580" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="14580" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF176"/>
+  <dimension ref="A1:AF178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="S174" sqref="S174"/>
+      <selection pane="bottomLeft" activeCell="AE178" sqref="AE178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13439,7 +13439,7 @@
         <v>1</v>
       </c>
       <c r="J175">
-        <v>1000</v>
+        <v>1137</v>
       </c>
       <c r="K175">
         <v>1</v>
@@ -13549,6 +13549,151 @@
         <v>13</v>
       </c>
       <c r="AD176">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>73</v>
+      </c>
+      <c r="B177">
+        <v>2022</v>
+      </c>
+      <c r="C177">
+        <v>21</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177">
+        <v>22</v>
+      </c>
+      <c r="F177" t="s">
+        <v>35</v>
+      </c>
+      <c r="G177" t="s">
+        <v>7</v>
+      </c>
+      <c r="H177" t="s">
+        <v>28</v>
+      </c>
+      <c r="I177">
+        <v>1</v>
+      </c>
+      <c r="J177">
+        <v>808</v>
+      </c>
+      <c r="K177">
+        <v>0.5</v>
+      </c>
+      <c r="L177">
+        <v>0.5</v>
+      </c>
+      <c r="M177">
+        <v>10.5</v>
+      </c>
+      <c r="N177">
+        <v>3</v>
+      </c>
+      <c r="P177">
+        <v>5</v>
+      </c>
+      <c r="Q177">
+        <v>3.5</v>
+      </c>
+      <c r="R177">
+        <v>24.5</v>
+      </c>
+      <c r="S177">
+        <v>16.5</v>
+      </c>
+      <c r="V177">
+        <v>1</v>
+      </c>
+      <c r="W177">
+        <v>2</v>
+      </c>
+      <c r="X177">
+        <v>18</v>
+      </c>
+      <c r="Y177">
+        <v>12</v>
+      </c>
+      <c r="AD177">
+        <v>3</v>
+      </c>
+      <c r="AE177" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="178" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>74</v>
+      </c>
+      <c r="B178">
+        <v>2022</v>
+      </c>
+      <c r="C178">
+        <v>21</v>
+      </c>
+      <c r="D178">
+        <v>1</v>
+      </c>
+      <c r="E178">
+        <v>20</v>
+      </c>
+      <c r="F178" t="s">
+        <v>40</v>
+      </c>
+      <c r="G178" t="s">
+        <v>7</v>
+      </c>
+      <c r="H178" t="s">
+        <v>27</v>
+      </c>
+      <c r="I178">
+        <v>0</v>
+      </c>
+      <c r="J178">
+        <v>712</v>
+      </c>
+      <c r="K178">
+        <v>1</v>
+      </c>
+      <c r="L178" t="s">
+        <v>37</v>
+      </c>
+      <c r="M178">
+        <v>9</v>
+      </c>
+      <c r="N178">
+        <v>3</v>
+      </c>
+      <c r="P178">
+        <v>5</v>
+      </c>
+      <c r="Q178">
+        <v>2</v>
+      </c>
+      <c r="R178">
+        <v>24</v>
+      </c>
+      <c r="S178">
+        <v>18</v>
+      </c>
+      <c r="V178">
+        <v>1</v>
+      </c>
+      <c r="W178">
+        <v>1</v>
+      </c>
+      <c r="X178">
+        <v>18</v>
+      </c>
+      <c r="Y178">
+        <v>13</v>
+      </c>
+      <c r="AD178">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update w/ cluster17 poll (1/25)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E48CFA-D529-DE46-AD3E-EA167D60076F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C37B154-B0F3-7343-8F3D-E59A2AC9191D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="14580" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="31280" yWindow="500" windowWidth="19800" windowHeight="14580" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF178"/>
+  <dimension ref="A1:AF179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AE178" sqref="AE178"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AE179" sqref="AE179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13695,6 +13695,83 @@
       </c>
       <c r="AD178">
         <v>5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>75</v>
+      </c>
+      <c r="B179">
+        <v>2022</v>
+      </c>
+      <c r="C179">
+        <v>21</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+      <c r="E179">
+        <v>20</v>
+      </c>
+      <c r="F179" t="s">
+        <v>42</v>
+      </c>
+      <c r="G179" t="s">
+        <v>7</v>
+      </c>
+      <c r="H179" t="s">
+        <v>27</v>
+      </c>
+      <c r="I179">
+        <v>0</v>
+      </c>
+      <c r="J179">
+        <v>2548</v>
+      </c>
+      <c r="K179">
+        <v>1</v>
+      </c>
+      <c r="L179" t="s">
+        <v>30</v>
+      </c>
+      <c r="M179">
+        <v>13</v>
+      </c>
+      <c r="N179">
+        <v>2</v>
+      </c>
+      <c r="O179">
+        <v>0.5</v>
+      </c>
+      <c r="P179">
+        <v>5</v>
+      </c>
+      <c r="Q179">
+        <v>2</v>
+      </c>
+      <c r="R179">
+        <v>22</v>
+      </c>
+      <c r="S179">
+        <v>14</v>
+      </c>
+      <c r="V179">
+        <v>1.5</v>
+      </c>
+      <c r="W179">
+        <v>1.5</v>
+      </c>
+      <c r="X179">
+        <v>15</v>
+      </c>
+      <c r="Y179">
+        <v>14</v>
+      </c>
+      <c r="Z179">
+        <v>1</v>
+      </c>
+      <c r="AD179">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ harris and elabe polls (1/26)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C37B154-B0F3-7343-8F3D-E59A2AC9191D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2305F6-47CC-CF4E-82AC-C7335B36D63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31280" yWindow="500" windowWidth="19800" windowHeight="14580" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="25320" yWindow="14760" windowWidth="23880" windowHeight="13560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF179"/>
+  <dimension ref="A1:AF183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AE179" sqref="AE179"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="H181" sqref="H181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13772,6 +13772,314 @@
       </c>
       <c r="AD179">
         <v>6</v>
+      </c>
+    </row>
+    <row r="180" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>76</v>
+      </c>
+      <c r="B180">
+        <v>2022</v>
+      </c>
+      <c r="C180">
+        <v>21</v>
+      </c>
+      <c r="D180">
+        <v>1</v>
+      </c>
+      <c r="E180">
+        <v>23</v>
+      </c>
+      <c r="F180" t="s">
+        <v>26</v>
+      </c>
+      <c r="G180" t="s">
+        <v>7</v>
+      </c>
+      <c r="H180" t="s">
+        <v>28</v>
+      </c>
+      <c r="I180">
+        <v>0</v>
+      </c>
+      <c r="J180">
+        <v>2037</v>
+      </c>
+      <c r="K180">
+        <v>1</v>
+      </c>
+      <c r="L180" t="s">
+        <v>30</v>
+      </c>
+      <c r="M180">
+        <v>10</v>
+      </c>
+      <c r="N180">
+        <v>2</v>
+      </c>
+      <c r="P180">
+        <v>5</v>
+      </c>
+      <c r="Q180">
+        <v>3</v>
+      </c>
+      <c r="R180">
+        <v>24</v>
+      </c>
+      <c r="S180">
+        <v>15</v>
+      </c>
+      <c r="V180">
+        <v>1</v>
+      </c>
+      <c r="W180">
+        <v>2</v>
+      </c>
+      <c r="X180">
+        <v>17</v>
+      </c>
+      <c r="Y180">
+        <v>14</v>
+      </c>
+      <c r="Z180" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB180">
+        <v>1</v>
+      </c>
+      <c r="AD180">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>76</v>
+      </c>
+      <c r="B181">
+        <v>2022</v>
+      </c>
+      <c r="C181">
+        <v>21</v>
+      </c>
+      <c r="D181">
+        <v>1</v>
+      </c>
+      <c r="E181">
+        <v>23</v>
+      </c>
+      <c r="F181" t="s">
+        <v>26</v>
+      </c>
+      <c r="G181" t="s">
+        <v>7</v>
+      </c>
+      <c r="H181" t="s">
+        <v>28</v>
+      </c>
+      <c r="I181">
+        <v>0</v>
+      </c>
+      <c r="J181">
+        <v>2037</v>
+      </c>
+      <c r="K181">
+        <v>1</v>
+      </c>
+      <c r="L181" t="s">
+        <v>30</v>
+      </c>
+      <c r="M181">
+        <v>11</v>
+      </c>
+      <c r="N181">
+        <v>2</v>
+      </c>
+      <c r="P181">
+        <v>7</v>
+      </c>
+      <c r="Q181">
+        <v>4</v>
+      </c>
+      <c r="R181">
+        <v>25</v>
+      </c>
+      <c r="S181">
+        <v>15</v>
+      </c>
+      <c r="V181">
+        <v>1</v>
+      </c>
+      <c r="W181">
+        <v>2</v>
+      </c>
+      <c r="X181">
+        <v>17</v>
+      </c>
+      <c r="Y181">
+        <v>14</v>
+      </c>
+      <c r="Z181" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>77</v>
+      </c>
+      <c r="B182">
+        <v>2022</v>
+      </c>
+      <c r="C182">
+        <v>22</v>
+      </c>
+      <c r="D182">
+        <v>1</v>
+      </c>
+      <c r="E182">
+        <v>25</v>
+      </c>
+      <c r="F182" t="s">
+        <v>36</v>
+      </c>
+      <c r="G182" t="s">
+        <v>7</v>
+      </c>
+      <c r="H182" t="s">
+        <v>27</v>
+      </c>
+      <c r="I182">
+        <v>0</v>
+      </c>
+      <c r="J182">
+        <v>1008</v>
+      </c>
+      <c r="K182">
+        <v>1.5</v>
+      </c>
+      <c r="L182">
+        <v>0.5</v>
+      </c>
+      <c r="M182">
+        <v>10</v>
+      </c>
+      <c r="N182">
+        <v>3</v>
+      </c>
+      <c r="P182">
+        <v>6.5</v>
+      </c>
+      <c r="Q182">
+        <v>3</v>
+      </c>
+      <c r="R182">
+        <v>25</v>
+      </c>
+      <c r="S182">
+        <v>17</v>
+      </c>
+      <c r="V182">
+        <v>2</v>
+      </c>
+      <c r="W182">
+        <v>1.5</v>
+      </c>
+      <c r="X182">
+        <v>17</v>
+      </c>
+      <c r="Y182">
+        <v>11.5</v>
+      </c>
+      <c r="Z182">
+        <v>0.5</v>
+      </c>
+      <c r="AB182">
+        <v>0.5</v>
+      </c>
+      <c r="AE182">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>77</v>
+      </c>
+      <c r="B183">
+        <v>2022</v>
+      </c>
+      <c r="C183">
+        <v>22</v>
+      </c>
+      <c r="D183">
+        <v>1</v>
+      </c>
+      <c r="E183">
+        <v>25</v>
+      </c>
+      <c r="F183" t="s">
+        <v>36</v>
+      </c>
+      <c r="G183" t="s">
+        <v>7</v>
+      </c>
+      <c r="H183" t="s">
+        <v>27</v>
+      </c>
+      <c r="I183">
+        <v>0</v>
+      </c>
+      <c r="J183">
+        <v>1020</v>
+      </c>
+      <c r="K183">
+        <v>1</v>
+      </c>
+      <c r="L183" t="s">
+        <v>30</v>
+      </c>
+      <c r="M183">
+        <v>9</v>
+      </c>
+      <c r="N183">
+        <v>2.5</v>
+      </c>
+      <c r="P183">
+        <v>5.5</v>
+      </c>
+      <c r="Q183">
+        <v>2.5</v>
+      </c>
+      <c r="R183">
+        <v>24</v>
+      </c>
+      <c r="S183">
+        <v>17</v>
+      </c>
+      <c r="V183">
+        <v>2</v>
+      </c>
+      <c r="W183">
+        <v>2</v>
+      </c>
+      <c r="X183">
+        <v>16.5</v>
+      </c>
+      <c r="Y183">
+        <v>11.5</v>
+      </c>
+      <c r="Z183">
+        <v>0.5</v>
+      </c>
+      <c r="AB183">
+        <v>0.5</v>
+      </c>
+      <c r="AD183">
+        <v>5</v>
+      </c>
+      <c r="AE183">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ bva poll (1/28), and ifop and opinionway rollings (1/28 and 1/25)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2305F6-47CC-CF4E-82AC-C7335B36D63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BB24B7-4CCB-7F4C-8BA0-D8DF4658F0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25320" yWindow="14760" windowWidth="23880" windowHeight="13560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="8220" yWindow="500" windowWidth="19480" windowHeight="10500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF183"/>
+  <dimension ref="A1:AF186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H181" sqref="H181"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AF185" sqref="AF185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14080,6 +14080,228 @@
       </c>
       <c r="AE183">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>78</v>
+      </c>
+      <c r="B184">
+        <v>2022</v>
+      </c>
+      <c r="C184">
+        <v>22</v>
+      </c>
+      <c r="D184">
+        <v>1</v>
+      </c>
+      <c r="E184">
+        <v>25</v>
+      </c>
+      <c r="F184" t="s">
+        <v>41</v>
+      </c>
+      <c r="G184" t="s">
+        <v>7</v>
+      </c>
+      <c r="H184" t="s">
+        <v>27</v>
+      </c>
+      <c r="I184">
+        <v>0</v>
+      </c>
+      <c r="J184">
+        <v>910</v>
+      </c>
+      <c r="K184">
+        <v>0.5</v>
+      </c>
+      <c r="L184" t="s">
+        <v>30</v>
+      </c>
+      <c r="M184">
+        <v>10</v>
+      </c>
+      <c r="N184">
+        <v>3</v>
+      </c>
+      <c r="P184">
+        <v>6</v>
+      </c>
+      <c r="Q184">
+        <v>3</v>
+      </c>
+      <c r="R184">
+        <v>24</v>
+      </c>
+      <c r="S184">
+        <v>16</v>
+      </c>
+      <c r="V184">
+        <v>0.5</v>
+      </c>
+      <c r="W184">
+        <v>2</v>
+      </c>
+      <c r="X184">
+        <v>18</v>
+      </c>
+      <c r="Y184">
+        <v>12.5</v>
+      </c>
+      <c r="Z184">
+        <v>0.5</v>
+      </c>
+      <c r="AD184">
+        <v>4</v>
+      </c>
+      <c r="AE184" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="185" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>79</v>
+      </c>
+      <c r="B185">
+        <v>2022</v>
+      </c>
+      <c r="C185">
+        <v>22</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+      <c r="E185">
+        <v>27</v>
+      </c>
+      <c r="F185" t="s">
+        <v>35</v>
+      </c>
+      <c r="G185" t="s">
+        <v>7</v>
+      </c>
+      <c r="H185" t="s">
+        <v>28</v>
+      </c>
+      <c r="I185">
+        <v>1</v>
+      </c>
+      <c r="J185">
+        <v>1000</v>
+      </c>
+      <c r="K185">
+        <v>0.5</v>
+      </c>
+      <c r="L185" t="s">
+        <v>30</v>
+      </c>
+      <c r="M185">
+        <v>9.5</v>
+      </c>
+      <c r="N185">
+        <v>3</v>
+      </c>
+      <c r="P185">
+        <v>5.5</v>
+      </c>
+      <c r="Q185">
+        <v>3.5</v>
+      </c>
+      <c r="R185">
+        <v>24</v>
+      </c>
+      <c r="S185">
+        <v>16.5</v>
+      </c>
+      <c r="V185">
+        <v>1</v>
+      </c>
+      <c r="W185">
+        <v>1</v>
+      </c>
+      <c r="X185">
+        <v>18</v>
+      </c>
+      <c r="Y185">
+        <v>13.5</v>
+      </c>
+      <c r="AD185">
+        <v>4</v>
+      </c>
+      <c r="AE185" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="186" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>80</v>
+      </c>
+      <c r="B186">
+        <v>2022</v>
+      </c>
+      <c r="C186">
+        <v>22</v>
+      </c>
+      <c r="D186">
+        <v>1</v>
+      </c>
+      <c r="E186">
+        <v>24</v>
+      </c>
+      <c r="F186" t="s">
+        <v>40</v>
+      </c>
+      <c r="G186" t="s">
+        <v>7</v>
+      </c>
+      <c r="H186" t="s">
+        <v>28</v>
+      </c>
+      <c r="I186">
+        <v>1</v>
+      </c>
+      <c r="J186">
+        <v>1000</v>
+      </c>
+      <c r="K186">
+        <v>1</v>
+      </c>
+      <c r="L186" t="s">
+        <v>30</v>
+      </c>
+      <c r="M186">
+        <v>9</v>
+      </c>
+      <c r="N186">
+        <v>3</v>
+      </c>
+      <c r="P186">
+        <v>5</v>
+      </c>
+      <c r="Q186">
+        <v>3</v>
+      </c>
+      <c r="R186">
+        <v>25</v>
+      </c>
+      <c r="S186">
+        <v>17</v>
+      </c>
+      <c r="V186">
+        <v>1</v>
+      </c>
+      <c r="W186">
+        <v>1</v>
+      </c>
+      <c r="X186">
+        <v>16</v>
+      </c>
+      <c r="Y186">
+        <v>14</v>
+      </c>
+      <c r="AD186">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ opinionway poll (1/28) + previous polls' N
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BB24B7-4CCB-7F4C-8BA0-D8DF4658F0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F758A25-43F1-E843-982C-C72167FF5F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="500" windowWidth="19480" windowHeight="10500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="28100" yWindow="16780" windowWidth="19480" windowHeight="10500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF186"/>
+  <dimension ref="A1:AF187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AF185" sqref="AF185"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AE187" sqref="AE187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12900,7 +12900,7 @@
         <v>1</v>
       </c>
       <c r="J168">
-        <v>728</v>
+        <v>1037</v>
       </c>
       <c r="K168">
         <v>0.5</v>
@@ -12974,7 +12974,7 @@
         <v>1</v>
       </c>
       <c r="J169">
-        <v>745</v>
+        <v>1056</v>
       </c>
       <c r="K169">
         <v>0.5</v>
@@ -13282,7 +13282,7 @@
         <v>1</v>
       </c>
       <c r="J173">
-        <v>764</v>
+        <v>1065</v>
       </c>
       <c r="K173">
         <v>1</v>
@@ -13581,7 +13581,7 @@
         <v>1</v>
       </c>
       <c r="J177">
-        <v>808</v>
+        <v>1084</v>
       </c>
       <c r="K177">
         <v>0.5</v>
@@ -13803,7 +13803,7 @@
         <v>0</v>
       </c>
       <c r="J180">
-        <v>2037</v>
+        <v>1752</v>
       </c>
       <c r="K180">
         <v>1</v>
@@ -13880,7 +13880,7 @@
         <v>0</v>
       </c>
       <c r="J181">
-        <v>2037</v>
+        <v>1752</v>
       </c>
       <c r="K181">
         <v>1</v>
@@ -14188,7 +14188,7 @@
         <v>1</v>
       </c>
       <c r="J185">
-        <v>1000</v>
+        <v>993</v>
       </c>
       <c r="K185">
         <v>0.5</v>
@@ -14256,13 +14256,13 @@
         <v>7</v>
       </c>
       <c r="H186" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I186">
         <v>1</v>
       </c>
       <c r="J186">
-        <v>1000</v>
+        <v>939</v>
       </c>
       <c r="K186">
         <v>1</v>
@@ -14301,6 +14301,77 @@
         <v>14</v>
       </c>
       <c r="AD186">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>81</v>
+      </c>
+      <c r="B187">
+        <v>2022</v>
+      </c>
+      <c r="C187">
+        <v>22</v>
+      </c>
+      <c r="D187">
+        <v>1</v>
+      </c>
+      <c r="E187">
+        <v>27</v>
+      </c>
+      <c r="F187" t="s">
+        <v>40</v>
+      </c>
+      <c r="G187" t="s">
+        <v>7</v>
+      </c>
+      <c r="H187" t="s">
+        <v>27</v>
+      </c>
+      <c r="I187">
+        <v>0</v>
+      </c>
+      <c r="J187">
+        <v>567</v>
+      </c>
+      <c r="K187">
+        <v>1</v>
+      </c>
+      <c r="L187" t="s">
+        <v>37</v>
+      </c>
+      <c r="M187">
+        <v>9</v>
+      </c>
+      <c r="N187">
+        <v>3</v>
+      </c>
+      <c r="P187">
+        <v>6</v>
+      </c>
+      <c r="Q187">
+        <v>2</v>
+      </c>
+      <c r="R187">
+        <v>24</v>
+      </c>
+      <c r="S187">
+        <v>18</v>
+      </c>
+      <c r="V187">
+        <v>1</v>
+      </c>
+      <c r="W187">
+        <v>1</v>
+      </c>
+      <c r="X187">
+        <v>17</v>
+      </c>
+      <c r="Y187">
+        <v>13</v>
+      </c>
+      <c r="AD187">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update w/ cluster17 poll (2/1), and opinionway and ifop rollings (1/31 and 2/1)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F758A25-43F1-E843-982C-C72167FF5F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8523EB5-D9AB-CC4E-9809-9096894015A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28100" yWindow="16780" windowWidth="19480" windowHeight="10500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF187"/>
+  <dimension ref="A1:AF190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AE187" sqref="AE187"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="U189" sqref="U189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11402,7 +11402,7 @@
         <v>1</v>
       </c>
       <c r="J148">
-        <v>639</v>
+        <v>1006</v>
       </c>
       <c r="K148">
         <v>1</v>
@@ -11553,7 +11553,7 @@
         <v>1</v>
       </c>
       <c r="J150">
-        <v>966</v>
+        <v>1108</v>
       </c>
       <c r="K150">
         <v>1</v>
@@ -12589,7 +12589,7 @@
         <v>1</v>
       </c>
       <c r="J164">
-        <v>997</v>
+        <v>1015</v>
       </c>
       <c r="K164">
         <v>2</v>
@@ -13439,7 +13439,7 @@
         <v>1</v>
       </c>
       <c r="J175">
-        <v>1137</v>
+        <v>1057</v>
       </c>
       <c r="K175">
         <v>1</v>
@@ -14262,7 +14262,7 @@
         <v>1</v>
       </c>
       <c r="J186">
-        <v>939</v>
+        <v>1112</v>
       </c>
       <c r="K186">
         <v>1</v>
@@ -14372,6 +14372,228 @@
         <v>13</v>
       </c>
       <c r="AD187">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>82</v>
+      </c>
+      <c r="B188">
+        <v>2022</v>
+      </c>
+      <c r="C188">
+        <v>22</v>
+      </c>
+      <c r="D188">
+        <v>1</v>
+      </c>
+      <c r="E188">
+        <v>27</v>
+      </c>
+      <c r="F188" t="s">
+        <v>42</v>
+      </c>
+      <c r="G188" t="s">
+        <v>7</v>
+      </c>
+      <c r="H188" t="s">
+        <v>27</v>
+      </c>
+      <c r="I188">
+        <v>0</v>
+      </c>
+      <c r="J188">
+        <v>1997</v>
+      </c>
+      <c r="K188">
+        <v>1</v>
+      </c>
+      <c r="L188" t="s">
+        <v>30</v>
+      </c>
+      <c r="M188">
+        <v>13</v>
+      </c>
+      <c r="N188">
+        <v>2</v>
+      </c>
+      <c r="P188">
+        <v>5</v>
+      </c>
+      <c r="Q188">
+        <v>2</v>
+      </c>
+      <c r="R188">
+        <v>22.5</v>
+      </c>
+      <c r="S188">
+        <v>14</v>
+      </c>
+      <c r="V188">
+        <v>1</v>
+      </c>
+      <c r="W188">
+        <v>1.5</v>
+      </c>
+      <c r="X188">
+        <v>14.5</v>
+      </c>
+      <c r="Y188">
+        <v>14.5</v>
+      </c>
+      <c r="Z188">
+        <v>1</v>
+      </c>
+      <c r="AB188">
+        <v>1</v>
+      </c>
+      <c r="AD188">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="189" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>83</v>
+      </c>
+      <c r="B189">
+        <v>2022</v>
+      </c>
+      <c r="C189">
+        <v>22</v>
+      </c>
+      <c r="D189">
+        <v>1</v>
+      </c>
+      <c r="E189">
+        <v>31</v>
+      </c>
+      <c r="F189" t="s">
+        <v>35</v>
+      </c>
+      <c r="G189" t="s">
+        <v>7</v>
+      </c>
+      <c r="H189" t="s">
+        <v>28</v>
+      </c>
+      <c r="I189">
+        <v>1</v>
+      </c>
+      <c r="J189">
+        <v>1000</v>
+      </c>
+      <c r="K189">
+        <v>0.5</v>
+      </c>
+      <c r="L189" t="s">
+        <v>30</v>
+      </c>
+      <c r="M189">
+        <v>9.5</v>
+      </c>
+      <c r="N189">
+        <v>3.5</v>
+      </c>
+      <c r="P189">
+        <v>5</v>
+      </c>
+      <c r="Q189">
+        <v>3.5</v>
+      </c>
+      <c r="R189">
+        <v>24</v>
+      </c>
+      <c r="S189">
+        <v>16</v>
+      </c>
+      <c r="V189">
+        <v>1</v>
+      </c>
+      <c r="W189">
+        <v>1.5</v>
+      </c>
+      <c r="X189">
+        <v>17.5</v>
+      </c>
+      <c r="Y189">
+        <v>14</v>
+      </c>
+      <c r="AD189">
+        <v>4</v>
+      </c>
+      <c r="AE189" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="190" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>84</v>
+      </c>
+      <c r="B190">
+        <v>2022</v>
+      </c>
+      <c r="C190">
+        <v>22</v>
+      </c>
+      <c r="D190">
+        <v>1</v>
+      </c>
+      <c r="E190">
+        <v>29</v>
+      </c>
+      <c r="F190" t="s">
+        <v>40</v>
+      </c>
+      <c r="G190" t="s">
+        <v>7</v>
+      </c>
+      <c r="H190" t="s">
+        <v>27</v>
+      </c>
+      <c r="I190">
+        <v>1</v>
+      </c>
+      <c r="J190">
+        <v>800</v>
+      </c>
+      <c r="K190" t="s">
+        <v>37</v>
+      </c>
+      <c r="L190" t="s">
+        <v>37</v>
+      </c>
+      <c r="M190">
+        <v>10</v>
+      </c>
+      <c r="N190">
+        <v>3</v>
+      </c>
+      <c r="P190">
+        <v>5</v>
+      </c>
+      <c r="Q190">
+        <v>3</v>
+      </c>
+      <c r="R190">
+        <v>24</v>
+      </c>
+      <c r="S190">
+        <v>16</v>
+      </c>
+      <c r="V190">
+        <v>1</v>
+      </c>
+      <c r="W190">
+        <v>2</v>
+      </c>
+      <c r="X190">
+        <v>17</v>
+      </c>
+      <c r="Y190">
+        <v>14</v>
+      </c>
+      <c r="AD190">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update w/ harris poll (2/2) + update N for rollings
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8523EB5-D9AB-CC4E-9809-9096894015A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D79F60-64B6-AF4D-82E7-E119B8E75C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28100" yWindow="16780" windowWidth="19480" windowHeight="10500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF190"/>
+  <dimension ref="A1:AF191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="U189" sqref="U189"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="K186" sqref="K186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14481,7 +14481,7 @@
         <v>1</v>
       </c>
       <c r="J189">
-        <v>1000</v>
+        <v>986</v>
       </c>
       <c r="K189">
         <v>0.5</v>
@@ -14540,7 +14540,7 @@
         <v>1</v>
       </c>
       <c r="E190">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F190" t="s">
         <v>40</v>
@@ -14555,7 +14555,7 @@
         <v>1</v>
       </c>
       <c r="J190">
-        <v>800</v>
+        <v>1987</v>
       </c>
       <c r="K190" t="s">
         <v>37</v>
@@ -14594,6 +14594,83 @@
         <v>14</v>
       </c>
       <c r="AD190">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>85</v>
+      </c>
+      <c r="B191">
+        <v>2022</v>
+      </c>
+      <c r="C191">
+        <v>22</v>
+      </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
+      <c r="E191">
+        <v>30</v>
+      </c>
+      <c r="F191" t="s">
+        <v>26</v>
+      </c>
+      <c r="G191" t="s">
+        <v>7</v>
+      </c>
+      <c r="H191" t="s">
+        <v>28</v>
+      </c>
+      <c r="I191">
+        <v>0</v>
+      </c>
+      <c r="J191">
+        <v>1841</v>
+      </c>
+      <c r="K191">
+        <v>1</v>
+      </c>
+      <c r="L191" t="s">
+        <v>30</v>
+      </c>
+      <c r="M191">
+        <v>11</v>
+      </c>
+      <c r="N191">
+        <v>2</v>
+      </c>
+      <c r="P191">
+        <v>6</v>
+      </c>
+      <c r="Q191">
+        <v>2</v>
+      </c>
+      <c r="R191">
+        <v>24</v>
+      </c>
+      <c r="S191">
+        <v>15</v>
+      </c>
+      <c r="V191">
+        <v>1</v>
+      </c>
+      <c r="W191">
+        <v>2</v>
+      </c>
+      <c r="X191">
+        <v>17</v>
+      </c>
+      <c r="Y191">
+        <v>14</v>
+      </c>
+      <c r="Z191" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB191" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD191">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update w/ elabe poll (2/2)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D79F60-64B6-AF4D-82E7-E119B8E75C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6D9FD8-89E2-934A-B319-B6C72AEB82D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28100" yWindow="16780" windowWidth="19480" windowHeight="10500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF191"/>
+  <dimension ref="A1:AF192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K186" sqref="K186"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AF192" sqref="AF192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14672,6 +14672,86 @@
       </c>
       <c r="AD191">
         <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>86</v>
+      </c>
+      <c r="B192">
+        <v>2022</v>
+      </c>
+      <c r="C192">
+        <v>23</v>
+      </c>
+      <c r="D192">
+        <v>2</v>
+      </c>
+      <c r="E192">
+        <v>1</v>
+      </c>
+      <c r="F192" t="s">
+        <v>36</v>
+      </c>
+      <c r="G192" t="s">
+        <v>7</v>
+      </c>
+      <c r="H192" t="s">
+        <v>27</v>
+      </c>
+      <c r="I192">
+        <v>0</v>
+      </c>
+      <c r="J192">
+        <v>1001</v>
+      </c>
+      <c r="K192">
+        <v>0.5</v>
+      </c>
+      <c r="L192" t="s">
+        <v>30</v>
+      </c>
+      <c r="M192">
+        <v>9.5</v>
+      </c>
+      <c r="N192">
+        <v>2.5</v>
+      </c>
+      <c r="P192">
+        <v>4.5</v>
+      </c>
+      <c r="Q192">
+        <v>2</v>
+      </c>
+      <c r="R192">
+        <v>25</v>
+      </c>
+      <c r="S192">
+        <v>16</v>
+      </c>
+      <c r="V192">
+        <v>1</v>
+      </c>
+      <c r="W192">
+        <v>2.5</v>
+      </c>
+      <c r="X192">
+        <v>16.5</v>
+      </c>
+      <c r="Y192">
+        <v>12.5</v>
+      </c>
+      <c r="Z192">
+        <v>0.5</v>
+      </c>
+      <c r="AB192">
+        <v>0.5</v>
+      </c>
+      <c r="AD192">
+        <v>6</v>
+      </c>
+      <c r="AE192">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ ipsos poll (2/5) and opinionway rolling (2/4)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6D9FD8-89E2-934A-B319-B6C72AEB82D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2735F676-1E23-3247-89C4-4A5B7D21BE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28100" yWindow="16780" windowWidth="19480" windowHeight="10500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="27980" yWindow="13640" windowWidth="19480" windowHeight="10500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF192"/>
+  <dimension ref="A1:AF194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AF192" sqref="AF192"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AE194" sqref="AE194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14626,7 +14626,7 @@
         <v>0</v>
       </c>
       <c r="J191">
-        <v>1841</v>
+        <v>1863</v>
       </c>
       <c r="K191">
         <v>1</v>
@@ -14752,6 +14752,148 @@
       </c>
       <c r="AE192">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>87</v>
+      </c>
+      <c r="B193">
+        <v>2022</v>
+      </c>
+      <c r="C193">
+        <v>23</v>
+      </c>
+      <c r="D193">
+        <v>2</v>
+      </c>
+      <c r="E193">
+        <v>2</v>
+      </c>
+      <c r="F193" t="s">
+        <v>6</v>
+      </c>
+      <c r="G193" t="s">
+        <v>7</v>
+      </c>
+      <c r="H193" t="s">
+        <v>8</v>
+      </c>
+      <c r="I193">
+        <v>0</v>
+      </c>
+      <c r="J193">
+        <v>777</v>
+      </c>
+      <c r="K193">
+        <v>1</v>
+      </c>
+      <c r="L193">
+        <v>0.5</v>
+      </c>
+      <c r="M193">
+        <v>9</v>
+      </c>
+      <c r="N193">
+        <v>3</v>
+      </c>
+      <c r="P193">
+        <v>8</v>
+      </c>
+      <c r="Q193">
+        <v>3</v>
+      </c>
+      <c r="R193">
+        <v>24</v>
+      </c>
+      <c r="S193">
+        <v>16.5</v>
+      </c>
+      <c r="V193">
+        <v>1</v>
+      </c>
+      <c r="W193">
+        <v>2</v>
+      </c>
+      <c r="X193">
+        <v>14</v>
+      </c>
+      <c r="Y193">
+        <v>14</v>
+      </c>
+      <c r="AD193">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>88</v>
+      </c>
+      <c r="B194">
+        <v>2022</v>
+      </c>
+      <c r="C194">
+        <v>23</v>
+      </c>
+      <c r="D194">
+        <v>2</v>
+      </c>
+      <c r="E194">
+        <v>3</v>
+      </c>
+      <c r="F194" t="s">
+        <v>40</v>
+      </c>
+      <c r="G194" t="s">
+        <v>7</v>
+      </c>
+      <c r="H194" t="s">
+        <v>27</v>
+      </c>
+      <c r="I194">
+        <v>1</v>
+      </c>
+      <c r="J194">
+        <v>1000</v>
+      </c>
+      <c r="K194">
+        <v>1</v>
+      </c>
+      <c r="L194" t="s">
+        <v>37</v>
+      </c>
+      <c r="M194">
+        <v>10</v>
+      </c>
+      <c r="N194">
+        <v>4</v>
+      </c>
+      <c r="P194">
+        <v>4</v>
+      </c>
+      <c r="Q194">
+        <v>3</v>
+      </c>
+      <c r="R194">
+        <v>24</v>
+      </c>
+      <c r="S194">
+        <v>16</v>
+      </c>
+      <c r="V194">
+        <v>1</v>
+      </c>
+      <c r="W194">
+        <v>2</v>
+      </c>
+      <c r="X194">
+        <v>17</v>
+      </c>
+      <c r="Y194">
+        <v>14</v>
+      </c>
+      <c r="AD194">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ opinionway rolling (2/8) + updates Ns
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4A8604-FC18-CB40-9310-9727C9F47EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E19B46-5578-9B45-A36F-4DD4A2C0A401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="4360" windowWidth="32300" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="160" yWindow="5440" windowWidth="25920" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF192"/>
+  <dimension ref="A1:AF194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="J191" sqref="J191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14511,7 +14511,7 @@
         <v>1</v>
       </c>
       <c r="J189">
-        <v>1000</v>
+        <v>1067</v>
       </c>
       <c r="K189">
         <v>1</v>
@@ -14567,7 +14567,7 @@
         <v>2</v>
       </c>
       <c r="E190">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F190" t="s">
         <v>35</v>
@@ -14582,7 +14582,7 @@
         <v>0</v>
       </c>
       <c r="J190">
-        <v>1100</v>
+        <v>1020</v>
       </c>
       <c r="K190">
         <v>0.5</v>
@@ -14656,7 +14656,7 @@
         <v>0</v>
       </c>
       <c r="J191">
-        <v>560</v>
+        <v>637</v>
       </c>
       <c r="K191" t="s">
         <v>37</v>
@@ -14727,7 +14727,7 @@
         <v>1</v>
       </c>
       <c r="J192">
-        <v>1100</v>
+        <v>1003</v>
       </c>
       <c r="K192">
         <v>0.5</v>
@@ -14770,6 +14770,151 @@
       </c>
       <c r="AE192" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="193" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>90</v>
+      </c>
+      <c r="B193">
+        <v>2022</v>
+      </c>
+      <c r="C193">
+        <v>23</v>
+      </c>
+      <c r="D193">
+        <v>2</v>
+      </c>
+      <c r="E193">
+        <v>3</v>
+      </c>
+      <c r="F193" t="s">
+        <v>42</v>
+      </c>
+      <c r="G193" t="s">
+        <v>7</v>
+      </c>
+      <c r="H193" t="s">
+        <v>27</v>
+      </c>
+      <c r="I193">
+        <v>0</v>
+      </c>
+      <c r="J193">
+        <v>2204</v>
+      </c>
+      <c r="K193">
+        <v>0.5</v>
+      </c>
+      <c r="L193">
+        <v>1</v>
+      </c>
+      <c r="M193">
+        <v>13</v>
+      </c>
+      <c r="N193">
+        <v>3.5</v>
+      </c>
+      <c r="P193">
+        <v>5</v>
+      </c>
+      <c r="Q193">
+        <v>1.5</v>
+      </c>
+      <c r="R193">
+        <v>23</v>
+      </c>
+      <c r="S193">
+        <v>13.5</v>
+      </c>
+      <c r="V193">
+        <v>1.5</v>
+      </c>
+      <c r="W193">
+        <v>1.5</v>
+      </c>
+      <c r="X193">
+        <v>15.5</v>
+      </c>
+      <c r="Y193">
+        <v>15.5</v>
+      </c>
+      <c r="AB193">
+        <v>1.5</v>
+      </c>
+      <c r="AD193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>91</v>
+      </c>
+      <c r="B194">
+        <v>2022</v>
+      </c>
+      <c r="C194">
+        <v>24</v>
+      </c>
+      <c r="D194">
+        <v>2</v>
+      </c>
+      <c r="E194">
+        <v>7</v>
+      </c>
+      <c r="F194" t="s">
+        <v>40</v>
+      </c>
+      <c r="G194" t="s">
+        <v>7</v>
+      </c>
+      <c r="H194" t="s">
+        <v>27</v>
+      </c>
+      <c r="I194">
+        <v>1</v>
+      </c>
+      <c r="J194">
+        <v>1000</v>
+      </c>
+      <c r="K194">
+        <v>1</v>
+      </c>
+      <c r="L194" t="s">
+        <v>37</v>
+      </c>
+      <c r="M194">
+        <v>9</v>
+      </c>
+      <c r="N194">
+        <v>4</v>
+      </c>
+      <c r="P194">
+        <v>4</v>
+      </c>
+      <c r="Q194">
+        <v>3</v>
+      </c>
+      <c r="R194">
+        <v>24</v>
+      </c>
+      <c r="S194">
+        <v>17</v>
+      </c>
+      <c r="V194">
+        <v>1</v>
+      </c>
+      <c r="W194">
+        <v>2</v>
+      </c>
+      <c r="X194">
+        <v>17</v>
+      </c>
+      <c r="Y194">
+        <v>14</v>
+      </c>
+      <c r="AD194">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ elabe and harris polls (2/9)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E19B46-5578-9B45-A36F-4DD4A2C0A401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A640BDCA-BC13-7042-926C-E8979A563541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="5440" windowWidth="25920" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF194"/>
+  <dimension ref="A1:AF196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="J191" sqref="J191"/>
+      <selection pane="bottomLeft" activeCell="AE196" sqref="AE196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14772,7 +14772,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="193" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>90</v>
       </c>
@@ -14846,7 +14846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>91</v>
       </c>
@@ -14915,6 +14915,160 @@
       </c>
       <c r="AD194">
         <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>92</v>
+      </c>
+      <c r="B195">
+        <v>2022</v>
+      </c>
+      <c r="C195">
+        <v>24</v>
+      </c>
+      <c r="D195">
+        <v>2</v>
+      </c>
+      <c r="E195">
+        <v>8</v>
+      </c>
+      <c r="F195" t="s">
+        <v>36</v>
+      </c>
+      <c r="G195" t="s">
+        <v>7</v>
+      </c>
+      <c r="H195" t="s">
+        <v>27</v>
+      </c>
+      <c r="I195">
+        <v>0</v>
+      </c>
+      <c r="J195">
+        <v>999</v>
+      </c>
+      <c r="K195">
+        <v>1</v>
+      </c>
+      <c r="L195">
+        <v>0.5</v>
+      </c>
+      <c r="M195">
+        <v>10</v>
+      </c>
+      <c r="N195">
+        <v>4</v>
+      </c>
+      <c r="P195">
+        <v>4.5</v>
+      </c>
+      <c r="Q195">
+        <v>1.5</v>
+      </c>
+      <c r="R195">
+        <v>26</v>
+      </c>
+      <c r="S195">
+        <v>15</v>
+      </c>
+      <c r="V195">
+        <v>2</v>
+      </c>
+      <c r="W195">
+        <v>1.5</v>
+      </c>
+      <c r="X195">
+        <v>15.5</v>
+      </c>
+      <c r="Y195">
+        <v>13</v>
+      </c>
+      <c r="Z195">
+        <v>0.5</v>
+      </c>
+      <c r="AB195">
+        <v>1.5</v>
+      </c>
+      <c r="AD195">
+        <v>3.5</v>
+      </c>
+      <c r="AE195" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="196" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>93</v>
+      </c>
+      <c r="B196">
+        <v>2022</v>
+      </c>
+      <c r="C196">
+        <v>23</v>
+      </c>
+      <c r="D196">
+        <v>2</v>
+      </c>
+      <c r="E196">
+        <v>6</v>
+      </c>
+      <c r="F196" t="s">
+        <v>26</v>
+      </c>
+      <c r="G196" t="s">
+        <v>7</v>
+      </c>
+      <c r="H196" t="s">
+        <v>28</v>
+      </c>
+      <c r="I196">
+        <v>0</v>
+      </c>
+      <c r="J196">
+        <v>1800</v>
+      </c>
+      <c r="K196" t="s">
+        <v>30</v>
+      </c>
+      <c r="L196" t="s">
+        <v>30</v>
+      </c>
+      <c r="M196">
+        <v>10</v>
+      </c>
+      <c r="N196">
+        <v>3</v>
+      </c>
+      <c r="P196">
+        <v>6</v>
+      </c>
+      <c r="Q196">
+        <v>3</v>
+      </c>
+      <c r="R196">
+        <v>24</v>
+      </c>
+      <c r="S196">
+        <v>15</v>
+      </c>
+      <c r="V196">
+        <v>1</v>
+      </c>
+      <c r="W196">
+        <v>1</v>
+      </c>
+      <c r="X196">
+        <v>17</v>
+      </c>
+      <c r="Y196">
+        <v>14.5</v>
+      </c>
+      <c r="Z196">
+        <v>0.5</v>
+      </c>
+      <c r="AD196">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ ipsos and bva polls (2/11) + update Ns
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A640BDCA-BC13-7042-926C-E8979A563541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48158F2E-12A6-CA47-9BAE-0D9C04465826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="5440" windowWidth="25920" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF196"/>
+  <dimension ref="A1:AF198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AE196" sqref="AE196"/>
+      <selection pane="bottomLeft" activeCell="AF198" sqref="AF198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14875,7 +14875,7 @@
         <v>1</v>
       </c>
       <c r="J194">
-        <v>1000</v>
+        <v>1101</v>
       </c>
       <c r="K194">
         <v>1</v>
@@ -15026,7 +15026,7 @@
         <v>0</v>
       </c>
       <c r="J196">
-        <v>1800</v>
+        <v>1720</v>
       </c>
       <c r="K196" t="s">
         <v>30</v>
@@ -15069,6 +15069,154 @@
       </c>
       <c r="AD196">
         <v>5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>94</v>
+      </c>
+      <c r="B197">
+        <v>2022</v>
+      </c>
+      <c r="C197">
+        <v>23</v>
+      </c>
+      <c r="D197">
+        <v>2</v>
+      </c>
+      <c r="E197">
+        <v>5</v>
+      </c>
+      <c r="F197" t="s">
+        <v>6</v>
+      </c>
+      <c r="G197" t="s">
+        <v>7</v>
+      </c>
+      <c r="H197" t="s">
+        <v>8</v>
+      </c>
+      <c r="I197">
+        <v>0</v>
+      </c>
+      <c r="J197">
+        <v>7741</v>
+      </c>
+      <c r="K197">
+        <v>0.5</v>
+      </c>
+      <c r="L197">
+        <v>1</v>
+      </c>
+      <c r="M197">
+        <v>9</v>
+      </c>
+      <c r="N197">
+        <v>3.5</v>
+      </c>
+      <c r="P197">
+        <v>7</v>
+      </c>
+      <c r="Q197">
+        <v>2.5</v>
+      </c>
+      <c r="R197">
+        <v>24</v>
+      </c>
+      <c r="S197">
+        <v>15.5</v>
+      </c>
+      <c r="V197">
+        <v>1</v>
+      </c>
+      <c r="W197">
+        <v>1.5</v>
+      </c>
+      <c r="X197">
+        <v>15</v>
+      </c>
+      <c r="Y197">
+        <v>14.5</v>
+      </c>
+      <c r="AD197">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>95</v>
+      </c>
+      <c r="B198">
+        <v>2022</v>
+      </c>
+      <c r="C198">
+        <v>24</v>
+      </c>
+      <c r="D198">
+        <v>2</v>
+      </c>
+      <c r="E198">
+        <v>8</v>
+      </c>
+      <c r="F198" t="s">
+        <v>41</v>
+      </c>
+      <c r="G198" t="s">
+        <v>7</v>
+      </c>
+      <c r="H198" t="s">
+        <v>27</v>
+      </c>
+      <c r="I198">
+        <v>0</v>
+      </c>
+      <c r="J198">
+        <v>892</v>
+      </c>
+      <c r="K198">
+        <v>0.5</v>
+      </c>
+      <c r="L198">
+        <v>1.5</v>
+      </c>
+      <c r="M198">
+        <v>9</v>
+      </c>
+      <c r="N198">
+        <v>4</v>
+      </c>
+      <c r="P198">
+        <v>4.5</v>
+      </c>
+      <c r="Q198">
+        <v>2</v>
+      </c>
+      <c r="R198">
+        <v>25</v>
+      </c>
+      <c r="S198">
+        <v>14.5</v>
+      </c>
+      <c r="V198">
+        <v>1.5</v>
+      </c>
+      <c r="W198">
+        <v>2</v>
+      </c>
+      <c r="X198">
+        <v>17</v>
+      </c>
+      <c r="Y198">
+        <v>14</v>
+      </c>
+      <c r="Z198">
+        <v>0.5</v>
+      </c>
+      <c r="AD198">
+        <v>4</v>
+      </c>
+      <c r="AE198" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ ifop rolling (2/11)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48158F2E-12A6-CA47-9BAE-0D9C04465826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF914D66-18B6-FF42-8B62-813E596BE72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="5440" windowWidth="25920" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF198"/>
+  <dimension ref="A1:AF199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AF198" sqref="AF198"/>
+      <selection pane="bottomLeft" activeCell="AE200" sqref="AE200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15217,6 +15217,80 @@
       </c>
       <c r="AE198" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="199" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>96</v>
+      </c>
+      <c r="B199">
+        <v>2022</v>
+      </c>
+      <c r="C199">
+        <v>24</v>
+      </c>
+      <c r="D199">
+        <v>2</v>
+      </c>
+      <c r="E199">
+        <v>10</v>
+      </c>
+      <c r="F199" t="s">
+        <v>35</v>
+      </c>
+      <c r="G199" t="s">
+        <v>7</v>
+      </c>
+      <c r="H199" t="s">
+        <v>28</v>
+      </c>
+      <c r="I199">
+        <v>1</v>
+      </c>
+      <c r="J199">
+        <v>1100</v>
+      </c>
+      <c r="K199">
+        <v>0.5</v>
+      </c>
+      <c r="L199">
+        <v>0.5</v>
+      </c>
+      <c r="M199">
+        <v>10.5</v>
+      </c>
+      <c r="N199">
+        <v>3</v>
+      </c>
+      <c r="P199">
+        <v>5</v>
+      </c>
+      <c r="Q199">
+        <v>2.5</v>
+      </c>
+      <c r="R199">
+        <v>25.5</v>
+      </c>
+      <c r="S199">
+        <v>15</v>
+      </c>
+      <c r="V199">
+        <v>0.5</v>
+      </c>
+      <c r="W199">
+        <v>2</v>
+      </c>
+      <c r="X199">
+        <v>17</v>
+      </c>
+      <c r="Y199">
+        <v>15</v>
+      </c>
+      <c r="AD199">
+        <v>2.5</v>
+      </c>
+      <c r="AE199">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ opinionway poll (2/11) + update Ns
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF914D66-18B6-FF42-8B62-813E596BE72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953F58A0-D446-914A-8424-855C63762170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="5440" windowWidth="25920" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AF199"/>
+  <dimension ref="A1:AF200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AE200" sqref="AE200"/>
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD200" sqref="AD200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15248,7 +15248,7 @@
         <v>1</v>
       </c>
       <c r="J199">
-        <v>1100</v>
+        <v>1113</v>
       </c>
       <c r="K199">
         <v>0.5</v>
@@ -15291,6 +15291,77 @@
       </c>
       <c r="AE199">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>97</v>
+      </c>
+      <c r="B200">
+        <v>2022</v>
+      </c>
+      <c r="C200">
+        <v>24</v>
+      </c>
+      <c r="D200">
+        <v>2</v>
+      </c>
+      <c r="E200">
+        <v>10</v>
+      </c>
+      <c r="F200" t="s">
+        <v>40</v>
+      </c>
+      <c r="G200" t="s">
+        <v>7</v>
+      </c>
+      <c r="H200" t="s">
+        <v>27</v>
+      </c>
+      <c r="I200">
+        <v>0</v>
+      </c>
+      <c r="J200">
+        <v>636</v>
+      </c>
+      <c r="K200" t="s">
+        <v>37</v>
+      </c>
+      <c r="L200">
+        <v>1</v>
+      </c>
+      <c r="M200">
+        <v>10</v>
+      </c>
+      <c r="N200">
+        <v>4</v>
+      </c>
+      <c r="P200">
+        <v>6</v>
+      </c>
+      <c r="Q200">
+        <v>3</v>
+      </c>
+      <c r="R200">
+        <v>23</v>
+      </c>
+      <c r="S200">
+        <v>16</v>
+      </c>
+      <c r="V200">
+        <v>1</v>
+      </c>
+      <c r="W200">
+        <v>1</v>
+      </c>
+      <c r="X200">
+        <v>18</v>
+      </c>
+      <c r="Y200">
+        <v>13</v>
+      </c>
+      <c r="AD200">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update w/ ifop and ow rollings (2/15) and w/ harris and cluster17 polls (2/15)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954AA088-231D-A441-AF27-C2FD430E2789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F890671-0C17-B34C-A6B2-EEA2C551E62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="5440" windowWidth="25920" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="22780" yWindow="8900" windowWidth="25920" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="49">
   <si>
     <t>year</t>
   </si>
@@ -547,11 +547,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH202"/>
+  <dimension ref="A1:AH206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AH203" sqref="AH203"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B206" sqref="B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17315,6 +17315,338 @@
         <v>0.5</v>
       </c>
       <c r="AH202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>100</v>
+      </c>
+      <c r="B203">
+        <v>2022</v>
+      </c>
+      <c r="C203">
+        <v>24</v>
+      </c>
+      <c r="D203">
+        <v>2</v>
+      </c>
+      <c r="E203">
+        <v>10</v>
+      </c>
+      <c r="F203" t="s">
+        <v>42</v>
+      </c>
+      <c r="G203" t="s">
+        <v>7</v>
+      </c>
+      <c r="H203" t="s">
+        <v>27</v>
+      </c>
+      <c r="I203">
+        <v>0</v>
+      </c>
+      <c r="J203">
+        <v>2085</v>
+      </c>
+      <c r="K203">
+        <v>0</v>
+      </c>
+      <c r="L203">
+        <v>1</v>
+      </c>
+      <c r="M203">
+        <v>0.5</v>
+      </c>
+      <c r="N203">
+        <v>0.5</v>
+      </c>
+      <c r="O203">
+        <v>13</v>
+      </c>
+      <c r="P203">
+        <v>4</v>
+      </c>
+      <c r="R203">
+        <v>5</v>
+      </c>
+      <c r="S203">
+        <v>2</v>
+      </c>
+      <c r="T203">
+        <v>23</v>
+      </c>
+      <c r="U203">
+        <v>15</v>
+      </c>
+      <c r="X203">
+        <v>0.5</v>
+      </c>
+      <c r="Y203">
+        <v>1</v>
+      </c>
+      <c r="Z203">
+        <v>16.5</v>
+      </c>
+      <c r="AA203">
+        <v>15</v>
+      </c>
+      <c r="AB203">
+        <v>0.5</v>
+      </c>
+      <c r="AD203">
+        <v>1</v>
+      </c>
+      <c r="AF203">
+        <v>2.5</v>
+      </c>
+      <c r="AH203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>101</v>
+      </c>
+      <c r="B204">
+        <v>2022</v>
+      </c>
+      <c r="C204">
+        <v>25</v>
+      </c>
+      <c r="D204">
+        <v>2</v>
+      </c>
+      <c r="E204">
+        <v>14</v>
+      </c>
+      <c r="F204" t="s">
+        <v>40</v>
+      </c>
+      <c r="G204" t="s">
+        <v>7</v>
+      </c>
+      <c r="H204" t="s">
+        <v>27</v>
+      </c>
+      <c r="I204">
+        <v>1</v>
+      </c>
+      <c r="J204">
+        <v>1000</v>
+      </c>
+      <c r="K204">
+        <v>1</v>
+      </c>
+      <c r="L204">
+        <v>1</v>
+      </c>
+      <c r="M204" t="s">
+        <v>37</v>
+      </c>
+      <c r="N204" t="s">
+        <v>37</v>
+      </c>
+      <c r="O204">
+        <v>10</v>
+      </c>
+      <c r="P204">
+        <v>5</v>
+      </c>
+      <c r="R204">
+        <v>5</v>
+      </c>
+      <c r="S204">
+        <v>3</v>
+      </c>
+      <c r="T204">
+        <v>25</v>
+      </c>
+      <c r="U204">
+        <v>16</v>
+      </c>
+      <c r="X204">
+        <v>2</v>
+      </c>
+      <c r="Y204">
+        <v>2</v>
+      </c>
+      <c r="Z204">
+        <v>15</v>
+      </c>
+      <c r="AA204">
+        <v>14</v>
+      </c>
+      <c r="AF204">
+        <v>3</v>
+      </c>
+      <c r="AH204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>102</v>
+      </c>
+      <c r="B205">
+        <v>2022</v>
+      </c>
+      <c r="C205">
+        <v>24</v>
+      </c>
+      <c r="D205">
+        <v>2</v>
+      </c>
+      <c r="E205">
+        <v>13</v>
+      </c>
+      <c r="F205" t="s">
+        <v>26</v>
+      </c>
+      <c r="G205" t="s">
+        <v>7</v>
+      </c>
+      <c r="H205" t="s">
+        <v>28</v>
+      </c>
+      <c r="I205">
+        <v>0</v>
+      </c>
+      <c r="J205">
+        <v>1700</v>
+      </c>
+      <c r="K205">
+        <v>1</v>
+      </c>
+      <c r="L205">
+        <v>1</v>
+      </c>
+      <c r="M205">
+        <v>0.5</v>
+      </c>
+      <c r="N205">
+        <v>0.5</v>
+      </c>
+      <c r="O205">
+        <v>10.5</v>
+      </c>
+      <c r="P205">
+        <v>3.5</v>
+      </c>
+      <c r="R205">
+        <v>5.5</v>
+      </c>
+      <c r="S205">
+        <v>2.5</v>
+      </c>
+      <c r="T205">
+        <v>25</v>
+      </c>
+      <c r="U205">
+        <v>14</v>
+      </c>
+      <c r="X205">
+        <v>1</v>
+      </c>
+      <c r="Y205">
+        <v>1</v>
+      </c>
+      <c r="Z205">
+        <v>17.5</v>
+      </c>
+      <c r="AA205">
+        <v>14.5</v>
+      </c>
+      <c r="AB205">
+        <v>0.5</v>
+      </c>
+      <c r="AF205">
+        <v>3.5</v>
+      </c>
+      <c r="AH205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>103</v>
+      </c>
+      <c r="B206">
+        <v>2022</v>
+      </c>
+      <c r="C206">
+        <v>25</v>
+      </c>
+      <c r="D206">
+        <v>2</v>
+      </c>
+      <c r="E206">
+        <v>14</v>
+      </c>
+      <c r="F206" t="s">
+        <v>35</v>
+      </c>
+      <c r="G206" t="s">
+        <v>7</v>
+      </c>
+      <c r="H206" t="s">
+        <v>28</v>
+      </c>
+      <c r="I206">
+        <v>1</v>
+      </c>
+      <c r="J206">
+        <v>1200</v>
+      </c>
+      <c r="K206">
+        <v>1</v>
+      </c>
+      <c r="L206">
+        <v>1</v>
+      </c>
+      <c r="M206">
+        <v>0.5</v>
+      </c>
+      <c r="N206">
+        <v>0.5</v>
+      </c>
+      <c r="O206">
+        <v>11.5</v>
+      </c>
+      <c r="P206">
+        <v>3</v>
+      </c>
+      <c r="R206">
+        <v>4.5</v>
+      </c>
+      <c r="S206">
+        <v>2</v>
+      </c>
+      <c r="T206">
+        <v>25.5</v>
+      </c>
+      <c r="U206">
+        <v>14.5</v>
+      </c>
+      <c r="X206">
+        <v>1</v>
+      </c>
+      <c r="Y206">
+        <v>1.5</v>
+      </c>
+      <c r="Z206">
+        <v>17.5</v>
+      </c>
+      <c r="AA206">
+        <v>15</v>
+      </c>
+      <c r="AF206">
+        <v>3</v>
+      </c>
+      <c r="AG206" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH206">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update w/ elabe poll (2/16)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F890671-0C17-B34C-A6B2-EEA2C551E62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D233AD-8E10-CB4C-BC2B-158D7EA7C593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22780" yWindow="8900" windowWidth="25920" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="23940" yWindow="8840" windowWidth="25920" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="49">
   <si>
     <t>year</t>
   </si>
@@ -230,9 +230,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,11 +548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH206"/>
+  <dimension ref="A1:AH207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B206" sqref="B206"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AH208" sqref="AH208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +695,7 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="2">
         <v>1</v>
       </c>
       <c r="M2">
@@ -771,7 +772,7 @@
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="2">
         <v>1</v>
       </c>
       <c r="M3">
@@ -848,7 +849,7 @@
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4">
@@ -925,7 +926,7 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="2">
         <v>1</v>
       </c>
       <c r="M5" t="s">
@@ -1002,7 +1003,7 @@
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="2">
         <v>1</v>
       </c>
       <c r="M6" t="s">
@@ -1079,7 +1080,7 @@
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="2">
         <v>1</v>
       </c>
       <c r="M7" t="s">
@@ -1156,7 +1157,7 @@
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="2">
         <v>1</v>
       </c>
       <c r="M8" t="s">
@@ -1230,7 +1231,7 @@
       <c r="K9">
         <v>0</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="2">
         <v>1</v>
       </c>
       <c r="M9" t="s">
@@ -1304,7 +1305,7 @@
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="2">
         <v>1</v>
       </c>
       <c r="M10" t="s">
@@ -1378,7 +1379,7 @@
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="2">
         <v>1</v>
       </c>
       <c r="M11">
@@ -1458,7 +1459,7 @@
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="2">
         <v>1</v>
       </c>
       <c r="M12">
@@ -1538,7 +1539,7 @@
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="2">
         <v>1</v>
       </c>
       <c r="M13">
@@ -1618,7 +1619,7 @@
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="2">
         <v>1</v>
       </c>
       <c r="M14">
@@ -1701,7 +1702,7 @@
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="2">
         <v>1</v>
       </c>
       <c r="M15">
@@ -1781,7 +1782,7 @@
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="2">
         <v>1</v>
       </c>
       <c r="M16">
@@ -1861,7 +1862,7 @@
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="2">
         <v>1</v>
       </c>
       <c r="M17">
@@ -1941,7 +1942,7 @@
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="2">
         <v>1</v>
       </c>
       <c r="M18">
@@ -2021,7 +2022,7 @@
       <c r="K19">
         <v>0</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="2">
         <v>1</v>
       </c>
       <c r="M19">
@@ -2104,7 +2105,7 @@
       <c r="K20">
         <v>0</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="2">
         <v>1</v>
       </c>
       <c r="M20">
@@ -2191,7 +2192,7 @@
       <c r="K21">
         <v>0</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="2">
         <v>1</v>
       </c>
       <c r="M21">
@@ -2277,7 +2278,7 @@
       <c r="K22">
         <v>0</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="2">
         <v>1</v>
       </c>
       <c r="M22">
@@ -2366,7 +2367,7 @@
       <c r="K23">
         <v>0</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="2">
         <v>1</v>
       </c>
       <c r="M23">
@@ -2455,7 +2456,7 @@
       <c r="K24">
         <v>0</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="2">
         <v>1</v>
       </c>
       <c r="M24">
@@ -2541,7 +2542,7 @@
       <c r="K25">
         <v>0</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="2">
         <v>1</v>
       </c>
       <c r="M25">
@@ -2627,7 +2628,7 @@
       <c r="K26">
         <v>0</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="2">
         <v>1</v>
       </c>
       <c r="M26">
@@ -2704,7 +2705,7 @@
       <c r="K27">
         <v>0</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="2">
         <v>1</v>
       </c>
       <c r="M27">
@@ -2781,7 +2782,7 @@
       <c r="K28">
         <v>0</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="2">
         <v>1</v>
       </c>
       <c r="M28">
@@ -2858,7 +2859,7 @@
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="2">
         <v>1</v>
       </c>
       <c r="M29">
@@ -2932,7 +2933,7 @@
       <c r="K30">
         <v>0</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="2">
         <v>1</v>
       </c>
       <c r="M30">
@@ -3006,7 +3007,7 @@
       <c r="K31">
         <v>0</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="2">
         <v>1</v>
       </c>
       <c r="M31">
@@ -3089,7 +3090,7 @@
       <c r="K32">
         <v>0</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="2">
         <v>1</v>
       </c>
       <c r="M32">
@@ -3172,7 +3173,7 @@
       <c r="K33">
         <v>0</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="2">
         <v>1</v>
       </c>
       <c r="M33">
@@ -3255,7 +3256,7 @@
       <c r="K34">
         <v>0</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="2">
         <v>1</v>
       </c>
       <c r="M34">
@@ -3332,7 +3333,7 @@
       <c r="K35">
         <v>0</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="2">
         <v>1</v>
       </c>
       <c r="M35">
@@ -3409,7 +3410,7 @@
       <c r="K36">
         <v>0</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="2">
         <v>1</v>
       </c>
       <c r="M36">
@@ -3486,7 +3487,7 @@
       <c r="K37">
         <v>0</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="2">
         <v>1</v>
       </c>
       <c r="M37">
@@ -3566,7 +3567,7 @@
       <c r="K38">
         <v>0</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="2">
         <v>1</v>
       </c>
       <c r="M38">
@@ -3646,7 +3647,7 @@
       <c r="K39">
         <v>0</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="2">
         <v>1</v>
       </c>
       <c r="M39">
@@ -3726,7 +3727,7 @@
       <c r="K40">
         <v>0</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="2">
         <v>1</v>
       </c>
       <c r="M40">
@@ -3806,7 +3807,7 @@
       <c r="K41">
         <v>0</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="2">
         <v>1</v>
       </c>
       <c r="M41">
@@ -3886,7 +3887,7 @@
       <c r="K42">
         <v>0</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="2">
         <v>1</v>
       </c>
       <c r="M42">
@@ -3966,7 +3967,7 @@
       <c r="K43">
         <v>0</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="2">
         <v>1</v>
       </c>
       <c r="M43">
@@ -4043,7 +4044,7 @@
       <c r="K44">
         <v>0</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="2">
         <v>1</v>
       </c>
       <c r="M44">
@@ -4120,7 +4121,7 @@
       <c r="K45">
         <v>0</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="2">
         <v>1</v>
       </c>
       <c r="M45">
@@ -4197,7 +4198,7 @@
       <c r="K46">
         <v>0</v>
       </c>
-      <c r="L46">
+      <c r="L46" s="2">
         <v>1</v>
       </c>
       <c r="M46">
@@ -4290,7 +4291,7 @@
       <c r="K47">
         <v>0</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="2">
         <v>1</v>
       </c>
       <c r="M47">
@@ -4383,7 +4384,7 @@
       <c r="K48">
         <v>0</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="2">
         <v>1</v>
       </c>
       <c r="M48">
@@ -4476,7 +4477,7 @@
       <c r="K49">
         <v>0</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="2">
         <v>1</v>
       </c>
       <c r="M49">
@@ -4568,7 +4569,7 @@
       <c r="K50">
         <v>0</v>
       </c>
-      <c r="L50">
+      <c r="L50" s="2">
         <v>1</v>
       </c>
       <c r="M50">
@@ -4661,7 +4662,7 @@
       <c r="K51">
         <v>0</v>
       </c>
-      <c r="L51">
+      <c r="L51" s="2">
         <v>1</v>
       </c>
       <c r="M51">
@@ -4754,7 +4755,7 @@
       <c r="K52">
         <v>0</v>
       </c>
-      <c r="L52">
+      <c r="L52" s="2">
         <v>1</v>
       </c>
       <c r="M52">
@@ -4834,7 +4835,7 @@
       <c r="K53">
         <v>0</v>
       </c>
-      <c r="L53">
+      <c r="L53" s="2">
         <v>1</v>
       </c>
       <c r="M53">
@@ -4914,7 +4915,7 @@
       <c r="K54">
         <v>0</v>
       </c>
-      <c r="L54">
+      <c r="L54" s="2">
         <v>1</v>
       </c>
       <c r="M54">
@@ -4991,7 +4992,7 @@
       <c r="K55">
         <v>0</v>
       </c>
-      <c r="L55">
+      <c r="L55" s="2">
         <v>1</v>
       </c>
       <c r="M55">
@@ -5068,7 +5069,7 @@
       <c r="K56">
         <v>0</v>
       </c>
-      <c r="L56">
+      <c r="L56" s="2">
         <v>1</v>
       </c>
       <c r="M56">
@@ -5139,7 +5140,7 @@
       <c r="K57">
         <v>0</v>
       </c>
-      <c r="L57">
+      <c r="L57" s="2">
         <v>1</v>
       </c>
       <c r="M57">
@@ -5222,7 +5223,7 @@
       <c r="K58">
         <v>0</v>
       </c>
-      <c r="L58">
+      <c r="L58" s="2">
         <v>1</v>
       </c>
       <c r="M58">
@@ -5305,7 +5306,7 @@
       <c r="K59">
         <v>0</v>
       </c>
-      <c r="L59">
+      <c r="L59" s="2">
         <v>1</v>
       </c>
       <c r="M59">
@@ -5388,7 +5389,7 @@
       <c r="K60">
         <v>0</v>
       </c>
-      <c r="L60">
+      <c r="L60" s="2">
         <v>1</v>
       </c>
       <c r="M60">
@@ -5481,7 +5482,7 @@
       <c r="K61">
         <v>0</v>
       </c>
-      <c r="L61">
+      <c r="L61" s="2">
         <v>1</v>
       </c>
       <c r="M61">
@@ -5574,7 +5575,7 @@
       <c r="K62">
         <v>0</v>
       </c>
-      <c r="L62">
+      <c r="L62" s="2">
         <v>1</v>
       </c>
       <c r="M62">
@@ -5667,7 +5668,7 @@
       <c r="K63">
         <v>0</v>
       </c>
-      <c r="L63">
+      <c r="L63" s="2">
         <v>1</v>
       </c>
       <c r="M63">
@@ -5747,7 +5748,7 @@
       <c r="K64">
         <v>0</v>
       </c>
-      <c r="L64">
+      <c r="L64" s="2">
         <v>1</v>
       </c>
       <c r="M64">
@@ -5827,7 +5828,7 @@
       <c r="K65">
         <v>0</v>
       </c>
-      <c r="L65">
+      <c r="L65" s="2">
         <v>1</v>
       </c>
       <c r="M65">
@@ -5907,7 +5908,7 @@
       <c r="K66">
         <v>0</v>
       </c>
-      <c r="L66">
+      <c r="L66" s="2">
         <v>1</v>
       </c>
       <c r="M66">
@@ -5984,7 +5985,7 @@
       <c r="K67">
         <v>0</v>
       </c>
-      <c r="L67">
+      <c r="L67" s="2">
         <v>1</v>
       </c>
       <c r="M67">
@@ -6061,7 +6062,7 @@
       <c r="K68">
         <v>0</v>
       </c>
-      <c r="L68">
+      <c r="L68" s="2">
         <v>1</v>
       </c>
       <c r="M68">
@@ -6138,7 +6139,7 @@
       <c r="K69">
         <v>0</v>
       </c>
-      <c r="L69">
+      <c r="L69" s="2">
         <v>1</v>
       </c>
       <c r="M69">
@@ -6218,7 +6219,7 @@
       <c r="K70">
         <v>0</v>
       </c>
-      <c r="L70">
+      <c r="L70" s="2">
         <v>1</v>
       </c>
       <c r="M70">
@@ -6298,7 +6299,7 @@
       <c r="K71">
         <v>0</v>
       </c>
-      <c r="L71">
+      <c r="L71" s="2">
         <v>1</v>
       </c>
       <c r="M71">
@@ -6378,7 +6379,7 @@
       <c r="K72">
         <v>0</v>
       </c>
-      <c r="L72">
+      <c r="L72" s="2">
         <v>1</v>
       </c>
       <c r="M72">
@@ -6458,7 +6459,7 @@
       <c r="K73">
         <v>0</v>
       </c>
-      <c r="L73">
+      <c r="L73" s="2">
         <v>1</v>
       </c>
       <c r="M73">
@@ -6538,7 +6539,7 @@
       <c r="K74">
         <v>0</v>
       </c>
-      <c r="L74">
+      <c r="L74" s="2">
         <v>1</v>
       </c>
       <c r="M74">
@@ -6618,7 +6619,7 @@
       <c r="K75">
         <v>0</v>
       </c>
-      <c r="L75">
+      <c r="L75" s="2">
         <v>1</v>
       </c>
       <c r="M75">
@@ -6704,7 +6705,7 @@
       <c r="K76">
         <v>0</v>
       </c>
-      <c r="L76">
+      <c r="L76" s="2">
         <v>1</v>
       </c>
       <c r="M76">
@@ -6790,7 +6791,7 @@
       <c r="K77">
         <v>0</v>
       </c>
-      <c r="L77">
+      <c r="L77" s="2">
         <v>1</v>
       </c>
       <c r="M77">
@@ -6876,7 +6877,7 @@
       <c r="K78">
         <v>0</v>
       </c>
-      <c r="L78">
+      <c r="L78" s="2">
         <v>1</v>
       </c>
       <c r="M78">
@@ -6953,7 +6954,7 @@
       <c r="K79">
         <v>0</v>
       </c>
-      <c r="L79">
+      <c r="L79" s="2">
         <v>1</v>
       </c>
       <c r="M79">
@@ -7030,7 +7031,7 @@
       <c r="K80">
         <v>0</v>
       </c>
-      <c r="L80">
+      <c r="L80" s="2">
         <v>1</v>
       </c>
       <c r="M80">
@@ -7107,7 +7108,7 @@
       <c r="K81">
         <v>0</v>
       </c>
-      <c r="L81">
+      <c r="L81" s="2">
         <v>1</v>
       </c>
       <c r="M81">
@@ -7181,7 +7182,7 @@
       <c r="K82">
         <v>0</v>
       </c>
-      <c r="L82">
+      <c r="L82" s="2">
         <v>1</v>
       </c>
       <c r="M82">
@@ -7271,7 +7272,7 @@
       <c r="K83">
         <v>0</v>
       </c>
-      <c r="L83">
+      <c r="L83" s="2">
         <v>1</v>
       </c>
       <c r="M83">
@@ -7361,7 +7362,7 @@
       <c r="K84">
         <v>0</v>
       </c>
-      <c r="L84">
+      <c r="L84" s="2">
         <v>1</v>
       </c>
       <c r="M84">
@@ -7451,7 +7452,7 @@
       <c r="K85">
         <v>0</v>
       </c>
-      <c r="L85">
+      <c r="L85" s="2">
         <v>1</v>
       </c>
       <c r="M85">
@@ -7544,7 +7545,7 @@
       <c r="K86">
         <v>0</v>
       </c>
-      <c r="L86">
+      <c r="L86" s="2">
         <v>1</v>
       </c>
       <c r="M86">
@@ -7637,7 +7638,7 @@
       <c r="K87">
         <v>0</v>
       </c>
-      <c r="L87">
+      <c r="L87" s="2">
         <v>1</v>
       </c>
       <c r="M87">
@@ -7729,7 +7730,7 @@
       <c r="K88">
         <v>0</v>
       </c>
-      <c r="L88">
+      <c r="L88" s="2">
         <v>1</v>
       </c>
       <c r="M88">
@@ -7819,7 +7820,7 @@
       <c r="K89">
         <v>0</v>
       </c>
-      <c r="L89">
+      <c r="L89" s="2">
         <v>1</v>
       </c>
       <c r="M89">
@@ -7909,7 +7910,7 @@
       <c r="K90">
         <v>0</v>
       </c>
-      <c r="L90">
+      <c r="L90" s="2">
         <v>1</v>
       </c>
       <c r="M90">
@@ -7999,7 +8000,7 @@
       <c r="K91">
         <v>0</v>
       </c>
-      <c r="L91">
+      <c r="L91" s="2">
         <v>1</v>
       </c>
       <c r="M91">
@@ -8079,7 +8080,7 @@
       <c r="K92">
         <v>0</v>
       </c>
-      <c r="L92">
+      <c r="L92" s="2">
         <v>1</v>
       </c>
       <c r="M92">
@@ -8159,7 +8160,7 @@
       <c r="K93">
         <v>0</v>
       </c>
-      <c r="L93">
+      <c r="L93" s="2">
         <v>1</v>
       </c>
       <c r="M93">
@@ -8239,7 +8240,7 @@
       <c r="K94">
         <v>0</v>
       </c>
-      <c r="L94">
+      <c r="L94" s="2">
         <v>1</v>
       </c>
       <c r="M94">
@@ -8329,7 +8330,7 @@
       <c r="K95">
         <v>0</v>
       </c>
-      <c r="L95">
+      <c r="L95" s="2">
         <v>1</v>
       </c>
       <c r="M95">
@@ -8419,7 +8420,7 @@
       <c r="K96">
         <v>0</v>
       </c>
-      <c r="L96">
+      <c r="L96" s="2">
         <v>1</v>
       </c>
       <c r="M96">
@@ -8509,7 +8510,7 @@
       <c r="K97">
         <v>0</v>
       </c>
-      <c r="L97">
+      <c r="L97" s="2">
         <v>1</v>
       </c>
       <c r="M97">
@@ -8589,7 +8590,7 @@
       <c r="K98">
         <v>0</v>
       </c>
-      <c r="L98">
+      <c r="L98" s="2">
         <v>1</v>
       </c>
       <c r="M98">
@@ -8669,7 +8670,7 @@
       <c r="K99">
         <v>0</v>
       </c>
-      <c r="L99">
+      <c r="L99" s="2">
         <v>1</v>
       </c>
       <c r="M99">
@@ -8749,7 +8750,7 @@
       <c r="K100">
         <v>0</v>
       </c>
-      <c r="L100">
+      <c r="L100" s="2">
         <v>1</v>
       </c>
       <c r="M100">
@@ -8838,7 +8839,7 @@
       <c r="K101">
         <v>0</v>
       </c>
-      <c r="L101">
+      <c r="L101" s="2">
         <v>1</v>
       </c>
       <c r="M101">
@@ -8927,7 +8928,7 @@
       <c r="K102">
         <v>0</v>
       </c>
-      <c r="L102">
+      <c r="L102" s="2">
         <v>1</v>
       </c>
       <c r="M102">
@@ -9016,7 +9017,7 @@
       <c r="K103">
         <v>0</v>
       </c>
-      <c r="L103">
+      <c r="L103" s="2">
         <v>1</v>
       </c>
       <c r="M103">
@@ -9102,7 +9103,7 @@
       <c r="K104">
         <v>0</v>
       </c>
-      <c r="L104">
+      <c r="L104" s="2">
         <v>1</v>
       </c>
       <c r="M104">
@@ -9188,7 +9189,7 @@
       <c r="K105">
         <v>0</v>
       </c>
-      <c r="L105">
+      <c r="L105" s="2">
         <v>1</v>
       </c>
       <c r="M105">
@@ -9274,7 +9275,7 @@
       <c r="K106">
         <v>0</v>
       </c>
-      <c r="L106">
+      <c r="L106" s="2">
         <v>1</v>
       </c>
       <c r="M106">
@@ -9357,7 +9358,7 @@
       <c r="K107">
         <v>0</v>
       </c>
-      <c r="L107">
+      <c r="L107" s="2">
         <v>1</v>
       </c>
       <c r="M107">
@@ -9440,7 +9441,7 @@
       <c r="K108">
         <v>0</v>
       </c>
-      <c r="L108">
+      <c r="L108" s="2">
         <v>1</v>
       </c>
       <c r="M108">
@@ -9523,7 +9524,7 @@
       <c r="K109">
         <v>0</v>
       </c>
-      <c r="L109">
+      <c r="L109" s="2">
         <v>1</v>
       </c>
       <c r="M109">
@@ -9603,7 +9604,7 @@
       <c r="K110">
         <v>0</v>
       </c>
-      <c r="L110">
+      <c r="L110" s="2">
         <v>1</v>
       </c>
       <c r="M110">
@@ -9683,7 +9684,7 @@
       <c r="K111">
         <v>0</v>
       </c>
-      <c r="L111">
+      <c r="L111" s="2">
         <v>1</v>
       </c>
       <c r="M111">
@@ -9763,7 +9764,7 @@
       <c r="K112">
         <v>0</v>
       </c>
-      <c r="L112">
+      <c r="L112" s="2">
         <v>1</v>
       </c>
       <c r="M112">
@@ -9840,7 +9841,7 @@
       <c r="K113">
         <v>0</v>
       </c>
-      <c r="L113">
+      <c r="L113" s="2">
         <v>1</v>
       </c>
       <c r="M113">
@@ -9917,7 +9918,7 @@
       <c r="K114">
         <v>0</v>
       </c>
-      <c r="L114">
+      <c r="L114" s="2">
         <v>1</v>
       </c>
       <c r="M114">
@@ -9994,7 +9995,7 @@
       <c r="K115">
         <v>0</v>
       </c>
-      <c r="L115">
+      <c r="L115" s="2">
         <v>1</v>
       </c>
       <c r="M115">
@@ -10068,7 +10069,7 @@
       <c r="K116">
         <v>0</v>
       </c>
-      <c r="L116">
+      <c r="L116" s="2">
         <v>1</v>
       </c>
       <c r="M116">
@@ -10154,7 +10155,7 @@
       <c r="K117">
         <v>0</v>
       </c>
-      <c r="L117">
+      <c r="L117" s="2">
         <v>1</v>
       </c>
       <c r="M117">
@@ -10240,7 +10241,7 @@
       <c r="K118">
         <v>0</v>
       </c>
-      <c r="L118">
+      <c r="L118" s="2">
         <v>1</v>
       </c>
       <c r="M118">
@@ -10326,7 +10327,7 @@
       <c r="K119">
         <v>0</v>
       </c>
-      <c r="L119">
+      <c r="L119" s="2">
         <v>1</v>
       </c>
       <c r="M119">
@@ -10415,7 +10416,7 @@
       <c r="K120">
         <v>0</v>
       </c>
-      <c r="L120">
+      <c r="L120" s="2">
         <v>1</v>
       </c>
       <c r="M120">
@@ -10504,7 +10505,7 @@
       <c r="K121">
         <v>0</v>
       </c>
-      <c r="L121">
+      <c r="L121" s="2">
         <v>1</v>
       </c>
       <c r="M121">
@@ -10593,7 +10594,7 @@
       <c r="K122">
         <v>0</v>
       </c>
-      <c r="L122">
+      <c r="L122" s="2">
         <v>1</v>
       </c>
       <c r="M122">
@@ -10673,7 +10674,7 @@
       <c r="K123">
         <v>0</v>
       </c>
-      <c r="L123">
+      <c r="L123" s="2">
         <v>1</v>
       </c>
       <c r="M123">
@@ -10753,7 +10754,7 @@
       <c r="K124">
         <v>0</v>
       </c>
-      <c r="L124">
+      <c r="L124" s="2">
         <v>1</v>
       </c>
       <c r="M124">
@@ -10833,7 +10834,7 @@
       <c r="K125">
         <v>0</v>
       </c>
-      <c r="L125">
+      <c r="L125" s="2">
         <v>1</v>
       </c>
       <c r="M125">
@@ -10919,7 +10920,7 @@
       <c r="K126">
         <v>0</v>
       </c>
-      <c r="L126">
+      <c r="L126" s="2">
         <v>1</v>
       </c>
       <c r="M126">
@@ -11005,7 +11006,7 @@
       <c r="K127">
         <v>0</v>
       </c>
-      <c r="L127">
+      <c r="L127" s="2">
         <v>1</v>
       </c>
       <c r="M127">
@@ -11091,7 +11092,7 @@
       <c r="K128">
         <v>0</v>
       </c>
-      <c r="L128">
+      <c r="L128" s="2">
         <v>1</v>
       </c>
       <c r="M128">
@@ -11177,7 +11178,7 @@
       <c r="K129">
         <v>0</v>
       </c>
-      <c r="L129">
+      <c r="L129" s="2">
         <v>1</v>
       </c>
       <c r="M129">
@@ -11257,7 +11258,7 @@
       <c r="K130">
         <v>0</v>
       </c>
-      <c r="L130">
+      <c r="L130" s="2">
         <v>1</v>
       </c>
       <c r="M130">
@@ -11346,7 +11347,7 @@
       <c r="K131">
         <v>0</v>
       </c>
-      <c r="L131">
+      <c r="L131" s="2">
         <v>1</v>
       </c>
       <c r="M131">
@@ -11426,7 +11427,7 @@
       <c r="K132">
         <v>0</v>
       </c>
-      <c r="L132">
+      <c r="L132" s="2">
         <v>1</v>
       </c>
       <c r="M132">
@@ -11509,7 +11510,7 @@
       <c r="K133">
         <v>0</v>
       </c>
-      <c r="L133">
+      <c r="L133" s="2">
         <v>1</v>
       </c>
       <c r="M133">
@@ -11589,7 +11590,7 @@
       <c r="K134">
         <v>0</v>
       </c>
-      <c r="L134">
+      <c r="L134" s="2">
         <v>1</v>
       </c>
       <c r="M134">
@@ -11675,7 +11676,7 @@
       <c r="K135">
         <v>0</v>
       </c>
-      <c r="L135">
+      <c r="L135" s="2">
         <v>1</v>
       </c>
       <c r="M135">
@@ -11761,7 +11762,7 @@
       <c r="K136">
         <v>0</v>
       </c>
-      <c r="L136">
+      <c r="L136" s="2">
         <v>1</v>
       </c>
       <c r="M136">
@@ -11841,7 +11842,7 @@
       <c r="K137">
         <v>0</v>
       </c>
-      <c r="L137">
+      <c r="L137" s="2">
         <v>1</v>
       </c>
       <c r="M137">
@@ -11921,7 +11922,7 @@
       <c r="K138">
         <v>0</v>
       </c>
-      <c r="L138">
+      <c r="L138" s="2">
         <v>1</v>
       </c>
       <c r="M138">
@@ -12007,7 +12008,7 @@
       <c r="K139">
         <v>0</v>
       </c>
-      <c r="L139">
+      <c r="L139" s="2">
         <v>1</v>
       </c>
       <c r="M139">
@@ -12087,7 +12088,7 @@
       <c r="K140">
         <v>0</v>
       </c>
-      <c r="L140">
+      <c r="L140" s="2">
         <v>1</v>
       </c>
       <c r="M140">
@@ -12167,7 +12168,7 @@
       <c r="K141">
         <v>0</v>
       </c>
-      <c r="L141">
+      <c r="L141" s="2">
         <v>1</v>
       </c>
       <c r="M141">
@@ -12256,7 +12257,7 @@
       <c r="K142">
         <v>0</v>
       </c>
-      <c r="L142">
+      <c r="L142" s="2">
         <v>1</v>
       </c>
       <c r="M142">
@@ -12345,7 +12346,7 @@
       <c r="K143">
         <v>0</v>
       </c>
-      <c r="L143">
+      <c r="L143" s="2">
         <v>1</v>
       </c>
       <c r="M143">
@@ -12425,7 +12426,7 @@
       <c r="K144">
         <v>0</v>
       </c>
-      <c r="L144">
+      <c r="L144" s="2">
         <v>1</v>
       </c>
       <c r="M144">
@@ -12514,7 +12515,7 @@
       <c r="K145">
         <v>0</v>
       </c>
-      <c r="L145">
+      <c r="L145" s="2">
         <v>1</v>
       </c>
       <c r="M145">
@@ -12594,7 +12595,7 @@
       <c r="K146">
         <v>0</v>
       </c>
-      <c r="L146">
+      <c r="L146" s="2">
         <v>1</v>
       </c>
       <c r="M146">
@@ -12680,7 +12681,7 @@
       <c r="K147">
         <v>0</v>
       </c>
-      <c r="L147">
+      <c r="L147" s="2">
         <v>1</v>
       </c>
       <c r="M147">
@@ -12760,7 +12761,7 @@
       <c r="K148">
         <v>0</v>
       </c>
-      <c r="L148">
+      <c r="L148" s="2">
         <v>1</v>
       </c>
       <c r="M148">
@@ -12840,7 +12841,7 @@
       <c r="K149">
         <v>0</v>
       </c>
-      <c r="L149">
+      <c r="L149" s="2">
         <v>1</v>
       </c>
       <c r="M149">
@@ -12920,7 +12921,7 @@
       <c r="K150">
         <v>0</v>
       </c>
-      <c r="L150">
+      <c r="L150" s="2">
         <v>1</v>
       </c>
       <c r="M150">
@@ -13000,7 +13001,7 @@
       <c r="K151">
         <v>0</v>
       </c>
-      <c r="L151">
+      <c r="L151" s="2">
         <v>1</v>
       </c>
       <c r="M151">
@@ -13083,7 +13084,7 @@
       <c r="K152">
         <v>0</v>
       </c>
-      <c r="L152">
+      <c r="L152" s="2">
         <v>1</v>
       </c>
       <c r="M152">
@@ -13160,7 +13161,7 @@
       <c r="K153">
         <v>0</v>
       </c>
-      <c r="L153">
+      <c r="L153" s="2">
         <v>1</v>
       </c>
       <c r="M153">
@@ -13243,7 +13244,7 @@
       <c r="K154">
         <v>0</v>
       </c>
-      <c r="L154">
+      <c r="L154" s="2">
         <v>1</v>
       </c>
       <c r="M154">
@@ -13323,7 +13324,7 @@
       <c r="K155">
         <v>0</v>
       </c>
-      <c r="L155">
+      <c r="L155" s="2">
         <v>1</v>
       </c>
       <c r="M155">
@@ -13406,7 +13407,7 @@
       <c r="K156">
         <v>0</v>
       </c>
-      <c r="L156">
+      <c r="L156" s="2">
         <v>1</v>
       </c>
       <c r="M156">
@@ -13489,7 +13490,7 @@
       <c r="K157">
         <v>0</v>
       </c>
-      <c r="L157">
+      <c r="L157" s="2">
         <v>1</v>
       </c>
       <c r="M157">
@@ -13575,7 +13576,7 @@
       <c r="K158">
         <v>0</v>
       </c>
-      <c r="L158">
+      <c r="L158" s="2">
         <v>1</v>
       </c>
       <c r="M158">
@@ -13664,7 +13665,7 @@
       <c r="K159">
         <v>0</v>
       </c>
-      <c r="L159">
+      <c r="L159" s="2">
         <v>1</v>
       </c>
       <c r="M159">
@@ -13744,7 +13745,7 @@
       <c r="K160">
         <v>0</v>
       </c>
-      <c r="L160">
+      <c r="L160" s="2">
         <v>1</v>
       </c>
       <c r="M160">
@@ -13833,7 +13834,7 @@
       <c r="K161">
         <v>0</v>
       </c>
-      <c r="L161">
+      <c r="L161" s="2">
         <v>1</v>
       </c>
       <c r="M161">
@@ -13925,7 +13926,7 @@
       <c r="K162">
         <v>0</v>
       </c>
-      <c r="L162">
+      <c r="L162" s="2">
         <v>1</v>
       </c>
       <c r="M162">
@@ -14011,7 +14012,7 @@
       <c r="K163">
         <v>0</v>
       </c>
-      <c r="L163">
+      <c r="L163" s="2">
         <v>1</v>
       </c>
       <c r="M163">
@@ -14094,7 +14095,7 @@
       <c r="K164">
         <v>0</v>
       </c>
-      <c r="L164">
+      <c r="L164" s="2">
         <v>1</v>
       </c>
       <c r="M164">
@@ -14180,7 +14181,7 @@
       <c r="K165">
         <v>0</v>
       </c>
-      <c r="L165">
+      <c r="L165" s="2">
         <v>1</v>
       </c>
       <c r="M165">
@@ -14263,7 +14264,7 @@
       <c r="K166">
         <v>0</v>
       </c>
-      <c r="L166">
+      <c r="L166" s="2">
         <v>1</v>
       </c>
       <c r="M166">
@@ -14349,7 +14350,7 @@
       <c r="K167">
         <v>0</v>
       </c>
-      <c r="L167">
+      <c r="L167" s="2">
         <v>1</v>
       </c>
       <c r="M167" t="s">
@@ -14438,7 +14439,7 @@
       <c r="K168">
         <v>0</v>
       </c>
-      <c r="L168">
+      <c r="L168" s="2">
         <v>1</v>
       </c>
       <c r="M168">
@@ -14524,7 +14525,7 @@
       <c r="K169">
         <v>0</v>
       </c>
-      <c r="L169">
+      <c r="L169" s="2">
         <v>1</v>
       </c>
       <c r="M169">
@@ -14613,7 +14614,7 @@
       <c r="K170">
         <v>0</v>
       </c>
-      <c r="L170">
+      <c r="L170" s="2">
         <v>1</v>
       </c>
       <c r="M170">
@@ -14693,7 +14694,7 @@
       <c r="K171">
         <v>0</v>
       </c>
-      <c r="L171">
+      <c r="L171" s="2">
         <v>1</v>
       </c>
       <c r="M171">
@@ -14773,7 +14774,7 @@
       <c r="K172">
         <v>0</v>
       </c>
-      <c r="L172">
+      <c r="L172" s="2">
         <v>1</v>
       </c>
       <c r="M172">
@@ -14856,7 +14857,7 @@
       <c r="K173">
         <v>0</v>
       </c>
-      <c r="L173">
+      <c r="L173" s="2">
         <v>1</v>
       </c>
       <c r="M173">
@@ -14936,7 +14937,7 @@
       <c r="K174">
         <v>0</v>
       </c>
-      <c r="L174">
+      <c r="L174" s="2">
         <v>1</v>
       </c>
       <c r="M174">
@@ -15022,7 +15023,7 @@
       <c r="K175">
         <v>0</v>
       </c>
-      <c r="L175">
+      <c r="L175" s="2">
         <v>1</v>
       </c>
       <c r="M175">
@@ -15108,7 +15109,7 @@
       <c r="K176">
         <v>0</v>
       </c>
-      <c r="L176">
+      <c r="L176" s="2">
         <v>1</v>
       </c>
       <c r="M176">
@@ -15191,7 +15192,7 @@
       <c r="K177">
         <v>0</v>
       </c>
-      <c r="L177">
+      <c r="L177" s="2">
         <v>1</v>
       </c>
       <c r="M177">
@@ -15277,7 +15278,7 @@
       <c r="K178">
         <v>0</v>
       </c>
-      <c r="L178">
+      <c r="L178" s="2">
         <v>1</v>
       </c>
       <c r="M178">
@@ -15366,7 +15367,7 @@
       <c r="K179">
         <v>0</v>
       </c>
-      <c r="L179">
+      <c r="L179" s="2">
         <v>1</v>
       </c>
       <c r="M179">
@@ -15452,7 +15453,7 @@
       <c r="K180">
         <v>0</v>
       </c>
-      <c r="L180">
+      <c r="L180" s="2">
         <v>1</v>
       </c>
       <c r="M180">
@@ -15535,7 +15536,7 @@
       <c r="K181">
         <v>0</v>
       </c>
-      <c r="L181">
+      <c r="L181" s="2">
         <v>1</v>
       </c>
       <c r="M181">
@@ -15615,7 +15616,7 @@
       <c r="K182">
         <v>0</v>
       </c>
-      <c r="L182">
+      <c r="L182" s="2">
         <v>1</v>
       </c>
       <c r="M182">
@@ -15695,7 +15696,7 @@
       <c r="K183">
         <v>0</v>
       </c>
-      <c r="L183">
+      <c r="L183" s="2">
         <v>1</v>
       </c>
       <c r="M183">
@@ -15781,7 +15782,7 @@
       <c r="K184">
         <v>0</v>
       </c>
-      <c r="L184">
+      <c r="L184" s="2">
         <v>1</v>
       </c>
       <c r="M184">
@@ -15864,7 +15865,7 @@
       <c r="K185">
         <v>0</v>
       </c>
-      <c r="L185">
+      <c r="L185" s="2">
         <v>1</v>
       </c>
       <c r="M185" t="s">
@@ -15944,7 +15945,7 @@
       <c r="K186">
         <v>0</v>
       </c>
-      <c r="L186">
+      <c r="L186" s="2">
         <v>1</v>
       </c>
       <c r="M186">
@@ -16030,7 +16031,7 @@
       <c r="K187">
         <v>0</v>
       </c>
-      <c r="L187">
+      <c r="L187" s="2">
         <v>1</v>
       </c>
       <c r="M187">
@@ -16119,7 +16120,7 @@
       <c r="K188">
         <v>0</v>
       </c>
-      <c r="L188">
+      <c r="L188" s="2">
         <v>1</v>
       </c>
       <c r="M188">
@@ -16199,7 +16200,7 @@
       <c r="K189">
         <v>0</v>
       </c>
-      <c r="L189">
+      <c r="L189" s="2">
         <v>1</v>
       </c>
       <c r="M189">
@@ -16279,7 +16280,7 @@
       <c r="K190">
         <v>1</v>
       </c>
-      <c r="L190">
+      <c r="L190" s="2">
         <v>1</v>
       </c>
       <c r="M190">
@@ -16362,7 +16363,7 @@
       <c r="K191">
         <v>0</v>
       </c>
-      <c r="L191">
+      <c r="L191" s="2">
         <v>1</v>
       </c>
       <c r="M191" t="s">
@@ -16442,7 +16443,7 @@
       <c r="K192">
         <v>0</v>
       </c>
-      <c r="L192">
+      <c r="L192" s="2">
         <v>1</v>
       </c>
       <c r="M192">
@@ -16525,7 +16526,7 @@
       <c r="K193">
         <v>0</v>
       </c>
-      <c r="L193">
+      <c r="L193" s="2">
         <v>1</v>
       </c>
       <c r="M193">
@@ -16608,7 +16609,7 @@
       <c r="K194">
         <v>0</v>
       </c>
-      <c r="L194">
+      <c r="L194" s="2">
         <v>1</v>
       </c>
       <c r="M194">
@@ -16688,7 +16689,7 @@
       <c r="K195">
         <v>0</v>
       </c>
-      <c r="L195">
+      <c r="L195" s="2">
         <v>1</v>
       </c>
       <c r="M195">
@@ -16777,7 +16778,7 @@
       <c r="K196">
         <v>0</v>
       </c>
-      <c r="L196">
+      <c r="L196" s="2">
         <v>1</v>
       </c>
       <c r="M196" t="s">
@@ -16860,7 +16861,7 @@
       <c r="K197">
         <v>0</v>
       </c>
-      <c r="L197">
+      <c r="L197" s="2">
         <v>1</v>
       </c>
       <c r="M197">
@@ -16940,7 +16941,7 @@
       <c r="K198">
         <v>0</v>
       </c>
-      <c r="L198">
+      <c r="L198" s="2">
         <v>1</v>
       </c>
       <c r="M198">
@@ -17026,7 +17027,7 @@
       <c r="K199">
         <v>0</v>
       </c>
-      <c r="L199">
+      <c r="L199" s="2">
         <v>1</v>
       </c>
       <c r="M199">
@@ -17109,7 +17110,7 @@
       <c r="K200">
         <v>0</v>
       </c>
-      <c r="L200">
+      <c r="L200" s="2">
         <v>1</v>
       </c>
       <c r="M200">
@@ -17189,8 +17190,8 @@
       <c r="K201">
         <v>0</v>
       </c>
-      <c r="L201">
-        <v>0.75</v>
+      <c r="L201" s="2">
+        <v>0.33333333333333331</v>
       </c>
       <c r="M201">
         <v>1</v>
@@ -17269,7 +17270,7 @@
       <c r="K202">
         <v>1</v>
       </c>
-      <c r="L202">
+      <c r="L202" s="2">
         <v>1</v>
       </c>
       <c r="M202">
@@ -17352,7 +17353,7 @@
       <c r="K203">
         <v>0</v>
       </c>
-      <c r="L203">
+      <c r="L203" s="2">
         <v>1</v>
       </c>
       <c r="M203">
@@ -17433,12 +17434,12 @@
         <v>1</v>
       </c>
       <c r="J204">
-        <v>1000</v>
+        <v>1072</v>
       </c>
       <c r="K204">
-        <v>1</v>
-      </c>
-      <c r="L204">
+        <v>0</v>
+      </c>
+      <c r="L204" s="2">
         <v>1</v>
       </c>
       <c r="M204" t="s">
@@ -17513,12 +17514,12 @@
         <v>0</v>
       </c>
       <c r="J205">
-        <v>1700</v>
+        <v>1725</v>
       </c>
       <c r="K205">
-        <v>1</v>
-      </c>
-      <c r="L205">
+        <v>0</v>
+      </c>
+      <c r="L205" s="2">
         <v>1</v>
       </c>
       <c r="M205">
@@ -17596,12 +17597,12 @@
         <v>1</v>
       </c>
       <c r="J206">
-        <v>1200</v>
+        <v>1063</v>
       </c>
       <c r="K206">
-        <v>1</v>
-      </c>
-      <c r="L206">
+        <v>0</v>
+      </c>
+      <c r="L206" s="2">
         <v>1</v>
       </c>
       <c r="M206">
@@ -17647,6 +17648,95 @@
         <v>30</v>
       </c>
       <c r="AH206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>104</v>
+      </c>
+      <c r="B207">
+        <v>2022</v>
+      </c>
+      <c r="C207">
+        <v>25</v>
+      </c>
+      <c r="D207">
+        <v>2</v>
+      </c>
+      <c r="E207">
+        <v>15</v>
+      </c>
+      <c r="F207" t="s">
+        <v>36</v>
+      </c>
+      <c r="G207" t="s">
+        <v>7</v>
+      </c>
+      <c r="H207" t="s">
+        <v>27</v>
+      </c>
+      <c r="I207">
+        <v>0</v>
+      </c>
+      <c r="J207">
+        <v>964</v>
+      </c>
+      <c r="K207">
+        <v>0</v>
+      </c>
+      <c r="L207" s="2">
+        <v>1</v>
+      </c>
+      <c r="M207">
+        <v>1</v>
+      </c>
+      <c r="N207">
+        <v>0.5</v>
+      </c>
+      <c r="O207">
+        <v>10.5</v>
+      </c>
+      <c r="P207">
+        <v>4.5</v>
+      </c>
+      <c r="R207">
+        <v>5.5</v>
+      </c>
+      <c r="S207">
+        <v>1.5</v>
+      </c>
+      <c r="T207">
+        <v>24</v>
+      </c>
+      <c r="U207">
+        <v>14</v>
+      </c>
+      <c r="X207">
+        <v>1.5</v>
+      </c>
+      <c r="Y207">
+        <v>2</v>
+      </c>
+      <c r="Z207">
+        <v>15</v>
+      </c>
+      <c r="AA207">
+        <v>13.5</v>
+      </c>
+      <c r="AB207">
+        <v>1</v>
+      </c>
+      <c r="AD207" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF207">
+        <v>4.5</v>
+      </c>
+      <c r="AG207">
+        <v>1</v>
+      </c>
+      <c r="AH207">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update w/ odoxa poll (2/17)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D233AD-8E10-CB4C-BC2B-158D7EA7C593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9438387-FCA6-6C41-8F86-768002CA4FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23940" yWindow="8840" windowWidth="25920" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="2140" yWindow="1840" windowWidth="25920" windowHeight="18840" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="49">
   <si>
     <t>year</t>
   </si>
@@ -548,11 +548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH207"/>
+  <dimension ref="A1:AH208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AH208" sqref="AH208"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AH209" sqref="AH209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17737,6 +17737,86 @@
         <v>1</v>
       </c>
       <c r="AH207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>105</v>
+      </c>
+      <c r="B208">
+        <v>2022</v>
+      </c>
+      <c r="C208">
+        <v>25</v>
+      </c>
+      <c r="D208">
+        <v>2</v>
+      </c>
+      <c r="E208">
+        <v>16</v>
+      </c>
+      <c r="F208" t="s">
+        <v>34</v>
+      </c>
+      <c r="G208" t="s">
+        <v>7</v>
+      </c>
+      <c r="H208" t="s">
+        <v>27</v>
+      </c>
+      <c r="I208">
+        <v>0</v>
+      </c>
+      <c r="J208">
+        <v>1357</v>
+      </c>
+      <c r="K208">
+        <v>0</v>
+      </c>
+      <c r="L208" s="2">
+        <v>1</v>
+      </c>
+      <c r="M208">
+        <v>1.5</v>
+      </c>
+      <c r="N208">
+        <v>0.5</v>
+      </c>
+      <c r="O208">
+        <v>11</v>
+      </c>
+      <c r="P208">
+        <v>4.5</v>
+      </c>
+      <c r="R208">
+        <v>5</v>
+      </c>
+      <c r="S208">
+        <v>2</v>
+      </c>
+      <c r="T208">
+        <v>24.5</v>
+      </c>
+      <c r="U208">
+        <v>12</v>
+      </c>
+      <c r="X208">
+        <v>2</v>
+      </c>
+      <c r="Y208">
+        <v>2</v>
+      </c>
+      <c r="Z208">
+        <v>18</v>
+      </c>
+      <c r="AA208">
+        <v>14</v>
+      </c>
+      <c r="AF208">
+        <v>3</v>
+      </c>
+      <c r="AH208">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update w/ 2/22 rollings
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63DB122-4F5F-984E-A504-F3AC81B7D44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5136ED7-53A6-6242-B633-6DA2E37E710F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="500" windowWidth="25780" windowHeight="19000" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="24360" yWindow="7140" windowWidth="25960" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="50">
   <si>
     <t>year</t>
   </si>
@@ -553,9 +553,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
   <dimension ref="A1:AH433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="M219" sqref="M219"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A221" sqref="A221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16847,10 +16847,10 @@
         <v>47</v>
       </c>
       <c r="J197">
-        <v>1020</v>
+        <v>1096</v>
       </c>
       <c r="K197">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L197" s="2">
         <v>1</v>
@@ -18590,10 +18590,10 @@
         <v>47</v>
       </c>
       <c r="J218">
-        <v>845</v>
+        <v>670</v>
       </c>
       <c r="K218">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L218" s="2">
         <v>1</v>
@@ -18655,58 +18655,58 @@
         <v>2</v>
       </c>
       <c r="D219">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E219">
         <v>2</v>
       </c>
       <c r="F219">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G219" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H219" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I219" t="s">
         <v>38</v>
       </c>
       <c r="J219">
-        <v>1073</v>
+        <v>1018</v>
       </c>
       <c r="K219">
         <v>0</v>
       </c>
       <c r="L219" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M219" s="2">
-        <v>1</v>
-      </c>
-      <c r="N219" t="s">
-        <v>31</v>
-      </c>
-      <c r="O219">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="N219">
+        <v>0.5</v>
+      </c>
+      <c r="O219" t="s">
+        <v>24</v>
       </c>
       <c r="P219">
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="Q219">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S219">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="T219">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U219">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V219">
-        <v>24</v>
+        <v>24.5</v>
       </c>
       <c r="W219">
         <v>15</v>
@@ -18715,13 +18715,16 @@
         <v>1</v>
       </c>
       <c r="AA219">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB219">
-        <v>15</v>
+        <v>16.5</v>
       </c>
       <c r="AC219">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="AH219" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="220" spans="1:34" x14ac:dyDescent="0.2">
@@ -18735,61 +18738,61 @@
         <v>2</v>
       </c>
       <c r="D220">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E220">
         <v>2</v>
       </c>
       <c r="F220">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G220" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H220" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I220" t="s">
         <v>38</v>
       </c>
       <c r="J220">
-        <v>1025</v>
+        <v>1071</v>
       </c>
       <c r="K220">
         <v>0</v>
       </c>
       <c r="L220" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M220" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N220" t="s">
-        <v>24</v>
-      </c>
-      <c r="O220" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="N220">
+        <v>1</v>
+      </c>
+      <c r="O220">
+        <v>1</v>
       </c>
       <c r="P220">
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="Q220">
         <v>4</v>
       </c>
       <c r="S220">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="T220">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U220">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="V220">
         <v>25</v>
       </c>
       <c r="W220">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z220">
         <v>1</v>
@@ -18798,19 +18801,174 @@
         <v>2</v>
       </c>
       <c r="AB220">
+        <v>17</v>
+      </c>
+      <c r="AC220">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="221" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>118</v>
+      </c>
+      <c r="B221">
+        <v>2022</v>
+      </c>
+      <c r="C221">
+        <v>2</v>
+      </c>
+      <c r="D221">
+        <v>19</v>
+      </c>
+      <c r="E221">
+        <v>2</v>
+      </c>
+      <c r="F221">
+        <v>22</v>
+      </c>
+      <c r="G221" t="s">
+        <v>33</v>
+      </c>
+      <c r="H221" t="s">
+        <v>21</v>
+      </c>
+      <c r="I221" t="s">
+        <v>38</v>
+      </c>
+      <c r="J221">
+        <v>1049</v>
+      </c>
+      <c r="K221">
+        <v>0</v>
+      </c>
+      <c r="L221" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M221" s="2">
+        <v>1</v>
+      </c>
+      <c r="N221">
+        <v>1</v>
+      </c>
+      <c r="O221">
+        <v>1</v>
+      </c>
+      <c r="P221">
+        <v>10</v>
+      </c>
+      <c r="Q221">
+        <v>4</v>
+      </c>
+      <c r="S221">
+        <v>5</v>
+      </c>
+      <c r="T221">
+        <v>3</v>
+      </c>
+      <c r="U221">
+        <v>2</v>
+      </c>
+      <c r="V221">
+        <v>25</v>
+      </c>
+      <c r="W221">
+        <v>14</v>
+      </c>
+      <c r="Z221">
+        <v>2</v>
+      </c>
+      <c r="AA221">
+        <v>2</v>
+      </c>
+      <c r="AB221">
+        <v>17</v>
+      </c>
+      <c r="AC221">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="222" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>119</v>
+      </c>
+      <c r="B222">
+        <v>2022</v>
+      </c>
+      <c r="C222">
+        <v>2</v>
+      </c>
+      <c r="D222">
+        <v>19</v>
+      </c>
+      <c r="E222">
+        <v>2</v>
+      </c>
+      <c r="F222">
+        <v>22</v>
+      </c>
+      <c r="G222" t="s">
+        <v>29</v>
+      </c>
+      <c r="H222" t="s">
+        <v>22</v>
+      </c>
+      <c r="I222" t="s">
+        <v>38</v>
+      </c>
+      <c r="J222">
+        <v>1018</v>
+      </c>
+      <c r="K222">
+        <v>0</v>
+      </c>
+      <c r="L222" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M222" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N222">
+        <v>0.5</v>
+      </c>
+      <c r="O222" t="s">
+        <v>24</v>
+      </c>
+      <c r="P222">
+        <v>11.5</v>
+      </c>
+      <c r="Q222">
+        <v>4.5</v>
+      </c>
+      <c r="S222">
+        <v>5</v>
+      </c>
+      <c r="T222">
+        <v>2</v>
+      </c>
+      <c r="U222">
+        <v>2</v>
+      </c>
+      <c r="V222">
+        <v>25</v>
+      </c>
+      <c r="W222">
+        <v>14.5</v>
+      </c>
+      <c r="Z222">
+        <v>1</v>
+      </c>
+      <c r="AA222">
+        <v>2</v>
+      </c>
+      <c r="AB222">
         <v>16</v>
       </c>
-      <c r="AC220">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="221" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L221" s="2"/>
-      <c r="M221" s="2"/>
-    </row>
-    <row r="222" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L222" s="2"/>
-      <c r="M222" s="2"/>
+      <c r="AC222">
+        <v>16</v>
+      </c>
+      <c r="AH222" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="223" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L223" s="2"/>

</xml_diff>

<commit_message>
update w/ 2/23 rollings + harris and elabe polls (2/23)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5136ED7-53A6-6242-B633-6DA2E37E710F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA8F6CF-B951-EC4A-B004-4BBEA82FDB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24360" yWindow="7140" windowWidth="25960" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="21520" yWindow="7800" windowWidth="25960" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="50">
   <si>
     <t>year</t>
   </si>
@@ -551,11 +551,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH433"/>
+  <dimension ref="A1:AH432"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A221" sqref="A221"/>
+      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AH224" sqref="AH224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17268,7 +17268,7 @@
         <v>1</v>
       </c>
       <c r="M202" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N202" t="s">
         <v>24</v>
@@ -18095,7 +18095,7 @@
         <v>1</v>
       </c>
       <c r="M212" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N212">
         <v>0.5</v>
@@ -18818,43 +18818,43 @@
         <v>2</v>
       </c>
       <c r="D221">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E221">
         <v>2</v>
       </c>
       <c r="F221">
+        <v>21</v>
+      </c>
+      <c r="G221" t="s">
+        <v>20</v>
+      </c>
+      <c r="H221" t="s">
         <v>22</v>
       </c>
-      <c r="G221" t="s">
-        <v>33</v>
-      </c>
-      <c r="H221" t="s">
-        <v>21</v>
-      </c>
       <c r="I221" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J221">
-        <v>1049</v>
+        <v>1715</v>
       </c>
       <c r="K221">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L221" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M221" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N221">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O221">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P221">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q221">
         <v>4</v>
@@ -18863,28 +18863,31 @@
         <v>5</v>
       </c>
       <c r="T221">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U221">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V221">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="W221">
-        <v>14</v>
+        <v>13.5</v>
       </c>
       <c r="Z221">
         <v>2</v>
       </c>
       <c r="AA221">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB221">
         <v>17</v>
       </c>
       <c r="AC221">
-        <v>14</v>
+        <v>15.5</v>
+      </c>
+      <c r="AD221">
+        <v>0.5</v>
       </c>
     </row>
     <row r="222" spans="1:34" x14ac:dyDescent="0.2">
@@ -18898,7 +18901,7 @@
         <v>2</v>
       </c>
       <c r="D222">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E222">
         <v>2</v>
@@ -18907,76 +18910,234 @@
         <v>22</v>
       </c>
       <c r="G222" t="s">
+        <v>30</v>
+      </c>
+      <c r="H222" t="s">
+        <v>21</v>
+      </c>
+      <c r="I222" t="s">
+        <v>47</v>
+      </c>
+      <c r="J222">
+        <v>990</v>
+      </c>
+      <c r="K222">
+        <v>0</v>
+      </c>
+      <c r="L222" s="2">
+        <v>1</v>
+      </c>
+      <c r="M222" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N222">
+        <v>1</v>
+      </c>
+      <c r="O222">
+        <v>1</v>
+      </c>
+      <c r="P222">
+        <v>11</v>
+      </c>
+      <c r="Q222">
+        <v>4</v>
+      </c>
+      <c r="S222">
+        <v>5.5</v>
+      </c>
+      <c r="T222">
+        <v>2.5</v>
+      </c>
+      <c r="U222">
+        <v>2.5</v>
+      </c>
+      <c r="V222">
+        <v>24.5</v>
+      </c>
+      <c r="W222">
+        <v>11.5</v>
+      </c>
+      <c r="Z222">
+        <v>1.5</v>
+      </c>
+      <c r="AA222">
+        <v>2.5</v>
+      </c>
+      <c r="AB222">
+        <v>18</v>
+      </c>
+      <c r="AC222">
+        <v>13.5</v>
+      </c>
+      <c r="AD222">
+        <v>0.5</v>
+      </c>
+      <c r="AH222">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>120</v>
+      </c>
+      <c r="B223">
+        <v>2022</v>
+      </c>
+      <c r="C223">
+        <v>2</v>
+      </c>
+      <c r="D223">
+        <v>19</v>
+      </c>
+      <c r="E223">
+        <v>2</v>
+      </c>
+      <c r="F223">
+        <v>23</v>
+      </c>
+      <c r="G223" t="s">
         <v>29</v>
       </c>
-      <c r="H222" t="s">
+      <c r="H223" t="s">
         <v>22</v>
       </c>
-      <c r="I222" t="s">
+      <c r="I223" t="s">
         <v>38</v>
       </c>
-      <c r="J222">
+      <c r="J223">
         <v>1018</v>
       </c>
-      <c r="K222">
-        <v>0</v>
-      </c>
-      <c r="L222" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="M222" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N222">
-        <v>0.5</v>
-      </c>
-      <c r="O222" t="s">
-        <v>24</v>
-      </c>
-      <c r="P222">
+      <c r="K223">
+        <v>1</v>
+      </c>
+      <c r="L223" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M223" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N223">
+        <v>0.5</v>
+      </c>
+      <c r="O223">
+        <v>0.5</v>
+      </c>
+      <c r="P223">
         <v>11.5</v>
       </c>
-      <c r="Q222">
+      <c r="Q223">
         <v>4.5</v>
       </c>
-      <c r="S222">
+      <c r="S223">
+        <v>5.5</v>
+      </c>
+      <c r="T223">
+        <v>2</v>
+      </c>
+      <c r="U223">
+        <v>2</v>
+      </c>
+      <c r="V223">
+        <v>25</v>
+      </c>
+      <c r="W223">
+        <v>14.5</v>
+      </c>
+      <c r="Z223">
+        <v>0.5</v>
+      </c>
+      <c r="AA223">
+        <v>2</v>
+      </c>
+      <c r="AB223">
+        <v>15.5</v>
+      </c>
+      <c r="AC223">
+        <v>16</v>
+      </c>
+      <c r="AH223" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="224" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>121</v>
+      </c>
+      <c r="B224">
+        <v>2022</v>
+      </c>
+      <c r="C224">
+        <v>2</v>
+      </c>
+      <c r="D224">
+        <v>21</v>
+      </c>
+      <c r="E224">
+        <v>2</v>
+      </c>
+      <c r="F224">
+        <v>23</v>
+      </c>
+      <c r="G224" t="s">
+        <v>33</v>
+      </c>
+      <c r="H224" t="s">
+        <v>21</v>
+      </c>
+      <c r="I224" t="s">
+        <v>38</v>
+      </c>
+      <c r="J224">
+        <v>1049</v>
+      </c>
+      <c r="K224">
+        <v>1</v>
+      </c>
+      <c r="L224" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M224" s="2">
+        <v>1</v>
+      </c>
+      <c r="N224">
+        <v>1</v>
+      </c>
+      <c r="O224">
+        <v>1</v>
+      </c>
+      <c r="P224">
+        <v>11</v>
+      </c>
+      <c r="Q224">
         <v>5</v>
       </c>
-      <c r="T222">
-        <v>2</v>
-      </c>
-      <c r="U222">
-        <v>2</v>
-      </c>
-      <c r="V222">
+      <c r="S224">
+        <v>5</v>
+      </c>
+      <c r="T224">
+        <v>2</v>
+      </c>
+      <c r="U224">
+        <v>2</v>
+      </c>
+      <c r="V224">
         <v>25</v>
       </c>
-      <c r="W222">
-        <v>14.5</v>
-      </c>
-      <c r="Z222">
-        <v>1</v>
-      </c>
-      <c r="AA222">
-        <v>2</v>
-      </c>
-      <c r="AB222">
+      <c r="W224">
+        <v>14</v>
+      </c>
+      <c r="Z224">
+        <v>2</v>
+      </c>
+      <c r="AA224">
+        <v>2</v>
+      </c>
+      <c r="AB224">
         <v>16</v>
       </c>
-      <c r="AC222">
-        <v>16</v>
-      </c>
-      <c r="AH222" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="223" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L223" s="2"/>
-      <c r="M223" s="2"/>
-    </row>
-    <row r="224" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L224" s="2"/>
-      <c r="M224" s="2"/>
+      <c r="AC224">
+        <v>14</v>
+      </c>
     </row>
     <row r="225" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L225" s="2"/>
@@ -19809,10 +19970,6 @@
     <row r="432" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L432" s="2"/>
       <c r="M432" s="2"/>
-    </row>
-    <row r="433" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L433" s="2"/>
-      <c r="M433" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ 2/24 rollings + cluster17 and kantar polls (2/24)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA8F6CF-B951-EC4A-B004-4BBEA82FDB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC70ED7-B327-5F49-A8FF-91A59F6F7AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21520" yWindow="7800" windowWidth="25960" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="28960" yWindow="5820" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>rounding</t>
+  </si>
+  <si>
+    <t>kantar</t>
   </si>
 </sst>
 </file>
@@ -551,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH432"/>
+  <dimension ref="A1:AH434"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AH224" sqref="AH224"/>
+      <selection pane="bottomLeft" activeCell="AG223" sqref="AG223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18987,7 +18990,7 @@
         <v>2</v>
       </c>
       <c r="D223">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E223">
         <v>2</v>
@@ -18996,22 +18999,22 @@
         <v>23</v>
       </c>
       <c r="G223" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H223" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I223" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J223">
-        <v>1018</v>
+        <v>2521</v>
       </c>
       <c r="K223">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L223" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M223" s="2">
         <v>0.5</v>
@@ -19023,14 +19026,14 @@
         <v>0.5</v>
       </c>
       <c r="P223">
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
       <c r="Q223">
+        <v>4</v>
+      </c>
+      <c r="S223">
         <v>4.5</v>
       </c>
-      <c r="S223">
-        <v>5.5</v>
-      </c>
       <c r="T223">
         <v>2</v>
       </c>
@@ -19038,25 +19041,25 @@
         <v>2</v>
       </c>
       <c r="V223">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="W223">
-        <v>14.5</v>
+        <v>13</v>
       </c>
       <c r="Z223">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AA223">
         <v>2</v>
       </c>
       <c r="AB223">
-        <v>15.5</v>
+        <v>16</v>
       </c>
       <c r="AC223">
         <v>16</v>
       </c>
-      <c r="AH223" t="s">
-        <v>24</v>
+      <c r="AD223">
+        <v>1</v>
       </c>
     </row>
     <row r="224" spans="1:34" x14ac:dyDescent="0.2">
@@ -19079,127 +19082,285 @@
         <v>23</v>
       </c>
       <c r="G224" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H224" t="s">
         <v>21</v>
       </c>
       <c r="I224" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J224">
-        <v>1049</v>
+        <v>1020</v>
       </c>
       <c r="K224">
         <v>1</v>
       </c>
       <c r="L224" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M224" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N224">
         <v>1</v>
       </c>
       <c r="O224">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P224">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q224">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S224">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T224">
         <v>2</v>
       </c>
       <c r="U224">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V224">
         <v>25</v>
       </c>
       <c r="W224">
+        <v>12</v>
+      </c>
+      <c r="Z224">
+        <v>1</v>
+      </c>
+      <c r="AA224">
+        <v>2.5</v>
+      </c>
+      <c r="AB224">
+        <v>16.5</v>
+      </c>
+      <c r="AC224">
+        <v>16.5</v>
+      </c>
+      <c r="AD224">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>122</v>
+      </c>
+      <c r="B225">
+        <v>2022</v>
+      </c>
+      <c r="C225">
+        <v>2</v>
+      </c>
+      <c r="D225">
+        <v>21</v>
+      </c>
+      <c r="E225">
+        <v>2</v>
+      </c>
+      <c r="F225">
+        <v>24</v>
+      </c>
+      <c r="G225" t="s">
+        <v>29</v>
+      </c>
+      <c r="H225" t="s">
+        <v>22</v>
+      </c>
+      <c r="I225" t="s">
+        <v>38</v>
+      </c>
+      <c r="J225">
+        <v>1018</v>
+      </c>
+      <c r="K225">
+        <v>1</v>
+      </c>
+      <c r="L225" s="2">
+        <v>1</v>
+      </c>
+      <c r="M225" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N225">
+        <v>0.5</v>
+      </c>
+      <c r="O225" t="s">
+        <v>24</v>
+      </c>
+      <c r="P225">
+        <v>11</v>
+      </c>
+      <c r="Q225">
+        <v>4.5</v>
+      </c>
+      <c r="S225">
+        <v>5</v>
+      </c>
+      <c r="T225">
+        <v>2.5</v>
+      </c>
+      <c r="U225">
+        <v>2.5</v>
+      </c>
+      <c r="V225">
+        <v>25</v>
+      </c>
+      <c r="W225">
         <v>14</v>
       </c>
-      <c r="Z224">
-        <v>2</v>
-      </c>
-      <c r="AA224">
-        <v>2</v>
-      </c>
-      <c r="AB224">
+      <c r="Z225">
+        <v>1</v>
+      </c>
+      <c r="AA225">
+        <v>2</v>
+      </c>
+      <c r="AB225">
         <v>16</v>
       </c>
-      <c r="AC224">
+      <c r="AC225">
+        <v>16</v>
+      </c>
+      <c r="AH225" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="226" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>123</v>
+      </c>
+      <c r="B226">
+        <v>2022</v>
+      </c>
+      <c r="C226">
+        <v>2</v>
+      </c>
+      <c r="D226">
+        <v>21</v>
+      </c>
+      <c r="E226">
+        <v>2</v>
+      </c>
+      <c r="F226">
+        <v>24</v>
+      </c>
+      <c r="G226" t="s">
+        <v>33</v>
+      </c>
+      <c r="H226" t="s">
+        <v>21</v>
+      </c>
+      <c r="I226" t="s">
+        <v>38</v>
+      </c>
+      <c r="J226">
+        <v>1049</v>
+      </c>
+      <c r="K226">
+        <v>1</v>
+      </c>
+      <c r="L226" s="2">
+        <v>1</v>
+      </c>
+      <c r="M226" s="2">
+        <v>1</v>
+      </c>
+      <c r="N226">
+        <v>1</v>
+      </c>
+      <c r="O226">
+        <v>1</v>
+      </c>
+      <c r="P226">
+        <v>11</v>
+      </c>
+      <c r="Q226">
+        <v>5</v>
+      </c>
+      <c r="S226">
+        <v>5</v>
+      </c>
+      <c r="T226">
+        <v>2</v>
+      </c>
+      <c r="U226">
+        <v>3</v>
+      </c>
+      <c r="V226">
+        <v>24</v>
+      </c>
+      <c r="W226">
         <v>14</v>
       </c>
-    </row>
-    <row r="225" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L225" s="2"/>
-      <c r="M225" s="2"/>
-    </row>
-    <row r="226" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L226" s="2"/>
-      <c r="M226" s="2"/>
-    </row>
-    <row r="227" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="Z226">
+        <v>2</v>
+      </c>
+      <c r="AA226">
+        <v>2</v>
+      </c>
+      <c r="AB226">
+        <v>16</v>
+      </c>
+      <c r="AC226">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="227" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L227" s="2"/>
       <c r="M227" s="2"/>
     </row>
-    <row r="228" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L228" s="2"/>
       <c r="M228" s="2"/>
     </row>
-    <row r="229" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L229" s="2"/>
       <c r="M229" s="2"/>
     </row>
-    <row r="230" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L230" s="2"/>
       <c r="M230" s="2"/>
     </row>
-    <row r="231" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L231" s="2"/>
       <c r="M231" s="2"/>
     </row>
-    <row r="232" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L232" s="2"/>
       <c r="M232" s="2"/>
     </row>
-    <row r="233" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L233" s="2"/>
       <c r="M233" s="2"/>
     </row>
-    <row r="234" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L234" s="2"/>
       <c r="M234" s="2"/>
     </row>
-    <row r="235" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L235" s="2"/>
       <c r="M235" s="2"/>
     </row>
-    <row r="236" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L236" s="2"/>
       <c r="M236" s="2"/>
     </row>
-    <row r="237" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L237" s="2"/>
       <c r="M237" s="2"/>
     </row>
-    <row r="238" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L238" s="2"/>
       <c r="M238" s="2"/>
     </row>
-    <row r="239" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L239" s="2"/>
       <c r="M239" s="2"/>
     </row>
-    <row r="240" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L240" s="2"/>
       <c r="M240" s="2"/>
     </row>
@@ -19970,6 +20131,14 @@
     <row r="432" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L432" s="2"/>
       <c r="M432" s="2"/>
+    </row>
+    <row r="433" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L433" s="2"/>
+      <c r="M433" s="2"/>
+    </row>
+    <row r="434" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L434" s="2"/>
+      <c r="M434" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ 2/25 rollings
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC70ED7-B327-5F49-A8FF-91A59F6F7AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2705D6B9-CC00-FE49-AA17-709CEFDB85CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28960" yWindow="5820" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="25780" yWindow="10740" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -556,9 +556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
   <dimension ref="A1:AH434"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AG223" sqref="AG223"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="O228" sqref="O228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18839,10 +18839,10 @@
         <v>47</v>
       </c>
       <c r="J221">
-        <v>1715</v>
+        <v>1756</v>
       </c>
       <c r="K221">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L221" s="2">
         <v>1</v>
@@ -19094,7 +19094,7 @@
         <v>1020</v>
       </c>
       <c r="K224">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L224" s="2">
         <v>1</v>
@@ -19174,10 +19174,10 @@
         <v>38</v>
       </c>
       <c r="J225">
-        <v>1018</v>
+        <v>1030</v>
       </c>
       <c r="K225">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L225" s="2">
         <v>1</v>
@@ -19309,12 +19309,167 @@
       </c>
     </row>
     <row r="227" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L227" s="2"/>
-      <c r="M227" s="2"/>
+      <c r="A227">
+        <v>124</v>
+      </c>
+      <c r="B227">
+        <v>2022</v>
+      </c>
+      <c r="C227">
+        <v>2</v>
+      </c>
+      <c r="D227">
+        <v>22</v>
+      </c>
+      <c r="E227">
+        <v>2</v>
+      </c>
+      <c r="F227">
+        <v>25</v>
+      </c>
+      <c r="G227" t="s">
+        <v>33</v>
+      </c>
+      <c r="H227" t="s">
+        <v>21</v>
+      </c>
+      <c r="I227" t="s">
+        <v>38</v>
+      </c>
+      <c r="J227">
+        <v>1049</v>
+      </c>
+      <c r="K227">
+        <v>1</v>
+      </c>
+      <c r="L227" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M227" s="2">
+        <v>1</v>
+      </c>
+      <c r="N227">
+        <v>1</v>
+      </c>
+      <c r="O227">
+        <v>1</v>
+      </c>
+      <c r="P227">
+        <v>12</v>
+      </c>
+      <c r="Q227">
+        <v>4</v>
+      </c>
+      <c r="S227">
+        <v>5</v>
+      </c>
+      <c r="T227">
+        <v>2</v>
+      </c>
+      <c r="U227">
+        <v>3</v>
+      </c>
+      <c r="V227">
+        <v>24</v>
+      </c>
+      <c r="W227">
+        <v>14</v>
+      </c>
+      <c r="Z227">
+        <v>1</v>
+      </c>
+      <c r="AA227">
+        <v>2</v>
+      </c>
+      <c r="AB227">
+        <v>17</v>
+      </c>
+      <c r="AC227">
+        <v>14</v>
+      </c>
     </row>
     <row r="228" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L228" s="2"/>
-      <c r="M228" s="2"/>
+      <c r="A228">
+        <v>125</v>
+      </c>
+      <c r="B228">
+        <v>2022</v>
+      </c>
+      <c r="C228">
+        <v>2</v>
+      </c>
+      <c r="D228">
+        <v>22</v>
+      </c>
+      <c r="E228">
+        <v>2</v>
+      </c>
+      <c r="F228">
+        <v>25</v>
+      </c>
+      <c r="G228" t="s">
+        <v>29</v>
+      </c>
+      <c r="H228" t="s">
+        <v>22</v>
+      </c>
+      <c r="I228" t="s">
+        <v>38</v>
+      </c>
+      <c r="J228">
+        <v>1030</v>
+      </c>
+      <c r="K228">
+        <v>1</v>
+      </c>
+      <c r="L228" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M228" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N228">
+        <v>0.5</v>
+      </c>
+      <c r="O228" t="s">
+        <v>24</v>
+      </c>
+      <c r="P228">
+        <v>11</v>
+      </c>
+      <c r="Q228">
+        <v>4</v>
+      </c>
+      <c r="S228">
+        <v>5</v>
+      </c>
+      <c r="T228">
+        <v>2.5</v>
+      </c>
+      <c r="U228">
+        <v>2</v>
+      </c>
+      <c r="V228">
+        <v>26</v>
+      </c>
+      <c r="W228">
+        <v>14</v>
+      </c>
+      <c r="Z228">
+        <v>1.5</v>
+      </c>
+      <c r="AA228">
+        <v>1.5</v>
+      </c>
+      <c r="AB228">
+        <v>16.5</v>
+      </c>
+      <c r="AC228">
+        <v>15.5</v>
+      </c>
+      <c r="AH228" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="229" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L229" s="2"/>

</xml_diff>

<commit_message>
update w/ opinionway poll (2/25)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2705D6B9-CC00-FE49-AA17-709CEFDB85CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDECD71-ECA5-E949-943F-88400A8A4ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25780" yWindow="10740" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="1900" yWindow="6720" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH434"/>
+  <dimension ref="A1:AH435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="O228" sqref="O228"/>
+      <selection pane="bottomLeft" activeCell="K230" sqref="K230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19257,10 +19257,10 @@
         <v>38</v>
       </c>
       <c r="J226">
-        <v>1049</v>
+        <v>1032</v>
       </c>
       <c r="K226">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L226" s="2">
         <v>1</v>
@@ -19319,13 +19319,13 @@
         <v>2</v>
       </c>
       <c r="D227">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E227">
         <v>2</v>
       </c>
       <c r="F227">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G227" t="s">
         <v>33</v>
@@ -19334,16 +19334,16 @@
         <v>21</v>
       </c>
       <c r="I227" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J227">
-        <v>1049</v>
+        <v>670</v>
       </c>
       <c r="K227">
         <v>1</v>
       </c>
       <c r="L227" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M227" s="2">
         <v>1</v>
@@ -19355,22 +19355,22 @@
         <v>1</v>
       </c>
       <c r="P227">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q227">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S227">
         <v>5</v>
       </c>
       <c r="T227">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U227">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V227">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="W227">
         <v>14</v>
@@ -19379,7 +19379,7 @@
         <v>1</v>
       </c>
       <c r="AA227">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB227">
         <v>17</v>
@@ -19408,34 +19408,34 @@
         <v>25</v>
       </c>
       <c r="G228" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H228" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I228" t="s">
         <v>38</v>
       </c>
       <c r="J228">
-        <v>1030</v>
+        <v>1050</v>
       </c>
       <c r="K228">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L228" s="2">
         <v>0.33333333333333331</v>
       </c>
       <c r="M228" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N228">
-        <v>0.5</v>
-      </c>
-      <c r="O228" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="O228">
+        <v>1</v>
       </c>
       <c r="P228">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q228">
         <v>4</v>
@@ -19444,36 +19444,112 @@
         <v>5</v>
       </c>
       <c r="T228">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U228">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V228">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="W228">
         <v>14</v>
       </c>
       <c r="Z228">
+        <v>1</v>
+      </c>
+      <c r="AA228">
+        <v>2</v>
+      </c>
+      <c r="AB228">
+        <v>17</v>
+      </c>
+      <c r="AC228">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="229" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>126</v>
+      </c>
+      <c r="B229">
+        <v>2022</v>
+      </c>
+      <c r="C229">
+        <v>2</v>
+      </c>
+      <c r="D229">
+        <v>22</v>
+      </c>
+      <c r="E229">
+        <v>2</v>
+      </c>
+      <c r="F229">
+        <v>25</v>
+      </c>
+      <c r="G229" t="s">
+        <v>29</v>
+      </c>
+      <c r="H229" t="s">
+        <v>22</v>
+      </c>
+      <c r="I229" t="s">
+        <v>38</v>
+      </c>
+      <c r="J229">
+        <v>1042</v>
+      </c>
+      <c r="K229">
+        <v>1</v>
+      </c>
+      <c r="L229" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M229" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N229">
+        <v>0.5</v>
+      </c>
+      <c r="O229" t="s">
+        <v>24</v>
+      </c>
+      <c r="P229">
+        <v>11</v>
+      </c>
+      <c r="Q229">
+        <v>4</v>
+      </c>
+      <c r="S229">
+        <v>5</v>
+      </c>
+      <c r="T229">
+        <v>2.5</v>
+      </c>
+      <c r="U229">
+        <v>2</v>
+      </c>
+      <c r="V229">
+        <v>26</v>
+      </c>
+      <c r="W229">
+        <v>14</v>
+      </c>
+      <c r="Z229">
         <v>1.5</v>
       </c>
-      <c r="AA228">
+      <c r="AA229">
         <v>1.5</v>
       </c>
-      <c r="AB228">
+      <c r="AB229">
         <v>16.5</v>
       </c>
-      <c r="AC228">
+      <c r="AC229">
         <v>15.5</v>
       </c>
-      <c r="AH228" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="229" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L229" s="2"/>
-      <c r="M229" s="2"/>
+      <c r="AH229" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="230" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L230" s="2"/>
@@ -20294,6 +20370,10 @@
     <row r="434" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L434" s="2"/>
       <c r="M434" s="2"/>
+    </row>
+    <row r="435" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L435" s="2"/>
+      <c r="M435" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ opinionway and harris polls (2/28) + 2/28 rollings
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDECD71-ECA5-E949-943F-88400A8A4ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FE5238-815C-4543-A78F-066176D7D677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="6720" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH435"/>
+  <dimension ref="A1:AH436"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K230" sqref="K230"/>
+      <selection pane="bottomLeft" activeCell="A231" sqref="A231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19399,13 +19399,13 @@
         <v>2</v>
       </c>
       <c r="D228">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E228">
         <v>2</v>
       </c>
       <c r="F228">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G228" t="s">
         <v>33</v>
@@ -19414,19 +19414,19 @@
         <v>21</v>
       </c>
       <c r="I228" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J228">
-        <v>1050</v>
+        <v>800</v>
       </c>
       <c r="K228">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L228" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M228" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N228">
         <v>1</v>
@@ -19435,37 +19435,37 @@
         <v>1</v>
       </c>
       <c r="P228">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q228">
         <v>4</v>
       </c>
       <c r="S228">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T228">
         <v>2</v>
       </c>
       <c r="U228">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V228">
         <v>24</v>
       </c>
       <c r="W228">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Z228">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA228">
         <v>2</v>
       </c>
       <c r="AB228">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AC228">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="229" spans="1:34" x14ac:dyDescent="0.2">
@@ -19479,40 +19479,40 @@
         <v>2</v>
       </c>
       <c r="D229">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E229">
         <v>2</v>
       </c>
       <c r="F229">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G229" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H229" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I229" t="s">
         <v>38</v>
       </c>
       <c r="J229">
-        <v>1042</v>
+        <v>1050</v>
       </c>
       <c r="K229">
         <v>1</v>
       </c>
       <c r="L229" s="2">
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M229" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N229">
-        <v>0.5</v>
-      </c>
-      <c r="O229" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="O229">
+        <v>1</v>
       </c>
       <c r="P229">
         <v>11</v>
@@ -19524,40 +19524,195 @@
         <v>5</v>
       </c>
       <c r="T229">
+        <v>2</v>
+      </c>
+      <c r="U229">
+        <v>2</v>
+      </c>
+      <c r="V229">
+        <v>24</v>
+      </c>
+      <c r="W229">
+        <v>15</v>
+      </c>
+      <c r="Z229">
+        <v>1</v>
+      </c>
+      <c r="AA229">
+        <v>2</v>
+      </c>
+      <c r="AB229">
+        <v>19</v>
+      </c>
+      <c r="AC229">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="230" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>127</v>
+      </c>
+      <c r="B230">
+        <v>2022</v>
+      </c>
+      <c r="C230">
+        <v>2</v>
+      </c>
+      <c r="D230">
+        <v>24</v>
+      </c>
+      <c r="E230">
+        <v>2</v>
+      </c>
+      <c r="F230">
+        <v>28</v>
+      </c>
+      <c r="G230" t="s">
+        <v>29</v>
+      </c>
+      <c r="H230" t="s">
+        <v>22</v>
+      </c>
+      <c r="I230" t="s">
+        <v>38</v>
+      </c>
+      <c r="J230">
+        <v>1042</v>
+      </c>
+      <c r="K230">
+        <v>1</v>
+      </c>
+      <c r="L230" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M230" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N230">
+        <v>0.5</v>
+      </c>
+      <c r="O230">
+        <v>0.5</v>
+      </c>
+      <c r="P230">
+        <v>10.5</v>
+      </c>
+      <c r="Q230">
+        <v>3.5</v>
+      </c>
+      <c r="S230">
+        <v>5</v>
+      </c>
+      <c r="T230">
         <v>2.5</v>
       </c>
-      <c r="U229">
-        <v>2</v>
-      </c>
-      <c r="V229">
-        <v>26</v>
-      </c>
-      <c r="W229">
+      <c r="U230">
+        <v>1.5</v>
+      </c>
+      <c r="V230">
+        <v>28</v>
+      </c>
+      <c r="W230">
+        <v>13</v>
+      </c>
+      <c r="Z230">
+        <v>2</v>
+      </c>
+      <c r="AA230">
+        <v>2.5</v>
+      </c>
+      <c r="AB230">
+        <v>16</v>
+      </c>
+      <c r="AC230">
         <v>14</v>
       </c>
-      <c r="Z229">
+      <c r="AH230">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>128</v>
+      </c>
+      <c r="B231">
+        <v>2022</v>
+      </c>
+      <c r="C231">
+        <v>2</v>
+      </c>
+      <c r="D231">
+        <v>25</v>
+      </c>
+      <c r="E231">
+        <v>2</v>
+      </c>
+      <c r="F231">
+        <v>28</v>
+      </c>
+      <c r="G231" t="s">
+        <v>20</v>
+      </c>
+      <c r="H231" t="s">
+        <v>22</v>
+      </c>
+      <c r="I231" t="s">
+        <v>47</v>
+      </c>
+      <c r="J231">
+        <v>1700</v>
+      </c>
+      <c r="K231">
+        <v>1</v>
+      </c>
+      <c r="L231" s="2">
+        <v>1</v>
+      </c>
+      <c r="M231" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N231">
+        <v>1</v>
+      </c>
+      <c r="O231">
+        <v>0.5</v>
+      </c>
+      <c r="P231">
+        <v>12.5</v>
+      </c>
+      <c r="Q231">
+        <v>3.5</v>
+      </c>
+      <c r="S231">
+        <v>5</v>
+      </c>
+      <c r="T231">
+        <v>2</v>
+      </c>
+      <c r="U231">
         <v>1.5</v>
       </c>
-      <c r="AA229">
+      <c r="V231">
+        <v>27</v>
+      </c>
+      <c r="W231">
+        <v>11</v>
+      </c>
+      <c r="Z231">
         <v>1.5</v>
       </c>
-      <c r="AB229">
-        <v>16.5</v>
-      </c>
-      <c r="AC229">
-        <v>15.5</v>
-      </c>
-      <c r="AH229" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="230" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L230" s="2"/>
-      <c r="M230" s="2"/>
-    </row>
-    <row r="231" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L231" s="2"/>
-      <c r="M231" s="2"/>
+      <c r="AA231">
+        <v>1</v>
+      </c>
+      <c r="AB231">
+        <v>18</v>
+      </c>
+      <c r="AC231">
+        <v>15</v>
+      </c>
+      <c r="AD231">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="232" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L232" s="2"/>
@@ -20374,6 +20529,10 @@
     <row r="435" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L435" s="2"/>
       <c r="M435" s="2"/>
+    </row>
+    <row r="436" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L436" s="2"/>
+      <c r="M436" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ elabe poll (3/1) + rollings (3/1)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FE5238-815C-4543-A78F-066176D7D677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341E346B-B48E-194A-BB32-9EFBEFE49F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="6720" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -557,8 +557,8 @@
   <dimension ref="A1:AH436"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A231" sqref="A231"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AH235" sqref="AH235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19488,64 +19488,67 @@
         <v>28</v>
       </c>
       <c r="G229" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H229" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I229" t="s">
         <v>38</v>
       </c>
       <c r="J229">
-        <v>1050</v>
+        <v>1076</v>
       </c>
       <c r="K229">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L229" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M229" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N229">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O229">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P229">
-        <v>11</v>
+        <v>10.5</v>
       </c>
       <c r="Q229">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S229">
         <v>5</v>
       </c>
       <c r="T229">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="U229">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V229">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="W229">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z229">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA229">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB229">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AC229">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="AH229">
+        <v>0.5</v>
       </c>
     </row>
     <row r="230" spans="1:34" x14ac:dyDescent="0.2">
@@ -19559,7 +19562,7 @@
         <v>2</v>
       </c>
       <c r="D230">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E230">
         <v>2</v>
@@ -19568,67 +19571,64 @@
         <v>28</v>
       </c>
       <c r="G230" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H230" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I230" t="s">
         <v>38</v>
       </c>
       <c r="J230">
-        <v>1042</v>
+        <v>1119</v>
       </c>
       <c r="K230">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L230" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M230" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N230">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O230">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P230">
-        <v>10.5</v>
+        <v>11</v>
       </c>
       <c r="Q230">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S230">
         <v>5</v>
       </c>
       <c r="T230">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U230">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V230">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="W230">
+        <v>15</v>
+      </c>
+      <c r="Z230">
+        <v>1</v>
+      </c>
+      <c r="AA230">
+        <v>2</v>
+      </c>
+      <c r="AB230">
+        <v>19</v>
+      </c>
+      <c r="AC230">
         <v>13</v>
-      </c>
-      <c r="Z230">
-        <v>2</v>
-      </c>
-      <c r="AA230">
-        <v>2.5</v>
-      </c>
-      <c r="AB230">
-        <v>16</v>
-      </c>
-      <c r="AC230">
-        <v>14</v>
-      </c>
-      <c r="AH230">
-        <v>0.5</v>
       </c>
     </row>
     <row r="231" spans="1:34" x14ac:dyDescent="0.2">
@@ -19660,10 +19660,10 @@
         <v>47</v>
       </c>
       <c r="J231">
-        <v>1700</v>
+        <v>1727</v>
       </c>
       <c r="K231">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L231" s="2">
         <v>1</v>
@@ -19715,16 +19715,253 @@
       </c>
     </row>
     <row r="232" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L232" s="2"/>
-      <c r="M232" s="2"/>
+      <c r="A232">
+        <v>129</v>
+      </c>
+      <c r="B232">
+        <v>2022</v>
+      </c>
+      <c r="C232">
+        <v>2</v>
+      </c>
+      <c r="D232">
+        <v>27</v>
+      </c>
+      <c r="E232">
+        <v>2</v>
+      </c>
+      <c r="F232">
+        <v>28</v>
+      </c>
+      <c r="G232" t="s">
+        <v>30</v>
+      </c>
+      <c r="H232" t="s">
+        <v>21</v>
+      </c>
+      <c r="I232" t="s">
+        <v>47</v>
+      </c>
+      <c r="J232">
+        <v>1005</v>
+      </c>
+      <c r="K232">
+        <v>0</v>
+      </c>
+      <c r="L232" s="2">
+        <v>1</v>
+      </c>
+      <c r="M232" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N232">
+        <v>1</v>
+      </c>
+      <c r="O232">
+        <v>0.5</v>
+      </c>
+      <c r="P232">
+        <v>12.5</v>
+      </c>
+      <c r="Q232">
+        <v>4</v>
+      </c>
+      <c r="S232">
+        <v>6.5</v>
+      </c>
+      <c r="T232">
+        <v>1.5</v>
+      </c>
+      <c r="U232">
+        <v>1.5</v>
+      </c>
+      <c r="V232">
+        <v>25</v>
+      </c>
+      <c r="W232">
+        <v>12</v>
+      </c>
+      <c r="Z232">
+        <v>2</v>
+      </c>
+      <c r="AA232">
+        <v>2</v>
+      </c>
+      <c r="AB232">
+        <v>17</v>
+      </c>
+      <c r="AC232">
+        <v>14</v>
+      </c>
+      <c r="AD232">
+        <v>0.5</v>
+      </c>
+      <c r="AH232" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="233" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L233" s="2"/>
-      <c r="M233" s="2"/>
+      <c r="A233">
+        <v>130</v>
+      </c>
+      <c r="B233">
+        <v>2022</v>
+      </c>
+      <c r="C233">
+        <v>2</v>
+      </c>
+      <c r="D233">
+        <v>26</v>
+      </c>
+      <c r="E233">
+        <v>3</v>
+      </c>
+      <c r="F233">
+        <v>1</v>
+      </c>
+      <c r="G233" t="s">
+        <v>33</v>
+      </c>
+      <c r="H233" t="s">
+        <v>21</v>
+      </c>
+      <c r="I233" t="s">
+        <v>38</v>
+      </c>
+      <c r="J233">
+        <v>1119</v>
+      </c>
+      <c r="K233">
+        <v>1</v>
+      </c>
+      <c r="L233" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M233" s="2">
+        <v>1</v>
+      </c>
+      <c r="N233">
+        <v>1</v>
+      </c>
+      <c r="O233">
+        <v>1</v>
+      </c>
+      <c r="P233">
+        <v>11</v>
+      </c>
+      <c r="Q233">
+        <v>4</v>
+      </c>
+      <c r="S233">
+        <v>4</v>
+      </c>
+      <c r="T233">
+        <v>2</v>
+      </c>
+      <c r="U233">
+        <v>2</v>
+      </c>
+      <c r="V233">
+        <v>26</v>
+      </c>
+      <c r="W233">
+        <v>15</v>
+      </c>
+      <c r="Z233">
+        <v>1</v>
+      </c>
+      <c r="AA233">
+        <v>2</v>
+      </c>
+      <c r="AB233">
+        <v>19</v>
+      </c>
+      <c r="AC233">
+        <v>12</v>
+      </c>
     </row>
     <row r="234" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L234" s="2"/>
-      <c r="M234" s="2"/>
+      <c r="A234">
+        <v>131</v>
+      </c>
+      <c r="B234">
+        <v>2022</v>
+      </c>
+      <c r="C234">
+        <v>2</v>
+      </c>
+      <c r="D234">
+        <v>25</v>
+      </c>
+      <c r="E234">
+        <v>3</v>
+      </c>
+      <c r="F234">
+        <v>1</v>
+      </c>
+      <c r="G234" t="s">
+        <v>29</v>
+      </c>
+      <c r="H234" t="s">
+        <v>22</v>
+      </c>
+      <c r="I234" t="s">
+        <v>38</v>
+      </c>
+      <c r="J234">
+        <v>1076</v>
+      </c>
+      <c r="K234">
+        <v>1</v>
+      </c>
+      <c r="L234" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M234" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N234">
+        <v>0.5</v>
+      </c>
+      <c r="O234">
+        <v>0.5</v>
+      </c>
+      <c r="P234">
+        <v>10.5</v>
+      </c>
+      <c r="Q234">
+        <v>4.5</v>
+      </c>
+      <c r="S234">
+        <v>5</v>
+      </c>
+      <c r="T234">
+        <v>2.5</v>
+      </c>
+      <c r="U234">
+        <v>1.5</v>
+      </c>
+      <c r="V234">
+        <v>28</v>
+      </c>
+      <c r="W234">
+        <v>13</v>
+      </c>
+      <c r="Z234">
+        <v>1.5</v>
+      </c>
+      <c r="AA234">
+        <v>2.5</v>
+      </c>
+      <c r="AB234">
+        <v>17</v>
+      </c>
+      <c r="AC234">
+        <v>13</v>
+      </c>
+      <c r="AH234" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="235" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L235" s="2"/>

</xml_diff>

<commit_message>
update w/ rollings (3/2)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341E346B-B48E-194A-BB32-9EFBEFE49F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCAC59C-702C-EE48-B0DD-8FD449A89382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="6720" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="26940" yWindow="5360" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH436"/>
+  <dimension ref="A1:AH437"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AH235" sqref="AH235"/>
+      <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A235" sqref="A235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19417,10 +19417,10 @@
         <v>47</v>
       </c>
       <c r="J228">
-        <v>800</v>
+        <v>740</v>
       </c>
       <c r="K228">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L228" s="2">
         <v>1</v>
@@ -19811,13 +19811,13 @@
         <v>2</v>
       </c>
       <c r="D233">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E233">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F233">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G233" t="s">
         <v>33</v>
@@ -19826,16 +19826,16 @@
         <v>21</v>
       </c>
       <c r="I233" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J233">
-        <v>1119</v>
+        <v>731</v>
       </c>
       <c r="K233">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L233" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M233" s="2">
         <v>1</v>
@@ -19847,13 +19847,13 @@
         <v>1</v>
       </c>
       <c r="P233">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q233">
         <v>4</v>
       </c>
       <c r="S233">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T233">
         <v>2</v>
@@ -19862,7 +19862,7 @@
         <v>2</v>
       </c>
       <c r="V233">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="W233">
         <v>15</v>
@@ -19877,7 +19877,7 @@
         <v>19</v>
       </c>
       <c r="AC233">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="234" spans="1:34" x14ac:dyDescent="0.2">
@@ -19891,81 +19891,157 @@
         <v>2</v>
       </c>
       <c r="D234">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E234">
         <v>3</v>
       </c>
       <c r="F234">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G234" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H234" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I234" t="s">
         <v>38</v>
       </c>
       <c r="J234">
-        <v>1076</v>
+        <v>1081</v>
       </c>
       <c r="K234">
         <v>1</v>
       </c>
       <c r="L234" s="2">
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M234" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N234">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O234">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P234">
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="Q234">
+        <v>4</v>
+      </c>
+      <c r="S234">
+        <v>4</v>
+      </c>
+      <c r="T234">
+        <v>3</v>
+      </c>
+      <c r="U234">
+        <v>2</v>
+      </c>
+      <c r="V234">
+        <v>26</v>
+      </c>
+      <c r="W234">
+        <v>15</v>
+      </c>
+      <c r="Z234">
+        <v>1</v>
+      </c>
+      <c r="AA234">
+        <v>2</v>
+      </c>
+      <c r="AB234">
+        <v>19</v>
+      </c>
+      <c r="AC234">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="235" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>132</v>
+      </c>
+      <c r="B235">
+        <v>2022</v>
+      </c>
+      <c r="C235">
+        <v>2</v>
+      </c>
+      <c r="D235">
+        <v>26</v>
+      </c>
+      <c r="E235">
+        <v>3</v>
+      </c>
+      <c r="F235">
+        <v>2</v>
+      </c>
+      <c r="G235" t="s">
+        <v>29</v>
+      </c>
+      <c r="H235" t="s">
+        <v>22</v>
+      </c>
+      <c r="I235" t="s">
+        <v>38</v>
+      </c>
+      <c r="J235">
+        <v>1109</v>
+      </c>
+      <c r="K235">
+        <v>1</v>
+      </c>
+      <c r="L235" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M235" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N235">
+        <v>0.5</v>
+      </c>
+      <c r="O235">
+        <v>0.5</v>
+      </c>
+      <c r="P235">
+        <v>11</v>
+      </c>
+      <c r="Q235">
         <v>4.5</v>
       </c>
-      <c r="S234">
-        <v>5</v>
-      </c>
-      <c r="T234">
+      <c r="S235">
+        <v>4.5</v>
+      </c>
+      <c r="T235">
         <v>2.5</v>
       </c>
-      <c r="U234">
+      <c r="U235">
         <v>1.5</v>
       </c>
-      <c r="V234">
+      <c r="V235">
         <v>28</v>
       </c>
-      <c r="W234">
-        <v>13</v>
-      </c>
-      <c r="Z234">
+      <c r="W235">
+        <v>13.5</v>
+      </c>
+      <c r="Z235">
         <v>1.5</v>
       </c>
-      <c r="AA234">
-        <v>2.5</v>
-      </c>
-      <c r="AB234">
+      <c r="AA235">
+        <v>2</v>
+      </c>
+      <c r="AB235">
         <v>17</v>
       </c>
-      <c r="AC234">
-        <v>13</v>
-      </c>
-      <c r="AH234" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="235" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L235" s="2"/>
-      <c r="M235" s="2"/>
+      <c r="AC235">
+        <v>12.5</v>
+      </c>
+      <c r="AH235">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="236" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L236" s="2"/>
@@ -20770,6 +20846,10 @@
     <row r="436" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L436" s="2"/>
       <c r="M436" s="2"/>
+    </row>
+    <row r="437" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L437" s="2"/>
+      <c r="M437" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ cluster17 poll (3/3) + rollings (3/3)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCAC59C-702C-EE48-B0DD-8FD449A89382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E89EB5-4B28-0641-8E06-432671EBD2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26940" yWindow="5360" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="28180" yWindow="1340" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH437"/>
+  <dimension ref="A1:AH439"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A235" sqref="A235"/>
+      <selection pane="bottomLeft" activeCell="A234" sqref="A234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19891,61 +19891,61 @@
         <v>2</v>
       </c>
       <c r="D234">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E234">
         <v>3</v>
       </c>
       <c r="F234">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G234" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H234" t="s">
         <v>21</v>
       </c>
       <c r="I234" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J234">
-        <v>1081</v>
+        <v>2095</v>
       </c>
       <c r="K234">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L234" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M234" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N234">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O234">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P234">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="Q234">
         <v>4</v>
       </c>
       <c r="S234">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="T234">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="U234">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V234">
-        <v>26</v>
+        <v>25.5</v>
       </c>
       <c r="W234">
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="Z234">
         <v>1</v>
@@ -19954,10 +19954,13 @@
         <v>2</v>
       </c>
       <c r="AB234">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AC234">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="AD234">
+        <v>1</v>
       </c>
     </row>
     <row r="235" spans="1:34" x14ac:dyDescent="0.2">
@@ -19971,85 +19974,237 @@
         <v>2</v>
       </c>
       <c r="D235">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E235">
         <v>3</v>
       </c>
       <c r="F235">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G235" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H235" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I235" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J235">
-        <v>1109</v>
+        <v>700</v>
       </c>
       <c r="K235">
         <v>1</v>
       </c>
       <c r="L235" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M235" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N235">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O235">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P235">
         <v>11</v>
       </c>
       <c r="Q235">
+        <v>3</v>
+      </c>
+      <c r="S235">
+        <v>6</v>
+      </c>
+      <c r="T235">
+        <v>3</v>
+      </c>
+      <c r="U235">
+        <v>2</v>
+      </c>
+      <c r="V235">
+        <v>27</v>
+      </c>
+      <c r="W235">
+        <v>14</v>
+      </c>
+      <c r="Z235">
+        <v>1</v>
+      </c>
+      <c r="AA235">
+        <v>1</v>
+      </c>
+      <c r="AB235">
+        <v>18</v>
+      </c>
+      <c r="AC235">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="236" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>133</v>
+      </c>
+      <c r="B236">
+        <v>2022</v>
+      </c>
+      <c r="C236">
+        <v>2</v>
+      </c>
+      <c r="D236">
+        <v>28</v>
+      </c>
+      <c r="E236">
+        <v>3</v>
+      </c>
+      <c r="F236">
+        <v>3</v>
+      </c>
+      <c r="G236" t="s">
+        <v>33</v>
+      </c>
+      <c r="H236" t="s">
+        <v>21</v>
+      </c>
+      <c r="I236" t="s">
+        <v>38</v>
+      </c>
+      <c r="J236">
+        <v>1078</v>
+      </c>
+      <c r="K236">
+        <v>1</v>
+      </c>
+      <c r="L236" s="2">
+        <v>1</v>
+      </c>
+      <c r="M236" s="2">
+        <v>1</v>
+      </c>
+      <c r="N236">
+        <v>1</v>
+      </c>
+      <c r="O236">
+        <v>1</v>
+      </c>
+      <c r="P236">
+        <v>10</v>
+      </c>
+      <c r="Q236">
+        <v>4</v>
+      </c>
+      <c r="S236">
+        <v>5</v>
+      </c>
+      <c r="T236">
+        <v>2</v>
+      </c>
+      <c r="U236">
+        <v>2</v>
+      </c>
+      <c r="V236">
+        <v>27</v>
+      </c>
+      <c r="W236">
+        <v>14</v>
+      </c>
+      <c r="Z236">
+        <v>2</v>
+      </c>
+      <c r="AA236">
+        <v>2</v>
+      </c>
+      <c r="AB236">
+        <v>18</v>
+      </c>
+      <c r="AC236">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="237" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>134</v>
+      </c>
+      <c r="B237">
+        <v>2022</v>
+      </c>
+      <c r="C237">
+        <v>2</v>
+      </c>
+      <c r="D237">
+        <v>28</v>
+      </c>
+      <c r="E237">
+        <v>3</v>
+      </c>
+      <c r="F237">
+        <v>3</v>
+      </c>
+      <c r="G237" t="s">
+        <v>29</v>
+      </c>
+      <c r="H237" t="s">
+        <v>22</v>
+      </c>
+      <c r="I237" t="s">
+        <v>38</v>
+      </c>
+      <c r="J237">
+        <v>1124</v>
+      </c>
+      <c r="K237">
+        <v>1</v>
+      </c>
+      <c r="L237" s="2">
+        <v>1</v>
+      </c>
+      <c r="M237" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N237">
+        <v>0.5</v>
+      </c>
+      <c r="O237">
+        <v>0.5</v>
+      </c>
+      <c r="P237">
+        <v>11.5</v>
+      </c>
+      <c r="Q237">
+        <v>4</v>
+      </c>
+      <c r="S237">
         <v>4.5</v>
       </c>
-      <c r="S235">
-        <v>4.5</v>
-      </c>
-      <c r="T235">
-        <v>2.5</v>
-      </c>
-      <c r="U235">
+      <c r="T237">
+        <v>3</v>
+      </c>
+      <c r="U237">
+        <v>1</v>
+      </c>
+      <c r="V237">
+        <v>28</v>
+      </c>
+      <c r="W237">
+        <v>14</v>
+      </c>
+      <c r="Z237">
         <v>1.5</v>
       </c>
-      <c r="V235">
-        <v>28</v>
-      </c>
-      <c r="W235">
-        <v>13.5</v>
-      </c>
-      <c r="Z235">
-        <v>1.5</v>
-      </c>
-      <c r="AA235">
-        <v>2</v>
-      </c>
-      <c r="AB235">
+      <c r="AA237">
+        <v>2</v>
+      </c>
+      <c r="AB237">
         <v>17</v>
       </c>
-      <c r="AC235">
-        <v>12.5</v>
-      </c>
-      <c r="AH235">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="236" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L236" s="2"/>
-      <c r="M236" s="2"/>
-    </row>
-    <row r="237" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L237" s="2"/>
-      <c r="M237" s="2"/>
+      <c r="AC237">
+        <v>12</v>
+      </c>
+      <c r="AH237">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="238" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L238" s="2"/>
@@ -20850,6 +21005,14 @@
     <row r="437" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L437" s="2"/>
       <c r="M437" s="2"/>
+    </row>
+    <row r="438" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L438" s="2"/>
+      <c r="M438" s="2"/>
+    </row>
+    <row r="439" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L439" s="2"/>
+      <c r="M439" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ bva poll (3/4) + rollings
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E89EB5-4B28-0641-8E06-432671EBD2C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1D721A-1D05-D84E-9177-495BB78547E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28180" yWindow="1340" windowWidth="21480" windowHeight="14560" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH439"/>
+  <dimension ref="A1:AH441"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A234" sqref="A234"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AH240" sqref="AH240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19992,10 +19992,10 @@
         <v>47</v>
       </c>
       <c r="J235">
-        <v>700</v>
+        <v>718</v>
       </c>
       <c r="K235">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L235" s="2">
         <v>1</v>
@@ -20051,16 +20051,16 @@
         <v>2022</v>
       </c>
       <c r="C236">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D236">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="E236">
         <v>3</v>
       </c>
       <c r="F236">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G236" t="s">
         <v>33</v>
@@ -20069,13 +20069,13 @@
         <v>21</v>
       </c>
       <c r="I236" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J236">
-        <v>1078</v>
+        <v>718</v>
       </c>
       <c r="K236">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L236" s="2">
         <v>1</v>
@@ -20090,16 +20090,16 @@
         <v>1</v>
       </c>
       <c r="P236">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q236">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S236">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T236">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U236">
         <v>2</v>
@@ -20111,10 +20111,10 @@
         <v>14</v>
       </c>
       <c r="Z236">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA236">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB236">
         <v>18</v>
@@ -20131,31 +20131,31 @@
         <v>2022</v>
       </c>
       <c r="C237">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D237">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="E237">
         <v>3</v>
       </c>
       <c r="F237">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G237" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H237" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I237" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J237">
-        <v>1124</v>
+        <v>922</v>
       </c>
       <c r="K237">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L237" s="2">
         <v>1</v>
@@ -20173,46 +20173,204 @@
         <v>11.5</v>
       </c>
       <c r="Q237">
+        <v>3.5</v>
+      </c>
+      <c r="S237">
+        <v>5.5</v>
+      </c>
+      <c r="T237">
+        <v>2</v>
+      </c>
+      <c r="U237">
+        <v>1.5</v>
+      </c>
+      <c r="V237">
+        <v>29</v>
+      </c>
+      <c r="W237">
+        <v>13</v>
+      </c>
+      <c r="Z237">
+        <v>2</v>
+      </c>
+      <c r="AA237">
+        <v>2</v>
+      </c>
+      <c r="AB237">
+        <v>16</v>
+      </c>
+      <c r="AC237">
+        <v>13</v>
+      </c>
+      <c r="AD237" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH237" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="238" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>135</v>
+      </c>
+      <c r="B238">
+        <v>2022</v>
+      </c>
+      <c r="C238">
+        <v>2</v>
+      </c>
+      <c r="D238">
+        <v>1</v>
+      </c>
+      <c r="E238">
+        <v>3</v>
+      </c>
+      <c r="F238">
         <v>4</v>
       </c>
-      <c r="S237">
-        <v>4.5</v>
-      </c>
-      <c r="T237">
+      <c r="G238" t="s">
+        <v>33</v>
+      </c>
+      <c r="H238" t="s">
+        <v>21</v>
+      </c>
+      <c r="I238" t="s">
+        <v>38</v>
+      </c>
+      <c r="J238">
+        <v>1037</v>
+      </c>
+      <c r="K238">
+        <v>1</v>
+      </c>
+      <c r="L238" s="2">
+        <v>1</v>
+      </c>
+      <c r="M238" s="2">
+        <v>1</v>
+      </c>
+      <c r="N238">
+        <v>1</v>
+      </c>
+      <c r="O238" t="s">
+        <v>31</v>
+      </c>
+      <c r="P238">
+        <v>11</v>
+      </c>
+      <c r="Q238">
+        <v>4</v>
+      </c>
+      <c r="S238">
+        <v>5</v>
+      </c>
+      <c r="T238">
+        <v>2</v>
+      </c>
+      <c r="U238">
+        <v>2</v>
+      </c>
+      <c r="V238">
+        <v>28</v>
+      </c>
+      <c r="W238">
+        <v>13</v>
+      </c>
+      <c r="Z238">
+        <v>2</v>
+      </c>
+      <c r="AA238">
+        <v>2</v>
+      </c>
+      <c r="AB238">
+        <v>18</v>
+      </c>
+      <c r="AC238">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="239" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>136</v>
+      </c>
+      <c r="B239">
+        <v>2022</v>
+      </c>
+      <c r="C239">
+        <v>2</v>
+      </c>
+      <c r="D239">
+        <v>1</v>
+      </c>
+      <c r="E239">
         <v>3</v>
       </c>
-      <c r="U237">
-        <v>1</v>
-      </c>
-      <c r="V237">
-        <v>28</v>
-      </c>
-      <c r="W237">
+      <c r="F239">
+        <v>4</v>
+      </c>
+      <c r="G239" t="s">
+        <v>29</v>
+      </c>
+      <c r="H239" t="s">
+        <v>22</v>
+      </c>
+      <c r="I239" t="s">
+        <v>38</v>
+      </c>
+      <c r="J239">
+        <v>1117</v>
+      </c>
+      <c r="K239">
+        <v>1</v>
+      </c>
+      <c r="L239" s="2">
+        <v>1</v>
+      </c>
+      <c r="M239" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N239">
+        <v>0.5</v>
+      </c>
+      <c r="O239">
+        <v>1</v>
+      </c>
+      <c r="P239">
+        <v>11.5</v>
+      </c>
+      <c r="Q239">
+        <v>4</v>
+      </c>
+      <c r="S239">
+        <v>5</v>
+      </c>
+      <c r="T239">
+        <v>3</v>
+      </c>
+      <c r="U239" t="s">
+        <v>31</v>
+      </c>
+      <c r="V239">
+        <v>29</v>
+      </c>
+      <c r="W239">
         <v>14</v>
       </c>
-      <c r="Z237">
+      <c r="Z239">
         <v>1.5</v>
       </c>
-      <c r="AA237">
-        <v>2</v>
-      </c>
-      <c r="AB237">
+      <c r="AA239">
+        <v>1.5</v>
+      </c>
+      <c r="AB239">
         <v>17</v>
       </c>
-      <c r="AC237">
+      <c r="AC239">
         <v>12</v>
       </c>
-      <c r="AH237">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="238" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L238" s="2"/>
-      <c r="M238" s="2"/>
-    </row>
-    <row r="239" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L239" s="2"/>
-      <c r="M239" s="2"/>
+      <c r="AH239" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="240" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L240" s="2"/>
@@ -21013,6 +21171,14 @@
     <row r="439" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L439" s="2"/>
       <c r="M439" s="2"/>
+    </row>
+    <row r="440" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L440" s="2"/>
+      <c r="M440" s="2"/>
+    </row>
+    <row r="441" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L441" s="2"/>
+      <c r="M441" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ ipsos polls (3/5)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1D721A-1D05-D84E-9177-495BB78547E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBED0D7A-4F71-164B-BD1F-5DD74C6D0621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="25540" yWindow="500" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH441"/>
+  <dimension ref="A1:AH443"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AH240" sqref="AH240"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D227" sqref="D227:F227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19399,7 +19399,7 @@
         <v>2</v>
       </c>
       <c r="D228">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E228">
         <v>2</v>
@@ -19408,16 +19408,16 @@
         <v>27</v>
       </c>
       <c r="G228" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="H228" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I228" t="s">
         <v>47</v>
       </c>
       <c r="J228">
-        <v>740</v>
+        <v>8598</v>
       </c>
       <c r="K228">
         <v>0</v>
@@ -19432,40 +19432,37 @@
         <v>1</v>
       </c>
       <c r="O228">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P228">
-        <v>10</v>
+        <v>11.5</v>
       </c>
       <c r="Q228">
         <v>4</v>
       </c>
       <c r="S228">
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="T228">
-        <v>2</v>
-      </c>
-      <c r="U228">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V228">
-        <v>24</v>
+        <v>26.5</v>
       </c>
       <c r="W228">
+        <v>12.5</v>
+      </c>
+      <c r="Z228">
+        <v>1.5</v>
+      </c>
+      <c r="AA228">
+        <v>2</v>
+      </c>
+      <c r="AB228">
+        <v>15.5</v>
+      </c>
+      <c r="AC228">
         <v>15</v>
-      </c>
-      <c r="Z228">
-        <v>2</v>
-      </c>
-      <c r="AA228">
-        <v>2</v>
-      </c>
-      <c r="AB228">
-        <v>18</v>
-      </c>
-      <c r="AC228">
-        <v>13</v>
       </c>
     </row>
     <row r="229" spans="1:34" x14ac:dyDescent="0.2">
@@ -19479,25 +19476,25 @@
         <v>2</v>
       </c>
       <c r="D229">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E229">
         <v>2</v>
       </c>
       <c r="F229">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G229" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H229" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I229" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J229">
-        <v>1076</v>
+        <v>740</v>
       </c>
       <c r="K229">
         <v>0</v>
@@ -19509,46 +19506,43 @@
         <v>0.5</v>
       </c>
       <c r="N229">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O229">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P229">
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="Q229">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S229">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T229">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U229">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V229">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="W229">
+        <v>15</v>
+      </c>
+      <c r="Z229">
+        <v>2</v>
+      </c>
+      <c r="AA229">
+        <v>2</v>
+      </c>
+      <c r="AB229">
+        <v>18</v>
+      </c>
+      <c r="AC229">
         <v>13</v>
-      </c>
-      <c r="Z229">
-        <v>2</v>
-      </c>
-      <c r="AA229">
-        <v>2.5</v>
-      </c>
-      <c r="AB229">
-        <v>16</v>
-      </c>
-      <c r="AC229">
-        <v>14</v>
-      </c>
-      <c r="AH229">
-        <v>0.5</v>
       </c>
     </row>
     <row r="230" spans="1:34" x14ac:dyDescent="0.2">
@@ -19562,7 +19556,7 @@
         <v>2</v>
       </c>
       <c r="D230">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E230">
         <v>2</v>
@@ -19571,16 +19565,16 @@
         <v>28</v>
       </c>
       <c r="G230" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H230" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I230" t="s">
         <v>38</v>
       </c>
       <c r="J230">
-        <v>1119</v>
+        <v>1076</v>
       </c>
       <c r="K230">
         <v>0</v>
@@ -19589,46 +19583,49 @@
         <v>1</v>
       </c>
       <c r="M230" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N230">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O230">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P230">
-        <v>11</v>
+        <v>10.5</v>
       </c>
       <c r="Q230">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S230">
         <v>5</v>
       </c>
       <c r="T230">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="U230">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V230">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="W230">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z230">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA230">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB230">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AC230">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="AH230">
+        <v>0.5</v>
       </c>
     </row>
     <row r="231" spans="1:34" x14ac:dyDescent="0.2">
@@ -19651,16 +19648,16 @@
         <v>28</v>
       </c>
       <c r="G231" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="H231" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I231" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J231">
-        <v>1727</v>
+        <v>1119</v>
       </c>
       <c r="K231">
         <v>0</v>
@@ -19669,19 +19666,19 @@
         <v>1</v>
       </c>
       <c r="M231" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N231">
         <v>1</v>
       </c>
       <c r="O231">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P231">
-        <v>12.5</v>
+        <v>11</v>
       </c>
       <c r="Q231">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S231">
         <v>5</v>
@@ -19690,28 +19687,25 @@
         <v>2</v>
       </c>
       <c r="U231">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V231">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="W231">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="Z231">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AA231">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB231">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AC231">
-        <v>15</v>
-      </c>
-      <c r="AD231">
-        <v>0.5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="232" spans="1:34" x14ac:dyDescent="0.2">
@@ -19725,7 +19719,7 @@
         <v>2</v>
       </c>
       <c r="D232">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E232">
         <v>2</v>
@@ -19734,16 +19728,16 @@
         <v>28</v>
       </c>
       <c r="G232" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H232" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I232" t="s">
         <v>47</v>
       </c>
       <c r="J232">
-        <v>1005</v>
+        <v>1727</v>
       </c>
       <c r="K232">
         <v>0</v>
@@ -19764,40 +19758,37 @@
         <v>12.5</v>
       </c>
       <c r="Q232">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S232">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="T232">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="U232">
         <v>1.5</v>
       </c>
       <c r="V232">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="W232">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z232">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AA232">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB232">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AC232">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AD232">
         <v>0.5</v>
-      </c>
-      <c r="AH232" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="233" spans="1:34" x14ac:dyDescent="0.2">
@@ -19820,7 +19811,7 @@
         <v>28</v>
       </c>
       <c r="G233" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H233" t="s">
         <v>21</v>
@@ -19829,7 +19820,7 @@
         <v>47</v>
       </c>
       <c r="J233">
-        <v>731</v>
+        <v>1005</v>
       </c>
       <c r="K233">
         <v>0</v>
@@ -19838,46 +19829,52 @@
         <v>1</v>
       </c>
       <c r="M233" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N233">
         <v>1</v>
       </c>
       <c r="O233">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P233">
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="Q233">
         <v>4</v>
       </c>
       <c r="S233">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="T233">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="U233">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V233">
         <v>25</v>
       </c>
       <c r="W233">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Z233">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA233">
         <v>2</v>
       </c>
       <c r="AB233">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AC233">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="AD233">
+        <v>0.5</v>
+      </c>
+      <c r="AH233" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="234" spans="1:34" x14ac:dyDescent="0.2">
@@ -19894,13 +19891,13 @@
         <v>27</v>
       </c>
       <c r="E234">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F234">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G234" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H234" t="s">
         <v>21</v>
@@ -19909,7 +19906,7 @@
         <v>47</v>
       </c>
       <c r="J234">
-        <v>2095</v>
+        <v>731</v>
       </c>
       <c r="K234">
         <v>0</v>
@@ -19918,34 +19915,34 @@
         <v>1</v>
       </c>
       <c r="M234" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N234">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O234">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P234">
-        <v>13.5</v>
+        <v>10</v>
       </c>
       <c r="Q234">
         <v>4</v>
       </c>
       <c r="S234">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T234">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="U234">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V234">
-        <v>25.5</v>
+        <v>25</v>
       </c>
       <c r="W234">
-        <v>12.5</v>
+        <v>15</v>
       </c>
       <c r="Z234">
         <v>1</v>
@@ -19954,13 +19951,10 @@
         <v>2</v>
       </c>
       <c r="AB234">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AC234">
-        <v>16</v>
-      </c>
-      <c r="AD234">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="235" spans="1:34" x14ac:dyDescent="0.2">
@@ -19974,7 +19968,7 @@
         <v>2</v>
       </c>
       <c r="D235">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E235">
         <v>3</v>
@@ -19983,7 +19977,7 @@
         <v>1</v>
       </c>
       <c r="G235" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H235" t="s">
         <v>21</v>
@@ -19992,7 +19986,7 @@
         <v>47</v>
       </c>
       <c r="J235">
-        <v>718</v>
+        <v>2095</v>
       </c>
       <c r="K235">
         <v>0</v>
@@ -20001,46 +19995,49 @@
         <v>1</v>
       </c>
       <c r="M235" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N235">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O235">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P235">
-        <v>11</v>
+        <v>13.5</v>
       </c>
       <c r="Q235">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S235">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="T235">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="U235">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V235">
-        <v>27</v>
+        <v>25.5</v>
       </c>
       <c r="W235">
-        <v>14</v>
+        <v>12.5</v>
       </c>
       <c r="Z235">
         <v>1</v>
       </c>
       <c r="AA235">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB235">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC235">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="AD235">
+        <v>1</v>
       </c>
     </row>
     <row r="236" spans="1:34" x14ac:dyDescent="0.2">
@@ -20051,16 +20048,16 @@
         <v>2022</v>
       </c>
       <c r="C236">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D236">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E236">
         <v>3</v>
       </c>
       <c r="F236">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G236" t="s">
         <v>33</v>
@@ -20143,7 +20140,7 @@
         <v>2</v>
       </c>
       <c r="G237" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H237" t="s">
         <v>21</v>
@@ -20152,7 +20149,7 @@
         <v>47</v>
       </c>
       <c r="J237">
-        <v>922</v>
+        <v>718</v>
       </c>
       <c r="K237">
         <v>0</v>
@@ -20161,52 +20158,46 @@
         <v>1</v>
       </c>
       <c r="M237" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N237">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O237">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P237">
-        <v>11.5</v>
+        <v>11</v>
       </c>
       <c r="Q237">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S237">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="T237">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U237">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V237">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="W237">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Z237">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA237">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB237">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AC237">
-        <v>13</v>
-      </c>
-      <c r="AD237" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH237" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="238" spans="1:34" x14ac:dyDescent="0.2">
@@ -20217,7 +20208,7 @@
         <v>2022</v>
       </c>
       <c r="C238">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D238">
         <v>1</v>
@@ -20226,52 +20217,52 @@
         <v>3</v>
       </c>
       <c r="F238">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G238" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H238" t="s">
         <v>21</v>
       </c>
       <c r="I238" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J238">
-        <v>1037</v>
+        <v>922</v>
       </c>
       <c r="K238">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L238" s="2">
         <v>1</v>
       </c>
       <c r="M238" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N238">
-        <v>1</v>
-      </c>
-      <c r="O238" t="s">
-        <v>31</v>
+        <v>0.5</v>
+      </c>
+      <c r="O238">
+        <v>0.5</v>
       </c>
       <c r="P238">
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="Q238">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S238">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="T238">
         <v>2</v>
       </c>
       <c r="U238">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V238">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W238">
         <v>13</v>
@@ -20283,10 +20274,16 @@
         <v>2</v>
       </c>
       <c r="AB238">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC238">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="AD238" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH238" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="239" spans="1:34" x14ac:dyDescent="0.2">
@@ -20297,31 +20294,31 @@
         <v>2022</v>
       </c>
       <c r="C239">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D239">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E239">
         <v>3</v>
       </c>
       <c r="F239">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G239" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="H239" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I239" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J239">
-        <v>1117</v>
+        <v>2269</v>
       </c>
       <c r="K239">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L239" s="2">
         <v>1</v>
@@ -20330,31 +20327,28 @@
         <v>0.5</v>
       </c>
       <c r="N239">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O239">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P239">
-        <v>11.5</v>
+        <v>12</v>
       </c>
       <c r="Q239">
         <v>4</v>
       </c>
       <c r="S239">
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="T239">
-        <v>3</v>
-      </c>
-      <c r="U239" t="s">
-        <v>31</v>
+        <v>2.5</v>
       </c>
       <c r="V239">
-        <v>29</v>
+        <v>30.5</v>
       </c>
       <c r="W239">
-        <v>14</v>
+        <v>11.5</v>
       </c>
       <c r="Z239">
         <v>1.5</v>
@@ -20363,80 +20357,232 @@
         <v>1.5</v>
       </c>
       <c r="AB239">
+        <v>14.5</v>
+      </c>
+      <c r="AC239">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="240" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>137</v>
+      </c>
+      <c r="B240">
+        <v>2022</v>
+      </c>
+      <c r="C240">
+        <v>2</v>
+      </c>
+      <c r="D240">
+        <v>1</v>
+      </c>
+      <c r="E240">
+        <v>3</v>
+      </c>
+      <c r="F240">
+        <v>4</v>
+      </c>
+      <c r="G240" t="s">
+        <v>33</v>
+      </c>
+      <c r="H240" t="s">
+        <v>21</v>
+      </c>
+      <c r="I240" t="s">
+        <v>38</v>
+      </c>
+      <c r="J240">
+        <v>1037</v>
+      </c>
+      <c r="K240">
+        <v>1</v>
+      </c>
+      <c r="L240" s="2">
+        <v>1</v>
+      </c>
+      <c r="M240" s="2">
+        <v>1</v>
+      </c>
+      <c r="N240">
+        <v>1</v>
+      </c>
+      <c r="O240" t="s">
+        <v>31</v>
+      </c>
+      <c r="P240">
+        <v>11</v>
+      </c>
+      <c r="Q240">
+        <v>4</v>
+      </c>
+      <c r="S240">
+        <v>5</v>
+      </c>
+      <c r="T240">
+        <v>2</v>
+      </c>
+      <c r="U240">
+        <v>2</v>
+      </c>
+      <c r="V240">
+        <v>28</v>
+      </c>
+      <c r="W240">
+        <v>13</v>
+      </c>
+      <c r="Z240">
+        <v>2</v>
+      </c>
+      <c r="AA240">
+        <v>2</v>
+      </c>
+      <c r="AB240">
+        <v>18</v>
+      </c>
+      <c r="AC240">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="241" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>138</v>
+      </c>
+      <c r="B241">
+        <v>2022</v>
+      </c>
+      <c r="C241">
+        <v>2</v>
+      </c>
+      <c r="D241">
+        <v>1</v>
+      </c>
+      <c r="E241">
+        <v>3</v>
+      </c>
+      <c r="F241">
+        <v>4</v>
+      </c>
+      <c r="G241" t="s">
+        <v>29</v>
+      </c>
+      <c r="H241" t="s">
+        <v>22</v>
+      </c>
+      <c r="I241" t="s">
+        <v>38</v>
+      </c>
+      <c r="J241">
+        <v>1117</v>
+      </c>
+      <c r="K241">
+        <v>1</v>
+      </c>
+      <c r="L241" s="2">
+        <v>1</v>
+      </c>
+      <c r="M241" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N241">
+        <v>0.5</v>
+      </c>
+      <c r="O241">
+        <v>1</v>
+      </c>
+      <c r="P241">
+        <v>11.5</v>
+      </c>
+      <c r="Q241">
+        <v>4</v>
+      </c>
+      <c r="S241">
+        <v>5</v>
+      </c>
+      <c r="T241">
+        <v>3</v>
+      </c>
+      <c r="U241" t="s">
+        <v>31</v>
+      </c>
+      <c r="V241">
+        <v>29</v>
+      </c>
+      <c r="W241">
+        <v>14</v>
+      </c>
+      <c r="Z241">
+        <v>1.5</v>
+      </c>
+      <c r="AA241">
+        <v>1.5</v>
+      </c>
+      <c r="AB241">
         <v>17</v>
       </c>
-      <c r="AC239">
+      <c r="AC241">
         <v>12</v>
       </c>
-      <c r="AH239" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="240" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L240" s="2"/>
-      <c r="M240" s="2"/>
-    </row>
-    <row r="241" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L241" s="2"/>
-      <c r="M241" s="2"/>
-    </row>
-    <row r="242" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="AH241" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="242" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L242" s="2"/>
       <c r="M242" s="2"/>
     </row>
-    <row r="243" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L243" s="2"/>
       <c r="M243" s="2"/>
     </row>
-    <row r="244" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L244" s="2"/>
       <c r="M244" s="2"/>
     </row>
-    <row r="245" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L245" s="2"/>
       <c r="M245" s="2"/>
     </row>
-    <row r="246" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L246" s="2"/>
       <c r="M246" s="2"/>
     </row>
-    <row r="247" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L247" s="2"/>
       <c r="M247" s="2"/>
     </row>
-    <row r="248" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L248" s="2"/>
       <c r="M248" s="2"/>
     </row>
-    <row r="249" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L249" s="2"/>
       <c r="M249" s="2"/>
     </row>
-    <row r="250" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L250" s="2"/>
       <c r="M250" s="2"/>
     </row>
-    <row r="251" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L251" s="2"/>
       <c r="M251" s="2"/>
     </row>
-    <row r="252" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L252" s="2"/>
       <c r="M252" s="2"/>
     </row>
-    <row r="253" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L253" s="2"/>
       <c r="M253" s="2"/>
     </row>
-    <row r="254" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L254" s="2"/>
       <c r="M254" s="2"/>
     </row>
-    <row r="255" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L255" s="2"/>
       <c r="M255" s="2"/>
     </row>
-    <row r="256" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L256" s="2"/>
       <c r="M256" s="2"/>
     </row>
@@ -21179,6 +21325,14 @@
     <row r="441" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L441" s="2"/>
       <c r="M441" s="2"/>
+    </row>
+    <row r="442" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L442" s="2"/>
+      <c r="M442" s="2"/>
+    </row>
+    <row r="443" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L443" s="2"/>
+      <c r="M443" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ ow polls (3/4 and 3/7) + rollings
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBED0D7A-4F71-164B-BD1F-5DD74C6D0621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2628C9EF-249C-E343-AEED-27F4C71EC4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25540" yWindow="500" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH443"/>
+  <dimension ref="A1:AH444"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D227" sqref="D227:F227"/>
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A243" sqref="A243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20294,10 +20294,10 @@
         <v>2022</v>
       </c>
       <c r="C239">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D239">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E239">
         <v>3</v>
@@ -20306,16 +20306,16 @@
         <v>3</v>
       </c>
       <c r="G239" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H239" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I239" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J239">
-        <v>2269</v>
+        <v>1037</v>
       </c>
       <c r="K239">
         <v>0</v>
@@ -20324,43 +20324,46 @@
         <v>1</v>
       </c>
       <c r="M239" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N239">
         <v>1</v>
       </c>
       <c r="O239">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P239">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q239">
         <v>4</v>
       </c>
       <c r="S239">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="T239">
-        <v>2.5</v>
+        <v>2</v>
+      </c>
+      <c r="U239">
+        <v>2</v>
       </c>
       <c r="V239">
-        <v>30.5</v>
+        <v>27</v>
       </c>
       <c r="W239">
-        <v>11.5</v>
+        <v>14</v>
       </c>
       <c r="Z239">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AA239">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB239">
-        <v>14.5</v>
+        <v>18</v>
       </c>
       <c r="AC239">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="240" spans="1:34" x14ac:dyDescent="0.2">
@@ -20374,76 +20377,79 @@
         <v>2</v>
       </c>
       <c r="D240">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E240">
         <v>3</v>
       </c>
       <c r="F240">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G240" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H240" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I240" t="s">
         <v>38</v>
       </c>
       <c r="J240">
-        <v>1037</v>
+        <v>1117</v>
       </c>
       <c r="K240">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L240" s="2">
         <v>1</v>
       </c>
       <c r="M240" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N240">
-        <v>1</v>
-      </c>
-      <c r="O240" t="s">
-        <v>31</v>
+        <v>0.5</v>
+      </c>
+      <c r="O240">
+        <v>0.5</v>
       </c>
       <c r="P240">
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="Q240">
         <v>4</v>
       </c>
       <c r="S240">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="T240">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U240">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V240">
         <v>28</v>
       </c>
       <c r="W240">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Z240">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AA240">
         <v>2</v>
       </c>
       <c r="AB240">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AC240">
         <v>12</v>
       </c>
-    </row>
-    <row r="241" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AH240">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>138</v>
       </c>
@@ -20451,31 +20457,31 @@
         <v>2022</v>
       </c>
       <c r="C241">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D241">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E241">
         <v>3</v>
       </c>
       <c r="F241">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G241" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="H241" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I241" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J241">
-        <v>1117</v>
+        <v>2269</v>
       </c>
       <c r="K241">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L241" s="2">
         <v>1</v>
@@ -20484,31 +20490,28 @@
         <v>0.5</v>
       </c>
       <c r="N241">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O241">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P241">
-        <v>11.5</v>
+        <v>12</v>
       </c>
       <c r="Q241">
         <v>4</v>
       </c>
       <c r="S241">
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="T241">
-        <v>3</v>
-      </c>
-      <c r="U241" t="s">
-        <v>31</v>
+        <v>2.5</v>
       </c>
       <c r="V241">
-        <v>29</v>
+        <v>30.5</v>
       </c>
       <c r="W241">
-        <v>14</v>
+        <v>11.5</v>
       </c>
       <c r="Z241">
         <v>1.5</v>
@@ -20517,72 +20520,434 @@
         <v>1.5</v>
       </c>
       <c r="AB241">
+        <v>14.5</v>
+      </c>
+      <c r="AC241">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="242" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>139</v>
+      </c>
+      <c r="B242">
+        <v>2022</v>
+      </c>
+      <c r="C242">
+        <v>3</v>
+      </c>
+      <c r="D242">
+        <v>2</v>
+      </c>
+      <c r="E242">
+        <v>3</v>
+      </c>
+      <c r="F242">
+        <v>3</v>
+      </c>
+      <c r="G242" t="s">
+        <v>33</v>
+      </c>
+      <c r="H242" t="s">
+        <v>21</v>
+      </c>
+      <c r="I242" t="s">
+        <v>47</v>
+      </c>
+      <c r="J242">
+        <v>700</v>
+      </c>
+      <c r="K242">
+        <v>0</v>
+      </c>
+      <c r="L242" s="2">
+        <v>1</v>
+      </c>
+      <c r="M242" s="2">
+        <v>1</v>
+      </c>
+      <c r="N242">
+        <v>1</v>
+      </c>
+      <c r="O242" t="s">
+        <v>31</v>
+      </c>
+      <c r="P242">
+        <v>11</v>
+      </c>
+      <c r="Q242">
+        <v>4</v>
+      </c>
+      <c r="S242">
+        <v>7</v>
+      </c>
+      <c r="T242">
+        <v>3</v>
+      </c>
+      <c r="V242">
+        <v>28</v>
+      </c>
+      <c r="W242">
+        <v>13</v>
+      </c>
+      <c r="Z242">
+        <v>2</v>
+      </c>
+      <c r="AA242">
+        <v>2</v>
+      </c>
+      <c r="AB242">
         <v>17</v>
       </c>
-      <c r="AC241">
+      <c r="AC242">
         <v>12</v>
       </c>
-      <c r="AH241" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="242" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L242" s="2"/>
-      <c r="M242" s="2"/>
-    </row>
-    <row r="243" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L243" s="2"/>
-      <c r="M243" s="2"/>
-    </row>
-    <row r="244" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L244" s="2"/>
-      <c r="M244" s="2"/>
-    </row>
-    <row r="245" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L245" s="2"/>
-      <c r="M245" s="2"/>
-    </row>
-    <row r="246" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="L246" s="2"/>
-      <c r="M246" s="2"/>
-    </row>
-    <row r="247" spans="1:34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="243" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>140</v>
+      </c>
+      <c r="B243">
+        <v>2022</v>
+      </c>
+      <c r="C243">
+        <v>3</v>
+      </c>
+      <c r="D243">
+        <v>5</v>
+      </c>
+      <c r="E243">
+        <v>3</v>
+      </c>
+      <c r="F243">
+        <v>6</v>
+      </c>
+      <c r="G243" t="s">
+        <v>33</v>
+      </c>
+      <c r="H243" t="s">
+        <v>21</v>
+      </c>
+      <c r="I243" t="s">
+        <v>47</v>
+      </c>
+      <c r="J243">
+        <v>700</v>
+      </c>
+      <c r="K243">
+        <v>0</v>
+      </c>
+      <c r="L243" s="2">
+        <v>1</v>
+      </c>
+      <c r="M243" s="2">
+        <v>1</v>
+      </c>
+      <c r="N243">
+        <v>1</v>
+      </c>
+      <c r="O243" t="s">
+        <v>31</v>
+      </c>
+      <c r="P243">
+        <v>10</v>
+      </c>
+      <c r="Q243">
+        <v>4</v>
+      </c>
+      <c r="S243">
+        <v>6</v>
+      </c>
+      <c r="T243">
+        <v>3</v>
+      </c>
+      <c r="V243">
+        <v>29</v>
+      </c>
+      <c r="W243">
+        <v>14</v>
+      </c>
+      <c r="Z243">
+        <v>2</v>
+      </c>
+      <c r="AA243">
+        <v>1</v>
+      </c>
+      <c r="AB243">
+        <v>18</v>
+      </c>
+      <c r="AC243">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="244" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>141</v>
+      </c>
+      <c r="B244">
+        <v>2022</v>
+      </c>
+      <c r="C244">
+        <v>3</v>
+      </c>
+      <c r="D244">
+        <v>3</v>
+      </c>
+      <c r="E244">
+        <v>3</v>
+      </c>
+      <c r="F244">
+        <v>7</v>
+      </c>
+      <c r="G244" t="s">
+        <v>29</v>
+      </c>
+      <c r="H244" t="s">
+        <v>22</v>
+      </c>
+      <c r="I244" t="s">
+        <v>38</v>
+      </c>
+      <c r="J244">
+        <v>1117</v>
+      </c>
+      <c r="K244">
+        <v>1</v>
+      </c>
+      <c r="L244" s="2">
+        <v>1</v>
+      </c>
+      <c r="M244" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N244">
+        <v>0.5</v>
+      </c>
+      <c r="O244" t="s">
+        <v>24</v>
+      </c>
+      <c r="P244">
+        <v>11.5</v>
+      </c>
+      <c r="Q244">
+        <v>4</v>
+      </c>
+      <c r="S244">
+        <v>5</v>
+      </c>
+      <c r="T244">
+        <v>2.5</v>
+      </c>
+      <c r="V244">
+        <v>30</v>
+      </c>
+      <c r="W244">
+        <v>13</v>
+      </c>
+      <c r="Z244">
+        <v>1.5</v>
+      </c>
+      <c r="AA244">
+        <v>1.5</v>
+      </c>
+      <c r="AB244">
+        <v>18</v>
+      </c>
+      <c r="AC244">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>142</v>
+      </c>
+      <c r="B245">
+        <v>2022</v>
+      </c>
+      <c r="C245">
+        <v>3</v>
+      </c>
+      <c r="D245">
+        <v>3</v>
+      </c>
+      <c r="E245">
+        <v>3</v>
+      </c>
+      <c r="F245">
+        <v>7</v>
+      </c>
+      <c r="G245" t="s">
+        <v>33</v>
+      </c>
+      <c r="H245" t="s">
+        <v>21</v>
+      </c>
+      <c r="I245" t="s">
+        <v>38</v>
+      </c>
+      <c r="J245">
+        <v>1037</v>
+      </c>
+      <c r="K245">
+        <v>1</v>
+      </c>
+      <c r="L245" s="2">
+        <v>1</v>
+      </c>
+      <c r="M245" s="2">
+        <v>1</v>
+      </c>
+      <c r="N245">
+        <v>1</v>
+      </c>
+      <c r="O245">
+        <v>1</v>
+      </c>
+      <c r="P245">
+        <v>10</v>
+      </c>
+      <c r="Q245">
+        <v>5</v>
+      </c>
+      <c r="S245">
+        <v>5</v>
+      </c>
+      <c r="T245">
+        <v>3</v>
+      </c>
+      <c r="V245">
+        <v>30</v>
+      </c>
+      <c r="W245">
+        <v>13</v>
+      </c>
+      <c r="Z245">
+        <v>2</v>
+      </c>
+      <c r="AA245">
+        <v>1</v>
+      </c>
+      <c r="AB245">
+        <v>18</v>
+      </c>
+      <c r="AC245">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="246" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>143</v>
+      </c>
+      <c r="B246">
+        <v>2022</v>
+      </c>
+      <c r="C246">
+        <v>3</v>
+      </c>
+      <c r="D246">
+        <v>5</v>
+      </c>
+      <c r="E246">
+        <v>3</v>
+      </c>
+      <c r="F246">
+        <v>6</v>
+      </c>
+      <c r="G246" t="s">
+        <v>33</v>
+      </c>
+      <c r="H246" t="s">
+        <v>21</v>
+      </c>
+      <c r="I246" t="s">
+        <v>47</v>
+      </c>
+      <c r="J246">
+        <v>700</v>
+      </c>
+      <c r="K246">
+        <v>0</v>
+      </c>
+      <c r="L246" s="2">
+        <v>1</v>
+      </c>
+      <c r="M246" s="2">
+        <v>1</v>
+      </c>
+      <c r="N246">
+        <v>1</v>
+      </c>
+      <c r="O246" t="s">
+        <v>31</v>
+      </c>
+      <c r="P246">
+        <v>11</v>
+      </c>
+      <c r="Q246">
+        <v>4</v>
+      </c>
+      <c r="S246">
+        <v>7</v>
+      </c>
+      <c r="T246">
+        <v>3</v>
+      </c>
+      <c r="V246">
+        <v>28</v>
+      </c>
+      <c r="W246">
+        <v>13</v>
+      </c>
+      <c r="Z246">
+        <v>2</v>
+      </c>
+      <c r="AA246">
+        <v>2</v>
+      </c>
+      <c r="AB246">
+        <v>17</v>
+      </c>
+      <c r="AC246">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="247" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L247" s="2"/>
       <c r="M247" s="2"/>
     </row>
-    <row r="248" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L248" s="2"/>
       <c r="M248" s="2"/>
     </row>
-    <row r="249" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L249" s="2"/>
       <c r="M249" s="2"/>
     </row>
-    <row r="250" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L250" s="2"/>
       <c r="M250" s="2"/>
     </row>
-    <row r="251" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L251" s="2"/>
       <c r="M251" s="2"/>
     </row>
-    <row r="252" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L252" s="2"/>
       <c r="M252" s="2"/>
     </row>
-    <row r="253" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L253" s="2"/>
       <c r="M253" s="2"/>
     </row>
-    <row r="254" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L254" s="2"/>
       <c r="M254" s="2"/>
     </row>
-    <row r="255" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L255" s="2"/>
       <c r="M255" s="2"/>
     </row>
-    <row r="256" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L256" s="2"/>
       <c r="M256" s="2"/>
     </row>
@@ -21333,6 +21698,10 @@
     <row r="443" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L443" s="2"/>
       <c r="M443" s="2"/>
+    </row>
+    <row r="444" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L444" s="2"/>
+      <c r="M444" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ cluster17 poll (3/8) + rollings
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2628C9EF-249C-E343-AEED-27F4C71EC4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AA5D6B-0936-C743-9B7A-7123CFB1B11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25540" yWindow="500" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH444"/>
+  <dimension ref="A1:AH446"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A243" sqref="A243"/>
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A247" sqref="A247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20614,7 +20614,7 @@
         <v>3</v>
       </c>
       <c r="D243">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E243">
         <v>3</v>
@@ -20623,7 +20623,7 @@
         <v>6</v>
       </c>
       <c r="G243" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H243" t="s">
         <v>21</v>
@@ -20632,7 +20632,7 @@
         <v>47</v>
       </c>
       <c r="J243">
-        <v>700</v>
+        <v>1978</v>
       </c>
       <c r="K243">
         <v>0</v>
@@ -20641,43 +20641,43 @@
         <v>1</v>
       </c>
       <c r="M243" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N243">
         <v>1</v>
       </c>
-      <c r="O243" t="s">
-        <v>31</v>
+      <c r="O243">
+        <v>1</v>
       </c>
       <c r="P243">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="Q243">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S243">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="T243">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="V243">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W243">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Z243">
         <v>2</v>
       </c>
       <c r="AA243">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB243">
-        <v>18</v>
+        <v>14.5</v>
       </c>
       <c r="AC243">
-        <v>12</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="244" spans="1:29" x14ac:dyDescent="0.2">
@@ -20691,70 +20691,70 @@
         <v>3</v>
       </c>
       <c r="D244">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E244">
         <v>3</v>
       </c>
       <c r="F244">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G244" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H244" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I244" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J244">
-        <v>1117</v>
+        <v>751</v>
       </c>
       <c r="K244">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L244" s="2">
         <v>1</v>
       </c>
       <c r="M244" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N244">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O244" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="P244">
-        <v>11.5</v>
+        <v>10</v>
       </c>
       <c r="Q244">
         <v>4</v>
       </c>
       <c r="S244">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T244">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="V244">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W244">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Z244">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AA244">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AB244">
         <v>18</v>
       </c>
       <c r="AC244">
-        <v>12.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="245" spans="1:29" x14ac:dyDescent="0.2">
@@ -20777,43 +20777,43 @@
         <v>7</v>
       </c>
       <c r="G245" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H245" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I245" t="s">
         <v>38</v>
       </c>
       <c r="J245">
-        <v>1037</v>
+        <v>1156</v>
       </c>
       <c r="K245">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L245" s="2">
         <v>1</v>
       </c>
       <c r="M245" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N245">
-        <v>1</v>
-      </c>
-      <c r="O245">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="O245" t="s">
+        <v>24</v>
       </c>
       <c r="P245">
-        <v>10</v>
+        <v>11.5</v>
       </c>
       <c r="Q245">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S245">
         <v>5</v>
       </c>
       <c r="T245">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="V245">
         <v>30</v>
@@ -20822,16 +20822,16 @@
         <v>13</v>
       </c>
       <c r="Z245">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AA245">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AB245">
         <v>18</v>
       </c>
       <c r="AC245">
-        <v>11</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="246" spans="1:29" x14ac:dyDescent="0.2">
@@ -20845,13 +20845,13 @@
         <v>3</v>
       </c>
       <c r="D246">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E246">
         <v>3</v>
       </c>
       <c r="F246">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G246" t="s">
         <v>33</v>
@@ -20860,10 +20860,10 @@
         <v>21</v>
       </c>
       <c r="I246" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J246">
-        <v>700</v>
+        <v>1150</v>
       </c>
       <c r="K246">
         <v>0</v>
@@ -20877,23 +20877,23 @@
       <c r="N246">
         <v>1</v>
       </c>
-      <c r="O246" t="s">
-        <v>31</v>
+      <c r="O246">
+        <v>1</v>
       </c>
       <c r="P246">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q246">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S246">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="T246">
         <v>3</v>
       </c>
       <c r="V246">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="W246">
         <v>13</v>
@@ -20902,22 +20902,168 @@
         <v>2</v>
       </c>
       <c r="AA246">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB246">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AC246">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="247" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>144</v>
+      </c>
+      <c r="B247">
+        <v>2022</v>
+      </c>
+      <c r="C247">
+        <v>3</v>
+      </c>
+      <c r="D247">
+        <v>4</v>
+      </c>
+      <c r="E247">
+        <v>3</v>
+      </c>
+      <c r="F247">
+        <v>8</v>
+      </c>
+      <c r="G247" t="s">
+        <v>29</v>
+      </c>
+      <c r="H247" t="s">
+        <v>22</v>
+      </c>
+      <c r="I247" t="s">
+        <v>38</v>
+      </c>
+      <c r="J247">
+        <v>1156</v>
+      </c>
+      <c r="K247">
+        <v>1</v>
+      </c>
+      <c r="L247" s="2">
+        <v>1</v>
+      </c>
+      <c r="M247" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N247">
+        <v>0.5</v>
+      </c>
+      <c r="O247" t="s">
+        <v>24</v>
+      </c>
+      <c r="P247">
+        <v>11.5</v>
+      </c>
+      <c r="Q247">
+        <v>4</v>
+      </c>
+      <c r="S247">
+        <v>5.5</v>
+      </c>
+      <c r="T247">
+        <v>2</v>
+      </c>
+      <c r="V247">
+        <v>30.5</v>
+      </c>
+      <c r="W247">
         <v>12</v>
       </c>
-    </row>
-    <row r="247" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L247" s="2"/>
-      <c r="M247" s="2"/>
+      <c r="Z247">
+        <v>1.5</v>
+      </c>
+      <c r="AA247">
+        <v>1.5</v>
+      </c>
+      <c r="AB247">
+        <v>18.5</v>
+      </c>
+      <c r="AC247">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="248" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L248" s="2"/>
-      <c r="M248" s="2"/>
+      <c r="A248">
+        <v>145</v>
+      </c>
+      <c r="B248">
+        <v>2022</v>
+      </c>
+      <c r="C248">
+        <v>3</v>
+      </c>
+      <c r="D248">
+        <v>5</v>
+      </c>
+      <c r="E248">
+        <v>3</v>
+      </c>
+      <c r="F248">
+        <v>8</v>
+      </c>
+      <c r="G248" t="s">
+        <v>33</v>
+      </c>
+      <c r="H248" t="s">
+        <v>21</v>
+      </c>
+      <c r="I248" t="s">
+        <v>38</v>
+      </c>
+      <c r="J248">
+        <v>1150</v>
+      </c>
+      <c r="K248">
+        <v>1</v>
+      </c>
+      <c r="L248" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M248" s="2">
+        <v>1</v>
+      </c>
+      <c r="N248">
+        <v>1</v>
+      </c>
+      <c r="O248">
+        <v>1</v>
+      </c>
+      <c r="P248">
+        <v>10</v>
+      </c>
+      <c r="Q248">
+        <v>5</v>
+      </c>
+      <c r="S248">
+        <v>5</v>
+      </c>
+      <c r="T248">
+        <v>3</v>
+      </c>
+      <c r="V248">
+        <v>30</v>
+      </c>
+      <c r="W248">
+        <v>12</v>
+      </c>
+      <c r="Z248">
+        <v>2</v>
+      </c>
+      <c r="AA248">
+        <v>2</v>
+      </c>
+      <c r="AB248">
+        <v>18</v>
+      </c>
+      <c r="AC248">
+        <v>11</v>
+      </c>
     </row>
     <row r="249" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L249" s="2"/>
@@ -21702,6 +21848,14 @@
     <row r="444" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L444" s="2"/>
       <c r="M444" s="2"/>
+    </row>
+    <row r="445" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L445" s="2"/>
+      <c r="M445" s="2"/>
+    </row>
+    <row r="446" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L446" s="2"/>
+      <c r="M446" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ elabe poll (3/8)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AA5D6B-0936-C743-9B7A-7123CFB1B11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9897150-4A8F-944F-A285-86F939E3E74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25540" yWindow="500" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -558,7 +558,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A247" sqref="A247"/>
+      <selection pane="bottomLeft" activeCell="M249" sqref="M249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21066,8 +21066,81 @@
       </c>
     </row>
     <row r="249" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L249" s="2"/>
-      <c r="M249" s="2"/>
+      <c r="A249">
+        <v>146</v>
+      </c>
+      <c r="B249">
+        <v>2022</v>
+      </c>
+      <c r="C249">
+        <v>3</v>
+      </c>
+      <c r="D249">
+        <v>7</v>
+      </c>
+      <c r="E249">
+        <v>3</v>
+      </c>
+      <c r="F249">
+        <v>8</v>
+      </c>
+      <c r="G249" t="s">
+        <v>30</v>
+      </c>
+      <c r="H249" t="s">
+        <v>21</v>
+      </c>
+      <c r="I249" t="s">
+        <v>47</v>
+      </c>
+      <c r="J249">
+        <v>1000</v>
+      </c>
+      <c r="K249">
+        <v>1</v>
+      </c>
+      <c r="L249" s="2">
+        <v>1</v>
+      </c>
+      <c r="M249" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N249">
+        <v>1</v>
+      </c>
+      <c r="O249">
+        <v>1</v>
+      </c>
+      <c r="P249">
+        <v>13</v>
+      </c>
+      <c r="Q249">
+        <v>3.5</v>
+      </c>
+      <c r="S249">
+        <v>5</v>
+      </c>
+      <c r="T249">
+        <v>1.5</v>
+      </c>
+      <c r="V249">
+        <v>33.5</v>
+      </c>
+      <c r="W249">
+        <v>10.5</v>
+      </c>
+      <c r="Z249">
+        <v>2.5</v>
+      </c>
+      <c r="AA249">
+        <v>2.5</v>
+      </c>
+      <c r="AB249">
+        <v>15</v>
+      </c>
+      <c r="AC249">
+        <v>11</v>
+      </c>
     </row>
     <row r="250" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L250" s="2"/>

</xml_diff>

<commit_message>
update w/ harris and ow polls (3/9) + rollings
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9897150-4A8F-944F-A285-86F939E3E74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC6DCA4-8360-5E42-AB21-214F46BCDA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25540" yWindow="500" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH446"/>
+  <dimension ref="A1:AH448"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="M249" sqref="M249"/>
+      <selection pane="bottomLeft" activeCell="A249" sqref="A249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20928,22 +20928,22 @@
         <v>3</v>
       </c>
       <c r="F247">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G247" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H247" t="s">
         <v>22</v>
       </c>
       <c r="I247" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J247">
-        <v>1156</v>
+        <v>1775</v>
       </c>
       <c r="K247">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L247" s="2">
         <v>1</v>
@@ -20952,19 +20952,19 @@
         <v>0.5</v>
       </c>
       <c r="N247">
-        <v>0.5</v>
-      </c>
-      <c r="O247" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="O247">
+        <v>0.5</v>
       </c>
       <c r="P247">
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
       <c r="Q247">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S247">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="T247">
         <v>2</v>
@@ -20973,10 +20973,10 @@
         <v>30.5</v>
       </c>
       <c r="W247">
-        <v>12</v>
+        <v>10.5</v>
       </c>
       <c r="Z247">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AA247">
         <v>1.5</v>
@@ -20999,13 +20999,13 @@
         <v>3</v>
       </c>
       <c r="D248">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E248">
         <v>3</v>
       </c>
       <c r="F248">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G248" t="s">
         <v>33</v>
@@ -21014,25 +21014,25 @@
         <v>21</v>
       </c>
       <c r="I248" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J248">
-        <v>1150</v>
+        <v>700</v>
       </c>
       <c r="K248">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L248" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M248" s="2">
         <v>1</v>
       </c>
       <c r="N248">
-        <v>1</v>
-      </c>
-      <c r="O248">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="O248" t="s">
+        <v>31</v>
       </c>
       <c r="P248">
         <v>10</v>
@@ -21050,19 +21050,19 @@
         <v>30</v>
       </c>
       <c r="W248">
+        <v>13</v>
+      </c>
+      <c r="Z248">
+        <v>2</v>
+      </c>
+      <c r="AA248">
+        <v>1</v>
+      </c>
+      <c r="AB248">
+        <v>17</v>
+      </c>
+      <c r="AC248">
         <v>12</v>
-      </c>
-      <c r="Z248">
-        <v>2</v>
-      </c>
-      <c r="AA248">
-        <v>2</v>
-      </c>
-      <c r="AB248">
-        <v>18</v>
-      </c>
-      <c r="AC248">
-        <v>11</v>
       </c>
     </row>
     <row r="249" spans="1:29" x14ac:dyDescent="0.2">
@@ -21076,79 +21076,225 @@
         <v>3</v>
       </c>
       <c r="D249">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E249">
         <v>3</v>
       </c>
       <c r="F249">
+        <v>9</v>
+      </c>
+      <c r="G249" t="s">
+        <v>29</v>
+      </c>
+      <c r="H249" t="s">
+        <v>22</v>
+      </c>
+      <c r="I249" t="s">
+        <v>38</v>
+      </c>
+      <c r="J249">
+        <v>1156</v>
+      </c>
+      <c r="K249">
+        <v>1</v>
+      </c>
+      <c r="L249" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M249" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N249">
+        <v>0.5</v>
+      </c>
+      <c r="O249" t="s">
+        <v>24</v>
+      </c>
+      <c r="P249">
+        <v>11</v>
+      </c>
+      <c r="Q249">
+        <v>4</v>
+      </c>
+      <c r="S249">
+        <v>5.5</v>
+      </c>
+      <c r="T249">
+        <v>2</v>
+      </c>
+      <c r="V249">
+        <v>31.5</v>
+      </c>
+      <c r="W249">
+        <v>12</v>
+      </c>
+      <c r="Z249">
+        <v>2</v>
+      </c>
+      <c r="AA249">
+        <v>1</v>
+      </c>
+      <c r="AB249">
+        <v>18.5</v>
+      </c>
+      <c r="AC249">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="250" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>147</v>
+      </c>
+      <c r="B250">
+        <v>2022</v>
+      </c>
+      <c r="C250">
+        <v>3</v>
+      </c>
+      <c r="D250">
+        <v>6</v>
+      </c>
+      <c r="E250">
+        <v>3</v>
+      </c>
+      <c r="F250">
+        <v>9</v>
+      </c>
+      <c r="G250" t="s">
+        <v>33</v>
+      </c>
+      <c r="H250" t="s">
+        <v>21</v>
+      </c>
+      <c r="I250" t="s">
+        <v>38</v>
+      </c>
+      <c r="J250">
+        <v>1150</v>
+      </c>
+      <c r="K250">
+        <v>1</v>
+      </c>
+      <c r="L250" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M250" s="2">
+        <v>1</v>
+      </c>
+      <c r="N250">
+        <v>1</v>
+      </c>
+      <c r="O250">
+        <v>1</v>
+      </c>
+      <c r="P250">
+        <v>11</v>
+      </c>
+      <c r="Q250">
+        <v>4</v>
+      </c>
+      <c r="S250">
+        <v>5</v>
+      </c>
+      <c r="T250">
+        <v>3</v>
+      </c>
+      <c r="V250">
+        <v>30</v>
+      </c>
+      <c r="W250">
+        <v>12</v>
+      </c>
+      <c r="Z250">
+        <v>2</v>
+      </c>
+      <c r="AA250">
+        <v>2</v>
+      </c>
+      <c r="AB250">
+        <v>18</v>
+      </c>
+      <c r="AC250">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="251" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>148</v>
+      </c>
+      <c r="B251">
+        <v>2022</v>
+      </c>
+      <c r="C251">
+        <v>3</v>
+      </c>
+      <c r="D251">
+        <v>7</v>
+      </c>
+      <c r="E251">
+        <v>3</v>
+      </c>
+      <c r="F251">
         <v>8</v>
       </c>
-      <c r="G249" t="s">
+      <c r="G251" t="s">
         <v>30</v>
       </c>
-      <c r="H249" t="s">
+      <c r="H251" t="s">
         <v>21</v>
       </c>
-      <c r="I249" t="s">
+      <c r="I251" t="s">
         <v>47</v>
       </c>
-      <c r="J249">
-        <v>1000</v>
-      </c>
-      <c r="K249">
-        <v>1</v>
-      </c>
-      <c r="L249" s="2">
-        <v>1</v>
-      </c>
-      <c r="M249" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N249">
-        <v>1</v>
-      </c>
-      <c r="O249">
-        <v>1</v>
-      </c>
-      <c r="P249">
+      <c r="J251">
+        <v>986</v>
+      </c>
+      <c r="K251">
+        <v>0</v>
+      </c>
+      <c r="L251" s="2">
+        <v>1</v>
+      </c>
+      <c r="M251" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N251">
+        <v>1</v>
+      </c>
+      <c r="O251">
+        <v>1</v>
+      </c>
+      <c r="P251">
         <v>13</v>
       </c>
-      <c r="Q249">
+      <c r="Q251">
         <v>3.5</v>
       </c>
-      <c r="S249">
+      <c r="S251">
         <v>5</v>
       </c>
-      <c r="T249">
+      <c r="T251">
         <v>1.5</v>
       </c>
-      <c r="V249">
+      <c r="V251">
         <v>33.5</v>
       </c>
-      <c r="W249">
+      <c r="W251">
         <v>10.5</v>
       </c>
-      <c r="Z249">
+      <c r="Z251">
         <v>2.5</v>
       </c>
-      <c r="AA249">
+      <c r="AA251">
         <v>2.5</v>
       </c>
-      <c r="AB249">
+      <c r="AB251">
         <v>15</v>
       </c>
-      <c r="AC249">
+      <c r="AC251">
         <v>11</v>
       </c>
-    </row>
-    <row r="250" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L250" s="2"/>
-      <c r="M250" s="2"/>
-    </row>
-    <row r="251" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L251" s="2"/>
-      <c r="M251" s="2"/>
     </row>
     <row r="252" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L252" s="2"/>
@@ -21929,6 +22075,14 @@
     <row r="446" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L446" s="2"/>
       <c r="M446" s="2"/>
+    </row>
+    <row r="447" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L447" s="2"/>
+      <c r="M447" s="2"/>
+    </row>
+    <row r="448" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L448" s="2"/>
+      <c r="M448" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ kantar + ow polls (3/10) + rollings
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC6DCA4-8360-5E42-AB21-214F46BCDA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BF4CD3-F841-0743-AF84-7CA84D50FFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH448"/>
+  <dimension ref="A1:AH447"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A249" sqref="A249"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AA252" sqref="AA252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21076,70 +21076,70 @@
         <v>3</v>
       </c>
       <c r="D249">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E249">
         <v>3</v>
       </c>
       <c r="F249">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G249" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H249" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I249" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J249">
-        <v>1156</v>
+        <v>986</v>
       </c>
       <c r="K249">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L249" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M249" s="2">
         <v>0.5</v>
       </c>
       <c r="N249">
-        <v>0.5</v>
-      </c>
-      <c r="O249" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="O249">
+        <v>1</v>
       </c>
       <c r="P249">
+        <v>13</v>
+      </c>
+      <c r="Q249">
+        <v>3.5</v>
+      </c>
+      <c r="S249">
+        <v>5</v>
+      </c>
+      <c r="T249">
+        <v>1.5</v>
+      </c>
+      <c r="V249">
+        <v>33.5</v>
+      </c>
+      <c r="W249">
+        <v>10.5</v>
+      </c>
+      <c r="Z249">
+        <v>2.5</v>
+      </c>
+      <c r="AA249">
+        <v>2.5</v>
+      </c>
+      <c r="AB249">
+        <v>15</v>
+      </c>
+      <c r="AC249">
         <v>11</v>
-      </c>
-      <c r="Q249">
-        <v>4</v>
-      </c>
-      <c r="S249">
-        <v>5.5</v>
-      </c>
-      <c r="T249">
-        <v>2</v>
-      </c>
-      <c r="V249">
-        <v>31.5</v>
-      </c>
-      <c r="W249">
-        <v>12</v>
-      </c>
-      <c r="Z249">
-        <v>2</v>
-      </c>
-      <c r="AA249">
-        <v>1</v>
-      </c>
-      <c r="AB249">
-        <v>18.5</v>
-      </c>
-      <c r="AC249">
-        <v>12</v>
       </c>
     </row>
     <row r="250" spans="1:29" x14ac:dyDescent="0.2">
@@ -21153,13 +21153,13 @@
         <v>3</v>
       </c>
       <c r="D250">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E250">
         <v>3</v>
       </c>
       <c r="F250">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G250" t="s">
         <v>33</v>
@@ -21168,25 +21168,25 @@
         <v>21</v>
       </c>
       <c r="I250" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J250">
-        <v>1150</v>
+        <v>717</v>
       </c>
       <c r="K250">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L250" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M250" s="2">
         <v>1</v>
       </c>
       <c r="N250">
-        <v>1</v>
-      </c>
-      <c r="O250">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="O250" t="s">
+        <v>31</v>
       </c>
       <c r="P250">
         <v>11</v>
@@ -21195,10 +21195,10 @@
         <v>4</v>
       </c>
       <c r="S250">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T250">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V250">
         <v>30</v>
@@ -21213,10 +21213,10 @@
         <v>2</v>
       </c>
       <c r="AB250">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AC250">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="251" spans="1:29" x14ac:dyDescent="0.2">
@@ -21236,10 +21236,10 @@
         <v>3</v>
       </c>
       <c r="F251">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G251" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H251" t="s">
         <v>21</v>
@@ -21248,7 +21248,7 @@
         <v>47</v>
       </c>
       <c r="J251">
-        <v>986</v>
+        <v>976</v>
       </c>
       <c r="K251">
         <v>0</v>
@@ -21260,53 +21260,272 @@
         <v>0.5</v>
       </c>
       <c r="N251">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O251">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P251">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q251">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S251">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T251">
         <v>1.5</v>
       </c>
       <c r="V251">
-        <v>33.5</v>
+        <v>31</v>
       </c>
       <c r="W251">
+        <v>12</v>
+      </c>
+      <c r="Z251">
+        <v>2</v>
+      </c>
+      <c r="AA251">
+        <v>3</v>
+      </c>
+      <c r="AB251">
+        <v>17</v>
+      </c>
+      <c r="AC251">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="252" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>149</v>
+      </c>
+      <c r="B252">
+        <v>2022</v>
+      </c>
+      <c r="C252">
+        <v>3</v>
+      </c>
+      <c r="D252">
+        <v>8</v>
+      </c>
+      <c r="E252">
+        <v>3</v>
+      </c>
+      <c r="F252">
+        <v>9</v>
+      </c>
+      <c r="G252" t="s">
+        <v>33</v>
+      </c>
+      <c r="H252" t="s">
+        <v>21</v>
+      </c>
+      <c r="I252" t="s">
+        <v>47</v>
+      </c>
+      <c r="J252">
+        <v>717</v>
+      </c>
+      <c r="K252">
+        <v>1</v>
+      </c>
+      <c r="L252" s="2">
+        <v>1</v>
+      </c>
+      <c r="M252" s="2">
+        <v>1</v>
+      </c>
+      <c r="N252">
+        <v>2</v>
+      </c>
+      <c r="O252" t="s">
+        <v>31</v>
+      </c>
+      <c r="P252">
+        <v>11</v>
+      </c>
+      <c r="Q252">
+        <v>3</v>
+      </c>
+      <c r="S252">
+        <v>7</v>
+      </c>
+      <c r="T252">
+        <v>2</v>
+      </c>
+      <c r="V252">
+        <v>30</v>
+      </c>
+      <c r="W252">
+        <v>13</v>
+      </c>
+      <c r="Z252">
+        <v>2</v>
+      </c>
+      <c r="AA252">
+        <v>2</v>
+      </c>
+      <c r="AB252">
+        <v>17</v>
+      </c>
+      <c r="AC252">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="253" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>150</v>
+      </c>
+      <c r="B253">
+        <v>2022</v>
+      </c>
+      <c r="C253">
+        <v>3</v>
+      </c>
+      <c r="D253">
+        <v>7</v>
+      </c>
+      <c r="E253">
+        <v>3</v>
+      </c>
+      <c r="F253">
+        <v>10</v>
+      </c>
+      <c r="G253" t="s">
+        <v>29</v>
+      </c>
+      <c r="H253" t="s">
+        <v>22</v>
+      </c>
+      <c r="I253" t="s">
+        <v>38</v>
+      </c>
+      <c r="J253">
+        <v>1113</v>
+      </c>
+      <c r="K253">
+        <v>1</v>
+      </c>
+      <c r="L253" s="2">
+        <v>1</v>
+      </c>
+      <c r="M253" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N253">
+        <v>0.5</v>
+      </c>
+      <c r="O253">
+        <v>0.5</v>
+      </c>
+      <c r="P253">
         <v>10.5</v>
       </c>
-      <c r="Z251">
-        <v>2.5</v>
-      </c>
-      <c r="AA251">
-        <v>2.5</v>
-      </c>
-      <c r="AB251">
-        <v>15</v>
-      </c>
-      <c r="AC251">
+      <c r="Q253">
+        <v>4</v>
+      </c>
+      <c r="S253">
+        <v>6</v>
+      </c>
+      <c r="T253">
+        <v>2</v>
+      </c>
+      <c r="V253">
+        <v>31</v>
+      </c>
+      <c r="W253">
+        <v>12.5</v>
+      </c>
+      <c r="Z253">
+        <v>2</v>
+      </c>
+      <c r="AA253">
+        <v>1</v>
+      </c>
+      <c r="AB253">
+        <v>18</v>
+      </c>
+      <c r="AC253">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="254" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>151</v>
+      </c>
+      <c r="B254">
+        <v>2022</v>
+      </c>
+      <c r="C254">
+        <v>3</v>
+      </c>
+      <c r="D254">
+        <v>7</v>
+      </c>
+      <c r="E254">
+        <v>3</v>
+      </c>
+      <c r="F254">
+        <v>10</v>
+      </c>
+      <c r="G254" t="s">
+        <v>33</v>
+      </c>
+      <c r="H254" t="s">
+        <v>21</v>
+      </c>
+      <c r="I254" t="s">
+        <v>38</v>
+      </c>
+      <c r="J254">
+        <v>1113</v>
+      </c>
+      <c r="K254">
+        <v>1</v>
+      </c>
+      <c r="L254" s="2">
+        <v>1</v>
+      </c>
+      <c r="M254" s="2">
+        <v>1</v>
+      </c>
+      <c r="N254">
+        <v>1</v>
+      </c>
+      <c r="O254">
+        <v>1</v>
+      </c>
+      <c r="P254">
         <v>11</v>
       </c>
-    </row>
-    <row r="252" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L252" s="2"/>
-      <c r="M252" s="2"/>
-    </row>
-    <row r="253" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L253" s="2"/>
-      <c r="M253" s="2"/>
-    </row>
-    <row r="254" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L254" s="2"/>
-      <c r="M254" s="2"/>
+      <c r="Q254">
+        <v>4</v>
+      </c>
+      <c r="S254">
+        <v>5</v>
+      </c>
+      <c r="T254">
+        <v>3</v>
+      </c>
+      <c r="V254">
+        <v>30</v>
+      </c>
+      <c r="W254">
+        <v>12</v>
+      </c>
+      <c r="Z254">
+        <v>2</v>
+      </c>
+      <c r="AA254">
+        <v>2</v>
+      </c>
+      <c r="AB254">
+        <v>18</v>
+      </c>
+      <c r="AC254">
+        <v>11</v>
+      </c>
     </row>
     <row r="255" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L255" s="2"/>
@@ -22079,10 +22298,6 @@
     <row r="447" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L447" s="2"/>
       <c r="M447" s="2"/>
-    </row>
-    <row r="448" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L448" s="2"/>
-      <c r="M448" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ bva and ow poll (3/11) + rollings
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BF4CD3-F841-0743-AF84-7CA84D50FFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCB7EE9-BA17-8149-A44C-922563A0C33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH447"/>
+  <dimension ref="A1:AH449"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AA252" sqref="AA252"/>
+      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="K254" sqref="K254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21325,10 +21325,10 @@
         <v>47</v>
       </c>
       <c r="J252">
-        <v>717</v>
+        <v>749</v>
       </c>
       <c r="K252">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L252" s="2">
         <v>1</v>
@@ -21384,28 +21384,28 @@
         <v>3</v>
       </c>
       <c r="D253">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E253">
         <v>3</v>
       </c>
       <c r="F253">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G253" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H253" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I253" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J253">
-        <v>1113</v>
+        <v>977</v>
       </c>
       <c r="K253">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L253" s="2">
         <v>1</v>
@@ -21414,40 +21414,40 @@
         <v>0.5</v>
       </c>
       <c r="N253">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O253">
         <v>0.5</v>
       </c>
       <c r="P253">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
       <c r="Q253">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S253">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="T253">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V253">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W253">
-        <v>12.5</v>
+        <v>12</v>
       </c>
       <c r="Z253">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AA253">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AB253">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AC253">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="254" spans="1:29" x14ac:dyDescent="0.2">
@@ -21470,132 +21470,424 @@
         <v>10</v>
       </c>
       <c r="G254" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H254" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I254" t="s">
         <v>38</v>
       </c>
       <c r="J254">
-        <v>1113</v>
+        <v>1076</v>
       </c>
       <c r="K254">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L254" s="2">
         <v>1</v>
       </c>
       <c r="M254" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N254">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O254">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P254">
-        <v>11</v>
+        <v>10.5</v>
       </c>
       <c r="Q254">
         <v>4</v>
       </c>
       <c r="S254">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T254">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V254">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W254">
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="Z254">
         <v>2</v>
       </c>
       <c r="AA254">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB254">
         <v>18</v>
       </c>
       <c r="AC254">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="255" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>152</v>
+      </c>
+      <c r="B255">
+        <v>2022</v>
+      </c>
+      <c r="C255">
+        <v>3</v>
+      </c>
+      <c r="D255">
+        <v>7</v>
+      </c>
+      <c r="E255">
+        <v>3</v>
+      </c>
+      <c r="F255">
+        <v>10</v>
+      </c>
+      <c r="G255" t="s">
+        <v>33</v>
+      </c>
+      <c r="H255" t="s">
+        <v>21</v>
+      </c>
+      <c r="I255" t="s">
+        <v>38</v>
+      </c>
+      <c r="J255">
+        <v>1087</v>
+      </c>
+      <c r="K255">
+        <v>0</v>
+      </c>
+      <c r="L255" s="2">
+        <v>1</v>
+      </c>
+      <c r="M255" s="2">
+        <v>1</v>
+      </c>
+      <c r="N255">
+        <v>1</v>
+      </c>
+      <c r="O255">
+        <v>1</v>
+      </c>
+      <c r="P255">
         <v>11</v>
       </c>
-    </row>
-    <row r="255" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L255" s="2"/>
-      <c r="M255" s="2"/>
+      <c r="Q255">
+        <v>4</v>
+      </c>
+      <c r="S255">
+        <v>5</v>
+      </c>
+      <c r="T255">
+        <v>3</v>
+      </c>
+      <c r="V255">
+        <v>30</v>
+      </c>
+      <c r="W255">
+        <v>12</v>
+      </c>
+      <c r="Z255">
+        <v>2</v>
+      </c>
+      <c r="AA255">
+        <v>2</v>
+      </c>
+      <c r="AB255">
+        <v>18</v>
+      </c>
+      <c r="AC255">
+        <v>11</v>
+      </c>
     </row>
     <row r="256" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L256" s="2"/>
-      <c r="M256" s="2"/>
-    </row>
-    <row r="257" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L257" s="2"/>
-      <c r="M257" s="2"/>
-    </row>
-    <row r="258" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L258" s="2"/>
-      <c r="M258" s="2"/>
-    </row>
-    <row r="259" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>153</v>
+      </c>
+      <c r="B256">
+        <v>2022</v>
+      </c>
+      <c r="C256">
+        <v>3</v>
+      </c>
+      <c r="D256">
+        <v>9</v>
+      </c>
+      <c r="E256">
+        <v>3</v>
+      </c>
+      <c r="F256">
+        <v>10</v>
+      </c>
+      <c r="G256" t="s">
+        <v>33</v>
+      </c>
+      <c r="H256" t="s">
+        <v>21</v>
+      </c>
+      <c r="I256" t="s">
+        <v>47</v>
+      </c>
+      <c r="J256">
+        <v>707</v>
+      </c>
+      <c r="K256">
+        <v>0</v>
+      </c>
+      <c r="L256" s="2">
+        <v>1</v>
+      </c>
+      <c r="M256" s="2">
+        <v>1</v>
+      </c>
+      <c r="N256">
+        <v>1</v>
+      </c>
+      <c r="O256" t="s">
+        <v>31</v>
+      </c>
+      <c r="P256">
+        <v>11</v>
+      </c>
+      <c r="Q256">
+        <v>4</v>
+      </c>
+      <c r="S256">
+        <v>7</v>
+      </c>
+      <c r="T256">
+        <v>2</v>
+      </c>
+      <c r="V256">
+        <v>30</v>
+      </c>
+      <c r="W256">
+        <v>12</v>
+      </c>
+      <c r="Z256">
+        <v>1</v>
+      </c>
+      <c r="AA256">
+        <v>2</v>
+      </c>
+      <c r="AB256">
+        <v>18</v>
+      </c>
+      <c r="AC256">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="257" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>154</v>
+      </c>
+      <c r="B257">
+        <v>2022</v>
+      </c>
+      <c r="C257">
+        <v>3</v>
+      </c>
+      <c r="D257">
+        <v>8</v>
+      </c>
+      <c r="E257">
+        <v>3</v>
+      </c>
+      <c r="F257">
+        <v>11</v>
+      </c>
+      <c r="G257" t="s">
+        <v>29</v>
+      </c>
+      <c r="H257" t="s">
+        <v>22</v>
+      </c>
+      <c r="I257" t="s">
+        <v>38</v>
+      </c>
+      <c r="J257">
+        <v>1090</v>
+      </c>
+      <c r="K257">
+        <v>0</v>
+      </c>
+      <c r="L257" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M257" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N257">
+        <v>0.5</v>
+      </c>
+      <c r="O257">
+        <v>0.5</v>
+      </c>
+      <c r="P257">
+        <v>10.5</v>
+      </c>
+      <c r="Q257">
+        <v>4.5</v>
+      </c>
+      <c r="S257">
+        <v>6</v>
+      </c>
+      <c r="T257">
+        <v>2</v>
+      </c>
+      <c r="V257">
+        <v>31</v>
+      </c>
+      <c r="W257">
+        <v>12</v>
+      </c>
+      <c r="Z257">
+        <v>2</v>
+      </c>
+      <c r="AA257">
+        <v>1</v>
+      </c>
+      <c r="AB257">
+        <v>17.5</v>
+      </c>
+      <c r="AC257">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="258" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>155</v>
+      </c>
+      <c r="B258">
+        <v>2022</v>
+      </c>
+      <c r="C258">
+        <v>3</v>
+      </c>
+      <c r="D258">
+        <v>8</v>
+      </c>
+      <c r="E258">
+        <v>3</v>
+      </c>
+      <c r="F258">
+        <v>11</v>
+      </c>
+      <c r="G258" t="s">
+        <v>33</v>
+      </c>
+      <c r="H258" t="s">
+        <v>21</v>
+      </c>
+      <c r="I258" t="s">
+        <v>38</v>
+      </c>
+      <c r="J258">
+        <v>1113</v>
+      </c>
+      <c r="K258">
+        <v>1</v>
+      </c>
+      <c r="L258" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M258" s="2">
+        <v>1</v>
+      </c>
+      <c r="N258">
+        <v>1</v>
+      </c>
+      <c r="O258">
+        <v>0.5</v>
+      </c>
+      <c r="P258">
+        <v>12</v>
+      </c>
+      <c r="Q258">
+        <v>3</v>
+      </c>
+      <c r="S258">
+        <v>6</v>
+      </c>
+      <c r="T258">
+        <v>3</v>
+      </c>
+      <c r="V258">
+        <v>30</v>
+      </c>
+      <c r="W258">
+        <v>12</v>
+      </c>
+      <c r="Z258">
+        <v>2</v>
+      </c>
+      <c r="AA258">
+        <v>2</v>
+      </c>
+      <c r="AB258">
+        <v>17</v>
+      </c>
+      <c r="AC258">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="259" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L259" s="2"/>
       <c r="M259" s="2"/>
     </row>
-    <row r="260" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L260" s="2"/>
       <c r="M260" s="2"/>
     </row>
-    <row r="261" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L261" s="2"/>
       <c r="M261" s="2"/>
     </row>
-    <row r="262" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L262" s="2"/>
       <c r="M262" s="2"/>
     </row>
-    <row r="263" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L263" s="2"/>
       <c r="M263" s="2"/>
     </row>
-    <row r="264" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L264" s="2"/>
       <c r="M264" s="2"/>
     </row>
-    <row r="265" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L265" s="2"/>
       <c r="M265" s="2"/>
     </row>
-    <row r="266" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L266" s="2"/>
       <c r="M266" s="2"/>
     </row>
-    <row r="267" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L267" s="2"/>
       <c r="M267" s="2"/>
     </row>
-    <row r="268" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L268" s="2"/>
       <c r="M268" s="2"/>
     </row>
-    <row r="269" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L269" s="2"/>
       <c r="M269" s="2"/>
     </row>
-    <row r="270" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L270" s="2"/>
       <c r="M270" s="2"/>
     </row>
-    <row r="271" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L271" s="2"/>
       <c r="M271" s="2"/>
     </row>
-    <row r="272" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L272" s="2"/>
       <c r="M272" s="2"/>
     </row>
@@ -22298,6 +22590,14 @@
     <row r="447" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L447" s="2"/>
       <c r="M447" s="2"/>
+    </row>
+    <row r="448" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L448" s="2"/>
+      <c r="M448" s="2"/>
+    </row>
+    <row r="449" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L449" s="2"/>
+      <c r="M449" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ ipsos rolling (3/12)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCB7EE9-BA17-8149-A44C-922563A0C33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9BEB93-1718-9444-90AC-ED1914A34531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -556,9 +556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
   <dimension ref="A1:AH449"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K254" sqref="K254"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD259" sqref="AD259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21836,8 +21836,81 @@
       </c>
     </row>
     <row r="259" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L259" s="2"/>
-      <c r="M259" s="2"/>
+      <c r="A259">
+        <v>156</v>
+      </c>
+      <c r="B259">
+        <v>2022</v>
+      </c>
+      <c r="C259">
+        <v>3</v>
+      </c>
+      <c r="D259">
+        <v>9</v>
+      </c>
+      <c r="E259">
+        <v>3</v>
+      </c>
+      <c r="F259">
+        <v>12</v>
+      </c>
+      <c r="G259" t="s">
+        <v>1</v>
+      </c>
+      <c r="H259" t="s">
+        <v>2</v>
+      </c>
+      <c r="I259" t="s">
+        <v>38</v>
+      </c>
+      <c r="J259">
+        <v>878</v>
+      </c>
+      <c r="K259">
+        <v>0</v>
+      </c>
+      <c r="L259" s="2">
+        <v>1</v>
+      </c>
+      <c r="M259" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N259">
+        <v>1.5</v>
+      </c>
+      <c r="O259">
+        <v>0.5</v>
+      </c>
+      <c r="P259">
+        <v>12</v>
+      </c>
+      <c r="Q259">
+        <v>3</v>
+      </c>
+      <c r="S259">
+        <v>6.5</v>
+      </c>
+      <c r="T259">
+        <v>2.5</v>
+      </c>
+      <c r="V259">
+        <v>30.5</v>
+      </c>
+      <c r="W259">
+        <v>11</v>
+      </c>
+      <c r="Z259">
+        <v>1.5</v>
+      </c>
+      <c r="AA259">
+        <v>1.5</v>
+      </c>
+      <c r="AB259">
+        <v>16</v>
+      </c>
+      <c r="AC259">
+        <v>13.5</v>
+      </c>
     </row>
     <row r="260" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L260" s="2"/>

</xml_diff>

<commit_message>
update w/ rollings (3/14)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9BEB93-1718-9444-90AC-ED1914A34531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CABC63E-E70C-5246-A99C-A1067402EC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH449"/>
+  <dimension ref="A1:AH448"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD259" sqref="AD259"/>
+      <selection pane="bottomLeft" activeCell="C263" sqref="C263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21692,70 +21692,70 @@
         <v>3</v>
       </c>
       <c r="D257">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E257">
         <v>3</v>
       </c>
       <c r="F257">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G257" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="H257" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I257" t="s">
         <v>38</v>
       </c>
       <c r="J257">
-        <v>1090</v>
+        <v>878</v>
       </c>
       <c r="K257">
         <v>0</v>
       </c>
       <c r="L257" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M257" s="2">
         <v>0.5</v>
       </c>
       <c r="N257">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="O257">
         <v>0.5</v>
       </c>
       <c r="P257">
-        <v>10.5</v>
+        <v>12</v>
       </c>
       <c r="Q257">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="S257">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="T257">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V257">
-        <v>31</v>
+        <v>30.5</v>
       </c>
       <c r="W257">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z257">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AA257">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AB257">
-        <v>17.5</v>
+        <v>16</v>
       </c>
       <c r="AC257">
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="258" spans="1:29" x14ac:dyDescent="0.2">
@@ -21769,70 +21769,70 @@
         <v>3</v>
       </c>
       <c r="D258">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E258">
         <v>3</v>
       </c>
       <c r="F258">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G258" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H258" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I258" t="s">
         <v>38</v>
       </c>
       <c r="J258">
-        <v>1113</v>
+        <v>1090</v>
       </c>
       <c r="K258">
         <v>1</v>
       </c>
       <c r="L258" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M258" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N258">
         <v>1</v>
       </c>
-      <c r="O258">
-        <v>0.5</v>
+      <c r="O258" t="s">
+        <v>24</v>
       </c>
       <c r="P258">
-        <v>12</v>
+        <v>11.5</v>
       </c>
       <c r="Q258">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="S258">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T258">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V258">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W258">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z258">
         <v>2</v>
       </c>
       <c r="AA258">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB258">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AC258">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="259" spans="1:29" x14ac:dyDescent="0.2">
@@ -21846,75 +21846,148 @@
         <v>3</v>
       </c>
       <c r="D259">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E259">
         <v>3</v>
       </c>
       <c r="F259">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G259" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H259" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I259" t="s">
         <v>38</v>
       </c>
       <c r="J259">
-        <v>878</v>
+        <v>1113</v>
       </c>
       <c r="K259">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L259" s="2">
         <v>1</v>
       </c>
       <c r="M259" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N259">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O259">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P259">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q259">
+        <v>4</v>
+      </c>
+      <c r="S259">
+        <v>6</v>
+      </c>
+      <c r="T259">
         <v>3</v>
       </c>
-      <c r="S259">
-        <v>6.5</v>
-      </c>
-      <c r="T259">
-        <v>2.5</v>
-      </c>
       <c r="V259">
-        <v>30.5</v>
+        <v>30</v>
       </c>
       <c r="W259">
         <v>11</v>
       </c>
       <c r="Z259">
+        <v>2</v>
+      </c>
+      <c r="AA259">
+        <v>2</v>
+      </c>
+      <c r="AB259">
+        <v>18</v>
+      </c>
+      <c r="AC259">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="260" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>157</v>
+      </c>
+      <c r="B260">
+        <v>2022</v>
+      </c>
+      <c r="C260">
+        <v>3</v>
+      </c>
+      <c r="D260">
+        <v>10</v>
+      </c>
+      <c r="E260">
+        <v>3</v>
+      </c>
+      <c r="F260">
+        <v>14</v>
+      </c>
+      <c r="G260" t="s">
+        <v>1</v>
+      </c>
+      <c r="H260" t="s">
+        <v>2</v>
+      </c>
+      <c r="I260" t="s">
+        <v>38</v>
+      </c>
+      <c r="J260">
+        <v>870</v>
+      </c>
+      <c r="K260">
+        <v>0</v>
+      </c>
+      <c r="L260" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M260" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N260">
         <v>1.5</v>
       </c>
-      <c r="AA259">
-        <v>1.5</v>
-      </c>
-      <c r="AB259">
+      <c r="O260">
+        <v>0.5</v>
+      </c>
+      <c r="P260">
+        <v>11.5</v>
+      </c>
+      <c r="Q260">
+        <v>3.5</v>
+      </c>
+      <c r="S260">
+        <v>6.5</v>
+      </c>
+      <c r="T260">
+        <v>2.5</v>
+      </c>
+      <c r="V260">
+        <v>30</v>
+      </c>
+      <c r="W260">
+        <v>11</v>
+      </c>
+      <c r="Z260">
+        <v>2</v>
+      </c>
+      <c r="AA260">
+        <v>2</v>
+      </c>
+      <c r="AB260">
         <v>16</v>
       </c>
-      <c r="AC259">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="260" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L260" s="2"/>
-      <c r="M260" s="2"/>
+      <c r="AC260">
+        <v>13</v>
+      </c>
     </row>
     <row r="261" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L261" s="2"/>
@@ -22667,10 +22740,6 @@
     <row r="448" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L448" s="2"/>
       <c r="M448" s="2"/>
-    </row>
-    <row r="449" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L449" s="2"/>
-      <c r="M449" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ ow poll (3/14)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CABC63E-E70C-5246-A99C-A1067402EC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FBC5EE-D61F-3D4C-99B2-04717E9F9890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH448"/>
+  <dimension ref="A1:AH449"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C263" sqref="C263"/>
+      <selection pane="bottomLeft" activeCell="AE258" sqref="AE258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21769,25 +21769,25 @@
         <v>3</v>
       </c>
       <c r="D258">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E258">
         <v>3</v>
       </c>
       <c r="F258">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G258" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H258" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I258" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J258">
-        <v>1090</v>
+        <v>700</v>
       </c>
       <c r="K258">
         <v>1</v>
@@ -21796,28 +21796,28 @@
         <v>1</v>
       </c>
       <c r="M258" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N258">
         <v>1</v>
       </c>
-      <c r="O258" t="s">
-        <v>24</v>
+      <c r="O258">
+        <v>1</v>
       </c>
       <c r="P258">
-        <v>11.5</v>
+        <v>11</v>
       </c>
       <c r="Q258">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="S258">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T258">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V258">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W258">
         <v>11</v>
@@ -21826,13 +21826,13 @@
         <v>2</v>
       </c>
       <c r="AA258">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB258">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AC258">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="259" spans="1:29" x14ac:dyDescent="0.2">
@@ -21855,16 +21855,16 @@
         <v>14</v>
       </c>
       <c r="G259" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H259" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I259" t="s">
         <v>38</v>
       </c>
       <c r="J259">
-        <v>1113</v>
+        <v>1090</v>
       </c>
       <c r="K259">
         <v>1</v>
@@ -21873,28 +21873,28 @@
         <v>1</v>
       </c>
       <c r="M259" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N259">
         <v>1</v>
       </c>
-      <c r="O259">
-        <v>1</v>
+      <c r="O259" t="s">
+        <v>24</v>
       </c>
       <c r="P259">
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="Q259">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="S259">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T259">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V259">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W259">
         <v>11</v>
@@ -21903,13 +21903,13 @@
         <v>2</v>
       </c>
       <c r="AA259">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB259">
         <v>18</v>
       </c>
       <c r="AC259">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="260" spans="1:29" x14ac:dyDescent="0.2">
@@ -21932,43 +21932,43 @@
         <v>14</v>
       </c>
       <c r="G260" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H260" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I260" t="s">
         <v>38</v>
       </c>
       <c r="J260">
-        <v>870</v>
+        <v>1113</v>
       </c>
       <c r="K260">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L260" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M260" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N260">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O260">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P260">
-        <v>11.5</v>
+        <v>11</v>
       </c>
       <c r="Q260">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S260">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="T260">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="V260">
         <v>30</v>
@@ -21983,15 +21983,88 @@
         <v>2</v>
       </c>
       <c r="AB260">
+        <v>18</v>
+      </c>
+      <c r="AC260">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="261" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>158</v>
+      </c>
+      <c r="B261">
+        <v>2022</v>
+      </c>
+      <c r="C261">
+        <v>3</v>
+      </c>
+      <c r="D261">
+        <v>10</v>
+      </c>
+      <c r="E261">
+        <v>3</v>
+      </c>
+      <c r="F261">
+        <v>14</v>
+      </c>
+      <c r="G261" t="s">
+        <v>1</v>
+      </c>
+      <c r="H261" t="s">
+        <v>2</v>
+      </c>
+      <c r="I261" t="s">
+        <v>38</v>
+      </c>
+      <c r="J261">
+        <v>870</v>
+      </c>
+      <c r="K261">
+        <v>0</v>
+      </c>
+      <c r="L261" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M261" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N261">
+        <v>1.5</v>
+      </c>
+      <c r="O261">
+        <v>0.5</v>
+      </c>
+      <c r="P261">
+        <v>11.5</v>
+      </c>
+      <c r="Q261">
+        <v>3.5</v>
+      </c>
+      <c r="S261">
+        <v>6.5</v>
+      </c>
+      <c r="T261">
+        <v>2.5</v>
+      </c>
+      <c r="V261">
+        <v>30</v>
+      </c>
+      <c r="W261">
+        <v>11</v>
+      </c>
+      <c r="Z261">
+        <v>2</v>
+      </c>
+      <c r="AA261">
+        <v>2</v>
+      </c>
+      <c r="AB261">
         <v>16</v>
       </c>
-      <c r="AC260">
+      <c r="AC261">
         <v>13</v>
       </c>
-    </row>
-    <row r="261" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L261" s="2"/>
-      <c r="M261" s="2"/>
     </row>
     <row r="262" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L262" s="2"/>
@@ -22740,6 +22813,10 @@
     <row r="448" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L448" s="2"/>
       <c r="M448" s="2"/>
+    </row>
+    <row r="449" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L449" s="2"/>
+      <c r="M449" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ rolling polls (3/15)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FBC5EE-D61F-3D4C-99B2-04717E9F9890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17FA9FD-A32C-5547-B5B9-993237F9BD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -557,8 +557,8 @@
   <dimension ref="A1:AH449"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AE258" sqref="AE258"/>
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D267" sqref="D267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21695,22 +21695,22 @@
         <v>9</v>
       </c>
       <c r="E257">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F257">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G257" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="H257" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I257" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J257">
-        <v>878</v>
+        <v>1461</v>
       </c>
       <c r="K257">
         <v>0</v>
@@ -21722,40 +21722,40 @@
         <v>0.5</v>
       </c>
       <c r="N257">
+        <v>2</v>
+      </c>
+      <c r="O257">
+        <v>1</v>
+      </c>
+      <c r="P257">
+        <v>11.5</v>
+      </c>
+      <c r="Q257">
+        <v>3.5</v>
+      </c>
+      <c r="S257">
+        <v>4.5</v>
+      </c>
+      <c r="T257">
         <v>1.5</v>
       </c>
-      <c r="O257">
-        <v>0.5</v>
-      </c>
-      <c r="P257">
-        <v>12</v>
-      </c>
-      <c r="Q257">
-        <v>3</v>
-      </c>
-      <c r="S257">
-        <v>6.5</v>
-      </c>
-      <c r="T257">
-        <v>2.5</v>
-      </c>
       <c r="V257">
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="W257">
         <v>11</v>
       </c>
       <c r="Z257">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AA257">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB257">
-        <v>16</v>
+        <v>19.5</v>
       </c>
       <c r="AC257">
-        <v>13.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="258" spans="1:29" x14ac:dyDescent="0.2">
@@ -21769,70 +21769,70 @@
         <v>3</v>
       </c>
       <c r="D258">
+        <v>9</v>
+      </c>
+      <c r="E258">
+        <v>3</v>
+      </c>
+      <c r="F258">
         <v>12</v>
       </c>
-      <c r="E258">
-        <v>3</v>
-      </c>
-      <c r="F258">
-        <v>13</v>
-      </c>
       <c r="G258" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="H258" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I258" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J258">
-        <v>700</v>
+        <v>878</v>
       </c>
       <c r="K258">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L258" s="2">
         <v>1</v>
       </c>
       <c r="M258" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N258">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O258">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P258">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q258">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S258">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="T258">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="V258">
-        <v>30</v>
+        <v>30.5</v>
       </c>
       <c r="W258">
         <v>11</v>
       </c>
       <c r="Z258">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AA258">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB258">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AC258">
-        <v>10</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="259" spans="1:29" x14ac:dyDescent="0.2">
@@ -21846,25 +21846,25 @@
         <v>3</v>
       </c>
       <c r="D259">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E259">
         <v>3</v>
       </c>
       <c r="F259">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G259" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H259" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I259" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J259">
-        <v>1090</v>
+        <v>700</v>
       </c>
       <c r="K259">
         <v>1</v>
@@ -21873,28 +21873,28 @@
         <v>1</v>
       </c>
       <c r="M259" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N259">
         <v>1</v>
       </c>
-      <c r="O259" t="s">
-        <v>24</v>
+      <c r="O259">
+        <v>1</v>
       </c>
       <c r="P259">
-        <v>11.5</v>
+        <v>11</v>
       </c>
       <c r="Q259">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="S259">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T259">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V259">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W259">
         <v>11</v>
@@ -21903,13 +21903,13 @@
         <v>2</v>
       </c>
       <c r="AA259">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB259">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AC259">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="260" spans="1:29" x14ac:dyDescent="0.2">
@@ -21932,16 +21932,16 @@
         <v>14</v>
       </c>
       <c r="G260" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H260" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I260" t="s">
         <v>38</v>
       </c>
       <c r="J260">
-        <v>1113</v>
+        <v>1090</v>
       </c>
       <c r="K260">
         <v>1</v>
@@ -21950,28 +21950,28 @@
         <v>1</v>
       </c>
       <c r="M260" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N260">
         <v>1</v>
       </c>
-      <c r="O260">
-        <v>1</v>
+      <c r="O260" t="s">
+        <v>24</v>
       </c>
       <c r="P260">
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="Q260">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="S260">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T260">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V260">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W260">
         <v>11</v>
@@ -21980,13 +21980,13 @@
         <v>2</v>
       </c>
       <c r="AA260">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB260">
         <v>18</v>
       </c>
       <c r="AC260">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="261" spans="1:29" x14ac:dyDescent="0.2">
@@ -22009,43 +22009,43 @@
         <v>14</v>
       </c>
       <c r="G261" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H261" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I261" t="s">
         <v>38</v>
       </c>
       <c r="J261">
-        <v>870</v>
+        <v>1113</v>
       </c>
       <c r="K261">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L261" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M261" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N261">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O261">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P261">
-        <v>11.5</v>
+        <v>11</v>
       </c>
       <c r="Q261">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S261">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="T261">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="V261">
         <v>30</v>
@@ -22060,23 +22060,242 @@
         <v>2</v>
       </c>
       <c r="AB261">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AC261">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="262" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>159</v>
+      </c>
+      <c r="B262">
+        <v>2022</v>
+      </c>
+      <c r="C262">
+        <v>3</v>
+      </c>
+      <c r="D262">
+        <v>11</v>
+      </c>
+      <c r="E262">
+        <v>3</v>
+      </c>
+      <c r="F262">
+        <v>15</v>
+      </c>
+      <c r="G262" t="s">
+        <v>1</v>
+      </c>
+      <c r="H262" t="s">
+        <v>2</v>
+      </c>
+      <c r="I262" t="s">
+        <v>38</v>
+      </c>
+      <c r="J262">
+        <v>850</v>
+      </c>
+      <c r="K262">
+        <v>0</v>
+      </c>
+      <c r="L262" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M262" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N262">
+        <v>1.5</v>
+      </c>
+      <c r="O262">
+        <v>0.5</v>
+      </c>
+      <c r="P262">
+        <v>11</v>
+      </c>
+      <c r="Q262">
+        <v>4</v>
+      </c>
+      <c r="S262">
+        <v>6</v>
+      </c>
+      <c r="T262">
+        <v>2.5</v>
+      </c>
+      <c r="V262">
+        <v>30</v>
+      </c>
+      <c r="W262">
+        <v>11</v>
+      </c>
+      <c r="Z262">
+        <v>2.5</v>
+      </c>
+      <c r="AA262">
+        <v>2.5</v>
+      </c>
+      <c r="AB262">
+        <v>15.5</v>
+      </c>
+      <c r="AC262">
         <v>13</v>
       </c>
     </row>
-    <row r="262" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L262" s="2"/>
-      <c r="M262" s="2"/>
-    </row>
     <row r="263" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L263" s="2"/>
-      <c r="M263" s="2"/>
+      <c r="A263">
+        <v>160</v>
+      </c>
+      <c r="B263">
+        <v>2022</v>
+      </c>
+      <c r="C263">
+        <v>3</v>
+      </c>
+      <c r="D263">
+        <v>11</v>
+      </c>
+      <c r="E263">
+        <v>3</v>
+      </c>
+      <c r="F263">
+        <v>15</v>
+      </c>
+      <c r="G263" t="s">
+        <v>33</v>
+      </c>
+      <c r="H263" t="s">
+        <v>21</v>
+      </c>
+      <c r="I263" t="s">
+        <v>38</v>
+      </c>
+      <c r="J263">
+        <v>1100</v>
+      </c>
+      <c r="K263">
+        <v>1</v>
+      </c>
+      <c r="L263" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M263" s="2">
+        <v>1</v>
+      </c>
+      <c r="N263">
+        <v>1</v>
+      </c>
+      <c r="O263">
+        <v>1</v>
+      </c>
+      <c r="P263">
+        <v>11</v>
+      </c>
+      <c r="Q263">
+        <v>4</v>
+      </c>
+      <c r="S263">
+        <v>6</v>
+      </c>
+      <c r="T263">
+        <v>3</v>
+      </c>
+      <c r="V263">
+        <v>30</v>
+      </c>
+      <c r="W263">
+        <v>11</v>
+      </c>
+      <c r="Z263">
+        <v>2</v>
+      </c>
+      <c r="AA263">
+        <v>2</v>
+      </c>
+      <c r="AB263">
+        <v>11</v>
+      </c>
+      <c r="AC263">
+        <v>11</v>
+      </c>
     </row>
     <row r="264" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L264" s="2"/>
-      <c r="M264" s="2"/>
+      <c r="A264">
+        <v>161</v>
+      </c>
+      <c r="B264">
+        <v>2022</v>
+      </c>
+      <c r="C264">
+        <v>3</v>
+      </c>
+      <c r="D264">
+        <v>11</v>
+      </c>
+      <c r="E264">
+        <v>3</v>
+      </c>
+      <c r="F264">
+        <v>15</v>
+      </c>
+      <c r="G264" t="s">
+        <v>29</v>
+      </c>
+      <c r="H264" t="s">
+        <v>22</v>
+      </c>
+      <c r="I264" t="s">
+        <v>38</v>
+      </c>
+      <c r="J264">
+        <v>1090</v>
+      </c>
+      <c r="K264">
+        <v>1</v>
+      </c>
+      <c r="L264" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M264" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N264">
+        <v>1</v>
+      </c>
+      <c r="O264" t="s">
+        <v>24</v>
+      </c>
+      <c r="P264">
+        <v>12</v>
+      </c>
+      <c r="Q264">
+        <v>4.5</v>
+      </c>
+      <c r="S264">
+        <v>5</v>
+      </c>
+      <c r="T264">
+        <v>2</v>
+      </c>
+      <c r="V264">
+        <v>31</v>
+      </c>
+      <c r="W264">
+        <v>11</v>
+      </c>
+      <c r="Z264">
+        <v>2</v>
+      </c>
+      <c r="AA264">
+        <v>1</v>
+      </c>
+      <c r="AB264">
+        <v>18</v>
+      </c>
+      <c r="AC264">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="265" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L265" s="2"/>

</xml_diff>

<commit_message>
update w/ ow polls (3/15 + 3/16), harris poll (3/16) + rollings (3/16)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17FA9FD-A32C-5547-B5B9-993237F9BD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDE68F1-D697-6D40-ABB7-FDDF7FD435E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH449"/>
+  <dimension ref="A1:AH452"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D267" sqref="D267"/>
+      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="K268" sqref="K268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21864,10 +21864,10 @@
         <v>47</v>
       </c>
       <c r="J259">
-        <v>700</v>
+        <v>752</v>
       </c>
       <c r="K259">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L259" s="2">
         <v>1</v>
@@ -21941,10 +21941,10 @@
         <v>38</v>
       </c>
       <c r="J260">
-        <v>1090</v>
+        <v>1070</v>
       </c>
       <c r="K260">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L260" s="2">
         <v>1</v>
@@ -22018,10 +22018,10 @@
         <v>38</v>
       </c>
       <c r="J261">
-        <v>1113</v>
+        <v>1157</v>
       </c>
       <c r="K261">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L261" s="2">
         <v>1</v>
@@ -22083,43 +22083,43 @@
         <v>3</v>
       </c>
       <c r="F262">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G262" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="H262" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I262" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J262">
-        <v>850</v>
+        <v>1817</v>
       </c>
       <c r="K262">
         <v>0</v>
       </c>
       <c r="L262" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M262" s="2">
         <v>0.5</v>
       </c>
       <c r="N262">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O262">
         <v>0.5</v>
       </c>
       <c r="P262">
-        <v>11</v>
+        <v>13.5</v>
       </c>
       <c r="Q262">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S262">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T262">
         <v>2.5</v>
@@ -22128,19 +22128,19 @@
         <v>30</v>
       </c>
       <c r="W262">
+        <v>10.5</v>
+      </c>
+      <c r="Z262">
+        <v>2</v>
+      </c>
+      <c r="AA262">
+        <v>1.5</v>
+      </c>
+      <c r="AB262">
+        <v>19.5</v>
+      </c>
+      <c r="AC262">
         <v>11</v>
-      </c>
-      <c r="Z262">
-        <v>2.5</v>
-      </c>
-      <c r="AA262">
-        <v>2.5</v>
-      </c>
-      <c r="AB262">
-        <v>15.5</v>
-      </c>
-      <c r="AC262">
-        <v>13</v>
       </c>
     </row>
     <row r="263" spans="1:29" x14ac:dyDescent="0.2">
@@ -22154,13 +22154,13 @@
         <v>3</v>
       </c>
       <c r="D263">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E263">
         <v>3</v>
       </c>
       <c r="F263">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G263" t="s">
         <v>33</v>
@@ -22169,16 +22169,16 @@
         <v>21</v>
       </c>
       <c r="I263" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J263">
-        <v>1100</v>
+        <v>718</v>
       </c>
       <c r="K263">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L263" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M263" s="2">
         <v>1</v>
@@ -22205,16 +22205,16 @@
         <v>30</v>
       </c>
       <c r="W263">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z263">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA263">
         <v>2</v>
       </c>
       <c r="AB263">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="AC263">
         <v>11</v>
@@ -22231,7 +22231,7 @@
         <v>3</v>
       </c>
       <c r="D264">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E264">
         <v>3</v>
@@ -22240,74 +22240,293 @@
         <v>15</v>
       </c>
       <c r="G264" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H264" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I264" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J264">
-        <v>1090</v>
+        <v>729</v>
       </c>
       <c r="K264">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L264" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M264" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N264">
         <v>1</v>
       </c>
-      <c r="O264" t="s">
-        <v>24</v>
+      <c r="O264">
+        <v>1</v>
       </c>
       <c r="P264">
         <v>12</v>
       </c>
       <c r="Q264">
+        <v>4</v>
+      </c>
+      <c r="S264">
+        <v>6</v>
+      </c>
+      <c r="T264">
+        <v>2</v>
+      </c>
+      <c r="V264">
+        <v>30</v>
+      </c>
+      <c r="W264">
+        <v>10</v>
+      </c>
+      <c r="Z264">
+        <v>2</v>
+      </c>
+      <c r="AA264">
+        <v>2</v>
+      </c>
+      <c r="AB264">
+        <v>19</v>
+      </c>
+      <c r="AC264">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="265" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>162</v>
+      </c>
+      <c r="B265">
+        <v>2022</v>
+      </c>
+      <c r="C265">
+        <v>3</v>
+      </c>
+      <c r="D265">
+        <v>13</v>
+      </c>
+      <c r="E265">
+        <v>3</v>
+      </c>
+      <c r="F265">
+        <v>16</v>
+      </c>
+      <c r="G265" t="s">
+        <v>1</v>
+      </c>
+      <c r="H265" t="s">
+        <v>2</v>
+      </c>
+      <c r="I265" t="s">
+        <v>38</v>
+      </c>
+      <c r="J265">
+        <v>838</v>
+      </c>
+      <c r="K265">
+        <v>0</v>
+      </c>
+      <c r="L265" s="2">
+        <v>1</v>
+      </c>
+      <c r="M265" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N265">
+        <v>1.5</v>
+      </c>
+      <c r="O265">
+        <v>0.5</v>
+      </c>
+      <c r="P265">
+        <v>11</v>
+      </c>
+      <c r="Q265">
+        <v>4</v>
+      </c>
+      <c r="S265">
+        <v>6.5</v>
+      </c>
+      <c r="T265">
+        <v>2.5</v>
+      </c>
+      <c r="V265">
+        <v>31</v>
+      </c>
+      <c r="W265">
+        <v>10.5</v>
+      </c>
+      <c r="Z265">
+        <v>2.5</v>
+      </c>
+      <c r="AA265">
+        <v>2</v>
+      </c>
+      <c r="AB265">
+        <v>16</v>
+      </c>
+      <c r="AC265">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="266" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>163</v>
+      </c>
+      <c r="B266">
+        <v>2022</v>
+      </c>
+      <c r="C266">
+        <v>3</v>
+      </c>
+      <c r="D266">
+        <v>12</v>
+      </c>
+      <c r="E266">
+        <v>3</v>
+      </c>
+      <c r="F266">
+        <v>16</v>
+      </c>
+      <c r="G266" t="s">
+        <v>33</v>
+      </c>
+      <c r="H266" t="s">
+        <v>21</v>
+      </c>
+      <c r="I266" t="s">
+        <v>38</v>
+      </c>
+      <c r="J266">
+        <v>1111</v>
+      </c>
+      <c r="K266">
+        <v>0</v>
+      </c>
+      <c r="L266" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M266" s="2">
+        <v>1</v>
+      </c>
+      <c r="N266">
+        <v>1</v>
+      </c>
+      <c r="O266" t="s">
+        <v>31</v>
+      </c>
+      <c r="P266">
+        <v>12</v>
+      </c>
+      <c r="Q266">
+        <v>4</v>
+      </c>
+      <c r="S266">
+        <v>6</v>
+      </c>
+      <c r="T266">
+        <v>3</v>
+      </c>
+      <c r="V266">
+        <v>29</v>
+      </c>
+      <c r="W266">
+        <v>11</v>
+      </c>
+      <c r="Z266">
+        <v>2</v>
+      </c>
+      <c r="AA266">
+        <v>3</v>
+      </c>
+      <c r="AB266">
+        <v>17</v>
+      </c>
+      <c r="AC266">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="267" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>164</v>
+      </c>
+      <c r="B267">
+        <v>2022</v>
+      </c>
+      <c r="C267">
+        <v>3</v>
+      </c>
+      <c r="D267">
+        <v>12</v>
+      </c>
+      <c r="E267">
+        <v>3</v>
+      </c>
+      <c r="F267">
+        <v>16</v>
+      </c>
+      <c r="G267" t="s">
+        <v>29</v>
+      </c>
+      <c r="H267" t="s">
+        <v>22</v>
+      </c>
+      <c r="I267" t="s">
+        <v>38</v>
+      </c>
+      <c r="J267">
+        <v>1079</v>
+      </c>
+      <c r="K267">
+        <v>0</v>
+      </c>
+      <c r="L267" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M267" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N267">
+        <v>0.5</v>
+      </c>
+      <c r="O267" t="s">
+        <v>24</v>
+      </c>
+      <c r="P267">
+        <v>12</v>
+      </c>
+      <c r="Q267">
         <v>4.5</v>
       </c>
-      <c r="S264">
-        <v>5</v>
-      </c>
-      <c r="T264">
-        <v>2</v>
-      </c>
-      <c r="V264">
-        <v>31</v>
-      </c>
-      <c r="W264">
+      <c r="S267">
+        <v>5.5</v>
+      </c>
+      <c r="T267">
+        <v>2</v>
+      </c>
+      <c r="V267">
+        <v>30</v>
+      </c>
+      <c r="W267">
         <v>11</v>
       </c>
-      <c r="Z264">
-        <v>2</v>
-      </c>
-      <c r="AA264">
-        <v>1</v>
-      </c>
-      <c r="AB264">
+      <c r="Z267">
+        <v>2.5</v>
+      </c>
+      <c r="AA267">
+        <v>1</v>
+      </c>
+      <c r="AB267">
         <v>18</v>
       </c>
-      <c r="AC264">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="265" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L265" s="2"/>
-      <c r="M265" s="2"/>
-    </row>
-    <row r="266" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L266" s="2"/>
-      <c r="M266" s="2"/>
-    </row>
-    <row r="267" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L267" s="2"/>
-      <c r="M267" s="2"/>
+      <c r="AC267">
+        <v>13</v>
+      </c>
     </row>
     <row r="268" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L268" s="2"/>
@@ -23036,6 +23255,18 @@
     <row r="449" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L449" s="2"/>
       <c r="M449" s="2"/>
+    </row>
+    <row r="450" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L450" s="2"/>
+      <c r="M450" s="2"/>
+    </row>
+    <row r="451" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L451" s="2"/>
+      <c r="M451" s="2"/>
+    </row>
+    <row r="452" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L452" s="2"/>
+      <c r="M452" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ elabe poll (3/16)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDE68F1-D697-6D40-ABB7-FDDF7FD435E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C145FF-F4C5-5246-9B6B-EB15882F4F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -558,7 +558,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K268" sqref="K268"/>
+      <selection pane="bottomLeft" activeCell="AD268" sqref="AD268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22529,8 +22529,81 @@
       </c>
     </row>
     <row r="268" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L268" s="2"/>
-      <c r="M268" s="2"/>
+      <c r="A268">
+        <v>165</v>
+      </c>
+      <c r="B268">
+        <v>2022</v>
+      </c>
+      <c r="C268">
+        <v>3</v>
+      </c>
+      <c r="D268">
+        <v>15</v>
+      </c>
+      <c r="E268">
+        <v>3</v>
+      </c>
+      <c r="F268">
+        <v>16</v>
+      </c>
+      <c r="G268" t="s">
+        <v>30</v>
+      </c>
+      <c r="H268" t="s">
+        <v>21</v>
+      </c>
+      <c r="I268" t="s">
+        <v>47</v>
+      </c>
+      <c r="J268">
+        <v>992</v>
+      </c>
+      <c r="K268">
+        <v>0</v>
+      </c>
+      <c r="L268" s="2">
+        <v>1</v>
+      </c>
+      <c r="M268" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N268">
+        <v>1</v>
+      </c>
+      <c r="O268">
+        <v>0.5</v>
+      </c>
+      <c r="P268">
+        <v>14</v>
+      </c>
+      <c r="Q268">
+        <v>3.5</v>
+      </c>
+      <c r="S268">
+        <v>5</v>
+      </c>
+      <c r="T268">
+        <v>1.5</v>
+      </c>
+      <c r="V268">
+        <v>31</v>
+      </c>
+      <c r="W268">
+        <v>11.5</v>
+      </c>
+      <c r="Z268">
+        <v>2</v>
+      </c>
+      <c r="AA268">
+        <v>1.5</v>
+      </c>
+      <c r="AB268">
+        <v>18</v>
+      </c>
+      <c r="AC268">
+        <v>10.5</v>
+      </c>
     </row>
     <row r="269" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L269" s="2"/>

</xml_diff>

<commit_message>
update w/ rollings (3/17)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C145FF-F4C5-5246-9B6B-EB15882F4F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D96FE4-0955-C042-9AAC-C373DB6E5E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH452"/>
+  <dimension ref="A1:AH454"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD268" sqref="AD268"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AE268" sqref="AE268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22385,7 +22385,7 @@
         <v>3</v>
       </c>
       <c r="D266">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E266">
         <v>3</v>
@@ -22394,61 +22394,61 @@
         <v>16</v>
       </c>
       <c r="G266" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H266" t="s">
         <v>21</v>
       </c>
       <c r="I266" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J266">
-        <v>1111</v>
+        <v>1873</v>
       </c>
       <c r="K266">
         <v>0</v>
       </c>
       <c r="L266" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M266" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N266">
-        <v>1</v>
-      </c>
-      <c r="O266" t="s">
-        <v>31</v>
+        <v>1.5</v>
+      </c>
+      <c r="O266">
+        <v>0.5</v>
       </c>
       <c r="P266">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Q266">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S266">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T266">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V266">
-        <v>29</v>
+        <v>29.5</v>
       </c>
       <c r="W266">
-        <v>11</v>
+        <v>10.5</v>
       </c>
       <c r="Z266">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA266">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AB266">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AC266">
-        <v>12</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="267" spans="1:29" x14ac:dyDescent="0.2">
@@ -22462,7 +22462,7 @@
         <v>3</v>
       </c>
       <c r="D267">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E267">
         <v>3</v>
@@ -22471,61 +22471,61 @@
         <v>16</v>
       </c>
       <c r="G267" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H267" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I267" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J267">
-        <v>1079</v>
+        <v>992</v>
       </c>
       <c r="K267">
         <v>0</v>
       </c>
       <c r="L267" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M267" s="2">
         <v>0.5</v>
       </c>
       <c r="N267">
-        <v>0.5</v>
-      </c>
-      <c r="O267" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="O267">
+        <v>0.5</v>
       </c>
       <c r="P267">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Q267">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="S267">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="T267">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V267">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W267">
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="Z267">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AA267">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AB267">
         <v>18</v>
       </c>
       <c r="AC267">
-        <v>13</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="268" spans="1:29" x14ac:dyDescent="0.2">
@@ -22548,7 +22548,7 @@
         <v>16</v>
       </c>
       <c r="G268" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H268" t="s">
         <v>21</v>
@@ -22557,65 +22557,284 @@
         <v>47</v>
       </c>
       <c r="J268">
-        <v>992</v>
+        <v>700</v>
       </c>
       <c r="K268">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L268" s="2">
         <v>1</v>
       </c>
       <c r="M268" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N268">
         <v>1</v>
       </c>
       <c r="O268">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P268">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="Q268">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S268">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T268">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V268">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="W268">
-        <v>11.5</v>
+        <v>11</v>
       </c>
       <c r="Z268">
         <v>2</v>
       </c>
       <c r="AA268">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AB268">
         <v>18</v>
       </c>
       <c r="AC268">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="269" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>166</v>
+      </c>
+      <c r="B269">
+        <v>2022</v>
+      </c>
+      <c r="C269">
+        <v>3</v>
+      </c>
+      <c r="D269">
+        <v>14</v>
+      </c>
+      <c r="E269">
+        <v>3</v>
+      </c>
+      <c r="F269">
+        <v>17</v>
+      </c>
+      <c r="G269" t="s">
+        <v>33</v>
+      </c>
+      <c r="H269" t="s">
+        <v>21</v>
+      </c>
+      <c r="I269" t="s">
+        <v>38</v>
+      </c>
+      <c r="J269">
+        <v>1111</v>
+      </c>
+      <c r="K269">
+        <v>1</v>
+      </c>
+      <c r="L269" s="2">
+        <v>1</v>
+      </c>
+      <c r="M269" s="2">
+        <v>1</v>
+      </c>
+      <c r="N269">
+        <v>1</v>
+      </c>
+      <c r="O269" t="s">
+        <v>31</v>
+      </c>
+      <c r="P269">
+        <v>12</v>
+      </c>
+      <c r="Q269">
+        <v>4</v>
+      </c>
+      <c r="S269">
+        <v>6</v>
+      </c>
+      <c r="T269">
+        <v>3</v>
+      </c>
+      <c r="V269">
+        <v>29</v>
+      </c>
+      <c r="W269">
+        <v>12</v>
+      </c>
+      <c r="Z269">
+        <v>2</v>
+      </c>
+      <c r="AA269">
+        <v>3</v>
+      </c>
+      <c r="AB269">
+        <v>17</v>
+      </c>
+      <c r="AC269">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="270" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>167</v>
+      </c>
+      <c r="B270">
+        <v>2022</v>
+      </c>
+      <c r="C270">
+        <v>3</v>
+      </c>
+      <c r="D270">
+        <v>14</v>
+      </c>
+      <c r="E270">
+        <v>3</v>
+      </c>
+      <c r="F270">
+        <v>17</v>
+      </c>
+      <c r="G270" t="s">
+        <v>29</v>
+      </c>
+      <c r="H270" t="s">
+        <v>22</v>
+      </c>
+      <c r="I270" t="s">
+        <v>38</v>
+      </c>
+      <c r="J270">
+        <v>1079</v>
+      </c>
+      <c r="K270">
+        <v>1</v>
+      </c>
+      <c r="L270" s="2">
+        <v>1</v>
+      </c>
+      <c r="M270" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N270">
+        <v>0.5</v>
+      </c>
+      <c r="O270">
+        <v>0.5</v>
+      </c>
+      <c r="P270">
+        <v>12.5</v>
+      </c>
+      <c r="Q270">
+        <v>4.5</v>
+      </c>
+      <c r="S270">
+        <v>5</v>
+      </c>
+      <c r="T270">
+        <v>2</v>
+      </c>
+      <c r="V270">
+        <v>30</v>
+      </c>
+      <c r="W270">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="269" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L269" s="2"/>
-      <c r="M269" s="2"/>
-    </row>
-    <row r="270" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L270" s="2"/>
-      <c r="M270" s="2"/>
+      <c r="Z270">
+        <v>2.5</v>
+      </c>
+      <c r="AA270">
+        <v>1.5</v>
+      </c>
+      <c r="AB270">
+        <v>17.5</v>
+      </c>
+      <c r="AC270">
+        <v>13</v>
+      </c>
     </row>
     <row r="271" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L271" s="2"/>
-      <c r="M271" s="2"/>
+      <c r="A271">
+        <v>168</v>
+      </c>
+      <c r="B271">
+        <v>2022</v>
+      </c>
+      <c r="C271">
+        <v>3</v>
+      </c>
+      <c r="D271">
+        <v>14</v>
+      </c>
+      <c r="E271">
+        <v>3</v>
+      </c>
+      <c r="F271">
+        <v>17</v>
+      </c>
+      <c r="G271" t="s">
+        <v>1</v>
+      </c>
+      <c r="H271" t="s">
+        <v>2</v>
+      </c>
+      <c r="I271" t="s">
+        <v>38</v>
+      </c>
+      <c r="J271">
+        <v>837</v>
+      </c>
+      <c r="K271">
+        <v>0</v>
+      </c>
+      <c r="L271" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M271" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N271">
+        <v>1.5</v>
+      </c>
+      <c r="O271">
+        <v>0.5</v>
+      </c>
+      <c r="P271">
+        <v>12</v>
+      </c>
+      <c r="Q271">
+        <v>3.5</v>
+      </c>
+      <c r="S271">
+        <v>6</v>
+      </c>
+      <c r="T271">
+        <v>2.5</v>
+      </c>
+      <c r="V271">
+        <v>31</v>
+      </c>
+      <c r="W271">
+        <v>11</v>
+      </c>
+      <c r="Z271">
+        <v>2.5</v>
+      </c>
+      <c r="AA271">
+        <v>2</v>
+      </c>
+      <c r="AB271">
+        <v>15.5</v>
+      </c>
+      <c r="AC271">
+        <v>12</v>
+      </c>
     </row>
     <row r="272" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L272" s="2"/>
@@ -23340,6 +23559,14 @@
     <row r="452" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L452" s="2"/>
       <c r="M452" s="2"/>
+    </row>
+    <row r="453" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L453" s="2"/>
+      <c r="M453" s="2"/>
+    </row>
+    <row r="454" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L454" s="2"/>
+      <c r="M454" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ ipsos and bva polls (3/18) + rollings (3/18)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D96FE4-0955-C042-9AAC-C373DB6E5E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACD85EA-E2DF-164D-8D2C-741130ACA421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH454"/>
+  <dimension ref="A1:AH456"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AE268" sqref="AE268"/>
+      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD273" sqref="AD273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22077,7 +22077,7 @@
         <v>3</v>
       </c>
       <c r="D262">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E262">
         <v>3</v>
@@ -22086,16 +22086,16 @@
         <v>14</v>
       </c>
       <c r="G262" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="H262" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I262" t="s">
         <v>47</v>
       </c>
       <c r="J262">
-        <v>1817</v>
+        <v>8790</v>
       </c>
       <c r="K262">
         <v>0</v>
@@ -22107,25 +22107,25 @@
         <v>0.5</v>
       </c>
       <c r="N262">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O262">
         <v>0.5</v>
       </c>
       <c r="P262">
-        <v>13.5</v>
+        <v>12</v>
       </c>
       <c r="Q262">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S262">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="T262">
         <v>2.5</v>
       </c>
       <c r="V262">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W262">
         <v>10.5</v>
@@ -22134,13 +22134,13 @@
         <v>2</v>
       </c>
       <c r="AA262">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB262">
-        <v>19.5</v>
+        <v>16</v>
       </c>
       <c r="AC262">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="263" spans="1:29" x14ac:dyDescent="0.2">
@@ -22154,7 +22154,7 @@
         <v>3</v>
       </c>
       <c r="D263">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E263">
         <v>3</v>
@@ -22163,16 +22163,16 @@
         <v>14</v>
       </c>
       <c r="G263" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H263" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I263" t="s">
         <v>47</v>
       </c>
       <c r="J263">
-        <v>718</v>
+        <v>1817</v>
       </c>
       <c r="K263">
         <v>0</v>
@@ -22181,40 +22181,40 @@
         <v>1</v>
       </c>
       <c r="M263" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N263">
         <v>1</v>
       </c>
       <c r="O263">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P263">
-        <v>11</v>
+        <v>13.5</v>
       </c>
       <c r="Q263">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S263">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T263">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="V263">
         <v>30</v>
       </c>
       <c r="W263">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="Z263">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA263">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB263">
-        <v>18</v>
+        <v>19.5</v>
       </c>
       <c r="AC263">
         <v>11</v>
@@ -22231,13 +22231,13 @@
         <v>3</v>
       </c>
       <c r="D264">
+        <v>13</v>
+      </c>
+      <c r="E264">
+        <v>3</v>
+      </c>
+      <c r="F264">
         <v>14</v>
-      </c>
-      <c r="E264">
-        <v>3</v>
-      </c>
-      <c r="F264">
-        <v>15</v>
       </c>
       <c r="G264" t="s">
         <v>33</v>
@@ -22249,7 +22249,7 @@
         <v>47</v>
       </c>
       <c r="J264">
-        <v>729</v>
+        <v>718</v>
       </c>
       <c r="K264">
         <v>0</v>
@@ -22267,7 +22267,7 @@
         <v>1</v>
       </c>
       <c r="P264">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q264">
         <v>4</v>
@@ -22276,7 +22276,7 @@
         <v>6</v>
       </c>
       <c r="T264">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V264">
         <v>30</v>
@@ -22285,13 +22285,13 @@
         <v>10</v>
       </c>
       <c r="Z264">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA264">
         <v>2</v>
       </c>
       <c r="AB264">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AC264">
         <v>11</v>
@@ -22308,25 +22308,25 @@
         <v>3</v>
       </c>
       <c r="D265">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E265">
         <v>3</v>
       </c>
       <c r="F265">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G265" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H265" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I265" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J265">
-        <v>838</v>
+        <v>729</v>
       </c>
       <c r="K265">
         <v>0</v>
@@ -22335,43 +22335,43 @@
         <v>1</v>
       </c>
       <c r="M265" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N265">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O265">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P265">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q265">
         <v>4</v>
       </c>
       <c r="S265">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="T265">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V265">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W265">
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="Z265">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AA265">
         <v>2</v>
       </c>
       <c r="AB265">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AC265">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="266" spans="1:29" x14ac:dyDescent="0.2">
@@ -22385,7 +22385,7 @@
         <v>3</v>
       </c>
       <c r="D266">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E266">
         <v>3</v>
@@ -22394,16 +22394,16 @@
         <v>16</v>
       </c>
       <c r="G266" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="H266" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I266" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J266">
-        <v>1873</v>
+        <v>838</v>
       </c>
       <c r="K266">
         <v>0</v>
@@ -22421,34 +22421,34 @@
         <v>0.5</v>
       </c>
       <c r="P266">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="Q266">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S266">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="T266">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V266">
-        <v>29.5</v>
+        <v>31</v>
       </c>
       <c r="W266">
         <v>10.5</v>
       </c>
       <c r="Z266">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AA266">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AB266">
         <v>16</v>
       </c>
       <c r="AC266">
-        <v>12.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="267" spans="1:29" x14ac:dyDescent="0.2">
@@ -22462,7 +22462,7 @@
         <v>3</v>
       </c>
       <c r="D267">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E267">
         <v>3</v>
@@ -22471,7 +22471,7 @@
         <v>16</v>
       </c>
       <c r="G267" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H267" t="s">
         <v>21</v>
@@ -22480,7 +22480,7 @@
         <v>47</v>
       </c>
       <c r="J267">
-        <v>992</v>
+        <v>1873</v>
       </c>
       <c r="K267">
         <v>0</v>
@@ -22492,7 +22492,7 @@
         <v>0.5</v>
       </c>
       <c r="N267">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O267">
         <v>0.5</v>
@@ -22507,25 +22507,25 @@
         <v>5</v>
       </c>
       <c r="T267">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V267">
-        <v>31</v>
+        <v>29.5</v>
       </c>
       <c r="W267">
-        <v>11.5</v>
+        <v>10.5</v>
       </c>
       <c r="Z267">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA267">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="AB267">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC267">
-        <v>10.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="268" spans="1:29" x14ac:dyDescent="0.2">
@@ -22548,7 +22548,7 @@
         <v>16</v>
       </c>
       <c r="G268" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H268" t="s">
         <v>21</v>
@@ -22557,52 +22557,52 @@
         <v>47</v>
       </c>
       <c r="J268">
-        <v>700</v>
+        <v>992</v>
       </c>
       <c r="K268">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L268" s="2">
         <v>1</v>
       </c>
       <c r="M268" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N268">
         <v>1</v>
       </c>
       <c r="O268">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P268">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="Q268">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S268">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T268">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V268">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="W268">
-        <v>11</v>
+        <v>11.5</v>
       </c>
       <c r="Z268">
         <v>2</v>
       </c>
       <c r="AA268">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="AB268">
         <v>18</v>
       </c>
       <c r="AC268">
-        <v>12</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="269" spans="1:29" x14ac:dyDescent="0.2">
@@ -22616,13 +22616,13 @@
         <v>3</v>
       </c>
       <c r="D269">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E269">
         <v>3</v>
       </c>
       <c r="F269">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G269" t="s">
         <v>33</v>
@@ -22631,10 +22631,10 @@
         <v>21</v>
       </c>
       <c r="I269" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J269">
-        <v>1111</v>
+        <v>700</v>
       </c>
       <c r="K269">
         <v>1</v>
@@ -22648,11 +22648,11 @@
       <c r="N269">
         <v>1</v>
       </c>
-      <c r="O269" t="s">
-        <v>31</v>
+      <c r="O269">
+        <v>1</v>
       </c>
       <c r="P269">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q269">
         <v>4</v>
@@ -22661,25 +22661,25 @@
         <v>6</v>
       </c>
       <c r="T269">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V269">
         <v>29</v>
       </c>
       <c r="W269">
+        <v>11</v>
+      </c>
+      <c r="Z269">
+        <v>2</v>
+      </c>
+      <c r="AA269">
+        <v>3</v>
+      </c>
+      <c r="AB269">
+        <v>18</v>
+      </c>
+      <c r="AC269">
         <v>12</v>
-      </c>
-      <c r="Z269">
-        <v>2</v>
-      </c>
-      <c r="AA269">
-        <v>3</v>
-      </c>
-      <c r="AB269">
-        <v>17</v>
-      </c>
-      <c r="AC269">
-        <v>11</v>
       </c>
     </row>
     <row r="270" spans="1:29" x14ac:dyDescent="0.2">
@@ -22693,28 +22693,28 @@
         <v>3</v>
       </c>
       <c r="D270">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E270">
         <v>3</v>
       </c>
       <c r="F270">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G270" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H270" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I270" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J270">
-        <v>1079</v>
+        <v>933</v>
       </c>
       <c r="K270">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L270" s="2">
         <v>1</v>
@@ -22729,31 +22729,31 @@
         <v>0.5</v>
       </c>
       <c r="P270">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="Q270">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="S270">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="T270">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V270">
         <v>30</v>
       </c>
       <c r="W270">
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="Z270">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AA270">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB270">
-        <v>17.5</v>
+        <v>18</v>
       </c>
       <c r="AC270">
         <v>13</v>
@@ -22779,128 +22779,420 @@
         <v>17</v>
       </c>
       <c r="G271" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H271" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I271" t="s">
         <v>38</v>
       </c>
       <c r="J271">
-        <v>837</v>
+        <v>1111</v>
       </c>
       <c r="K271">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L271" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M271" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N271">
-        <v>1.5</v>
-      </c>
-      <c r="O271">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="O271" t="s">
+        <v>31</v>
       </c>
       <c r="P271">
         <v>12</v>
       </c>
       <c r="Q271">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S271">
         <v>6</v>
       </c>
       <c r="T271">
+        <v>3</v>
+      </c>
+      <c r="V271">
+        <v>29</v>
+      </c>
+      <c r="W271">
+        <v>12</v>
+      </c>
+      <c r="Z271">
+        <v>3</v>
+      </c>
+      <c r="AA271">
+        <v>2</v>
+      </c>
+      <c r="AB271">
+        <v>17</v>
+      </c>
+      <c r="AC271">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="272" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>169</v>
+      </c>
+      <c r="B272">
+        <v>2022</v>
+      </c>
+      <c r="C272">
+        <v>3</v>
+      </c>
+      <c r="D272">
+        <v>14</v>
+      </c>
+      <c r="E272">
+        <v>3</v>
+      </c>
+      <c r="F272">
+        <v>17</v>
+      </c>
+      <c r="G272" t="s">
+        <v>29</v>
+      </c>
+      <c r="H272" t="s">
+        <v>22</v>
+      </c>
+      <c r="I272" t="s">
+        <v>38</v>
+      </c>
+      <c r="J272">
+        <v>1079</v>
+      </c>
+      <c r="K272">
+        <v>1</v>
+      </c>
+      <c r="L272" s="2">
+        <v>1</v>
+      </c>
+      <c r="M272" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N272">
+        <v>0.5</v>
+      </c>
+      <c r="O272">
+        <v>0.5</v>
+      </c>
+      <c r="P272">
+        <v>12.5</v>
+      </c>
+      <c r="Q272">
+        <v>4.5</v>
+      </c>
+      <c r="S272">
+        <v>5</v>
+      </c>
+      <c r="T272">
+        <v>2</v>
+      </c>
+      <c r="V272">
+        <v>30</v>
+      </c>
+      <c r="W272">
+        <v>10.5</v>
+      </c>
+      <c r="Z272">
         <v>2.5</v>
       </c>
-      <c r="V271">
+      <c r="AA272">
+        <v>1.5</v>
+      </c>
+      <c r="AB272">
+        <v>17.5</v>
+      </c>
+      <c r="AC272">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="273" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>170</v>
+      </c>
+      <c r="B273">
+        <v>2022</v>
+      </c>
+      <c r="C273">
+        <v>3</v>
+      </c>
+      <c r="D273">
+        <v>15</v>
+      </c>
+      <c r="E273">
+        <v>3</v>
+      </c>
+      <c r="F273">
+        <v>18</v>
+      </c>
+      <c r="G273" t="s">
+        <v>1</v>
+      </c>
+      <c r="H273" t="s">
+        <v>2</v>
+      </c>
+      <c r="I273" t="s">
+        <v>38</v>
+      </c>
+      <c r="J273">
+        <v>861</v>
+      </c>
+      <c r="K273">
+        <v>0</v>
+      </c>
+      <c r="L273" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M273" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N273">
+        <v>1.5</v>
+      </c>
+      <c r="O273">
+        <v>0.5</v>
+      </c>
+      <c r="P273">
+        <v>12</v>
+      </c>
+      <c r="Q273">
+        <v>3.5</v>
+      </c>
+      <c r="S273">
+        <v>6</v>
+      </c>
+      <c r="T273">
+        <v>2.5</v>
+      </c>
+      <c r="V273">
         <v>31</v>
       </c>
-      <c r="W271">
+      <c r="W273">
         <v>11</v>
       </c>
-      <c r="Z271">
+      <c r="Z273">
+        <v>3</v>
+      </c>
+      <c r="AA273">
+        <v>2</v>
+      </c>
+      <c r="AB273">
+        <v>15.5</v>
+      </c>
+      <c r="AC273">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="274" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>171</v>
+      </c>
+      <c r="B274">
+        <v>2022</v>
+      </c>
+      <c r="C274">
+        <v>3</v>
+      </c>
+      <c r="D274">
+        <v>15</v>
+      </c>
+      <c r="E274">
+        <v>3</v>
+      </c>
+      <c r="F274">
+        <v>18</v>
+      </c>
+      <c r="G274" t="s">
+        <v>33</v>
+      </c>
+      <c r="H274" t="s">
+        <v>21</v>
+      </c>
+      <c r="I274" t="s">
+        <v>38</v>
+      </c>
+      <c r="J274">
+        <v>1111</v>
+      </c>
+      <c r="K274">
+        <v>1</v>
+      </c>
+      <c r="L274" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M274" s="2">
+        <v>1</v>
+      </c>
+      <c r="N274">
+        <v>1</v>
+      </c>
+      <c r="O274" t="s">
+        <v>31</v>
+      </c>
+      <c r="P274">
+        <v>13</v>
+      </c>
+      <c r="Q274">
+        <v>4</v>
+      </c>
+      <c r="S274">
+        <v>5</v>
+      </c>
+      <c r="T274">
+        <v>3</v>
+      </c>
+      <c r="V274">
+        <v>29</v>
+      </c>
+      <c r="W274">
+        <v>12</v>
+      </c>
+      <c r="Z274">
+        <v>3</v>
+      </c>
+      <c r="AA274">
+        <v>2</v>
+      </c>
+      <c r="AB274">
+        <v>17</v>
+      </c>
+      <c r="AC274">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="275" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>172</v>
+      </c>
+      <c r="B275">
+        <v>2022</v>
+      </c>
+      <c r="C275">
+        <v>3</v>
+      </c>
+      <c r="D275">
+        <v>15</v>
+      </c>
+      <c r="E275">
+        <v>3</v>
+      </c>
+      <c r="F275">
+        <v>18</v>
+      </c>
+      <c r="G275" t="s">
+        <v>29</v>
+      </c>
+      <c r="H275" t="s">
+        <v>22</v>
+      </c>
+      <c r="I275" t="s">
+        <v>38</v>
+      </c>
+      <c r="J275">
+        <v>1079</v>
+      </c>
+      <c r="K275">
+        <v>1</v>
+      </c>
+      <c r="L275" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M275" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N275">
+        <v>0.5</v>
+      </c>
+      <c r="O275" t="s">
+        <v>24</v>
+      </c>
+      <c r="P275">
+        <v>13.5</v>
+      </c>
+      <c r="Q275">
+        <v>4.5</v>
+      </c>
+      <c r="S275">
+        <v>5</v>
+      </c>
+      <c r="T275">
+        <v>2</v>
+      </c>
+      <c r="V275">
+        <v>29</v>
+      </c>
+      <c r="W275">
+        <v>11</v>
+      </c>
+      <c r="Z275">
         <v>2.5</v>
       </c>
-      <c r="AA271">
-        <v>2</v>
-      </c>
-      <c r="AB271">
-        <v>15.5</v>
-      </c>
-      <c r="AC271">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="272" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L272" s="2"/>
-      <c r="M272" s="2"/>
-    </row>
-    <row r="273" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L273" s="2"/>
-      <c r="M273" s="2"/>
-    </row>
-    <row r="274" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L274" s="2"/>
-      <c r="M274" s="2"/>
-    </row>
-    <row r="275" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L275" s="2"/>
-      <c r="M275" s="2"/>
-    </row>
-    <row r="276" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="AA275">
+        <v>1.5</v>
+      </c>
+      <c r="AB275">
+        <v>17.5</v>
+      </c>
+      <c r="AC275">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="276" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L276" s="2"/>
       <c r="M276" s="2"/>
     </row>
-    <row r="277" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L277" s="2"/>
       <c r="M277" s="2"/>
     </row>
-    <row r="278" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L278" s="2"/>
       <c r="M278" s="2"/>
     </row>
-    <row r="279" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L279" s="2"/>
       <c r="M279" s="2"/>
     </row>
-    <row r="280" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L280" s="2"/>
       <c r="M280" s="2"/>
     </row>
-    <row r="281" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L281" s="2"/>
       <c r="M281" s="2"/>
     </row>
-    <row r="282" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L282" s="2"/>
       <c r="M282" s="2"/>
     </row>
-    <row r="283" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L283" s="2"/>
       <c r="M283" s="2"/>
     </row>
-    <row r="284" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L284" s="2"/>
       <c r="M284" s="2"/>
     </row>
-    <row r="285" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L285" s="2"/>
       <c r="M285" s="2"/>
     </row>
-    <row r="286" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L286" s="2"/>
       <c r="M286" s="2"/>
     </row>
-    <row r="287" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L287" s="2"/>
       <c r="M287" s="2"/>
     </row>
-    <row r="288" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L288" s="2"/>
       <c r="M288" s="2"/>
     </row>
@@ -23567,6 +23859,14 @@
     <row r="454" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L454" s="2"/>
       <c r="M454" s="2"/>
+    </row>
+    <row r="455" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L455" s="2"/>
+      <c r="M455" s="2"/>
+    </row>
+    <row r="456" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L456" s="2"/>
+      <c r="M456" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ ipsos rolling (3/19)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACD85EA-E2DF-164D-8D2C-741130ACA421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33D6BAE-C7A8-F043-AA10-EC8DC7E5FD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH456"/>
+  <dimension ref="A1:AH455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD273" sqref="AD273"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AC275" sqref="AC275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22933,61 +22933,61 @@
         <v>18</v>
       </c>
       <c r="G273" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H273" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I273" t="s">
         <v>38</v>
       </c>
       <c r="J273">
-        <v>861</v>
+        <v>1111</v>
       </c>
       <c r="K273">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L273" s="2">
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M273" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N273">
-        <v>1.5</v>
-      </c>
-      <c r="O273">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="O273" t="s">
+        <v>31</v>
       </c>
       <c r="P273">
+        <v>13</v>
+      </c>
+      <c r="Q273">
+        <v>4</v>
+      </c>
+      <c r="S273">
+        <v>5</v>
+      </c>
+      <c r="T273">
+        <v>3</v>
+      </c>
+      <c r="V273">
+        <v>29</v>
+      </c>
+      <c r="W273">
         <v>12</v>
       </c>
-      <c r="Q273">
-        <v>3.5</v>
-      </c>
-      <c r="S273">
-        <v>6</v>
-      </c>
-      <c r="T273">
-        <v>2.5</v>
-      </c>
-      <c r="V273">
-        <v>31</v>
-      </c>
-      <c r="W273">
+      <c r="Z273">
+        <v>3</v>
+      </c>
+      <c r="AA273">
+        <v>2</v>
+      </c>
+      <c r="AB273">
+        <v>17</v>
+      </c>
+      <c r="AC273">
         <v>11</v>
-      </c>
-      <c r="Z273">
-        <v>3</v>
-      </c>
-      <c r="AA273">
-        <v>2</v>
-      </c>
-      <c r="AB273">
-        <v>15.5</v>
-      </c>
-      <c r="AC273">
-        <v>11.5</v>
       </c>
     </row>
     <row r="274" spans="1:29" x14ac:dyDescent="0.2">
@@ -23010,16 +23010,16 @@
         <v>18</v>
       </c>
       <c r="G274" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H274" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I274" t="s">
         <v>38</v>
       </c>
       <c r="J274">
-        <v>1111</v>
+        <v>1079</v>
       </c>
       <c r="K274">
         <v>1</v>
@@ -23028,43 +23028,43 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="M274" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N274">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O274" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="P274">
-        <v>13</v>
+        <v>13.5</v>
       </c>
       <c r="Q274">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="S274">
         <v>5</v>
       </c>
       <c r="T274">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V274">
         <v>29</v>
       </c>
       <c r="W274">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z274">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AA274">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB274">
-        <v>17</v>
+        <v>17.5</v>
       </c>
       <c r="AC274">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="275" spans="1:29" x14ac:dyDescent="0.2">
@@ -23078,70 +23078,70 @@
         <v>3</v>
       </c>
       <c r="D275">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E275">
         <v>3</v>
       </c>
       <c r="F275">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G275" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="H275" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I275" t="s">
         <v>38</v>
       </c>
       <c r="J275">
-        <v>1079</v>
+        <v>911</v>
       </c>
       <c r="K275">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L275" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M275" s="2">
         <v>0.5</v>
       </c>
       <c r="N275">
-        <v>0.5</v>
-      </c>
-      <c r="O275" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="O275">
+        <v>0.5</v>
       </c>
       <c r="P275">
-        <v>13.5</v>
+        <v>13</v>
       </c>
       <c r="Q275">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="S275">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T275">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V275">
-        <v>29</v>
+        <v>30.5</v>
       </c>
       <c r="W275">
+        <v>10</v>
+      </c>
+      <c r="Z275">
+        <v>3</v>
+      </c>
+      <c r="AA275">
+        <v>2</v>
+      </c>
+      <c r="AB275">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="AC275">
         <v>11</v>
-      </c>
-      <c r="Z275">
-        <v>2.5</v>
-      </c>
-      <c r="AA275">
-        <v>1.5</v>
-      </c>
-      <c r="AB275">
-        <v>17.5</v>
-      </c>
-      <c r="AC275">
-        <v>13</v>
       </c>
     </row>
     <row r="276" spans="1:29" x14ac:dyDescent="0.2">
@@ -23863,10 +23863,6 @@
     <row r="455" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L455" s="2"/>
       <c r="M455" s="2"/>
-    </row>
-    <row r="456" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L456" s="2"/>
-      <c r="M456" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ ifop poll (3/19)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33D6BAE-C7A8-F043-AA10-EC8DC7E5FD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC93E12A-161F-8243-B744-059376D84784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -557,8 +557,8 @@
   <dimension ref="A1:AH455"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AC275" sqref="AC275"/>
+      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD276" sqref="AD276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23145,8 +23145,81 @@
       </c>
     </row>
     <row r="276" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L276" s="2"/>
-      <c r="M276" s="2"/>
+      <c r="A276">
+        <v>173</v>
+      </c>
+      <c r="B276">
+        <v>2022</v>
+      </c>
+      <c r="C276">
+        <v>3</v>
+      </c>
+      <c r="D276">
+        <v>17</v>
+      </c>
+      <c r="E276">
+        <v>3</v>
+      </c>
+      <c r="F276">
+        <v>18</v>
+      </c>
+      <c r="G276" t="s">
+        <v>29</v>
+      </c>
+      <c r="H276" t="s">
+        <v>22</v>
+      </c>
+      <c r="I276" t="s">
+        <v>47</v>
+      </c>
+      <c r="J276">
+        <v>1200</v>
+      </c>
+      <c r="K276">
+        <v>1</v>
+      </c>
+      <c r="L276" s="2">
+        <v>1</v>
+      </c>
+      <c r="M276" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N276">
+        <v>0.5</v>
+      </c>
+      <c r="O276" t="s">
+        <v>24</v>
+      </c>
+      <c r="P276">
+        <v>13</v>
+      </c>
+      <c r="Q276">
+        <v>4</v>
+      </c>
+      <c r="S276">
+        <v>5.5</v>
+      </c>
+      <c r="T276">
+        <v>2</v>
+      </c>
+      <c r="V276">
+        <v>29.5</v>
+      </c>
+      <c r="W276">
+        <v>11</v>
+      </c>
+      <c r="Z276">
+        <v>2</v>
+      </c>
+      <c r="AA276">
+        <v>2</v>
+      </c>
+      <c r="AB276">
+        <v>18.5</v>
+      </c>
+      <c r="AC276">
+        <v>12</v>
+      </c>
     </row>
     <row r="277" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L277" s="2"/>

</xml_diff>

<commit_message>
update w/ rollings + ow poll (3/21)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC93E12A-161F-8243-B744-059376D84784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15BACAD-F279-4E4F-8B05-8104A6932AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH455"/>
+  <dimension ref="A1:AH453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD276" sqref="AD276"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A255" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AC277" sqref="AC277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22924,58 +22924,58 @@
         <v>3</v>
       </c>
       <c r="D273">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E273">
         <v>3</v>
       </c>
       <c r="F273">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G273" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="H273" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I273" t="s">
         <v>38</v>
       </c>
       <c r="J273">
-        <v>1111</v>
+        <v>911</v>
       </c>
       <c r="K273">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L273" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M273" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N273">
         <v>1</v>
       </c>
-      <c r="O273" t="s">
-        <v>31</v>
+      <c r="O273">
+        <v>0.5</v>
       </c>
       <c r="P273">
         <v>13</v>
       </c>
       <c r="Q273">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S273">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T273">
         <v>3</v>
       </c>
       <c r="V273">
-        <v>29</v>
+        <v>30.5</v>
       </c>
       <c r="W273">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Z273">
         <v>3</v>
@@ -22984,7 +22984,7 @@
         <v>2</v>
       </c>
       <c r="AB273">
-        <v>17</v>
+        <v>16.5</v>
       </c>
       <c r="AC273">
         <v>11</v>
@@ -23001,7 +23001,7 @@
         <v>3</v>
       </c>
       <c r="D274">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E274">
         <v>3</v>
@@ -23016,16 +23016,16 @@
         <v>22</v>
       </c>
       <c r="I274" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J274">
-        <v>1079</v>
+        <v>1200</v>
       </c>
       <c r="K274">
         <v>1</v>
       </c>
       <c r="L274" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M274" s="2">
         <v>0.5</v>
@@ -23037,34 +23037,34 @@
         <v>24</v>
       </c>
       <c r="P274">
-        <v>13.5</v>
+        <v>13</v>
       </c>
       <c r="Q274">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="S274">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="T274">
         <v>2</v>
       </c>
       <c r="V274">
-        <v>29</v>
+        <v>29.5</v>
       </c>
       <c r="W274">
         <v>11</v>
       </c>
       <c r="Z274">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AA274">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB274">
-        <v>17.5</v>
+        <v>18.5</v>
       </c>
       <c r="AC274">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="275" spans="1:29" x14ac:dyDescent="0.2">
@@ -23078,70 +23078,70 @@
         <v>3</v>
       </c>
       <c r="D275">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E275">
         <v>3</v>
       </c>
       <c r="F275">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G275" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H275" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I275" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J275">
-        <v>911</v>
+        <v>700</v>
       </c>
       <c r="K275">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L275" s="2">
         <v>1</v>
       </c>
       <c r="M275" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N275">
         <v>1</v>
       </c>
       <c r="O275">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P275">
         <v>13</v>
       </c>
       <c r="Q275">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S275">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T275">
         <v>3</v>
       </c>
       <c r="V275">
-        <v>30.5</v>
+        <v>29</v>
       </c>
       <c r="W275">
+        <v>13</v>
+      </c>
+      <c r="Z275">
+        <v>3</v>
+      </c>
+      <c r="AA275">
+        <v>1</v>
+      </c>
+      <c r="AB275">
+        <v>17</v>
+      </c>
+      <c r="AC275">
         <v>10</v>
-      </c>
-      <c r="Z275">
-        <v>3</v>
-      </c>
-      <c r="AA275">
-        <v>2</v>
-      </c>
-      <c r="AB275">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="AC275">
-        <v>11</v>
       </c>
     </row>
     <row r="276" spans="1:29" x14ac:dyDescent="0.2">
@@ -23161,19 +23161,19 @@
         <v>3</v>
       </c>
       <c r="F276">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G276" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H276" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I276" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J276">
-        <v>1200</v>
+        <v>1111</v>
       </c>
       <c r="K276">
         <v>1</v>
@@ -23182,13 +23182,13 @@
         <v>1</v>
       </c>
       <c r="M276" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N276">
-        <v>0.5</v>
-      </c>
-      <c r="O276" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="O276">
+        <v>1</v>
       </c>
       <c r="P276">
         <v>13</v>
@@ -23197,37 +23197,183 @@
         <v>4</v>
       </c>
       <c r="S276">
+        <v>5</v>
+      </c>
+      <c r="T276">
+        <v>3</v>
+      </c>
+      <c r="V276">
+        <v>29</v>
+      </c>
+      <c r="W276">
+        <v>13</v>
+      </c>
+      <c r="Z276">
+        <v>2</v>
+      </c>
+      <c r="AA276">
+        <v>2</v>
+      </c>
+      <c r="AB276">
+        <v>18</v>
+      </c>
+      <c r="AC276">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="277" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>174</v>
+      </c>
+      <c r="B277">
+        <v>2022</v>
+      </c>
+      <c r="C277">
+        <v>3</v>
+      </c>
+      <c r="D277">
+        <v>17</v>
+      </c>
+      <c r="E277">
+        <v>3</v>
+      </c>
+      <c r="F277">
+        <v>21</v>
+      </c>
+      <c r="G277" t="s">
+        <v>29</v>
+      </c>
+      <c r="H277" t="s">
+        <v>22</v>
+      </c>
+      <c r="I277" t="s">
+        <v>38</v>
+      </c>
+      <c r="J277">
+        <v>1079</v>
+      </c>
+      <c r="K277">
+        <v>1</v>
+      </c>
+      <c r="L277" s="2">
+        <v>1</v>
+      </c>
+      <c r="M277" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N277">
+        <v>0.5</v>
+      </c>
+      <c r="O277" t="s">
+        <v>24</v>
+      </c>
+      <c r="P277">
+        <v>14</v>
+      </c>
+      <c r="Q277">
+        <v>4</v>
+      </c>
+      <c r="S277">
         <v>5.5</v>
       </c>
-      <c r="T276">
-        <v>2</v>
-      </c>
-      <c r="V276">
-        <v>29.5</v>
-      </c>
-      <c r="W276">
-        <v>11</v>
-      </c>
-      <c r="Z276">
-        <v>2</v>
-      </c>
-      <c r="AA276">
-        <v>2</v>
-      </c>
-      <c r="AB276">
+      <c r="T277">
+        <v>2</v>
+      </c>
+      <c r="V277">
+        <v>28</v>
+      </c>
+      <c r="W277">
+        <v>10.5</v>
+      </c>
+      <c r="Z277">
+        <v>3</v>
+      </c>
+      <c r="AA277">
+        <v>1.5</v>
+      </c>
+      <c r="AB277">
         <v>18.5</v>
       </c>
-      <c r="AC276">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="277" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L277" s="2"/>
-      <c r="M277" s="2"/>
+      <c r="AC277">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="278" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L278" s="2"/>
-      <c r="M278" s="2"/>
+      <c r="A278">
+        <v>175</v>
+      </c>
+      <c r="B278">
+        <v>2022</v>
+      </c>
+      <c r="C278">
+        <v>3</v>
+      </c>
+      <c r="D278">
+        <v>17</v>
+      </c>
+      <c r="E278">
+        <v>3</v>
+      </c>
+      <c r="F278">
+        <v>21</v>
+      </c>
+      <c r="G278" t="s">
+        <v>1</v>
+      </c>
+      <c r="H278" t="s">
+        <v>2</v>
+      </c>
+      <c r="I278" t="s">
+        <v>38</v>
+      </c>
+      <c r="J278">
+        <v>919</v>
+      </c>
+      <c r="K278">
+        <v>0</v>
+      </c>
+      <c r="L278" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M278" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N278">
+        <v>1</v>
+      </c>
+      <c r="O278">
+        <v>0.5</v>
+      </c>
+      <c r="P278">
+        <v>13</v>
+      </c>
+      <c r="Q278">
+        <v>3.5</v>
+      </c>
+      <c r="S278">
+        <v>6.5</v>
+      </c>
+      <c r="T278">
+        <v>3</v>
+      </c>
+      <c r="V278">
+        <v>30.5</v>
+      </c>
+      <c r="W278">
+        <v>10</v>
+      </c>
+      <c r="Z278">
+        <v>3</v>
+      </c>
+      <c r="AA278">
+        <v>2</v>
+      </c>
+      <c r="AB278">
+        <v>17</v>
+      </c>
+      <c r="AC278">
+        <v>10</v>
+      </c>
     </row>
     <row r="279" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L279" s="2"/>
@@ -23928,14 +24074,6 @@
     <row r="453" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L453" s="2"/>
       <c r="M453" s="2"/>
-    </row>
-    <row r="454" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L454" s="2"/>
-      <c r="M454" s="2"/>
-    </row>
-    <row r="455" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L455" s="2"/>
-      <c r="M455" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ rollings + elabe and cluster17 poll (3/22)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15BACAD-F279-4E4F-8B05-8104A6932AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0035828-955E-E141-8DB6-A8BC3DFA6A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25680" yWindow="2640" windowWidth="25340" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="29720" yWindow="500" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH453"/>
+  <dimension ref="A1:AH456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A255" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AC277" sqref="AC277"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD283" sqref="AD283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22634,10 +22634,10 @@
         <v>47</v>
       </c>
       <c r="J269">
-        <v>700</v>
+        <v>719</v>
       </c>
       <c r="K269">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L269" s="2">
         <v>1</v>
@@ -22788,10 +22788,10 @@
         <v>38</v>
       </c>
       <c r="J271">
-        <v>1111</v>
+        <v>1067</v>
       </c>
       <c r="K271">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L271" s="2">
         <v>1</v>
@@ -22865,10 +22865,10 @@
         <v>38</v>
       </c>
       <c r="J272">
-        <v>1079</v>
+        <v>1072</v>
       </c>
       <c r="K272">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L272" s="2">
         <v>1</v>
@@ -22930,19 +22930,19 @@
         <v>3</v>
       </c>
       <c r="F273">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G273" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H273" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I273" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J273">
-        <v>911</v>
+        <v>681</v>
       </c>
       <c r="K273">
         <v>0</v>
@@ -22951,31 +22951,31 @@
         <v>1</v>
       </c>
       <c r="M273" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N273">
         <v>1</v>
       </c>
       <c r="O273">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P273">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q273">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S273">
         <v>6</v>
       </c>
       <c r="T273">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V273">
-        <v>30.5</v>
+        <v>29</v>
       </c>
       <c r="W273">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Z273">
         <v>3</v>
@@ -22984,7 +22984,7 @@
         <v>2</v>
       </c>
       <c r="AB273">
-        <v>16.5</v>
+        <v>18</v>
       </c>
       <c r="AC273">
         <v>11</v>
@@ -23078,70 +23078,70 @@
         <v>3</v>
       </c>
       <c r="D275">
+        <v>16</v>
+      </c>
+      <c r="E275">
+        <v>3</v>
+      </c>
+      <c r="F275">
         <v>19</v>
       </c>
-      <c r="E275">
-        <v>3</v>
-      </c>
-      <c r="F275">
-        <v>20</v>
-      </c>
       <c r="G275" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="H275" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I275" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J275">
-        <v>700</v>
+        <v>911</v>
       </c>
       <c r="K275">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L275" s="2">
         <v>1</v>
       </c>
       <c r="M275" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N275">
         <v>1</v>
       </c>
       <c r="O275">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P275">
         <v>13</v>
       </c>
       <c r="Q275">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S275">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T275">
         <v>3</v>
       </c>
       <c r="V275">
-        <v>29</v>
+        <v>30.5</v>
       </c>
       <c r="W275">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="Z275">
         <v>3</v>
       </c>
       <c r="AA275">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB275">
-        <v>17</v>
+        <v>16.5</v>
       </c>
       <c r="AC275">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="276" spans="1:29" x14ac:dyDescent="0.2">
@@ -23155,70 +23155,70 @@
         <v>3</v>
       </c>
       <c r="D276">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E276">
         <v>3</v>
       </c>
       <c r="F276">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G276" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H276" t="s">
         <v>21</v>
       </c>
       <c r="I276" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J276">
-        <v>1111</v>
+        <v>2382</v>
       </c>
       <c r="K276">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L276" s="2">
         <v>1</v>
       </c>
       <c r="M276" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N276">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O276">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="P276">
-        <v>13</v>
+        <v>14.5</v>
       </c>
       <c r="Q276">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S276">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="T276">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="V276">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W276">
-        <v>13</v>
+        <v>10.5</v>
       </c>
       <c r="Z276">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA276">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB276">
-        <v>18</v>
+        <v>16.5</v>
       </c>
       <c r="AC276">
-        <v>9</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="277" spans="1:29" x14ac:dyDescent="0.2">
@@ -23232,70 +23232,70 @@
         <v>3</v>
       </c>
       <c r="D277">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E277">
         <v>3</v>
       </c>
       <c r="F277">
+        <v>20</v>
+      </c>
+      <c r="G277" t="s">
+        <v>33</v>
+      </c>
+      <c r="H277" t="s">
         <v>21</v>
       </c>
-      <c r="G277" t="s">
-        <v>29</v>
-      </c>
-      <c r="H277" t="s">
-        <v>22</v>
-      </c>
       <c r="I277" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J277">
-        <v>1079</v>
+        <v>760</v>
       </c>
       <c r="K277">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L277" s="2">
         <v>1</v>
       </c>
       <c r="M277" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N277">
-        <v>0.5</v>
-      </c>
-      <c r="O277" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="O277">
+        <v>1</v>
       </c>
       <c r="P277">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q277">
         <v>4</v>
       </c>
       <c r="S277">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="T277">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V277">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W277">
-        <v>10.5</v>
+        <v>13</v>
       </c>
       <c r="Z277">
         <v>3</v>
       </c>
       <c r="AA277">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AB277">
-        <v>18.5</v>
+        <v>17</v>
       </c>
       <c r="AC277">
-        <v>12.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="278" spans="1:29" x14ac:dyDescent="0.2">
@@ -23309,7 +23309,7 @@
         <v>3</v>
       </c>
       <c r="D278">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E278">
         <v>3</v>
@@ -23318,82 +23318,447 @@
         <v>21</v>
       </c>
       <c r="G278" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H278" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I278" t="s">
         <v>38</v>
       </c>
       <c r="J278">
-        <v>919</v>
+        <v>1135</v>
       </c>
       <c r="K278">
         <v>0</v>
       </c>
       <c r="L278" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M278" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N278">
         <v>1</v>
       </c>
       <c r="O278">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P278">
         <v>13</v>
       </c>
       <c r="Q278">
+        <v>4</v>
+      </c>
+      <c r="S278">
+        <v>5</v>
+      </c>
+      <c r="T278">
+        <v>3</v>
+      </c>
+      <c r="V278">
+        <v>29</v>
+      </c>
+      <c r="W278">
+        <v>13</v>
+      </c>
+      <c r="Z278">
+        <v>2</v>
+      </c>
+      <c r="AA278">
+        <v>2</v>
+      </c>
+      <c r="AB278">
+        <v>18</v>
+      </c>
+      <c r="AC278">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="279" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>176</v>
+      </c>
+      <c r="B279">
+        <v>2022</v>
+      </c>
+      <c r="C279">
+        <v>3</v>
+      </c>
+      <c r="D279">
+        <v>17</v>
+      </c>
+      <c r="E279">
+        <v>3</v>
+      </c>
+      <c r="F279">
+        <v>21</v>
+      </c>
+      <c r="G279" t="s">
+        <v>29</v>
+      </c>
+      <c r="H279" t="s">
+        <v>22</v>
+      </c>
+      <c r="I279" t="s">
+        <v>38</v>
+      </c>
+      <c r="J279">
+        <v>1051</v>
+      </c>
+      <c r="K279">
+        <v>1</v>
+      </c>
+      <c r="L279" s="2">
+        <v>1</v>
+      </c>
+      <c r="M279" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N279">
+        <v>0.5</v>
+      </c>
+      <c r="O279" t="s">
+        <v>24</v>
+      </c>
+      <c r="P279">
+        <v>14</v>
+      </c>
+      <c r="Q279">
+        <v>4</v>
+      </c>
+      <c r="S279">
+        <v>5.5</v>
+      </c>
+      <c r="T279">
+        <v>2</v>
+      </c>
+      <c r="V279">
+        <v>28</v>
+      </c>
+      <c r="W279">
+        <v>10.5</v>
+      </c>
+      <c r="Z279">
+        <v>3</v>
+      </c>
+      <c r="AA279">
+        <v>1.5</v>
+      </c>
+      <c r="AB279">
+        <v>18.5</v>
+      </c>
+      <c r="AC279">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="280" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>177</v>
+      </c>
+      <c r="B280">
+        <v>2022</v>
+      </c>
+      <c r="C280">
+        <v>3</v>
+      </c>
+      <c r="D280">
+        <v>20</v>
+      </c>
+      <c r="E280">
+        <v>3</v>
+      </c>
+      <c r="F280">
+        <v>21</v>
+      </c>
+      <c r="G280" t="s">
+        <v>30</v>
+      </c>
+      <c r="H280" t="s">
+        <v>21</v>
+      </c>
+      <c r="I280" t="s">
+        <v>47</v>
+      </c>
+      <c r="J280">
+        <v>966</v>
+      </c>
+      <c r="K280">
+        <v>0</v>
+      </c>
+      <c r="L280" s="2">
+        <v>1</v>
+      </c>
+      <c r="M280" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N280">
+        <v>1.5</v>
+      </c>
+      <c r="O280">
+        <v>0.5</v>
+      </c>
+      <c r="P280">
+        <v>15</v>
+      </c>
+      <c r="Q280">
         <v>3.5</v>
       </c>
-      <c r="S278">
-        <v>6.5</v>
-      </c>
-      <c r="T278">
-        <v>3</v>
-      </c>
-      <c r="V278">
-        <v>30.5</v>
-      </c>
-      <c r="W278">
+      <c r="S280">
+        <v>4.5</v>
+      </c>
+      <c r="T280">
+        <v>1.5</v>
+      </c>
+      <c r="V280">
+        <v>27.5</v>
+      </c>
+      <c r="W280">
         <v>10</v>
       </c>
-      <c r="Z278">
-        <v>3</v>
-      </c>
-      <c r="AA278">
-        <v>2</v>
-      </c>
-      <c r="AB278">
-        <v>17</v>
-      </c>
-      <c r="AC278">
+      <c r="Z280">
+        <v>3</v>
+      </c>
+      <c r="AA280">
+        <v>3</v>
+      </c>
+      <c r="AB280">
+        <v>20</v>
+      </c>
+      <c r="AC280">
         <v>10</v>
       </c>
     </row>
-    <row r="279" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L279" s="2"/>
-      <c r="M279" s="2"/>
-    </row>
-    <row r="280" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L280" s="2"/>
-      <c r="M280" s="2"/>
-    </row>
     <row r="281" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L281" s="2"/>
-      <c r="M281" s="2"/>
+      <c r="A281">
+        <v>178</v>
+      </c>
+      <c r="B281">
+        <v>2022</v>
+      </c>
+      <c r="C281">
+        <v>3</v>
+      </c>
+      <c r="D281">
+        <v>18</v>
+      </c>
+      <c r="E281">
+        <v>3</v>
+      </c>
+      <c r="F281">
+        <v>22</v>
+      </c>
+      <c r="G281" t="s">
+        <v>1</v>
+      </c>
+      <c r="H281" t="s">
+        <v>2</v>
+      </c>
+      <c r="I281" t="s">
+        <v>38</v>
+      </c>
+      <c r="J281">
+        <v>927</v>
+      </c>
+      <c r="K281">
+        <v>0</v>
+      </c>
+      <c r="L281" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M281" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N281">
+        <v>1</v>
+      </c>
+      <c r="O281">
+        <v>1</v>
+      </c>
+      <c r="P281">
+        <v>13</v>
+      </c>
+      <c r="Q281">
+        <v>4</v>
+      </c>
+      <c r="S281">
+        <v>7</v>
+      </c>
+      <c r="T281">
+        <v>2.5</v>
+      </c>
+      <c r="V281">
+        <v>29.5</v>
+      </c>
+      <c r="W281">
+        <v>9.5</v>
+      </c>
+      <c r="Z281">
+        <v>2.5</v>
+      </c>
+      <c r="AA281">
+        <v>1.5</v>
+      </c>
+      <c r="AB281">
+        <v>17.5</v>
+      </c>
+      <c r="AC281">
+        <v>11</v>
+      </c>
     </row>
     <row r="282" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L282" s="2"/>
-      <c r="M282" s="2"/>
+      <c r="A282">
+        <v>179</v>
+      </c>
+      <c r="B282">
+        <v>2022</v>
+      </c>
+      <c r="C282">
+        <v>3</v>
+      </c>
+      <c r="D282">
+        <v>19</v>
+      </c>
+      <c r="E282">
+        <v>3</v>
+      </c>
+      <c r="F282">
+        <v>22</v>
+      </c>
+      <c r="G282" t="s">
+        <v>33</v>
+      </c>
+      <c r="H282" t="s">
+        <v>21</v>
+      </c>
+      <c r="I282" t="s">
+        <v>38</v>
+      </c>
+      <c r="J282">
+        <v>1135</v>
+      </c>
+      <c r="K282">
+        <v>1</v>
+      </c>
+      <c r="L282" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M282" s="2">
+        <v>1</v>
+      </c>
+      <c r="N282">
+        <v>2</v>
+      </c>
+      <c r="O282">
+        <v>1</v>
+      </c>
+      <c r="P282">
+        <v>14</v>
+      </c>
+      <c r="Q282">
+        <v>3</v>
+      </c>
+      <c r="S282">
+        <v>5</v>
+      </c>
+      <c r="T282">
+        <v>2</v>
+      </c>
+      <c r="V282">
+        <v>29</v>
+      </c>
+      <c r="W282">
+        <v>12</v>
+      </c>
+      <c r="Z282">
+        <v>2</v>
+      </c>
+      <c r="AA282">
+        <v>2</v>
+      </c>
+      <c r="AB282">
+        <v>19</v>
+      </c>
+      <c r="AC282">
+        <v>9</v>
+      </c>
     </row>
     <row r="283" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L283" s="2"/>
-      <c r="M283" s="2"/>
+      <c r="A283">
+        <v>180</v>
+      </c>
+      <c r="B283">
+        <v>2022</v>
+      </c>
+      <c r="C283">
+        <v>3</v>
+      </c>
+      <c r="D283">
+        <v>18</v>
+      </c>
+      <c r="E283">
+        <v>3</v>
+      </c>
+      <c r="F283">
+        <v>22</v>
+      </c>
+      <c r="G283" t="s">
+        <v>29</v>
+      </c>
+      <c r="H283" t="s">
+        <v>22</v>
+      </c>
+      <c r="I283" t="s">
+        <v>38</v>
+      </c>
+      <c r="J283">
+        <v>1051</v>
+      </c>
+      <c r="K283">
+        <v>1</v>
+      </c>
+      <c r="L283" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M283" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N283">
+        <v>0.5</v>
+      </c>
+      <c r="O283">
+        <v>0.5</v>
+      </c>
+      <c r="P283">
+        <v>13.5</v>
+      </c>
+      <c r="Q283">
+        <v>4</v>
+      </c>
+      <c r="S283">
+        <v>5.5</v>
+      </c>
+      <c r="T283">
+        <v>2</v>
+      </c>
+      <c r="V283">
+        <v>28</v>
+      </c>
+      <c r="W283">
+        <v>10.5</v>
+      </c>
+      <c r="Z283">
+        <v>2.5</v>
+      </c>
+      <c r="AA283">
+        <v>1</v>
+      </c>
+      <c r="AB283">
+        <v>19.5</v>
+      </c>
+      <c r="AC283">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="284" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L284" s="2"/>
@@ -24074,6 +24439,18 @@
     <row r="453" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L453" s="2"/>
       <c r="M453" s="2"/>
+    </row>
+    <row r="454" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L454" s="2"/>
+      <c r="M454" s="2"/>
+    </row>
+    <row r="455" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L455" s="2"/>
+      <c r="M455" s="2"/>
+    </row>
+    <row r="456" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L456" s="2"/>
+      <c r="M456" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ harris poll + rollings (3/23)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0035828-955E-E141-8DB6-A8BC3DFA6A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8F7C67-7D8E-5548-A644-9BF7FF279DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29720" yWindow="500" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="28820" yWindow="12040" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH456"/>
+  <dimension ref="A1:AH458"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD283" sqref="AD283"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AA285" sqref="AA285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23463,7 +23463,7 @@
         <v>3</v>
       </c>
       <c r="D280">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E280">
         <v>3</v>
@@ -23472,19 +23472,19 @@
         <v>21</v>
       </c>
       <c r="G280" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H280" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I280" t="s">
         <v>47</v>
       </c>
       <c r="J280">
-        <v>966</v>
+        <v>1697</v>
       </c>
       <c r="K280">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L280" s="2">
         <v>1</v>
@@ -23493,40 +23493,40 @@
         <v>0.5</v>
       </c>
       <c r="N280">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O280">
         <v>0.5</v>
       </c>
       <c r="P280">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q280">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S280">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T280">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="V280">
-        <v>27.5</v>
+        <v>29.5</v>
       </c>
       <c r="W280">
         <v>10</v>
       </c>
       <c r="Z280">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA280">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB280">
-        <v>20</v>
+        <v>19.5</v>
       </c>
       <c r="AC280">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="281" spans="1:29" x14ac:dyDescent="0.2">
@@ -23540,70 +23540,70 @@
         <v>3</v>
       </c>
       <c r="D281">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E281">
         <v>3</v>
       </c>
       <c r="F281">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G281" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="H281" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I281" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J281">
-        <v>927</v>
+        <v>966</v>
       </c>
       <c r="K281">
         <v>0</v>
       </c>
       <c r="L281" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M281" s="2">
         <v>0.5</v>
       </c>
       <c r="N281">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O281">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P281">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Q281">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S281">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="T281">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="V281">
-        <v>29.5</v>
+        <v>27.5</v>
       </c>
       <c r="W281">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="Z281">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AA281">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AB281">
-        <v>17.5</v>
+        <v>20</v>
       </c>
       <c r="AC281">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="282" spans="1:29" x14ac:dyDescent="0.2">
@@ -23617,13 +23617,13 @@
         <v>3</v>
       </c>
       <c r="D282">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E282">
         <v>3</v>
       </c>
       <c r="F282">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G282" t="s">
         <v>33</v>
@@ -23632,16 +23632,16 @@
         <v>21</v>
       </c>
       <c r="I282" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J282">
-        <v>1135</v>
+        <v>738</v>
       </c>
       <c r="K282">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L282" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M282" s="2">
         <v>1</v>
@@ -23677,10 +23677,10 @@
         <v>2</v>
       </c>
       <c r="AB282">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AC282">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="283" spans="1:29" x14ac:dyDescent="0.2">
@@ -23694,79 +23694,225 @@
         <v>3</v>
       </c>
       <c r="D283">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E283">
         <v>3</v>
       </c>
       <c r="F283">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G283" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="H283" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I283" t="s">
         <v>38</v>
       </c>
       <c r="J283">
-        <v>1051</v>
+        <v>891</v>
       </c>
       <c r="K283">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L283" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M283" s="2">
         <v>0.5</v>
       </c>
       <c r="N283">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O283">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P283">
-        <v>13.5</v>
+        <v>12.5</v>
       </c>
       <c r="Q283">
         <v>4</v>
       </c>
       <c r="S283">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="T283">
         <v>2</v>
       </c>
       <c r="V283">
-        <v>28</v>
+        <v>29.5</v>
       </c>
       <c r="W283">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="Z283">
         <v>2.5</v>
       </c>
       <c r="AA283">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AB283">
-        <v>19.5</v>
+        <v>18.5</v>
       </c>
       <c r="AC283">
-        <v>12.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="284" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L284" s="2"/>
-      <c r="M284" s="2"/>
+      <c r="A284">
+        <v>181</v>
+      </c>
+      <c r="B284">
+        <v>2022</v>
+      </c>
+      <c r="C284">
+        <v>3</v>
+      </c>
+      <c r="D284">
+        <v>20</v>
+      </c>
+      <c r="E284">
+        <v>3</v>
+      </c>
+      <c r="F284">
+        <v>23</v>
+      </c>
+      <c r="G284" t="s">
+        <v>33</v>
+      </c>
+      <c r="H284" t="s">
+        <v>21</v>
+      </c>
+      <c r="I284" t="s">
+        <v>38</v>
+      </c>
+      <c r="J284">
+        <v>1107</v>
+      </c>
+      <c r="K284">
+        <v>1</v>
+      </c>
+      <c r="L284" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M284" s="2">
+        <v>1</v>
+      </c>
+      <c r="N284">
+        <v>2</v>
+      </c>
+      <c r="O284">
+        <v>1</v>
+      </c>
+      <c r="P284">
+        <v>14</v>
+      </c>
+      <c r="Q284">
+        <v>3</v>
+      </c>
+      <c r="S284">
+        <v>6</v>
+      </c>
+      <c r="T284">
+        <v>2</v>
+      </c>
+      <c r="V284">
+        <v>28</v>
+      </c>
+      <c r="W284">
+        <v>11</v>
+      </c>
+      <c r="Z284">
+        <v>2</v>
+      </c>
+      <c r="AA284">
+        <v>2</v>
+      </c>
+      <c r="AB284">
+        <v>20</v>
+      </c>
+      <c r="AC284">
+        <v>9</v>
+      </c>
     </row>
     <row r="285" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L285" s="2"/>
-      <c r="M285" s="2"/>
+      <c r="A285">
+        <v>182</v>
+      </c>
+      <c r="B285">
+        <v>2022</v>
+      </c>
+      <c r="C285">
+        <v>3</v>
+      </c>
+      <c r="D285">
+        <v>20</v>
+      </c>
+      <c r="E285">
+        <v>3</v>
+      </c>
+      <c r="F285">
+        <v>23</v>
+      </c>
+      <c r="G285" t="s">
+        <v>29</v>
+      </c>
+      <c r="H285" t="s">
+        <v>22</v>
+      </c>
+      <c r="I285" t="s">
+        <v>38</v>
+      </c>
+      <c r="J285">
+        <v>1079</v>
+      </c>
+      <c r="K285">
+        <v>1</v>
+      </c>
+      <c r="L285" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M285" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N285">
+        <v>0.5</v>
+      </c>
+      <c r="O285">
+        <v>0.5</v>
+      </c>
+      <c r="P285">
+        <v>14</v>
+      </c>
+      <c r="Q285">
+        <v>3.5</v>
+      </c>
+      <c r="S285">
+        <v>5</v>
+      </c>
+      <c r="T285">
+        <v>2</v>
+      </c>
+      <c r="V285">
+        <v>28</v>
+      </c>
+      <c r="W285">
+        <v>11</v>
+      </c>
+      <c r="Z285">
+        <v>2.5</v>
+      </c>
+      <c r="AA285">
+        <v>1</v>
+      </c>
+      <c r="AB285">
+        <v>20</v>
+      </c>
+      <c r="AC285">
+        <v>12</v>
+      </c>
     </row>
     <row r="286" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L286" s="2"/>
@@ -24451,6 +24597,14 @@
     <row r="456" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L456" s="2"/>
       <c r="M456" s="2"/>
+    </row>
+    <row r="457" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L457" s="2"/>
+      <c r="M457" s="2"/>
+    </row>
+    <row r="458" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L458" s="2"/>
+      <c r="M458" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ rollings + kantar poll (3/24)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8F7C67-7D8E-5548-A644-9BF7FF279DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEEA37B-FE74-BC43-AEB3-B25496EFC46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="12040" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="28800" yWindow="12040" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH458"/>
+  <dimension ref="A1:AH459"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AA285" sqref="AA285"/>
+      <selection pane="bottomLeft" activeCell="A286" sqref="A286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23694,7 +23694,7 @@
         <v>3</v>
       </c>
       <c r="D283">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E283">
         <v>3</v>
@@ -23703,16 +23703,16 @@
         <v>23</v>
       </c>
       <c r="G283" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="H283" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I283" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J283">
-        <v>891</v>
+        <v>1013</v>
       </c>
       <c r="K283">
         <v>0</v>
@@ -23730,31 +23730,31 @@
         <v>1</v>
       </c>
       <c r="P283">
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="Q283">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S283">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="T283">
         <v>2</v>
       </c>
       <c r="V283">
-        <v>29.5</v>
+        <v>29</v>
       </c>
       <c r="W283">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="Z283">
+        <v>2</v>
+      </c>
+      <c r="AA283">
         <v>2.5</v>
       </c>
-      <c r="AA283">
-        <v>1.5</v>
-      </c>
       <c r="AB283">
-        <v>18.5</v>
+        <v>20</v>
       </c>
       <c r="AC283">
         <v>11</v>
@@ -23780,61 +23780,61 @@
         <v>23</v>
       </c>
       <c r="G284" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="H284" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I284" t="s">
         <v>38</v>
       </c>
       <c r="J284">
-        <v>1107</v>
+        <v>891</v>
       </c>
       <c r="K284">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L284" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M284" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N284">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O284">
         <v>1</v>
       </c>
       <c r="P284">
-        <v>14</v>
+        <v>12.5</v>
       </c>
       <c r="Q284">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S284">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T284">
         <v>2</v>
       </c>
       <c r="V284">
-        <v>28</v>
+        <v>29.5</v>
       </c>
       <c r="W284">
+        <v>9.5</v>
+      </c>
+      <c r="Z284">
+        <v>2.5</v>
+      </c>
+      <c r="AA284">
+        <v>1.5</v>
+      </c>
+      <c r="AB284">
+        <v>18.5</v>
+      </c>
+      <c r="AC284">
         <v>11</v>
-      </c>
-      <c r="Z284">
-        <v>2</v>
-      </c>
-      <c r="AA284">
-        <v>2</v>
-      </c>
-      <c r="AB284">
-        <v>20</v>
-      </c>
-      <c r="AC284">
-        <v>9</v>
       </c>
     </row>
     <row r="285" spans="1:29" x14ac:dyDescent="0.2">
@@ -23848,46 +23848,46 @@
         <v>3</v>
       </c>
       <c r="D285">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E285">
         <v>3</v>
       </c>
       <c r="F285">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G285" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H285" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I285" t="s">
         <v>38</v>
       </c>
       <c r="J285">
-        <v>1079</v>
+        <v>1107</v>
       </c>
       <c r="K285">
         <v>1</v>
       </c>
       <c r="L285" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M285" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N285">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O285">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P285">
         <v>14</v>
       </c>
       <c r="Q285">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S285">
         <v>5</v>
@@ -23899,10 +23899,10 @@
         <v>28</v>
       </c>
       <c r="W285">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Z285">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AA285">
         <v>1</v>
@@ -23911,16 +23911,162 @@
         <v>20</v>
       </c>
       <c r="AC285">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="286" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L286" s="2"/>
-      <c r="M286" s="2"/>
+      <c r="A286">
+        <v>183</v>
+      </c>
+      <c r="B286">
+        <v>2022</v>
+      </c>
+      <c r="C286">
+        <v>3</v>
+      </c>
+      <c r="D286">
+        <v>21</v>
+      </c>
+      <c r="E286">
+        <v>3</v>
+      </c>
+      <c r="F286">
+        <v>24</v>
+      </c>
+      <c r="G286" t="s">
+        <v>29</v>
+      </c>
+      <c r="H286" t="s">
+        <v>22</v>
+      </c>
+      <c r="I286" t="s">
+        <v>38</v>
+      </c>
+      <c r="J286">
+        <v>1079</v>
+      </c>
+      <c r="K286">
+        <v>1</v>
+      </c>
+      <c r="L286" s="2">
+        <v>1</v>
+      </c>
+      <c r="M286" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N286">
+        <v>0.5</v>
+      </c>
+      <c r="O286">
+        <v>0.5</v>
+      </c>
+      <c r="P286">
+        <v>14</v>
+      </c>
+      <c r="Q286">
+        <v>3.5</v>
+      </c>
+      <c r="S286">
+        <v>4.5</v>
+      </c>
+      <c r="T286">
+        <v>2</v>
+      </c>
+      <c r="V286">
+        <v>28.5</v>
+      </c>
+      <c r="W286">
+        <v>11.5</v>
+      </c>
+      <c r="Z286">
+        <v>2</v>
+      </c>
+      <c r="AA286">
+        <v>1.5</v>
+      </c>
+      <c r="AB286">
+        <v>20</v>
+      </c>
+      <c r="AC286">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="287" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L287" s="2"/>
-      <c r="M287" s="2"/>
+      <c r="A287">
+        <v>184</v>
+      </c>
+      <c r="B287">
+        <v>2022</v>
+      </c>
+      <c r="C287">
+        <v>3</v>
+      </c>
+      <c r="D287">
+        <v>21</v>
+      </c>
+      <c r="E287">
+        <v>3</v>
+      </c>
+      <c r="F287">
+        <v>24</v>
+      </c>
+      <c r="G287" t="s">
+        <v>1</v>
+      </c>
+      <c r="H287" t="s">
+        <v>2</v>
+      </c>
+      <c r="I287" t="s">
+        <v>38</v>
+      </c>
+      <c r="J287">
+        <v>882</v>
+      </c>
+      <c r="K287">
+        <v>0</v>
+      </c>
+      <c r="L287" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M287" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N287">
+        <v>1</v>
+      </c>
+      <c r="O287">
+        <v>0.5</v>
+      </c>
+      <c r="P287">
+        <v>12.5</v>
+      </c>
+      <c r="Q287">
+        <v>4</v>
+      </c>
+      <c r="S287">
+        <v>6.5</v>
+      </c>
+      <c r="T287">
+        <v>2</v>
+      </c>
+      <c r="V287">
+        <v>29.5</v>
+      </c>
+      <c r="W287">
+        <v>10</v>
+      </c>
+      <c r="Z287">
+        <v>2.5</v>
+      </c>
+      <c r="AA287">
+        <v>2</v>
+      </c>
+      <c r="AB287">
+        <v>19</v>
+      </c>
+      <c r="AC287">
+        <v>10.5</v>
+      </c>
     </row>
     <row r="288" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L288" s="2"/>
@@ -24605,6 +24751,10 @@
     <row r="458" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L458" s="2"/>
       <c r="M458" s="2"/>
+    </row>
+    <row r="459" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L459" s="2"/>
+      <c r="M459" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ ow polls (3/23-24) + bva poll (3/25)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEEA37B-FE74-BC43-AEB3-B25496EFC46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1986E100-0241-3640-8EC6-D7E7E73A207E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="12040" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH459"/>
+  <dimension ref="A1:AH462"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A286" sqref="A286"/>
+      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD283" sqref="AD283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23481,10 +23481,10 @@
         <v>47</v>
       </c>
       <c r="J280">
-        <v>1697</v>
+        <v>1737</v>
       </c>
       <c r="K280">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L280" s="2">
         <v>1</v>
@@ -23700,10 +23700,10 @@
         <v>3</v>
       </c>
       <c r="F283">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G283" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="H283" t="s">
         <v>21</v>
@@ -23712,7 +23712,7 @@
         <v>47</v>
       </c>
       <c r="J283">
-        <v>1013</v>
+        <v>751</v>
       </c>
       <c r="K283">
         <v>0</v>
@@ -23721,10 +23721,10 @@
         <v>1</v>
       </c>
       <c r="M283" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N283">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O283">
         <v>1</v>
@@ -23736,28 +23736,28 @@
         <v>3</v>
       </c>
       <c r="S283">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="T283">
         <v>2</v>
       </c>
       <c r="V283">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W283">
+        <v>12</v>
+      </c>
+      <c r="Z283">
+        <v>2</v>
+      </c>
+      <c r="AA283">
+        <v>2</v>
+      </c>
+      <c r="AB283">
+        <v>18</v>
+      </c>
+      <c r="AC283">
         <v>10</v>
-      </c>
-      <c r="Z283">
-        <v>2</v>
-      </c>
-      <c r="AA283">
-        <v>2.5</v>
-      </c>
-      <c r="AB283">
-        <v>20</v>
-      </c>
-      <c r="AC283">
-        <v>11</v>
       </c>
     </row>
     <row r="284" spans="1:29" x14ac:dyDescent="0.2">
@@ -23854,28 +23854,28 @@
         <v>3</v>
       </c>
       <c r="F285">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G285" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H285" t="s">
         <v>21</v>
       </c>
       <c r="I285" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J285">
-        <v>1107</v>
+        <v>1013</v>
       </c>
       <c r="K285">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L285" s="2">
         <v>1</v>
       </c>
       <c r="M285" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N285">
         <v>1</v>
@@ -23887,31 +23887,31 @@
         <v>14</v>
       </c>
       <c r="Q285">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S285">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="T285">
         <v>2</v>
       </c>
       <c r="V285">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W285">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Z285">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA285">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB285">
         <v>20</v>
       </c>
       <c r="AC285">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="286" spans="1:29" x14ac:dyDescent="0.2">
@@ -23925,70 +23925,70 @@
         <v>3</v>
       </c>
       <c r="D286">
+        <v>22</v>
+      </c>
+      <c r="E286">
+        <v>3</v>
+      </c>
+      <c r="F286">
+        <v>23</v>
+      </c>
+      <c r="G286" t="s">
+        <v>33</v>
+      </c>
+      <c r="H286" t="s">
         <v>21</v>
       </c>
-      <c r="E286">
-        <v>3</v>
-      </c>
-      <c r="F286">
-        <v>24</v>
-      </c>
-      <c r="G286" t="s">
-        <v>29</v>
-      </c>
-      <c r="H286" t="s">
-        <v>22</v>
-      </c>
       <c r="I286" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J286">
-        <v>1079</v>
+        <v>743</v>
       </c>
       <c r="K286">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L286" s="2">
         <v>1</v>
       </c>
       <c r="M286" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N286">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O286">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P286">
         <v>14</v>
       </c>
       <c r="Q286">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S286">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="T286">
         <v>2</v>
       </c>
       <c r="V286">
-        <v>28.5</v>
+        <v>28</v>
       </c>
       <c r="W286">
-        <v>11.5</v>
+        <v>11</v>
       </c>
       <c r="Z286">
         <v>2</v>
       </c>
       <c r="AA286">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB286">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AC286">
-        <v>11.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="287" spans="1:29" x14ac:dyDescent="0.2">
@@ -24002,137 +24002,356 @@
         <v>3</v>
       </c>
       <c r="D287">
+        <v>22</v>
+      </c>
+      <c r="E287">
+        <v>3</v>
+      </c>
+      <c r="F287">
+        <v>23</v>
+      </c>
+      <c r="G287" t="s">
+        <v>34</v>
+      </c>
+      <c r="H287" t="s">
         <v>21</v>
       </c>
-      <c r="E287">
-        <v>3</v>
-      </c>
-      <c r="F287">
-        <v>24</v>
-      </c>
-      <c r="G287" t="s">
-        <v>1</v>
-      </c>
-      <c r="H287" t="s">
-        <v>2</v>
-      </c>
       <c r="I287" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J287">
-        <v>882</v>
+        <v>958</v>
       </c>
       <c r="K287">
         <v>0</v>
       </c>
       <c r="L287" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M287" s="2">
         <v>0.5</v>
       </c>
       <c r="N287">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O287">
         <v>0.5</v>
       </c>
       <c r="P287">
-        <v>12.5</v>
+        <v>14.5</v>
       </c>
       <c r="Q287">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S287">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="T287">
         <v>2</v>
       </c>
       <c r="V287">
-        <v>29.5</v>
+        <v>28</v>
       </c>
       <c r="W287">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="Z287">
         <v>2.5</v>
       </c>
       <c r="AA287">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB287">
         <v>19</v>
       </c>
       <c r="AC287">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="288" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>185</v>
+      </c>
+      <c r="B288">
+        <v>2022</v>
+      </c>
+      <c r="C288">
+        <v>3</v>
+      </c>
+      <c r="D288">
+        <v>21</v>
+      </c>
+      <c r="E288">
+        <v>3</v>
+      </c>
+      <c r="F288">
+        <v>24</v>
+      </c>
+      <c r="G288" t="s">
+        <v>33</v>
+      </c>
+      <c r="H288" t="s">
+        <v>21</v>
+      </c>
+      <c r="I288" t="s">
+        <v>38</v>
+      </c>
+      <c r="J288">
+        <v>1094</v>
+      </c>
+      <c r="K288">
+        <v>0</v>
+      </c>
+      <c r="L288" s="2">
+        <v>1</v>
+      </c>
+      <c r="M288" s="2">
+        <v>1</v>
+      </c>
+      <c r="N288">
+        <v>1</v>
+      </c>
+      <c r="O288">
+        <v>1</v>
+      </c>
+      <c r="P288">
+        <v>14</v>
+      </c>
+      <c r="Q288">
+        <v>4</v>
+      </c>
+      <c r="S288">
+        <v>5</v>
+      </c>
+      <c r="T288">
+        <v>2</v>
+      </c>
+      <c r="V288">
+        <v>28</v>
+      </c>
+      <c r="W288">
+        <v>12</v>
+      </c>
+      <c r="Z288">
+        <v>3</v>
+      </c>
+      <c r="AA288">
+        <v>1</v>
+      </c>
+      <c r="AB288">
+        <v>20</v>
+      </c>
+      <c r="AC288">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="289" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <v>186</v>
+      </c>
+      <c r="B289">
+        <v>2022</v>
+      </c>
+      <c r="C289">
+        <v>3</v>
+      </c>
+      <c r="D289">
+        <v>21</v>
+      </c>
+      <c r="E289">
+        <v>3</v>
+      </c>
+      <c r="F289">
+        <v>24</v>
+      </c>
+      <c r="G289" t="s">
+        <v>29</v>
+      </c>
+      <c r="H289" t="s">
+        <v>22</v>
+      </c>
+      <c r="I289" t="s">
+        <v>38</v>
+      </c>
+      <c r="J289">
+        <v>1103</v>
+      </c>
+      <c r="K289">
+        <v>0</v>
+      </c>
+      <c r="L289" s="2">
+        <v>1</v>
+      </c>
+      <c r="M289" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N289">
+        <v>0.5</v>
+      </c>
+      <c r="O289">
+        <v>0.5</v>
+      </c>
+      <c r="P289">
+        <v>14</v>
+      </c>
+      <c r="Q289">
+        <v>3.5</v>
+      </c>
+      <c r="S289">
+        <v>4.5</v>
+      </c>
+      <c r="T289">
+        <v>2</v>
+      </c>
+      <c r="V289">
+        <v>28.5</v>
+      </c>
+      <c r="W289">
+        <v>11.5</v>
+      </c>
+      <c r="Z289">
+        <v>2</v>
+      </c>
+      <c r="AA289">
+        <v>1.5</v>
+      </c>
+      <c r="AB289">
+        <v>20</v>
+      </c>
+      <c r="AC289">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="290" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <v>187</v>
+      </c>
+      <c r="B290">
+        <v>2022</v>
+      </c>
+      <c r="C290">
+        <v>3</v>
+      </c>
+      <c r="D290">
+        <v>21</v>
+      </c>
+      <c r="E290">
+        <v>3</v>
+      </c>
+      <c r="F290">
+        <v>24</v>
+      </c>
+      <c r="G290" t="s">
+        <v>1</v>
+      </c>
+      <c r="H290" t="s">
+        <v>2</v>
+      </c>
+      <c r="I290" t="s">
+        <v>38</v>
+      </c>
+      <c r="J290">
+        <v>882</v>
+      </c>
+      <c r="K290">
+        <v>0</v>
+      </c>
+      <c r="L290" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M290" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N290">
+        <v>1</v>
+      </c>
+      <c r="O290">
+        <v>0.5</v>
+      </c>
+      <c r="P290">
+        <v>12.5</v>
+      </c>
+      <c r="Q290">
+        <v>4</v>
+      </c>
+      <c r="S290">
+        <v>6.5</v>
+      </c>
+      <c r="T290">
+        <v>2</v>
+      </c>
+      <c r="V290">
+        <v>29.5</v>
+      </c>
+      <c r="W290">
+        <v>10</v>
+      </c>
+      <c r="Z290">
+        <v>2.5</v>
+      </c>
+      <c r="AA290">
+        <v>2</v>
+      </c>
+      <c r="AB290">
+        <v>19</v>
+      </c>
+      <c r="AC290">
         <v>10.5</v>
       </c>
     </row>
-    <row r="288" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L288" s="2"/>
-      <c r="M288" s="2"/>
-    </row>
-    <row r="289" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L289" s="2"/>
-      <c r="M289" s="2"/>
-    </row>
-    <row r="290" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L290" s="2"/>
-      <c r="M290" s="2"/>
-    </row>
-    <row r="291" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L291" s="2"/>
       <c r="M291" s="2"/>
     </row>
-    <row r="292" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L292" s="2"/>
       <c r="M292" s="2"/>
     </row>
-    <row r="293" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L293" s="2"/>
       <c r="M293" s="2"/>
     </row>
-    <row r="294" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L294" s="2"/>
       <c r="M294" s="2"/>
     </row>
-    <row r="295" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L295" s="2"/>
       <c r="M295" s="2"/>
     </row>
-    <row r="296" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L296" s="2"/>
       <c r="M296" s="2"/>
     </row>
-    <row r="297" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L297" s="2"/>
       <c r="M297" s="2"/>
     </row>
-    <row r="298" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L298" s="2"/>
       <c r="M298" s="2"/>
     </row>
-    <row r="299" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L299" s="2"/>
       <c r="M299" s="2"/>
     </row>
-    <row r="300" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L300" s="2"/>
       <c r="M300" s="2"/>
     </row>
-    <row r="301" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L301" s="2"/>
       <c r="M301" s="2"/>
     </row>
-    <row r="302" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L302" s="2"/>
       <c r="M302" s="2"/>
     </row>
-    <row r="303" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L303" s="2"/>
       <c r="M303" s="2"/>
     </row>
-    <row r="304" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L304" s="2"/>
       <c r="M304" s="2"/>
     </row>
@@ -24755,6 +24974,18 @@
     <row r="459" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L459" s="2"/>
       <c r="M459" s="2"/>
+    </row>
+    <row r="460" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L460" s="2"/>
+      <c r="M460" s="2"/>
+    </row>
+    <row r="461" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L461" s="2"/>
+      <c r="M461" s="2"/>
+    </row>
+    <row r="462" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L462" s="2"/>
+      <c r="M462" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ ow poll (3/25) + ipsos rolling (3/26)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1986E100-0241-3640-8EC6-D7E7E73A207E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE942C83-95FD-354D-80E3-98164E4C7448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12040" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="28540" yWindow="900" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH462"/>
+  <dimension ref="A1:AH463"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD283" sqref="AD283"/>
+      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A291" sqref="A291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24079,7 +24079,7 @@
         <v>3</v>
       </c>
       <c r="D288">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E288">
         <v>3</v>
@@ -24088,16 +24088,16 @@
         <v>24</v>
       </c>
       <c r="G288" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H288" t="s">
         <v>21</v>
       </c>
       <c r="I288" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J288">
-        <v>1094</v>
+        <v>2353</v>
       </c>
       <c r="K288">
         <v>0</v>
@@ -24106,16 +24106,16 @@
         <v>1</v>
       </c>
       <c r="M288" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N288">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O288">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P288">
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="Q288">
         <v>4</v>
@@ -24124,25 +24124,25 @@
         <v>5</v>
       </c>
       <c r="T288">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V288">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W288">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z288">
         <v>3</v>
       </c>
       <c r="AA288">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB288">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AC288">
-        <v>9</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="289" spans="1:29" x14ac:dyDescent="0.2">
@@ -24165,16 +24165,16 @@
         <v>24</v>
       </c>
       <c r="G289" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H289" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I289" t="s">
         <v>38</v>
       </c>
       <c r="J289">
-        <v>1103</v>
+        <v>1094</v>
       </c>
       <c r="K289">
         <v>0</v>
@@ -24183,43 +24183,43 @@
         <v>1</v>
       </c>
       <c r="M289" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N289">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O289">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P289">
         <v>14</v>
       </c>
       <c r="Q289">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S289">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T289">
         <v>2</v>
       </c>
       <c r="V289">
-        <v>28.5</v>
+        <v>28</v>
       </c>
       <c r="W289">
-        <v>11.5</v>
+        <v>12</v>
       </c>
       <c r="Z289">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA289">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AB289">
         <v>20</v>
       </c>
       <c r="AC289">
-        <v>11.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="290" spans="1:29" x14ac:dyDescent="0.2">
@@ -24242,78 +24242,370 @@
         <v>24</v>
       </c>
       <c r="G290" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="H290" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I290" t="s">
         <v>38</v>
       </c>
       <c r="J290">
-        <v>882</v>
+        <v>1103</v>
       </c>
       <c r="K290">
         <v>0</v>
       </c>
       <c r="L290" s="2">
+        <v>1</v>
+      </c>
+      <c r="M290" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N290">
+        <v>0.5</v>
+      </c>
+      <c r="O290">
+        <v>0.5</v>
+      </c>
+      <c r="P290">
+        <v>14</v>
+      </c>
+      <c r="Q290">
+        <v>3.5</v>
+      </c>
+      <c r="S290">
+        <v>4.5</v>
+      </c>
+      <c r="T290">
+        <v>2</v>
+      </c>
+      <c r="V290">
+        <v>28.5</v>
+      </c>
+      <c r="W290">
+        <v>11.5</v>
+      </c>
+      <c r="Z290">
+        <v>2</v>
+      </c>
+      <c r="AA290">
+        <v>1.5</v>
+      </c>
+      <c r="AB290">
+        <v>20</v>
+      </c>
+      <c r="AC290">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="291" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <v>188</v>
+      </c>
+      <c r="B291">
+        <v>2022</v>
+      </c>
+      <c r="C291">
+        <v>3</v>
+      </c>
+      <c r="D291">
+        <v>23</v>
+      </c>
+      <c r="E291">
+        <v>3</v>
+      </c>
+      <c r="F291">
+        <v>24</v>
+      </c>
+      <c r="G291" t="s">
+        <v>33</v>
+      </c>
+      <c r="H291" t="s">
+        <v>21</v>
+      </c>
+      <c r="I291" t="s">
+        <v>47</v>
+      </c>
+      <c r="J291">
+        <v>700</v>
+      </c>
+      <c r="K291">
+        <v>1</v>
+      </c>
+      <c r="L291" s="2">
+        <v>1</v>
+      </c>
+      <c r="M291" s="2">
+        <v>1</v>
+      </c>
+      <c r="N291">
+        <v>1</v>
+      </c>
+      <c r="O291">
+        <v>1</v>
+      </c>
+      <c r="P291">
+        <v>14</v>
+      </c>
+      <c r="Q291">
+        <v>4</v>
+      </c>
+      <c r="S291">
+        <v>6</v>
+      </c>
+      <c r="T291">
+        <v>2</v>
+      </c>
+      <c r="V291">
+        <v>27</v>
+      </c>
+      <c r="W291">
+        <v>11</v>
+      </c>
+      <c r="Z291">
+        <v>2</v>
+      </c>
+      <c r="AA291">
+        <v>2</v>
+      </c>
+      <c r="AB291">
+        <v>20</v>
+      </c>
+      <c r="AC291">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="292" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <v>189</v>
+      </c>
+      <c r="B292">
+        <v>2022</v>
+      </c>
+      <c r="C292">
+        <v>3</v>
+      </c>
+      <c r="D292">
+        <v>22</v>
+      </c>
+      <c r="E292">
+        <v>3</v>
+      </c>
+      <c r="F292">
+        <v>25</v>
+      </c>
+      <c r="G292" t="s">
+        <v>33</v>
+      </c>
+      <c r="H292" t="s">
+        <v>21</v>
+      </c>
+      <c r="I292" t="s">
+        <v>38</v>
+      </c>
+      <c r="J292">
+        <v>1094</v>
+      </c>
+      <c r="K292">
+        <v>1</v>
+      </c>
+      <c r="L292" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="M290" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N290">
-        <v>1</v>
-      </c>
-      <c r="O290">
-        <v>0.5</v>
-      </c>
-      <c r="P290">
-        <v>12.5</v>
-      </c>
-      <c r="Q290">
+      <c r="M292" s="2">
+        <v>1</v>
+      </c>
+      <c r="N292">
+        <v>1</v>
+      </c>
+      <c r="O292">
+        <v>1</v>
+      </c>
+      <c r="P292">
+        <v>13</v>
+      </c>
+      <c r="Q292">
         <v>4</v>
       </c>
-      <c r="S290">
-        <v>6.5</v>
-      </c>
-      <c r="T290">
-        <v>2</v>
-      </c>
-      <c r="V290">
-        <v>29.5</v>
-      </c>
-      <c r="W290">
+      <c r="S292">
+        <v>5</v>
+      </c>
+      <c r="T292">
+        <v>2</v>
+      </c>
+      <c r="V292">
+        <v>27</v>
+      </c>
+      <c r="W292">
+        <v>12</v>
+      </c>
+      <c r="Z292">
+        <v>3</v>
+      </c>
+      <c r="AA292">
+        <v>1</v>
+      </c>
+      <c r="AB292">
+        <v>21</v>
+      </c>
+      <c r="AC292">
         <v>10</v>
       </c>
-      <c r="Z290">
+    </row>
+    <row r="293" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <v>190</v>
+      </c>
+      <c r="B293">
+        <v>2022</v>
+      </c>
+      <c r="C293">
+        <v>3</v>
+      </c>
+      <c r="D293">
+        <v>22</v>
+      </c>
+      <c r="E293">
+        <v>3</v>
+      </c>
+      <c r="F293">
+        <v>25</v>
+      </c>
+      <c r="G293" t="s">
+        <v>29</v>
+      </c>
+      <c r="H293" t="s">
+        <v>22</v>
+      </c>
+      <c r="I293" t="s">
+        <v>38</v>
+      </c>
+      <c r="J293">
+        <v>1103</v>
+      </c>
+      <c r="K293">
+        <v>1</v>
+      </c>
+      <c r="L293" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M293" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N293">
+        <v>0.5</v>
+      </c>
+      <c r="O293">
+        <v>0.5</v>
+      </c>
+      <c r="P293">
+        <v>14</v>
+      </c>
+      <c r="Q293">
+        <v>3.5</v>
+      </c>
+      <c r="S293">
+        <v>5</v>
+      </c>
+      <c r="T293">
+        <v>2</v>
+      </c>
+      <c r="V293">
+        <v>18</v>
+      </c>
+      <c r="W293">
+        <v>11.5</v>
+      </c>
+      <c r="Z293">
+        <v>2</v>
+      </c>
+      <c r="AA293">
+        <v>1.5</v>
+      </c>
+      <c r="AB293">
+        <v>20.5</v>
+      </c>
+      <c r="AC293">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="294" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>191</v>
+      </c>
+      <c r="B294">
+        <v>2022</v>
+      </c>
+      <c r="C294">
+        <v>3</v>
+      </c>
+      <c r="D294">
+        <v>23</v>
+      </c>
+      <c r="E294">
+        <v>3</v>
+      </c>
+      <c r="F294">
+        <v>26</v>
+      </c>
+      <c r="G294" t="s">
+        <v>1</v>
+      </c>
+      <c r="H294" t="s">
+        <v>2</v>
+      </c>
+      <c r="I294" t="s">
+        <v>38</v>
+      </c>
+      <c r="J294">
+        <v>878</v>
+      </c>
+      <c r="K294">
+        <v>0</v>
+      </c>
+      <c r="L294" s="2">
+        <v>1</v>
+      </c>
+      <c r="M294" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N294">
+        <v>1</v>
+      </c>
+      <c r="O294">
+        <v>0.5</v>
+      </c>
+      <c r="P294">
+        <v>14.5</v>
+      </c>
+      <c r="Q294">
+        <v>3.5</v>
+      </c>
+      <c r="S294">
+        <v>6</v>
+      </c>
+      <c r="T294">
         <v>2.5</v>
       </c>
-      <c r="AA290">
-        <v>2</v>
-      </c>
-      <c r="AB290">
-        <v>19</v>
-      </c>
-      <c r="AC290">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="291" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L291" s="2"/>
-      <c r="M291" s="2"/>
-    </row>
-    <row r="292" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L292" s="2"/>
-      <c r="M292" s="2"/>
-    </row>
-    <row r="293" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L293" s="2"/>
-      <c r="M293" s="2"/>
-    </row>
-    <row r="294" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L294" s="2"/>
-      <c r="M294" s="2"/>
+      <c r="V294">
+        <v>28.5</v>
+      </c>
+      <c r="W294">
+        <v>10</v>
+      </c>
+      <c r="Z294">
+        <v>2.5</v>
+      </c>
+      <c r="AA294">
+        <v>2.5</v>
+      </c>
+      <c r="AB294">
+        <v>17.5</v>
+      </c>
+      <c r="AC294">
+        <v>11</v>
+      </c>
     </row>
     <row r="295" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L295" s="2"/>
@@ -24986,6 +25278,10 @@
     <row r="462" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L462" s="2"/>
       <c r="M462" s="2"/>
+    </row>
+    <row r="463" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L463" s="2"/>
+      <c r="M463" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ rollings + ipsos-cevipof poll (3/28)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE942C83-95FD-354D-80E3-98164E4C7448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2E7275-613F-BE41-B481-EAF0955AB501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28540" yWindow="900" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH463"/>
+  <dimension ref="A1:AH462"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A291" sqref="A291"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AC296" sqref="AC296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18475,7 +18475,7 @@
         <v>1.5</v>
       </c>
       <c r="AB216">
-        <v>16.600000000000001</v>
+        <v>16.5</v>
       </c>
       <c r="AC216">
         <v>16</v>
@@ -24310,7 +24310,7 @@
         <v>3</v>
       </c>
       <c r="D291">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E291">
         <v>3</v>
@@ -24319,61 +24319,61 @@
         <v>24</v>
       </c>
       <c r="G291" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="H291" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I291" t="s">
         <v>47</v>
       </c>
       <c r="J291">
-        <v>700</v>
+        <v>7230</v>
       </c>
       <c r="K291">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L291" s="2">
         <v>1</v>
       </c>
       <c r="M291" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N291">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O291">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P291">
         <v>14</v>
       </c>
       <c r="Q291">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S291">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T291">
         <v>2</v>
       </c>
       <c r="V291">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W291">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z291">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AA291">
         <v>2</v>
       </c>
       <c r="AB291">
-        <v>20</v>
+        <v>17.5</v>
       </c>
       <c r="AC291">
-        <v>10</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="292" spans="1:29" x14ac:dyDescent="0.2">
@@ -24387,13 +24387,13 @@
         <v>3</v>
       </c>
       <c r="D292">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E292">
         <v>3</v>
       </c>
       <c r="F292">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G292" t="s">
         <v>33</v>
@@ -24402,16 +24402,16 @@
         <v>21</v>
       </c>
       <c r="I292" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J292">
-        <v>1094</v>
+        <v>682</v>
       </c>
       <c r="K292">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L292" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M292" s="2">
         <v>1</v>
@@ -24423,13 +24423,13 @@
         <v>1</v>
       </c>
       <c r="P292">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q292">
         <v>4</v>
       </c>
       <c r="S292">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T292">
         <v>2</v>
@@ -24438,16 +24438,16 @@
         <v>27</v>
       </c>
       <c r="W292">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z292">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA292">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB292">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC292">
         <v>10</v>
@@ -24464,67 +24464,67 @@
         <v>3</v>
       </c>
       <c r="D293">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E293">
         <v>3</v>
       </c>
       <c r="F293">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G293" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="H293" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I293" t="s">
         <v>38</v>
       </c>
       <c r="J293">
-        <v>1103</v>
+        <v>878</v>
       </c>
       <c r="K293">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L293" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M293" s="2">
         <v>0.5</v>
       </c>
       <c r="N293">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O293">
         <v>0.5</v>
       </c>
       <c r="P293">
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="Q293">
         <v>3.5</v>
       </c>
       <c r="S293">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T293">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V293">
-        <v>18</v>
+        <v>28.5</v>
       </c>
       <c r="W293">
-        <v>11.5</v>
+        <v>10</v>
       </c>
       <c r="Z293">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AA293">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="AB293">
-        <v>20.5</v>
+        <v>17.5</v>
       </c>
       <c r="AC293">
         <v>11</v>
@@ -24541,13 +24541,13 @@
         <v>3</v>
       </c>
       <c r="D294">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E294">
         <v>3</v>
       </c>
       <c r="F294">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G294" t="s">
         <v>1</v>
@@ -24559,13 +24559,13 @@
         <v>38</v>
       </c>
       <c r="J294">
-        <v>878</v>
+        <v>903</v>
       </c>
       <c r="K294">
         <v>0</v>
       </c>
       <c r="L294" s="2">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M294" s="2">
         <v>0.5</v>
@@ -24577,7 +24577,7 @@
         <v>0.5</v>
       </c>
       <c r="P294">
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
       <c r="Q294">
         <v>3.5</v>
@@ -24586,34 +24586,180 @@
         <v>6</v>
       </c>
       <c r="T294">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V294">
-        <v>28.5</v>
+        <v>27.5</v>
       </c>
       <c r="W294">
         <v>10</v>
       </c>
       <c r="Z294">
+        <v>2</v>
+      </c>
+      <c r="AA294">
+        <v>2</v>
+      </c>
+      <c r="AB294">
+        <v>18.5</v>
+      </c>
+      <c r="AC294">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="295" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>192</v>
+      </c>
+      <c r="B295">
+        <v>2022</v>
+      </c>
+      <c r="C295">
+        <v>3</v>
+      </c>
+      <c r="D295">
+        <v>24</v>
+      </c>
+      <c r="E295">
+        <v>3</v>
+      </c>
+      <c r="F295">
+        <v>28</v>
+      </c>
+      <c r="G295" t="s">
+        <v>33</v>
+      </c>
+      <c r="H295" t="s">
+        <v>21</v>
+      </c>
+      <c r="I295" t="s">
+        <v>38</v>
+      </c>
+      <c r="J295">
+        <v>1094</v>
+      </c>
+      <c r="K295">
+        <v>1</v>
+      </c>
+      <c r="L295" s="2">
+        <v>1</v>
+      </c>
+      <c r="M295" s="2">
+        <v>1</v>
+      </c>
+      <c r="N295">
+        <v>1</v>
+      </c>
+      <c r="O295">
+        <v>1</v>
+      </c>
+      <c r="P295">
+        <v>14</v>
+      </c>
+      <c r="Q295">
+        <v>3</v>
+      </c>
+      <c r="S295">
+        <v>5</v>
+      </c>
+      <c r="T295">
+        <v>2</v>
+      </c>
+      <c r="V295">
+        <v>28</v>
+      </c>
+      <c r="W295">
+        <v>11</v>
+      </c>
+      <c r="Z295">
+        <v>3</v>
+      </c>
+      <c r="AA295">
+        <v>2</v>
+      </c>
+      <c r="AB295">
+        <v>20</v>
+      </c>
+      <c r="AC295">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <v>193</v>
+      </c>
+      <c r="B296">
+        <v>2022</v>
+      </c>
+      <c r="C296">
+        <v>3</v>
+      </c>
+      <c r="D296">
+        <v>24</v>
+      </c>
+      <c r="E296">
+        <v>3</v>
+      </c>
+      <c r="F296">
+        <v>28</v>
+      </c>
+      <c r="G296" t="s">
+        <v>29</v>
+      </c>
+      <c r="H296" t="s">
+        <v>22</v>
+      </c>
+      <c r="I296" t="s">
+        <v>38</v>
+      </c>
+      <c r="J296">
+        <v>1103</v>
+      </c>
+      <c r="K296">
+        <v>1</v>
+      </c>
+      <c r="L296" s="2">
+        <v>1</v>
+      </c>
+      <c r="M296" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N296">
+        <v>0.5</v>
+      </c>
+      <c r="O296">
+        <v>0.5</v>
+      </c>
+      <c r="P296">
+        <v>14</v>
+      </c>
+      <c r="Q296">
+        <v>3.5</v>
+      </c>
+      <c r="S296">
+        <v>5</v>
+      </c>
+      <c r="T296">
         <v>2.5</v>
       </c>
-      <c r="AA294">
-        <v>2.5</v>
-      </c>
-      <c r="AB294">
-        <v>17.5</v>
-      </c>
-      <c r="AC294">
+      <c r="V296">
+        <v>28</v>
+      </c>
+      <c r="W296">
         <v>11</v>
       </c>
-    </row>
-    <row r="295" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L295" s="2"/>
-      <c r="M295" s="2"/>
-    </row>
-    <row r="296" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L296" s="2"/>
-      <c r="M296" s="2"/>
+      <c r="Z296">
+        <v>1.5</v>
+      </c>
+      <c r="AA296">
+        <v>1.5</v>
+      </c>
+      <c r="AB296">
+        <v>21</v>
+      </c>
+      <c r="AC296">
+        <v>11</v>
+      </c>
     </row>
     <row r="297" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L297" s="2"/>
@@ -25278,10 +25424,6 @@
     <row r="462" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L462" s="2"/>
       <c r="M462" s="2"/>
-    </row>
-    <row r="463" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L463" s="2"/>
-      <c r="M463" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ rollings + cluster17 poll (3/29)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2E7275-613F-BE41-B481-EAF0955AB501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588BA0A6-3A1A-DF4B-9F3D-4E25D07CE47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28540" yWindow="900" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -556,9 +556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
   <dimension ref="A1:AH462"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AC296" sqref="AC296"/>
+      <selection pane="bottomLeft" activeCell="AB300" sqref="AB300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24541,70 +24541,70 @@
         <v>3</v>
       </c>
       <c r="D294">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E294">
         <v>3</v>
       </c>
       <c r="F294">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G294" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="H294" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I294" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J294">
-        <v>903</v>
+        <v>2471</v>
       </c>
       <c r="K294">
         <v>0</v>
       </c>
       <c r="L294" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M294" s="2">
         <v>0.5</v>
       </c>
       <c r="N294">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O294">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P294">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="Q294">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S294">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="T294">
         <v>2</v>
       </c>
       <c r="V294">
-        <v>27.5</v>
+        <v>27</v>
       </c>
       <c r="W294">
         <v>10</v>
       </c>
       <c r="Z294">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA294">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB294">
-        <v>18.5</v>
+        <v>17</v>
       </c>
       <c r="AC294">
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="295" spans="1:29" x14ac:dyDescent="0.2">
@@ -24618,13 +24618,13 @@
         <v>3</v>
       </c>
       <c r="D295">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E295">
         <v>3</v>
       </c>
       <c r="F295">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G295" t="s">
         <v>33</v>
@@ -24633,13 +24633,13 @@
         <v>21</v>
       </c>
       <c r="I295" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J295">
-        <v>1094</v>
+        <v>725</v>
       </c>
       <c r="K295">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L295" s="2">
         <v>1</v>
@@ -24657,19 +24657,19 @@
         <v>14</v>
       </c>
       <c r="Q295">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S295">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T295">
         <v>2</v>
       </c>
       <c r="V295">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W295">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z295">
         <v>3</v>
@@ -24686,7 +24686,7 @@
     </row>
     <row r="296" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A296">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B296">
         <v>2022</v>
@@ -24704,43 +24704,43 @@
         <v>28</v>
       </c>
       <c r="G296" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H296" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I296" t="s">
         <v>38</v>
       </c>
       <c r="J296">
-        <v>1103</v>
+        <v>1119</v>
       </c>
       <c r="K296">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L296" s="2">
         <v>1</v>
       </c>
       <c r="M296" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N296">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O296">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P296">
         <v>14</v>
       </c>
       <c r="Q296">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S296">
         <v>5</v>
       </c>
       <c r="T296">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V296">
         <v>28</v>
@@ -24749,33 +24749,325 @@
         <v>11</v>
       </c>
       <c r="Z296">
+        <v>3</v>
+      </c>
+      <c r="AA296">
+        <v>2</v>
+      </c>
+      <c r="AB296">
+        <v>20</v>
+      </c>
+      <c r="AC296">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="297" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <v>195</v>
+      </c>
+      <c r="B297">
+        <v>2022</v>
+      </c>
+      <c r="C297">
+        <v>3</v>
+      </c>
+      <c r="D297">
+        <v>24</v>
+      </c>
+      <c r="E297">
+        <v>3</v>
+      </c>
+      <c r="F297">
+        <v>28</v>
+      </c>
+      <c r="G297" t="s">
+        <v>29</v>
+      </c>
+      <c r="H297" t="s">
+        <v>22</v>
+      </c>
+      <c r="I297" t="s">
+        <v>38</v>
+      </c>
+      <c r="J297">
+        <v>1161</v>
+      </c>
+      <c r="K297">
+        <v>0</v>
+      </c>
+      <c r="L297" s="2">
+        <v>1</v>
+      </c>
+      <c r="M297" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N297">
+        <v>0.5</v>
+      </c>
+      <c r="O297">
+        <v>0.5</v>
+      </c>
+      <c r="P297">
+        <v>14</v>
+      </c>
+      <c r="Q297">
+        <v>3.5</v>
+      </c>
+      <c r="S297">
+        <v>5</v>
+      </c>
+      <c r="T297">
+        <v>2.5</v>
+      </c>
+      <c r="V297">
+        <v>28</v>
+      </c>
+      <c r="W297">
+        <v>11</v>
+      </c>
+      <c r="Z297">
         <v>1.5</v>
       </c>
-      <c r="AA296">
+      <c r="AA297">
         <v>1.5</v>
       </c>
-      <c r="AB296">
+      <c r="AB297">
         <v>21</v>
       </c>
-      <c r="AC296">
+      <c r="AC297">
         <v>11</v>
       </c>
     </row>
-    <row r="297" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L297" s="2"/>
-      <c r="M297" s="2"/>
-    </row>
     <row r="298" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L298" s="2"/>
-      <c r="M298" s="2"/>
+      <c r="A298">
+        <v>196</v>
+      </c>
+      <c r="B298">
+        <v>2022</v>
+      </c>
+      <c r="C298">
+        <v>3</v>
+      </c>
+      <c r="D298">
+        <v>25</v>
+      </c>
+      <c r="E298">
+        <v>3</v>
+      </c>
+      <c r="F298">
+        <v>29</v>
+      </c>
+      <c r="G298" t="s">
+        <v>33</v>
+      </c>
+      <c r="H298" t="s">
+        <v>21</v>
+      </c>
+      <c r="I298" t="s">
+        <v>38</v>
+      </c>
+      <c r="J298">
+        <v>1119</v>
+      </c>
+      <c r="K298">
+        <v>1</v>
+      </c>
+      <c r="L298" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M298" s="2">
+        <v>1</v>
+      </c>
+      <c r="N298">
+        <v>1</v>
+      </c>
+      <c r="O298">
+        <v>1</v>
+      </c>
+      <c r="P298">
+        <v>15</v>
+      </c>
+      <c r="Q298">
+        <v>3</v>
+      </c>
+      <c r="S298">
+        <v>5</v>
+      </c>
+      <c r="T298">
+        <v>2</v>
+      </c>
+      <c r="V298">
+        <v>28</v>
+      </c>
+      <c r="W298">
+        <v>11</v>
+      </c>
+      <c r="Z298">
+        <v>3</v>
+      </c>
+      <c r="AA298">
+        <v>1</v>
+      </c>
+      <c r="AB298">
+        <v>20</v>
+      </c>
+      <c r="AC298">
+        <v>10</v>
+      </c>
     </row>
     <row r="299" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L299" s="2"/>
-      <c r="M299" s="2"/>
+      <c r="A299">
+        <v>197</v>
+      </c>
+      <c r="B299">
+        <v>2022</v>
+      </c>
+      <c r="C299">
+        <v>3</v>
+      </c>
+      <c r="D299">
+        <v>25</v>
+      </c>
+      <c r="E299">
+        <v>3</v>
+      </c>
+      <c r="F299">
+        <v>29</v>
+      </c>
+      <c r="G299" t="s">
+        <v>29</v>
+      </c>
+      <c r="H299" t="s">
+        <v>22</v>
+      </c>
+      <c r="I299" t="s">
+        <v>38</v>
+      </c>
+      <c r="J299">
+        <v>1161</v>
+      </c>
+      <c r="K299">
+        <v>1</v>
+      </c>
+      <c r="L299" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M299" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N299">
+        <v>1</v>
+      </c>
+      <c r="O299">
+        <v>0.5</v>
+      </c>
+      <c r="P299">
+        <v>14.5</v>
+      </c>
+      <c r="Q299">
+        <v>3.5</v>
+      </c>
+      <c r="S299">
+        <v>5</v>
+      </c>
+      <c r="T299">
+        <v>2</v>
+      </c>
+      <c r="V299">
+        <v>27.5</v>
+      </c>
+      <c r="W299">
+        <v>10.5</v>
+      </c>
+      <c r="Z299">
+        <v>2</v>
+      </c>
+      <c r="AA299">
+        <v>1.5</v>
+      </c>
+      <c r="AB299">
+        <v>21</v>
+      </c>
+      <c r="AC299">
+        <v>11</v>
+      </c>
     </row>
     <row r="300" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L300" s="2"/>
-      <c r="M300" s="2"/>
+      <c r="A300">
+        <v>193</v>
+      </c>
+      <c r="B300">
+        <v>2022</v>
+      </c>
+      <c r="C300">
+        <v>3</v>
+      </c>
+      <c r="D300">
+        <v>25</v>
+      </c>
+      <c r="E300">
+        <v>3</v>
+      </c>
+      <c r="F300">
+        <v>29</v>
+      </c>
+      <c r="G300" t="s">
+        <v>1</v>
+      </c>
+      <c r="H300" t="s">
+        <v>2</v>
+      </c>
+      <c r="I300" t="s">
+        <v>38</v>
+      </c>
+      <c r="J300">
+        <v>933</v>
+      </c>
+      <c r="K300">
+        <v>0</v>
+      </c>
+      <c r="L300" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M300" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N300">
+        <v>1.5</v>
+      </c>
+      <c r="O300">
+        <v>0.5</v>
+      </c>
+      <c r="P300">
+        <v>15</v>
+      </c>
+      <c r="Q300">
+        <v>3.5</v>
+      </c>
+      <c r="S300">
+        <v>6</v>
+      </c>
+      <c r="T300">
+        <v>2</v>
+      </c>
+      <c r="V300">
+        <v>27</v>
+      </c>
+      <c r="W300">
+        <v>9</v>
+      </c>
+      <c r="Z300">
+        <v>2</v>
+      </c>
+      <c r="AA300">
+        <v>2</v>
+      </c>
+      <c r="AB300">
+        <v>19.5</v>
+      </c>
+      <c r="AC300">
+        <v>12</v>
+      </c>
     </row>
     <row r="301" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L301" s="2"/>

</xml_diff>

<commit_message>
update w/ harris and elabe polls + rollings (3/30)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588BA0A6-3A1A-DF4B-9F3D-4E25D07CE47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69F1390-2347-B348-AFF6-C56227B1CDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28540" yWindow="900" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="28400" yWindow="2780" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH462"/>
+  <dimension ref="A1:AH464"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AB300" sqref="AB300"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D300" sqref="D300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24855,34 +24855,34 @@
         <v>3</v>
       </c>
       <c r="F298">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G298" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H298" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I298" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J298">
-        <v>1119</v>
+        <v>1700</v>
       </c>
       <c r="K298">
         <v>1</v>
       </c>
       <c r="L298" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M298" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N298">
         <v>1</v>
       </c>
       <c r="O298">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P298">
         <v>15</v>
@@ -24894,22 +24894,22 @@
         <v>5</v>
       </c>
       <c r="T298">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V298">
-        <v>28</v>
+        <v>28.5</v>
       </c>
       <c r="W298">
-        <v>11</v>
+        <v>9.5</v>
       </c>
       <c r="Z298">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA298">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB298">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AC298">
         <v>10</v>
@@ -24926,46 +24926,46 @@
         <v>3</v>
       </c>
       <c r="D299">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E299">
         <v>3</v>
       </c>
       <c r="F299">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G299" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H299" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I299" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J299">
-        <v>1161</v>
+        <v>772</v>
       </c>
       <c r="K299">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L299" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M299" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N299">
         <v>1</v>
       </c>
       <c r="O299">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P299">
-        <v>14.5</v>
+        <v>15</v>
       </c>
       <c r="Q299">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S299">
         <v>5</v>
@@ -24974,27 +24974,27 @@
         <v>2</v>
       </c>
       <c r="V299">
-        <v>27.5</v>
+        <v>28</v>
       </c>
       <c r="W299">
-        <v>10.5</v>
+        <v>11</v>
       </c>
       <c r="Z299">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA299">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AB299">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC299">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="300" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A300">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B300">
         <v>2022</v>
@@ -25003,83 +25003,302 @@
         <v>3</v>
       </c>
       <c r="D300">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E300">
         <v>3</v>
       </c>
       <c r="F300">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G300" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H300" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I300" t="s">
         <v>38</v>
       </c>
       <c r="J300">
-        <v>933</v>
+        <v>1119</v>
       </c>
       <c r="K300">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L300" s="2">
         <v>0.66666666666666663</v>
       </c>
       <c r="M300" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N300">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O300">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P300">
         <v>15</v>
       </c>
       <c r="Q300">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S300">
+        <v>5</v>
+      </c>
+      <c r="T300">
+        <v>2</v>
+      </c>
+      <c r="V300">
+        <v>28</v>
+      </c>
+      <c r="W300">
+        <v>11</v>
+      </c>
+      <c r="Z300">
+        <v>3</v>
+      </c>
+      <c r="AA300">
+        <v>1</v>
+      </c>
+      <c r="AB300">
+        <v>20</v>
+      </c>
+      <c r="AC300">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="301" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <v>199</v>
+      </c>
+      <c r="B301">
+        <v>2022</v>
+      </c>
+      <c r="C301">
+        <v>3</v>
+      </c>
+      <c r="D301">
+        <v>26</v>
+      </c>
+      <c r="E301">
+        <v>3</v>
+      </c>
+      <c r="F301">
+        <v>30</v>
+      </c>
+      <c r="G301" t="s">
+        <v>29</v>
+      </c>
+      <c r="H301" t="s">
+        <v>22</v>
+      </c>
+      <c r="I301" t="s">
+        <v>38</v>
+      </c>
+      <c r="J301">
+        <v>1500</v>
+      </c>
+      <c r="K301">
+        <v>1</v>
+      </c>
+      <c r="L301" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M301" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N301">
+        <v>0.5</v>
+      </c>
+      <c r="O301">
+        <v>0.5</v>
+      </c>
+      <c r="P301">
+        <v>15</v>
+      </c>
+      <c r="Q301">
+        <v>4</v>
+      </c>
+      <c r="S301">
+        <v>4.5</v>
+      </c>
+      <c r="T301">
+        <v>2</v>
+      </c>
+      <c r="V301">
+        <v>28</v>
+      </c>
+      <c r="W301">
+        <v>10.5</v>
+      </c>
+      <c r="Z301">
+        <v>1.5</v>
+      </c>
+      <c r="AA301">
+        <v>1.5</v>
+      </c>
+      <c r="AB301">
+        <v>21.5</v>
+      </c>
+      <c r="AC301">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="302" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>200</v>
+      </c>
+      <c r="B302">
+        <v>2022</v>
+      </c>
+      <c r="C302">
+        <v>3</v>
+      </c>
+      <c r="D302">
+        <v>27</v>
+      </c>
+      <c r="E302">
+        <v>3</v>
+      </c>
+      <c r="F302">
+        <v>30</v>
+      </c>
+      <c r="G302" t="s">
+        <v>1</v>
+      </c>
+      <c r="H302" t="s">
+        <v>2</v>
+      </c>
+      <c r="I302" t="s">
+        <v>38</v>
+      </c>
+      <c r="J302">
+        <v>951</v>
+      </c>
+      <c r="K302">
+        <v>0</v>
+      </c>
+      <c r="L302" s="2">
+        <v>1</v>
+      </c>
+      <c r="M302" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N302">
+        <v>1.5</v>
+      </c>
+      <c r="O302">
+        <v>0.5</v>
+      </c>
+      <c r="P302">
+        <v>15.5</v>
+      </c>
+      <c r="Q302">
+        <v>3</v>
+      </c>
+      <c r="S302">
         <v>6</v>
       </c>
-      <c r="T300">
-        <v>2</v>
-      </c>
-      <c r="V300">
+      <c r="T302">
+        <v>1.5</v>
+      </c>
+      <c r="V302">
         <v>27</v>
       </c>
-      <c r="W300">
+      <c r="W302">
         <v>9</v>
       </c>
-      <c r="Z300">
-        <v>2</v>
-      </c>
-      <c r="AA300">
-        <v>2</v>
-      </c>
-      <c r="AB300">
-        <v>19.5</v>
-      </c>
-      <c r="AC300">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="301" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L301" s="2"/>
-      <c r="M301" s="2"/>
-    </row>
-    <row r="302" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L302" s="2"/>
-      <c r="M302" s="2"/>
+      <c r="Z302">
+        <v>2</v>
+      </c>
+      <c r="AA302">
+        <v>2</v>
+      </c>
+      <c r="AB302">
+        <v>20.5</v>
+      </c>
+      <c r="AC302">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="303" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L303" s="2"/>
-      <c r="M303" s="2"/>
+      <c r="A303">
+        <v>201</v>
+      </c>
+      <c r="B303">
+        <v>2022</v>
+      </c>
+      <c r="C303">
+        <v>3</v>
+      </c>
+      <c r="D303">
+        <v>28</v>
+      </c>
+      <c r="E303">
+        <v>3</v>
+      </c>
+      <c r="F303">
+        <v>30</v>
+      </c>
+      <c r="G303" t="s">
+        <v>30</v>
+      </c>
+      <c r="H303" t="s">
+        <v>21</v>
+      </c>
+      <c r="I303" t="s">
+        <v>47</v>
+      </c>
+      <c r="J303">
+        <v>966</v>
+      </c>
+      <c r="K303">
+        <v>1</v>
+      </c>
+      <c r="L303" s="2">
+        <v>1</v>
+      </c>
+      <c r="M303" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N303">
+        <v>1.5</v>
+      </c>
+      <c r="O303">
+        <v>0.5</v>
+      </c>
+      <c r="P303">
+        <v>15.5</v>
+      </c>
+      <c r="Q303">
+        <v>2.5</v>
+      </c>
+      <c r="S303">
+        <v>4</v>
+      </c>
+      <c r="T303">
+        <v>2</v>
+      </c>
+      <c r="V303">
+        <v>28</v>
+      </c>
+      <c r="W303">
+        <v>9.5</v>
+      </c>
+      <c r="Z303">
+        <v>2.5</v>
+      </c>
+      <c r="AA303">
+        <v>2.5</v>
+      </c>
+      <c r="AB303">
+        <v>21</v>
+      </c>
+      <c r="AC303">
+        <v>10.5</v>
+      </c>
     </row>
     <row r="304" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L304" s="2"/>
@@ -25716,6 +25935,14 @@
     <row r="462" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L462" s="2"/>
       <c r="M462" s="2"/>
+    </row>
+    <row r="463" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L463" s="2"/>
+      <c r="M463" s="2"/>
+    </row>
+    <row r="464" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L464" s="2"/>
+      <c r="M464" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ rollings (3/31)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69F1390-2347-B348-AFF6-C56227B1CDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A6052F-731E-4844-AA95-5C7329A669F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28400" yWindow="2780" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="1100" yWindow="3580" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH464"/>
+  <dimension ref="A1:AH462"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D300" sqref="D300"/>
+      <selection pane="bottomLeft" activeCell="A303" sqref="A303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25003,7 +25003,7 @@
         <v>3</v>
       </c>
       <c r="D300">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E300">
         <v>3</v>
@@ -25012,61 +25012,61 @@
         <v>30</v>
       </c>
       <c r="G300" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="H300" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I300" t="s">
         <v>38</v>
       </c>
       <c r="J300">
-        <v>1119</v>
+        <v>951</v>
       </c>
       <c r="K300">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L300" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M300" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N300">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O300">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P300">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="Q300">
         <v>3</v>
       </c>
       <c r="S300">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T300">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V300">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W300">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z300">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA300">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB300">
-        <v>20</v>
+        <v>20.5</v>
       </c>
       <c r="AC300">
-        <v>10</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="301" spans="1:29" x14ac:dyDescent="0.2">
@@ -25080,7 +25080,7 @@
         <v>3</v>
       </c>
       <c r="D301">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E301">
         <v>3</v>
@@ -25089,40 +25089,40 @@
         <v>30</v>
       </c>
       <c r="G301" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H301" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I301" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J301">
-        <v>1500</v>
+        <v>966</v>
       </c>
       <c r="K301">
         <v>1</v>
       </c>
       <c r="L301" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M301" s="2">
         <v>0.5</v>
       </c>
       <c r="N301">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="O301">
         <v>0.5</v>
       </c>
       <c r="P301">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="Q301">
+        <v>2.5</v>
+      </c>
+      <c r="S301">
         <v>4</v>
-      </c>
-      <c r="S301">
-        <v>4.5</v>
       </c>
       <c r="T301">
         <v>2</v>
@@ -25131,16 +25131,16 @@
         <v>28</v>
       </c>
       <c r="W301">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="Z301">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="AA301">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="AB301">
-        <v>21.5</v>
+        <v>21</v>
       </c>
       <c r="AC301">
         <v>10.5</v>
@@ -25157,70 +25157,70 @@
         <v>3</v>
       </c>
       <c r="D302">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E302">
         <v>3</v>
       </c>
       <c r="F302">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G302" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H302" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I302" t="s">
         <v>38</v>
       </c>
       <c r="J302">
-        <v>951</v>
+        <v>1119</v>
       </c>
       <c r="K302">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L302" s="2">
         <v>1</v>
       </c>
       <c r="M302" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N302">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O302">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P302">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="Q302">
         <v>3</v>
       </c>
       <c r="S302">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T302">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V302">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W302">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Z302">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA302">
         <v>2</v>
       </c>
       <c r="AB302">
-        <v>20.5</v>
+        <v>20</v>
       </c>
       <c r="AC302">
-        <v>11.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="303" spans="1:29" x14ac:dyDescent="0.2">
@@ -25240,19 +25240,19 @@
         <v>3</v>
       </c>
       <c r="F303">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G303" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H303" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I303" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J303">
-        <v>966</v>
+        <v>1500</v>
       </c>
       <c r="K303">
         <v>1</v>
@@ -25264,7 +25264,7 @@
         <v>0.5</v>
       </c>
       <c r="N303">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="O303">
         <v>0.5</v>
@@ -25273,36 +25273,109 @@
         <v>15.5</v>
       </c>
       <c r="Q303">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="S303">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="T303">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V303">
         <v>28</v>
       </c>
       <c r="W303">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="Z303">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AA303">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AB303">
         <v>21</v>
       </c>
       <c r="AC303">
-        <v>10.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="304" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L304" s="2"/>
-      <c r="M304" s="2"/>
+      <c r="A304">
+        <v>202</v>
+      </c>
+      <c r="B304">
+        <v>2022</v>
+      </c>
+      <c r="C304">
+        <v>3</v>
+      </c>
+      <c r="D304">
+        <v>28</v>
+      </c>
+      <c r="E304">
+        <v>3</v>
+      </c>
+      <c r="F304">
+        <v>31</v>
+      </c>
+      <c r="G304" t="s">
+        <v>1</v>
+      </c>
+      <c r="H304" t="s">
+        <v>2</v>
+      </c>
+      <c r="I304" t="s">
+        <v>38</v>
+      </c>
+      <c r="J304">
+        <v>951</v>
+      </c>
+      <c r="K304">
+        <v>1</v>
+      </c>
+      <c r="L304" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M304" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N304">
+        <v>1.5</v>
+      </c>
+      <c r="O304">
+        <v>0.5</v>
+      </c>
+      <c r="P304">
+        <v>15.5</v>
+      </c>
+      <c r="Q304">
+        <v>3</v>
+      </c>
+      <c r="S304">
+        <v>6</v>
+      </c>
+      <c r="T304">
+        <v>2</v>
+      </c>
+      <c r="V304">
+        <v>27</v>
+      </c>
+      <c r="W304">
+        <v>9</v>
+      </c>
+      <c r="Z304">
+        <v>2.5</v>
+      </c>
+      <c r="AA304">
+        <v>1.5</v>
+      </c>
+      <c r="AB304">
+        <v>20</v>
+      </c>
+      <c r="AC304">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="305" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L305" s="2"/>
@@ -25935,14 +26008,6 @@
     <row r="462" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L462" s="2"/>
       <c r="M462" s="2"/>
-    </row>
-    <row r="463" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L463" s="2"/>
-      <c r="M463" s="2"/>
-    </row>
-    <row r="464" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L464" s="2"/>
-      <c r="M464" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ rollings + bva, ow, and cluster18 polls (4/1)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A6052F-731E-4844-AA95-5C7329A669F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945AE983-2156-5C47-87F1-98DC46C4B6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="3580" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="29100" yWindow="1580" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -556,9 +556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
   <dimension ref="A1:AH462"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A303" sqref="A303"/>
+      <selection pane="bottomLeft" activeCell="AC307" sqref="AC307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25311,7 +25311,7 @@
         <v>3</v>
       </c>
       <c r="D304">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E304">
         <v>3</v>
@@ -25320,40 +25320,40 @@
         <v>31</v>
       </c>
       <c r="G304" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="H304" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I304" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J304">
-        <v>951</v>
+        <v>2515</v>
       </c>
       <c r="K304">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L304" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M304" s="2">
         <v>0.5</v>
       </c>
       <c r="N304">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O304">
         <v>0.5</v>
       </c>
       <c r="P304">
-        <v>15.5</v>
+        <v>16</v>
       </c>
       <c r="Q304">
         <v>3</v>
       </c>
       <c r="S304">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T304">
         <v>2</v>
@@ -25362,82 +25362,447 @@
         <v>27</v>
       </c>
       <c r="W304">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Z304">
         <v>2.5</v>
       </c>
       <c r="AA304">
+        <v>3</v>
+      </c>
+      <c r="AB304">
+        <v>18</v>
+      </c>
+      <c r="AC304">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="305" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>203</v>
+      </c>
+      <c r="B305">
+        <v>2022</v>
+      </c>
+      <c r="C305">
+        <v>3</v>
+      </c>
+      <c r="D305">
+        <v>30</v>
+      </c>
+      <c r="E305">
+        <v>3</v>
+      </c>
+      <c r="F305">
+        <v>31</v>
+      </c>
+      <c r="G305" t="s">
+        <v>33</v>
+      </c>
+      <c r="H305" t="s">
+        <v>21</v>
+      </c>
+      <c r="I305" t="s">
+        <v>47</v>
+      </c>
+      <c r="J305">
+        <v>700</v>
+      </c>
+      <c r="K305">
+        <v>1</v>
+      </c>
+      <c r="L305" s="2">
+        <v>1</v>
+      </c>
+      <c r="M305" s="2">
+        <v>1</v>
+      </c>
+      <c r="N305">
+        <v>1</v>
+      </c>
+      <c r="O305">
+        <v>1</v>
+      </c>
+      <c r="P305">
+        <v>15</v>
+      </c>
+      <c r="Q305">
+        <v>4</v>
+      </c>
+      <c r="S305">
+        <v>5</v>
+      </c>
+      <c r="T305">
+        <v>2</v>
+      </c>
+      <c r="V305">
+        <v>27</v>
+      </c>
+      <c r="W305">
+        <v>10</v>
+      </c>
+      <c r="Z305">
+        <v>2</v>
+      </c>
+      <c r="AA305">
+        <v>3</v>
+      </c>
+      <c r="AB305">
+        <v>21</v>
+      </c>
+      <c r="AC305">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="306" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>204</v>
+      </c>
+      <c r="B306">
+        <v>2022</v>
+      </c>
+      <c r="C306">
+        <v>3</v>
+      </c>
+      <c r="D306">
+        <v>30</v>
+      </c>
+      <c r="E306">
+        <v>3</v>
+      </c>
+      <c r="F306">
+        <v>31</v>
+      </c>
+      <c r="G306" t="s">
+        <v>34</v>
+      </c>
+      <c r="H306" t="s">
+        <v>21</v>
+      </c>
+      <c r="I306" t="s">
+        <v>47</v>
+      </c>
+      <c r="J306">
+        <v>992</v>
+      </c>
+      <c r="K306">
+        <v>0</v>
+      </c>
+      <c r="L306" s="2">
+        <v>1</v>
+      </c>
+      <c r="M306" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N306">
+        <v>1</v>
+      </c>
+      <c r="O306">
+        <v>1</v>
+      </c>
+      <c r="P306">
+        <v>15.5</v>
+      </c>
+      <c r="Q306">
+        <v>3.5</v>
+      </c>
+      <c r="S306">
+        <v>5</v>
+      </c>
+      <c r="T306">
+        <v>2</v>
+      </c>
+      <c r="V306">
+        <v>27</v>
+      </c>
+      <c r="W306">
+        <v>9.5</v>
+      </c>
+      <c r="Z306">
+        <v>2.5</v>
+      </c>
+      <c r="AA306">
+        <v>2.5</v>
+      </c>
+      <c r="AB306">
+        <v>21</v>
+      </c>
+      <c r="AC306">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="307" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>205</v>
+      </c>
+      <c r="B307">
+        <v>2022</v>
+      </c>
+      <c r="C307">
+        <v>3</v>
+      </c>
+      <c r="D307">
+        <v>29</v>
+      </c>
+      <c r="E307">
+        <v>4</v>
+      </c>
+      <c r="F307">
+        <v>1</v>
+      </c>
+      <c r="G307" t="s">
+        <v>1</v>
+      </c>
+      <c r="H307" t="s">
+        <v>2</v>
+      </c>
+      <c r="I307" t="s">
+        <v>38</v>
+      </c>
+      <c r="J307">
+        <v>939</v>
+      </c>
+      <c r="K307">
+        <v>0</v>
+      </c>
+      <c r="L307" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M307" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N307">
+        <v>1</v>
+      </c>
+      <c r="O307">
+        <v>0.5</v>
+      </c>
+      <c r="P307">
+        <v>16</v>
+      </c>
+      <c r="Q307">
+        <v>3</v>
+      </c>
+      <c r="S307">
+        <v>6.5</v>
+      </c>
+      <c r="T307">
+        <v>2</v>
+      </c>
+      <c r="V307">
+        <v>26.5</v>
+      </c>
+      <c r="W307">
+        <v>9.5</v>
+      </c>
+      <c r="Z307">
+        <v>2.5</v>
+      </c>
+      <c r="AA307">
         <v>1.5</v>
       </c>
-      <c r="AB304">
+      <c r="AB307">
         <v>20</v>
       </c>
-      <c r="AC304">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="305" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L305" s="2"/>
-      <c r="M305" s="2"/>
-    </row>
-    <row r="306" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L306" s="2"/>
-      <c r="M306" s="2"/>
-    </row>
-    <row r="307" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L307" s="2"/>
-      <c r="M307" s="2"/>
-    </row>
-    <row r="308" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L308" s="2"/>
-      <c r="M308" s="2"/>
-    </row>
-    <row r="309" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L309" s="2"/>
-      <c r="M309" s="2"/>
-    </row>
-    <row r="310" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="AC307">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="308" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>206</v>
+      </c>
+      <c r="B308">
+        <v>2022</v>
+      </c>
+      <c r="C308">
+        <v>3</v>
+      </c>
+      <c r="D308">
+        <v>29</v>
+      </c>
+      <c r="E308">
+        <v>4</v>
+      </c>
+      <c r="F308">
+        <v>1</v>
+      </c>
+      <c r="G308" t="s">
+        <v>33</v>
+      </c>
+      <c r="H308" t="s">
+        <v>21</v>
+      </c>
+      <c r="I308" t="s">
+        <v>38</v>
+      </c>
+      <c r="J308">
+        <v>1119</v>
+      </c>
+      <c r="K308">
+        <v>1</v>
+      </c>
+      <c r="L308" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M308" s="2">
+        <v>1</v>
+      </c>
+      <c r="N308">
+        <v>1</v>
+      </c>
+      <c r="O308">
+        <v>1</v>
+      </c>
+      <c r="P308">
+        <v>15</v>
+      </c>
+      <c r="Q308">
+        <v>3</v>
+      </c>
+      <c r="S308">
+        <v>5</v>
+      </c>
+      <c r="T308">
+        <v>3</v>
+      </c>
+      <c r="V308">
+        <v>28</v>
+      </c>
+      <c r="W308">
+        <v>9</v>
+      </c>
+      <c r="Z308">
+        <v>3</v>
+      </c>
+      <c r="AA308">
+        <v>2</v>
+      </c>
+      <c r="AB308">
+        <v>20</v>
+      </c>
+      <c r="AC308">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="309" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>207</v>
+      </c>
+      <c r="B309">
+        <v>2022</v>
+      </c>
+      <c r="C309">
+        <v>3</v>
+      </c>
+      <c r="D309">
+        <v>29</v>
+      </c>
+      <c r="E309">
+        <v>4</v>
+      </c>
+      <c r="F309">
+        <v>1</v>
+      </c>
+      <c r="G309" t="s">
+        <v>29</v>
+      </c>
+      <c r="H309" t="s">
+        <v>22</v>
+      </c>
+      <c r="I309" t="s">
+        <v>38</v>
+      </c>
+      <c r="J309">
+        <v>1500</v>
+      </c>
+      <c r="K309">
+        <v>1</v>
+      </c>
+      <c r="L309" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M309" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N309">
+        <v>1</v>
+      </c>
+      <c r="O309">
+        <v>0.5</v>
+      </c>
+      <c r="P309">
+        <v>15</v>
+      </c>
+      <c r="Q309">
+        <v>3.5</v>
+      </c>
+      <c r="S309">
+        <v>4.5</v>
+      </c>
+      <c r="T309">
+        <v>1.5</v>
+      </c>
+      <c r="V309">
+        <v>28</v>
+      </c>
+      <c r="W309">
+        <v>9.5</v>
+      </c>
+      <c r="Z309">
+        <v>2</v>
+      </c>
+      <c r="AA309">
+        <v>2</v>
+      </c>
+      <c r="AB309">
+        <v>21.5</v>
+      </c>
+      <c r="AC309">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="310" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L310" s="2"/>
       <c r="M310" s="2"/>
     </row>
-    <row r="311" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L311" s="2"/>
       <c r="M311" s="2"/>
     </row>
-    <row r="312" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L312" s="2"/>
       <c r="M312" s="2"/>
     </row>
-    <row r="313" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L313" s="2"/>
       <c r="M313" s="2"/>
     </row>
-    <row r="314" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L314" s="2"/>
       <c r="M314" s="2"/>
     </row>
-    <row r="315" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L315" s="2"/>
       <c r="M315" s="2"/>
     </row>
-    <row r="316" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L316" s="2"/>
       <c r="M316" s="2"/>
     </row>
-    <row r="317" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L317" s="2"/>
       <c r="M317" s="2"/>
     </row>
-    <row r="318" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L318" s="2"/>
       <c r="M318" s="2"/>
     </row>
-    <row r="319" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L319" s="2"/>
       <c r="M319" s="2"/>
     </row>
-    <row r="320" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L320" s="2"/>
       <c r="M320" s="2"/>
     </row>

</xml_diff>

<commit_message>
update w/ rolling + elabe and ifop poll (4/2) + ow polls of the week
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945AE983-2156-5C47-87F1-98DC46C4B6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5D0AC5-F245-3941-9C19-9A95495729A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29100" yWindow="1580" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH462"/>
+  <dimension ref="A1:AH464"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AC307" sqref="AC307"/>
+      <pane ySplit="1" topLeftCell="A291" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD311" sqref="AD311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25003,70 +25003,70 @@
         <v>3</v>
       </c>
       <c r="D300">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E300">
         <v>3</v>
       </c>
       <c r="F300">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G300" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H300" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I300" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J300">
-        <v>951</v>
+        <v>772</v>
       </c>
       <c r="K300">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L300" s="2">
         <v>1</v>
       </c>
       <c r="M300" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N300">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O300">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P300">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="Q300">
         <v>3</v>
       </c>
       <c r="S300">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T300">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V300">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W300">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="Z300">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA300">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB300">
-        <v>20.5</v>
+        <v>20</v>
       </c>
       <c r="AC300">
-        <v>11.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="301" spans="1:29" x14ac:dyDescent="0.2">
@@ -25080,7 +25080,7 @@
         <v>3</v>
       </c>
       <c r="D301">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E301">
         <v>3</v>
@@ -25089,19 +25089,19 @@
         <v>30</v>
       </c>
       <c r="G301" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H301" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I301" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J301">
-        <v>966</v>
+        <v>951</v>
       </c>
       <c r="K301">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L301" s="2">
         <v>1</v>
@@ -25119,31 +25119,31 @@
         <v>15.5</v>
       </c>
       <c r="Q301">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="S301">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="T301">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V301">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W301">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="Z301">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AA301">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AB301">
-        <v>21</v>
+        <v>20.5</v>
       </c>
       <c r="AC301">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="302" spans="1:29" x14ac:dyDescent="0.2">
@@ -25163,19 +25163,19 @@
         <v>3</v>
       </c>
       <c r="F302">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G302" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H302" t="s">
         <v>21</v>
       </c>
       <c r="I302" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J302">
-        <v>1119</v>
+        <v>966</v>
       </c>
       <c r="K302">
         <v>1</v>
@@ -25184,22 +25184,22 @@
         <v>1</v>
       </c>
       <c r="M302" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N302">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O302">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P302">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="Q302">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="S302">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T302">
         <v>2</v>
@@ -25208,19 +25208,19 @@
         <v>28</v>
       </c>
       <c r="W302">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="Z302">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AA302">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB302">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AC302">
-        <v>10</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="303" spans="1:29" x14ac:dyDescent="0.2">
@@ -25234,25 +25234,25 @@
         <v>3</v>
       </c>
       <c r="D303">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E303">
         <v>3</v>
       </c>
       <c r="F303">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G303" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H303" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I303" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J303">
-        <v>1500</v>
+        <v>772</v>
       </c>
       <c r="K303">
         <v>1</v>
@@ -25261,43 +25261,43 @@
         <v>1</v>
       </c>
       <c r="M303" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N303">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O303">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P303">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="Q303">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S303">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T303">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V303">
         <v>28</v>
       </c>
       <c r="W303">
+        <v>11</v>
+      </c>
+      <c r="Z303">
+        <v>3</v>
+      </c>
+      <c r="AA303">
+        <v>1</v>
+      </c>
+      <c r="AB303">
+        <v>20</v>
+      </c>
+      <c r="AC303">
         <v>10</v>
-      </c>
-      <c r="Z303">
-        <v>2</v>
-      </c>
-      <c r="AA303">
-        <v>1.5</v>
-      </c>
-      <c r="AB303">
-        <v>21</v>
-      </c>
-      <c r="AC303">
-        <v>11</v>
       </c>
     </row>
     <row r="304" spans="1:29" x14ac:dyDescent="0.2">
@@ -25311,7 +25311,7 @@
         <v>3</v>
       </c>
       <c r="D304">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E304">
         <v>3</v>
@@ -25320,34 +25320,34 @@
         <v>31</v>
       </c>
       <c r="G304" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H304" t="s">
         <v>21</v>
       </c>
       <c r="I304" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J304">
-        <v>2515</v>
+        <v>1119</v>
       </c>
       <c r="K304">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L304" s="2">
         <v>1</v>
       </c>
       <c r="M304" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N304">
         <v>1</v>
       </c>
       <c r="O304">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P304">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q304">
         <v>3</v>
@@ -25359,22 +25359,22 @@
         <v>2</v>
       </c>
       <c r="V304">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W304">
         <v>10</v>
       </c>
       <c r="Z304">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AA304">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB304">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AC304">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="305" spans="1:29" x14ac:dyDescent="0.2">
@@ -25388,7 +25388,7 @@
         <v>3</v>
       </c>
       <c r="D305">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E305">
         <v>3</v>
@@ -25397,16 +25397,16 @@
         <v>31</v>
       </c>
       <c r="G305" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H305" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I305" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J305">
-        <v>700</v>
+        <v>1500</v>
       </c>
       <c r="K305">
         <v>1</v>
@@ -25415,28 +25415,28 @@
         <v>1</v>
       </c>
       <c r="M305" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N305">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O305">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P305">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="Q305">
         <v>4</v>
       </c>
       <c r="S305">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="T305">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V305">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W305">
         <v>10</v>
@@ -25445,13 +25445,13 @@
         <v>2</v>
       </c>
       <c r="AA305">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="AB305">
         <v>21</v>
       </c>
       <c r="AC305">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="306" spans="1:29" x14ac:dyDescent="0.2">
@@ -25465,7 +25465,7 @@
         <v>3</v>
       </c>
       <c r="D306">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E306">
         <v>3</v>
@@ -25474,7 +25474,7 @@
         <v>31</v>
       </c>
       <c r="G306" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H306" t="s">
         <v>21</v>
@@ -25483,7 +25483,7 @@
         <v>47</v>
       </c>
       <c r="J306">
-        <v>992</v>
+        <v>2515</v>
       </c>
       <c r="K306">
         <v>0</v>
@@ -25498,13 +25498,13 @@
         <v>1</v>
       </c>
       <c r="O306">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P306">
-        <v>15.5</v>
+        <v>16</v>
       </c>
       <c r="Q306">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S306">
         <v>5</v>
@@ -25516,19 +25516,19 @@
         <v>27</v>
       </c>
       <c r="W306">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="Z306">
         <v>2.5</v>
       </c>
       <c r="AA306">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AB306">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AC306">
-        <v>9.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="307" spans="1:29" x14ac:dyDescent="0.2">
@@ -25542,70 +25542,70 @@
         <v>3</v>
       </c>
       <c r="D307">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E307">
+        <v>3</v>
+      </c>
+      <c r="F307">
+        <v>31</v>
+      </c>
+      <c r="G307" t="s">
+        <v>33</v>
+      </c>
+      <c r="H307" t="s">
+        <v>21</v>
+      </c>
+      <c r="I307" t="s">
+        <v>47</v>
+      </c>
+      <c r="J307">
+        <v>700</v>
+      </c>
+      <c r="K307">
+        <v>1</v>
+      </c>
+      <c r="L307" s="2">
+        <v>1</v>
+      </c>
+      <c r="M307" s="2">
+        <v>1</v>
+      </c>
+      <c r="N307">
+        <v>1</v>
+      </c>
+      <c r="O307">
+        <v>1</v>
+      </c>
+      <c r="P307">
+        <v>15</v>
+      </c>
+      <c r="Q307">
         <v>4</v>
       </c>
-      <c r="F307">
-        <v>1</v>
-      </c>
-      <c r="G307" t="s">
-        <v>1</v>
-      </c>
-      <c r="H307" t="s">
-        <v>2</v>
-      </c>
-      <c r="I307" t="s">
-        <v>38</v>
-      </c>
-      <c r="J307">
-        <v>939</v>
-      </c>
-      <c r="K307">
-        <v>0</v>
-      </c>
-      <c r="L307" s="2">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="M307" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N307">
-        <v>1</v>
-      </c>
-      <c r="O307">
-        <v>0.5</v>
-      </c>
-      <c r="P307">
-        <v>16</v>
-      </c>
-      <c r="Q307">
-        <v>3</v>
-      </c>
       <c r="S307">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="T307">
         <v>2</v>
       </c>
       <c r="V307">
-        <v>26.5</v>
+        <v>27</v>
       </c>
       <c r="W307">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="Z307">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AA307">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AB307">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AC307">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="308" spans="1:29" x14ac:dyDescent="0.2">
@@ -25619,34 +25619,34 @@
         <v>3</v>
       </c>
       <c r="D308">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E308">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F308">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="G308" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H308" t="s">
         <v>21</v>
       </c>
       <c r="I308" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J308">
-        <v>1119</v>
+        <v>992</v>
       </c>
       <c r="K308">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L308" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M308" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N308">
         <v>1</v>
@@ -25655,34 +25655,34 @@
         <v>1</v>
       </c>
       <c r="P308">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="Q308">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="S308">
         <v>5</v>
       </c>
       <c r="T308">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V308">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W308">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="Z308">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AA308">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB308">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AC308">
-        <v>10</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="309" spans="1:29" x14ac:dyDescent="0.2">
@@ -25705,16 +25705,16 @@
         <v>1</v>
       </c>
       <c r="G309" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H309" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I309" t="s">
         <v>38</v>
       </c>
       <c r="J309">
-        <v>1500</v>
+        <v>1119</v>
       </c>
       <c r="K309">
         <v>1</v>
@@ -25723,60 +25723,352 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="M309" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N309">
         <v>1</v>
       </c>
       <c r="O309">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P309">
         <v>15</v>
       </c>
       <c r="Q309">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S309">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T309">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="V309">
         <v>28</v>
       </c>
       <c r="W309">
+        <v>9</v>
+      </c>
+      <c r="Z309">
+        <v>3</v>
+      </c>
+      <c r="AA309">
+        <v>2</v>
+      </c>
+      <c r="AB309">
+        <v>20</v>
+      </c>
+      <c r="AC309">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="310" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>208</v>
+      </c>
+      <c r="B310">
+        <v>2022</v>
+      </c>
+      <c r="C310">
+        <v>3</v>
+      </c>
+      <c r="D310">
+        <v>29</v>
+      </c>
+      <c r="E310">
+        <v>4</v>
+      </c>
+      <c r="F310">
+        <v>1</v>
+      </c>
+      <c r="G310" t="s">
+        <v>29</v>
+      </c>
+      <c r="H310" t="s">
+        <v>22</v>
+      </c>
+      <c r="I310" t="s">
+        <v>38</v>
+      </c>
+      <c r="J310">
+        <v>1500</v>
+      </c>
+      <c r="K310">
+        <v>1</v>
+      </c>
+      <c r="L310" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M310" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N310">
+        <v>1</v>
+      </c>
+      <c r="O310">
+        <v>0.5</v>
+      </c>
+      <c r="P310">
+        <v>15</v>
+      </c>
+      <c r="Q310">
+        <v>3.5</v>
+      </c>
+      <c r="S310">
+        <v>4.5</v>
+      </c>
+      <c r="T310">
+        <v>1.5</v>
+      </c>
+      <c r="V310">
+        <v>28</v>
+      </c>
+      <c r="W310">
         <v>9.5</v>
       </c>
-      <c r="Z309">
-        <v>2</v>
-      </c>
-      <c r="AA309">
-        <v>2</v>
-      </c>
-      <c r="AB309">
+      <c r="Z310">
+        <v>2</v>
+      </c>
+      <c r="AA310">
+        <v>2</v>
+      </c>
+      <c r="AB310">
         <v>21.5</v>
       </c>
-      <c r="AC309">
+      <c r="AC310">
         <v>11</v>
       </c>
     </row>
-    <row r="310" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L310" s="2"/>
-      <c r="M310" s="2"/>
-    </row>
     <row r="311" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L311" s="2"/>
-      <c r="M311" s="2"/>
+      <c r="A311">
+        <v>209</v>
+      </c>
+      <c r="B311">
+        <v>2022</v>
+      </c>
+      <c r="C311">
+        <v>3</v>
+      </c>
+      <c r="D311">
+        <v>31</v>
+      </c>
+      <c r="E311">
+        <v>4</v>
+      </c>
+      <c r="F311">
+        <v>1</v>
+      </c>
+      <c r="G311" t="s">
+        <v>29</v>
+      </c>
+      <c r="H311" t="s">
+        <v>22</v>
+      </c>
+      <c r="I311" t="s">
+        <v>47</v>
+      </c>
+      <c r="J311">
+        <v>1000</v>
+      </c>
+      <c r="K311">
+        <v>1</v>
+      </c>
+      <c r="L311" s="2">
+        <v>1</v>
+      </c>
+      <c r="M311" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N311">
+        <v>1</v>
+      </c>
+      <c r="O311">
+        <v>0.5</v>
+      </c>
+      <c r="P311">
+        <v>15</v>
+      </c>
+      <c r="Q311">
+        <v>3.5</v>
+      </c>
+      <c r="S311">
+        <v>5</v>
+      </c>
+      <c r="T311">
+        <v>2</v>
+      </c>
+      <c r="V311">
+        <v>27</v>
+      </c>
+      <c r="W311">
+        <v>9</v>
+      </c>
+      <c r="Z311">
+        <v>2.5</v>
+      </c>
+      <c r="AA311">
+        <v>2</v>
+      </c>
+      <c r="AB311">
+        <v>22</v>
+      </c>
+      <c r="AC311">
+        <v>10.5</v>
+      </c>
     </row>
     <row r="312" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L312" s="2"/>
-      <c r="M312" s="2"/>
+      <c r="A312">
+        <v>210</v>
+      </c>
+      <c r="B312">
+        <v>2022</v>
+      </c>
+      <c r="C312">
+        <v>3</v>
+      </c>
+      <c r="D312">
+        <v>30</v>
+      </c>
+      <c r="E312">
+        <v>4</v>
+      </c>
+      <c r="F312">
+        <v>2</v>
+      </c>
+      <c r="G312" t="s">
+        <v>1</v>
+      </c>
+      <c r="H312" t="s">
+        <v>2</v>
+      </c>
+      <c r="I312" t="s">
+        <v>38</v>
+      </c>
+      <c r="J312">
+        <v>1066</v>
+      </c>
+      <c r="K312">
+        <v>0</v>
+      </c>
+      <c r="L312" s="2">
+        <v>1</v>
+      </c>
+      <c r="M312" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N312">
+        <v>1.5</v>
+      </c>
+      <c r="O312">
+        <v>0.5</v>
+      </c>
+      <c r="P312">
+        <v>15.5</v>
+      </c>
+      <c r="Q312">
+        <v>3</v>
+      </c>
+      <c r="S312">
+        <v>6</v>
+      </c>
+      <c r="T312">
+        <v>2</v>
+      </c>
+      <c r="V312">
+        <v>26</v>
+      </c>
+      <c r="W312">
+        <v>9.5</v>
+      </c>
+      <c r="Z312">
+        <v>2.5</v>
+      </c>
+      <c r="AA312">
+        <v>1.5</v>
+      </c>
+      <c r="AB312">
+        <v>21</v>
+      </c>
+      <c r="AC312">
+        <v>11</v>
+      </c>
     </row>
     <row r="313" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L313" s="2"/>
-      <c r="M313" s="2"/>
+      <c r="A313">
+        <v>211</v>
+      </c>
+      <c r="B313">
+        <v>2022</v>
+      </c>
+      <c r="C313">
+        <v>3</v>
+      </c>
+      <c r="D313">
+        <v>31</v>
+      </c>
+      <c r="E313">
+        <v>4</v>
+      </c>
+      <c r="F313">
+        <v>2</v>
+      </c>
+      <c r="G313" t="s">
+        <v>30</v>
+      </c>
+      <c r="H313" t="s">
+        <v>21</v>
+      </c>
+      <c r="I313" t="s">
+        <v>47</v>
+      </c>
+      <c r="J313">
+        <v>999</v>
+      </c>
+      <c r="K313">
+        <v>0</v>
+      </c>
+      <c r="L313" s="2">
+        <v>1</v>
+      </c>
+      <c r="M313" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N313">
+        <v>1.5</v>
+      </c>
+      <c r="O313">
+        <v>0.5</v>
+      </c>
+      <c r="P313">
+        <v>15</v>
+      </c>
+      <c r="Q313">
+        <v>3.5</v>
+      </c>
+      <c r="S313">
+        <v>4.5</v>
+      </c>
+      <c r="T313">
+        <v>1.5</v>
+      </c>
+      <c r="V313">
+        <v>28.5</v>
+      </c>
+      <c r="W313">
+        <v>8.5</v>
+      </c>
+      <c r="Z313">
+        <v>2.5</v>
+      </c>
+      <c r="AA313">
+        <v>2.5</v>
+      </c>
+      <c r="AB313">
+        <v>22</v>
+      </c>
+      <c r="AC313">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="314" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L314" s="2"/>
@@ -26373,6 +26665,14 @@
     <row r="462" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L462" s="2"/>
       <c r="M462" s="2"/>
+    </row>
+    <row r="463" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L463" s="2"/>
+      <c r="M463" s="2"/>
+    </row>
+    <row r="464" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L464" s="2"/>
+      <c r="M464" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ rollings + harris poll (4/4)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5D0AC5-F245-3941-9C19-9A95495729A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDC2711-BF57-E148-A562-D70AD17AD282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29100" yWindow="1580" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="28180" yWindow="1880" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH464"/>
+  <dimension ref="A1:AH463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A291" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD311" sqref="AD311"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="Z310" sqref="Z310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24867,10 +24867,10 @@
         <v>47</v>
       </c>
       <c r="J298">
-        <v>1700</v>
+        <v>1791</v>
       </c>
       <c r="K298">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L298" s="2">
         <v>1</v>
@@ -25021,10 +25021,10 @@
         <v>47</v>
       </c>
       <c r="J300">
-        <v>772</v>
+        <v>720</v>
       </c>
       <c r="K300">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L300" s="2">
         <v>1</v>
@@ -25175,10 +25175,10 @@
         <v>47</v>
       </c>
       <c r="J302">
-        <v>966</v>
+        <v>977</v>
       </c>
       <c r="K302">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L302" s="2">
         <v>1</v>
@@ -25252,10 +25252,10 @@
         <v>47</v>
       </c>
       <c r="J303">
-        <v>772</v>
+        <v>723</v>
       </c>
       <c r="K303">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L303" s="2">
         <v>1</v>
@@ -25329,10 +25329,10 @@
         <v>38</v>
       </c>
       <c r="J304">
-        <v>1119</v>
+        <v>1083</v>
       </c>
       <c r="K304">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L304" s="2">
         <v>1</v>
@@ -25406,10 +25406,10 @@
         <v>38</v>
       </c>
       <c r="J305">
-        <v>1500</v>
+        <v>2256</v>
       </c>
       <c r="K305">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L305" s="2">
         <v>1</v>
@@ -25560,10 +25560,10 @@
         <v>47</v>
       </c>
       <c r="J307">
-        <v>700</v>
+        <v>743</v>
       </c>
       <c r="K307">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L307" s="2">
         <v>1</v>
@@ -25574,8 +25574,8 @@
       <c r="N307">
         <v>1</v>
       </c>
-      <c r="O307">
-        <v>1</v>
+      <c r="O307" t="s">
+        <v>31</v>
       </c>
       <c r="P307">
         <v>15</v>
@@ -25696,7 +25696,7 @@
         <v>3</v>
       </c>
       <c r="D309">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E309">
         <v>4</v>
@@ -25705,61 +25705,61 @@
         <v>1</v>
       </c>
       <c r="G309" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H309" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I309" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J309">
-        <v>1119</v>
+        <v>1000</v>
       </c>
       <c r="K309">
         <v>1</v>
       </c>
       <c r="L309" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M309" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N309">
         <v>1</v>
       </c>
       <c r="O309">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P309">
         <v>15</v>
       </c>
       <c r="Q309">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="S309">
         <v>5</v>
       </c>
       <c r="T309">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V309">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W309">
         <v>9</v>
       </c>
       <c r="Z309">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AA309">
         <v>2</v>
       </c>
       <c r="AB309">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AC309">
-        <v>10</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="310" spans="1:29" x14ac:dyDescent="0.2">
@@ -25773,67 +25773,67 @@
         <v>3</v>
       </c>
       <c r="D310">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E310">
         <v>4</v>
       </c>
       <c r="F310">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G310" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="H310" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I310" t="s">
         <v>38</v>
       </c>
       <c r="J310">
-        <v>1500</v>
+        <v>1066</v>
       </c>
       <c r="K310">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L310" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M310" s="2">
         <v>0.5</v>
       </c>
       <c r="N310">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O310">
         <v>0.5</v>
       </c>
       <c r="P310">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="Q310">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S310">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="T310">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V310">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W310">
         <v>9.5</v>
       </c>
       <c r="Z310">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AA310">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB310">
-        <v>21.5</v>
+        <v>21</v>
       </c>
       <c r="AC310">
         <v>11</v>
@@ -25856,22 +25856,22 @@
         <v>4</v>
       </c>
       <c r="F311">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G311" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H311" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I311" t="s">
         <v>47</v>
       </c>
       <c r="J311">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="K311">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L311" s="2">
         <v>1</v>
@@ -25880,7 +25880,7 @@
         <v>0.5</v>
       </c>
       <c r="N311">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O311">
         <v>0.5</v>
@@ -25892,28 +25892,28 @@
         <v>3.5</v>
       </c>
       <c r="S311">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="T311">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V311">
-        <v>27</v>
+        <v>28.5</v>
       </c>
       <c r="W311">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="Z311">
         <v>2.5</v>
       </c>
       <c r="AA311">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB311">
         <v>22</v>
       </c>
       <c r="AC311">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="312" spans="1:29" x14ac:dyDescent="0.2">
@@ -25924,49 +25924,49 @@
         <v>2022</v>
       </c>
       <c r="C312">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D312">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E312">
         <v>4</v>
       </c>
       <c r="F312">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G312" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H312" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I312" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J312">
-        <v>1066</v>
+        <v>700</v>
       </c>
       <c r="K312">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L312" s="2">
         <v>1</v>
       </c>
       <c r="M312" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N312">
-        <v>1.5</v>
-      </c>
-      <c r="O312">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="O312" t="s">
+        <v>31</v>
       </c>
       <c r="P312">
-        <v>15.5</v>
+        <v>14</v>
       </c>
       <c r="Q312">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S312">
         <v>6</v>
@@ -25975,22 +25975,22 @@
         <v>2</v>
       </c>
       <c r="V312">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W312">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="Z312">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AA312">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB312">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AC312">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="313" spans="1:29" x14ac:dyDescent="0.2">
@@ -26010,77 +26010,296 @@
         <v>4</v>
       </c>
       <c r="F313">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G313" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H313" t="s">
         <v>21</v>
       </c>
       <c r="I313" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J313">
-        <v>999</v>
+        <v>1119</v>
       </c>
       <c r="K313">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L313" s="2">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M313" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N313">
-        <v>1.5</v>
-      </c>
-      <c r="O313">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="O313" t="s">
+        <v>31</v>
       </c>
       <c r="P313">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q313">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S313">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="T313">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V313">
-        <v>28.5</v>
+        <v>28</v>
       </c>
       <c r="W313">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="Z313">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AA313">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AB313">
         <v>22</v>
       </c>
       <c r="AC313">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="314" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>212</v>
+      </c>
+      <c r="B314">
+        <v>2022</v>
+      </c>
+      <c r="C314">
+        <v>3</v>
+      </c>
+      <c r="D314">
+        <v>31</v>
+      </c>
+      <c r="E314">
+        <v>4</v>
+      </c>
+      <c r="F314">
+        <v>4</v>
+      </c>
+      <c r="G314" t="s">
+        <v>29</v>
+      </c>
+      <c r="H314" t="s">
+        <v>22</v>
+      </c>
+      <c r="I314" t="s">
+        <v>38</v>
+      </c>
+      <c r="J314">
+        <v>2500</v>
+      </c>
+      <c r="K314">
+        <v>1</v>
+      </c>
+      <c r="L314" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M314" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N314">
+        <v>1</v>
+      </c>
+      <c r="O314">
+        <v>0.5</v>
+      </c>
+      <c r="P314">
+        <v>15.5</v>
+      </c>
+      <c r="Q314">
+        <v>3</v>
+      </c>
+      <c r="S314">
+        <v>4.5</v>
+      </c>
+      <c r="T314">
+        <v>2</v>
+      </c>
+      <c r="V314">
+        <v>27.5</v>
+      </c>
+      <c r="W314">
+        <v>10</v>
+      </c>
+      <c r="Z314">
+        <v>2</v>
+      </c>
+      <c r="AA314">
+        <v>2</v>
+      </c>
+      <c r="AB314">
+        <v>22</v>
+      </c>
+      <c r="AC314">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="315" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>213</v>
+      </c>
+      <c r="B315">
+        <v>2022</v>
+      </c>
+      <c r="C315">
+        <v>3</v>
+      </c>
+      <c r="D315">
+        <v>31</v>
+      </c>
+      <c r="E315">
+        <v>4</v>
+      </c>
+      <c r="F315">
+        <v>4</v>
+      </c>
+      <c r="G315" t="s">
+        <v>1</v>
+      </c>
+      <c r="H315" t="s">
+        <v>2</v>
+      </c>
+      <c r="I315" t="s">
+        <v>38</v>
+      </c>
+      <c r="J315">
+        <v>913</v>
+      </c>
+      <c r="K315">
+        <v>0</v>
+      </c>
+      <c r="L315" s="2">
+        <v>1</v>
+      </c>
+      <c r="M315" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N315">
+        <v>1</v>
+      </c>
+      <c r="O315">
+        <v>0.5</v>
+      </c>
+      <c r="P315">
+        <v>16</v>
+      </c>
+      <c r="Q315">
+        <v>3.5</v>
+      </c>
+      <c r="S315">
+        <v>5.5</v>
+      </c>
+      <c r="T315">
+        <v>2</v>
+      </c>
+      <c r="V315">
+        <v>26.5</v>
+      </c>
+      <c r="W315">
+        <v>8.5</v>
+      </c>
+      <c r="Z315">
+        <v>3</v>
+      </c>
+      <c r="AA315">
+        <v>2</v>
+      </c>
+      <c r="AB315">
+        <v>21</v>
+      </c>
+      <c r="AC315">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="316" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>214</v>
+      </c>
+      <c r="B316">
+        <v>2022</v>
+      </c>
+      <c r="C316">
+        <v>4</v>
+      </c>
+      <c r="D316">
+        <v>1</v>
+      </c>
+      <c r="E316">
+        <v>4</v>
+      </c>
+      <c r="F316">
+        <v>4</v>
+      </c>
+      <c r="G316" t="s">
+        <v>20</v>
+      </c>
+      <c r="H316" t="s">
+        <v>22</v>
+      </c>
+      <c r="I316" t="s">
+        <v>47</v>
+      </c>
+      <c r="J316">
+        <v>1800</v>
+      </c>
+      <c r="K316">
+        <v>1</v>
+      </c>
+      <c r="L316" s="2">
+        <v>1</v>
+      </c>
+      <c r="M316" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N316">
+        <v>1</v>
+      </c>
+      <c r="O316">
+        <v>0.5</v>
+      </c>
+      <c r="P316">
+        <v>17</v>
+      </c>
+      <c r="Q316">
+        <v>2.5</v>
+      </c>
+      <c r="S316">
+        <v>5</v>
+      </c>
+      <c r="T316">
+        <v>2</v>
+      </c>
+      <c r="V316">
+        <v>26.5</v>
+      </c>
+      <c r="W316">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="314" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L314" s="2"/>
-      <c r="M314" s="2"/>
-    </row>
-    <row r="315" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L315" s="2"/>
-      <c r="M315" s="2"/>
-    </row>
-    <row r="316" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L316" s="2"/>
-      <c r="M316" s="2"/>
+      <c r="Z316">
+        <v>2</v>
+      </c>
+      <c r="AA316">
+        <v>1.5</v>
+      </c>
+      <c r="AB316">
+        <v>23</v>
+      </c>
+      <c r="AC316">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="317" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L317" s="2"/>
@@ -26669,10 +26888,6 @@
     <row r="463" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L463" s="2"/>
       <c r="M463" s="2"/>
-    </row>
-    <row r="464" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L464" s="2"/>
-      <c r="M464" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ rollings + cluster 17 poll (4/5)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDC2711-BF57-E148-A562-D70AD17AD282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BFCF6A-6A84-4A40-BC08-F09B5E3710DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28180" yWindow="1880" windowWidth="21480" windowHeight="13900" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
+    <workbookView xWindow="21800" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH463"/>
+  <dimension ref="A1:AH462"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="Z310" sqref="Z310"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AC317" sqref="AC317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25311,25 +25311,25 @@
         <v>3</v>
       </c>
       <c r="D304">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E304">
         <v>3</v>
       </c>
       <c r="F304">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G304" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="H304" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I304" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J304">
-        <v>1083</v>
+        <v>1103</v>
       </c>
       <c r="K304">
         <v>0</v>
@@ -25338,43 +25338,43 @@
         <v>1</v>
       </c>
       <c r="M304" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N304">
         <v>1</v>
       </c>
       <c r="O304">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P304">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="Q304">
         <v>3</v>
       </c>
       <c r="S304">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T304">
         <v>2</v>
       </c>
       <c r="V304">
-        <v>28</v>
+        <v>27.5</v>
       </c>
       <c r="W304">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Z304">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA304">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB304">
         <v>20</v>
       </c>
       <c r="AC304">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="305" spans="1:29" x14ac:dyDescent="0.2">
@@ -25397,16 +25397,16 @@
         <v>31</v>
       </c>
       <c r="G305" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H305" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I305" t="s">
         <v>38</v>
       </c>
       <c r="J305">
-        <v>2256</v>
+        <v>1083</v>
       </c>
       <c r="K305">
         <v>0</v>
@@ -25415,25 +25415,25 @@
         <v>1</v>
       </c>
       <c r="M305" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N305">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O305">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P305">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="Q305">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S305">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T305">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V305">
         <v>28</v>
@@ -25442,16 +25442,16 @@
         <v>10</v>
       </c>
       <c r="Z305">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA305">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB305">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC305">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="306" spans="1:29" x14ac:dyDescent="0.2">
@@ -25465,7 +25465,7 @@
         <v>3</v>
       </c>
       <c r="D306">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E306">
         <v>3</v>
@@ -25474,16 +25474,16 @@
         <v>31</v>
       </c>
       <c r="G306" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H306" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I306" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J306">
-        <v>2515</v>
+        <v>2256</v>
       </c>
       <c r="K306">
         <v>0</v>
@@ -25495,40 +25495,40 @@
         <v>0.5</v>
       </c>
       <c r="N306">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O306">
         <v>0.5</v>
       </c>
       <c r="P306">
-        <v>16</v>
+        <v>15.5</v>
       </c>
       <c r="Q306">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S306">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="T306">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V306">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W306">
         <v>10</v>
       </c>
       <c r="Z306">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AA306">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="AB306">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="AC306">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="307" spans="1:29" x14ac:dyDescent="0.2">
@@ -25542,7 +25542,7 @@
         <v>3</v>
       </c>
       <c r="D307">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E307">
         <v>3</v>
@@ -25551,7 +25551,7 @@
         <v>31</v>
       </c>
       <c r="G307" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H307" t="s">
         <v>21</v>
@@ -25560,7 +25560,7 @@
         <v>47</v>
       </c>
       <c r="J307">
-        <v>743</v>
+        <v>2515</v>
       </c>
       <c r="K307">
         <v>0</v>
@@ -25569,19 +25569,19 @@
         <v>1</v>
       </c>
       <c r="M307" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N307">
         <v>1</v>
       </c>
-      <c r="O307" t="s">
-        <v>31</v>
+      <c r="O307">
+        <v>0.5</v>
       </c>
       <c r="P307">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q307">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S307">
         <v>5</v>
@@ -25596,16 +25596,16 @@
         <v>10</v>
       </c>
       <c r="Z307">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AA307">
         <v>3</v>
       </c>
       <c r="AB307">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AC307">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="308" spans="1:29" x14ac:dyDescent="0.2">
@@ -25628,7 +25628,7 @@
         <v>31</v>
       </c>
       <c r="G308" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H308" t="s">
         <v>21</v>
@@ -25637,7 +25637,7 @@
         <v>47</v>
       </c>
       <c r="J308">
-        <v>992</v>
+        <v>743</v>
       </c>
       <c r="K308">
         <v>0</v>
@@ -25646,19 +25646,19 @@
         <v>1</v>
       </c>
       <c r="M308" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N308">
         <v>1</v>
       </c>
-      <c r="O308">
-        <v>1</v>
+      <c r="O308" t="s">
+        <v>31</v>
       </c>
       <c r="P308">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="Q308">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S308">
         <v>5</v>
@@ -25670,19 +25670,19 @@
         <v>27</v>
       </c>
       <c r="W308">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="Z308">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AA308">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AB308">
         <v>21</v>
       </c>
       <c r="AC308">
-        <v>9.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="309" spans="1:29" x14ac:dyDescent="0.2">
@@ -25696,28 +25696,28 @@
         <v>3</v>
       </c>
       <c r="D309">
+        <v>30</v>
+      </c>
+      <c r="E309">
+        <v>3</v>
+      </c>
+      <c r="F309">
         <v>31</v>
       </c>
-      <c r="E309">
-        <v>4</v>
-      </c>
-      <c r="F309">
-        <v>1</v>
-      </c>
       <c r="G309" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H309" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I309" t="s">
         <v>47</v>
       </c>
       <c r="J309">
-        <v>1000</v>
+        <v>992</v>
       </c>
       <c r="K309">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L309" s="2">
         <v>1</v>
@@ -25729,10 +25729,10 @@
         <v>1</v>
       </c>
       <c r="O309">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P309">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="Q309">
         <v>3.5</v>
@@ -25747,19 +25747,19 @@
         <v>27</v>
       </c>
       <c r="W309">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="Z309">
         <v>2.5</v>
       </c>
       <c r="AA309">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB309">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AC309">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="310" spans="1:29" x14ac:dyDescent="0.2">
@@ -25773,25 +25773,25 @@
         <v>3</v>
       </c>
       <c r="D310">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E310">
         <v>4</v>
       </c>
       <c r="F310">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G310" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="H310" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I310" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J310">
-        <v>1066</v>
+        <v>1052</v>
       </c>
       <c r="K310">
         <v>0</v>
@@ -25803,40 +25803,40 @@
         <v>0.5</v>
       </c>
       <c r="N310">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O310">
         <v>0.5</v>
       </c>
       <c r="P310">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="Q310">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="S310">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T310">
         <v>2</v>
       </c>
       <c r="V310">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W310">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="Z310">
         <v>2.5</v>
       </c>
       <c r="AA310">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB310">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AC310">
-        <v>11</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="311" spans="1:29" x14ac:dyDescent="0.2">
@@ -25850,7 +25850,7 @@
         <v>3</v>
       </c>
       <c r="D311">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E311">
         <v>4</v>
@@ -25859,16 +25859,16 @@
         <v>2</v>
       </c>
       <c r="G311" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H311" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I311" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J311">
-        <v>999</v>
+        <v>1066</v>
       </c>
       <c r="K311">
         <v>0</v>
@@ -25886,34 +25886,34 @@
         <v>0.5</v>
       </c>
       <c r="P311">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="Q311">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S311">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="T311">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V311">
-        <v>28.5</v>
+        <v>26</v>
       </c>
       <c r="W311">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="Z311">
         <v>2.5</v>
       </c>
       <c r="AA311">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AB311">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AC311">
-        <v>9.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="312" spans="1:29" x14ac:dyDescent="0.2">
@@ -25924,19 +25924,19 @@
         <v>2022</v>
       </c>
       <c r="C312">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D312">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="E312">
         <v>4</v>
       </c>
       <c r="F312">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G312" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H312" t="s">
         <v>21</v>
@@ -25945,52 +25945,52 @@
         <v>47</v>
       </c>
       <c r="J312">
-        <v>700</v>
+        <v>999</v>
       </c>
       <c r="K312">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L312" s="2">
         <v>1</v>
       </c>
       <c r="M312" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N312">
-        <v>1</v>
-      </c>
-      <c r="O312" t="s">
-        <v>31</v>
+        <v>1.5</v>
+      </c>
+      <c r="O312">
+        <v>0.5</v>
       </c>
       <c r="P312">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q312">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S312">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="T312">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V312">
-        <v>27</v>
+        <v>28.5</v>
       </c>
       <c r="W312">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="Z312">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AA312">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB312">
         <v>22</v>
       </c>
       <c r="AC312">
-        <v>9</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="313" spans="1:29" x14ac:dyDescent="0.2">
@@ -26001,16 +26001,16 @@
         <v>2022</v>
       </c>
       <c r="C313">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D313">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E313">
         <v>4</v>
       </c>
       <c r="F313">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G313" t="s">
         <v>33</v>
@@ -26019,16 +26019,16 @@
         <v>21</v>
       </c>
       <c r="I313" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J313">
-        <v>1119</v>
+        <v>700</v>
       </c>
       <c r="K313">
         <v>1</v>
       </c>
       <c r="L313" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M313" s="2">
         <v>1</v>
@@ -26043,7 +26043,7 @@
         <v>14</v>
       </c>
       <c r="Q313">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S313">
         <v>6</v>
@@ -26052,16 +26052,16 @@
         <v>2</v>
       </c>
       <c r="V313">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W313">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Z313">
         <v>3</v>
       </c>
       <c r="AA313">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB313">
         <v>22</v>
@@ -26078,10 +26078,10 @@
         <v>2022</v>
       </c>
       <c r="C314">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D314">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E314">
         <v>4</v>
@@ -26090,22 +26090,22 @@
         <v>4</v>
       </c>
       <c r="G314" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H314" t="s">
         <v>22</v>
       </c>
       <c r="I314" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J314">
-        <v>2500</v>
+        <v>1892</v>
       </c>
       <c r="K314">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L314" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M314" s="2">
         <v>0.5</v>
@@ -26117,34 +26117,34 @@
         <v>0.5</v>
       </c>
       <c r="P314">
-        <v>15.5</v>
+        <v>17</v>
       </c>
       <c r="Q314">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="S314">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T314">
         <v>2</v>
       </c>
       <c r="V314">
-        <v>27.5</v>
+        <v>26.5</v>
       </c>
       <c r="W314">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="Z314">
         <v>2</v>
       </c>
       <c r="AA314">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB314">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AC314">
-        <v>10</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="315" spans="1:29" x14ac:dyDescent="0.2">
@@ -26155,10 +26155,10 @@
         <v>2022</v>
       </c>
       <c r="C315">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D315">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E315">
         <v>4</v>
@@ -26167,16 +26167,16 @@
         <v>4</v>
       </c>
       <c r="G315" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="H315" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I315" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J315">
-        <v>913</v>
+        <v>2793</v>
       </c>
       <c r="K315">
         <v>0</v>
@@ -26194,34 +26194,34 @@
         <v>0.5</v>
       </c>
       <c r="P315">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q315">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="S315">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="T315">
         <v>2</v>
       </c>
       <c r="V315">
-        <v>26.5</v>
+        <v>26</v>
       </c>
       <c r="W315">
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="Z315">
         <v>3</v>
       </c>
       <c r="AA315">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB315">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC315">
-        <v>10.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="316" spans="1:29" x14ac:dyDescent="0.2">
@@ -26241,19 +26241,19 @@
         <v>4</v>
       </c>
       <c r="F316">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G316" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="H316" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I316" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J316">
-        <v>1800</v>
+        <v>1119</v>
       </c>
       <c r="K316">
         <v>1</v>
@@ -26262,52 +26262,198 @@
         <v>1</v>
       </c>
       <c r="M316" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N316">
         <v>1</v>
       </c>
-      <c r="O316">
-        <v>0.5</v>
+      <c r="O316" t="s">
+        <v>31</v>
       </c>
       <c r="P316">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q316">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="S316">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T316">
         <v>2</v>
       </c>
       <c r="V316">
-        <v>26.5</v>
+        <v>27</v>
       </c>
       <c r="W316">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="Z316">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA316">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AB316">
         <v>23</v>
       </c>
       <c r="AC316">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="317" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>215</v>
+      </c>
+      <c r="B317">
+        <v>2022</v>
+      </c>
+      <c r="C317">
+        <v>4</v>
+      </c>
+      <c r="D317">
+        <v>1</v>
+      </c>
+      <c r="E317">
+        <v>4</v>
+      </c>
+      <c r="F317">
+        <v>5</v>
+      </c>
+      <c r="G317" t="s">
+        <v>29</v>
+      </c>
+      <c r="H317" t="s">
+        <v>22</v>
+      </c>
+      <c r="I317" t="s">
+        <v>38</v>
+      </c>
+      <c r="J317">
+        <v>2500</v>
+      </c>
+      <c r="K317">
+        <v>1</v>
+      </c>
+      <c r="L317" s="2">
+        <v>1</v>
+      </c>
+      <c r="M317" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N317">
+        <v>0.5</v>
+      </c>
+      <c r="O317">
+        <v>0.5</v>
+      </c>
+      <c r="P317">
+        <v>16.5</v>
+      </c>
+      <c r="Q317">
+        <v>3</v>
+      </c>
+      <c r="S317">
+        <v>4.5</v>
+      </c>
+      <c r="T317">
+        <v>2.5</v>
+      </c>
+      <c r="V317">
+        <v>27</v>
+      </c>
+      <c r="W317">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="317" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L317" s="2"/>
-      <c r="M317" s="2"/>
+      <c r="Z317">
+        <v>2</v>
+      </c>
+      <c r="AA317">
+        <v>1.5</v>
+      </c>
+      <c r="AB317">
+        <v>23</v>
+      </c>
+      <c r="AC317">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="318" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L318" s="2"/>
-      <c r="M318" s="2"/>
+      <c r="A318">
+        <v>216</v>
+      </c>
+      <c r="B318">
+        <v>2022</v>
+      </c>
+      <c r="C318">
+        <v>4</v>
+      </c>
+      <c r="D318">
+        <v>3</v>
+      </c>
+      <c r="E318">
+        <v>4</v>
+      </c>
+      <c r="F318">
+        <v>5</v>
+      </c>
+      <c r="G318" t="s">
+        <v>1</v>
+      </c>
+      <c r="H318" t="s">
+        <v>2</v>
+      </c>
+      <c r="I318" t="s">
+        <v>38</v>
+      </c>
+      <c r="J318">
+        <v>949</v>
+      </c>
+      <c r="K318">
+        <v>0</v>
+      </c>
+      <c r="L318" s="2">
+        <v>1</v>
+      </c>
+      <c r="M318" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N318">
+        <v>1</v>
+      </c>
+      <c r="O318">
+        <v>0.5</v>
+      </c>
+      <c r="P318">
+        <v>16.5</v>
+      </c>
+      <c r="Q318">
+        <v>3.5</v>
+      </c>
+      <c r="S318">
+        <v>5.5</v>
+      </c>
+      <c r="T318">
+        <v>2</v>
+      </c>
+      <c r="V318">
+        <v>27</v>
+      </c>
+      <c r="W318">
+        <v>8</v>
+      </c>
+      <c r="Z318">
+        <v>3</v>
+      </c>
+      <c r="AA318">
+        <v>2.5</v>
+      </c>
+      <c r="AB318">
+        <v>20.5</v>
+      </c>
+      <c r="AC318">
+        <v>10</v>
+      </c>
     </row>
     <row r="319" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L319" s="2"/>
@@ -26884,10 +27030,6 @@
     <row r="462" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L462" s="2"/>
       <c r="M462" s="2"/>
-    </row>
-    <row r="463" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L463" s="2"/>
-      <c r="M463" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ elabe and kantar polls (5/4)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BFCF6A-6A84-4A40-BC08-F09B5E3710DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2447C3E-4554-D444-BC5A-339223F29921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21800" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -556,9 +556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
   <dimension ref="A1:AH462"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AC317" sqref="AC317"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AB316" sqref="AB316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26456,12 +26456,158 @@
       </c>
     </row>
     <row r="319" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L319" s="2"/>
-      <c r="M319" s="2"/>
+      <c r="A319">
+        <v>217</v>
+      </c>
+      <c r="B319">
+        <v>2022</v>
+      </c>
+      <c r="C319">
+        <v>4</v>
+      </c>
+      <c r="D319">
+        <v>4</v>
+      </c>
+      <c r="E319">
+        <v>4</v>
+      </c>
+      <c r="F319">
+        <v>5</v>
+      </c>
+      <c r="G319" t="s">
+        <v>30</v>
+      </c>
+      <c r="H319" t="s">
+        <v>21</v>
+      </c>
+      <c r="I319" t="s">
+        <v>47</v>
+      </c>
+      <c r="J319">
+        <v>1000</v>
+      </c>
+      <c r="K319">
+        <v>1</v>
+      </c>
+      <c r="L319" s="2">
+        <v>1</v>
+      </c>
+      <c r="M319" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N319">
+        <v>1.5</v>
+      </c>
+      <c r="O319">
+        <v>0.5</v>
+      </c>
+      <c r="P319">
+        <v>15.5</v>
+      </c>
+      <c r="Q319">
+        <v>2.5</v>
+      </c>
+      <c r="S319">
+        <v>5</v>
+      </c>
+      <c r="T319">
+        <v>2</v>
+      </c>
+      <c r="V319">
+        <v>28</v>
+      </c>
+      <c r="W319">
+        <v>8</v>
+      </c>
+      <c r="Z319">
+        <v>3</v>
+      </c>
+      <c r="AA319">
+        <v>2</v>
+      </c>
+      <c r="AB319">
+        <v>23</v>
+      </c>
+      <c r="AC319">
+        <v>9</v>
+      </c>
     </row>
     <row r="320" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L320" s="2"/>
-      <c r="M320" s="2"/>
+      <c r="A320">
+        <v>218</v>
+      </c>
+      <c r="B320">
+        <v>2022</v>
+      </c>
+      <c r="C320">
+        <v>4</v>
+      </c>
+      <c r="D320">
+        <v>4</v>
+      </c>
+      <c r="E320">
+        <v>4</v>
+      </c>
+      <c r="F320">
+        <v>5</v>
+      </c>
+      <c r="G320" t="s">
+        <v>50</v>
+      </c>
+      <c r="H320" t="s">
+        <v>21</v>
+      </c>
+      <c r="I320" t="s">
+        <v>47</v>
+      </c>
+      <c r="J320">
+        <v>1032</v>
+      </c>
+      <c r="K320">
+        <v>0</v>
+      </c>
+      <c r="L320" s="2">
+        <v>1</v>
+      </c>
+      <c r="M320" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N320">
+        <v>1</v>
+      </c>
+      <c r="O320">
+        <v>0.5</v>
+      </c>
+      <c r="P320">
+        <v>16</v>
+      </c>
+      <c r="Q320">
+        <v>3</v>
+      </c>
+      <c r="S320">
+        <v>5</v>
+      </c>
+      <c r="T320">
+        <v>2.5</v>
+      </c>
+      <c r="V320">
+        <v>25</v>
+      </c>
+      <c r="W320">
+        <v>8</v>
+      </c>
+      <c r="Z320">
+        <v>3</v>
+      </c>
+      <c r="AA320">
+        <v>2</v>
+      </c>
+      <c r="AB320">
+        <v>23</v>
+      </c>
+      <c r="AC320">
+        <v>11</v>
+      </c>
     </row>
     <row r="321" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L321" s="2"/>

</xml_diff>

<commit_message>
update w/ rollings + ipsos poll (4/6)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2447C3E-4554-D444-BC5A-339223F29921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7438ED62-2EF5-7F42-87E6-BEFA933CF599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21800" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="51">
   <si>
     <t>year</t>
   </si>
@@ -554,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH462"/>
+  <dimension ref="A1:AH466"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AB316" sqref="AB316"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A301" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AC323" sqref="AC323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23407,7 +23407,7 @@
         <v>1051</v>
       </c>
       <c r="K279">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L279" s="2">
         <v>1</v>
@@ -26235,46 +26235,46 @@
         <v>4</v>
       </c>
       <c r="D316">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E316">
         <v>4</v>
       </c>
       <c r="F316">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G316" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="H316" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I316" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J316">
-        <v>1119</v>
+        <v>7037</v>
       </c>
       <c r="K316">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L316" s="2">
         <v>1</v>
       </c>
       <c r="M316" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N316">
         <v>1</v>
       </c>
-      <c r="O316" t="s">
-        <v>31</v>
+      <c r="O316">
+        <v>0.5</v>
       </c>
       <c r="P316">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q316">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="S316">
         <v>6</v>
@@ -26283,22 +26283,22 @@
         <v>2</v>
       </c>
       <c r="V316">
-        <v>27</v>
+        <v>26.5</v>
       </c>
       <c r="W316">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="Z316">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AA316">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB316">
-        <v>23</v>
+        <v>21.5</v>
       </c>
       <c r="AC316">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="317" spans="1:29" x14ac:dyDescent="0.2">
@@ -26312,70 +26312,70 @@
         <v>4</v>
       </c>
       <c r="D317">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E317">
         <v>4</v>
       </c>
       <c r="F317">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G317" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H317" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I317" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J317">
-        <v>2500</v>
+        <v>801</v>
       </c>
       <c r="K317">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L317" s="2">
         <v>1</v>
       </c>
       <c r="M317" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N317">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O317">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P317">
-        <v>16.5</v>
+        <v>14</v>
       </c>
       <c r="Q317">
         <v>3</v>
       </c>
       <c r="S317">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="T317">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="V317">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W317">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="Z317">
         <v>2</v>
       </c>
       <c r="AA317">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AB317">
         <v>23</v>
       </c>
       <c r="AC317">
-        <v>9.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="318" spans="1:29" x14ac:dyDescent="0.2">
@@ -26389,7 +26389,7 @@
         <v>4</v>
       </c>
       <c r="D318">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E318">
         <v>4</v>
@@ -26398,16 +26398,16 @@
         <v>5</v>
       </c>
       <c r="G318" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H318" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I318" t="s">
         <v>38</v>
       </c>
       <c r="J318">
-        <v>949</v>
+        <v>1280</v>
       </c>
       <c r="K318">
         <v>0</v>
@@ -26416,22 +26416,22 @@
         <v>1</v>
       </c>
       <c r="M318" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N318">
         <v>1</v>
       </c>
-      <c r="O318">
-        <v>0.5</v>
+      <c r="O318" t="s">
+        <v>31</v>
       </c>
       <c r="P318">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="Q318">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S318">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="T318">
         <v>2</v>
@@ -26440,19 +26440,19 @@
         <v>27</v>
       </c>
       <c r="W318">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Z318">
         <v>3</v>
       </c>
       <c r="AA318">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AB318">
-        <v>20.5</v>
+        <v>23</v>
       </c>
       <c r="AC318">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="319" spans="1:29" x14ac:dyDescent="0.2">
@@ -26466,7 +26466,7 @@
         <v>4</v>
       </c>
       <c r="D319">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E319">
         <v>4</v>
@@ -26475,19 +26475,19 @@
         <v>5</v>
       </c>
       <c r="G319" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H319" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I319" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J319">
-        <v>1000</v>
+        <v>2293</v>
       </c>
       <c r="K319">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L319" s="2">
         <v>1</v>
@@ -26496,40 +26496,40 @@
         <v>0.5</v>
       </c>
       <c r="N319">
+        <v>0.5</v>
+      </c>
+      <c r="O319">
+        <v>0.5</v>
+      </c>
+      <c r="P319">
+        <v>16.5</v>
+      </c>
+      <c r="Q319">
+        <v>3</v>
+      </c>
+      <c r="S319">
+        <v>4.5</v>
+      </c>
+      <c r="T319">
+        <v>2.5</v>
+      </c>
+      <c r="V319">
+        <v>27</v>
+      </c>
+      <c r="W319">
+        <v>9.5</v>
+      </c>
+      <c r="Z319">
+        <v>2</v>
+      </c>
+      <c r="AA319">
         <v>1.5</v>
-      </c>
-      <c r="O319">
-        <v>0.5</v>
-      </c>
-      <c r="P319">
-        <v>15.5</v>
-      </c>
-      <c r="Q319">
-        <v>2.5</v>
-      </c>
-      <c r="S319">
-        <v>5</v>
-      </c>
-      <c r="T319">
-        <v>2</v>
-      </c>
-      <c r="V319">
-        <v>28</v>
-      </c>
-      <c r="W319">
-        <v>8</v>
-      </c>
-      <c r="Z319">
-        <v>3</v>
-      </c>
-      <c r="AA319">
-        <v>2</v>
       </c>
       <c r="AB319">
         <v>23</v>
       </c>
       <c r="AC319">
-        <v>9</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="320" spans="1:29" x14ac:dyDescent="0.2">
@@ -26543,7 +26543,7 @@
         <v>4</v>
       </c>
       <c r="D320">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E320">
         <v>4</v>
@@ -26552,16 +26552,16 @@
         <v>5</v>
       </c>
       <c r="G320" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="H320" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I320" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J320">
-        <v>1032</v>
+        <v>949</v>
       </c>
       <c r="K320">
         <v>0</v>
@@ -26579,19 +26579,19 @@
         <v>0.5</v>
       </c>
       <c r="P320">
-        <v>16</v>
+        <v>16.5</v>
       </c>
       <c r="Q320">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="S320">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="T320">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V320">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="W320">
         <v>8</v>
@@ -26600,76 +26600,514 @@
         <v>3</v>
       </c>
       <c r="AA320">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB320">
+        <v>20.5</v>
+      </c>
+      <c r="AC320">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="321" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <v>219</v>
+      </c>
+      <c r="B321">
+        <v>2022</v>
+      </c>
+      <c r="C321">
+        <v>4</v>
+      </c>
+      <c r="D321">
+        <v>4</v>
+      </c>
+      <c r="E321">
+        <v>4</v>
+      </c>
+      <c r="F321">
+        <v>5</v>
+      </c>
+      <c r="G321" t="s">
+        <v>30</v>
+      </c>
+      <c r="H321" t="s">
+        <v>21</v>
+      </c>
+      <c r="I321" t="s">
+        <v>47</v>
+      </c>
+      <c r="J321">
+        <v>993</v>
+      </c>
+      <c r="K321">
+        <v>0</v>
+      </c>
+      <c r="L321" s="2">
+        <v>1</v>
+      </c>
+      <c r="M321" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N321">
+        <v>1.5</v>
+      </c>
+      <c r="O321">
+        <v>0.5</v>
+      </c>
+      <c r="P321">
+        <v>15.5</v>
+      </c>
+      <c r="Q321">
+        <v>2.5</v>
+      </c>
+      <c r="S321">
+        <v>5</v>
+      </c>
+      <c r="T321">
+        <v>2</v>
+      </c>
+      <c r="V321">
+        <v>28</v>
+      </c>
+      <c r="W321">
+        <v>8</v>
+      </c>
+      <c r="Z321">
+        <v>3</v>
+      </c>
+      <c r="AA321">
+        <v>2</v>
+      </c>
+      <c r="AB321">
         <v>23</v>
       </c>
-      <c r="AC320">
+      <c r="AC321">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="322" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A322">
+        <v>220</v>
+      </c>
+      <c r="B322">
+        <v>2022</v>
+      </c>
+      <c r="C322">
+        <v>4</v>
+      </c>
+      <c r="D322">
+        <v>4</v>
+      </c>
+      <c r="E322">
+        <v>4</v>
+      </c>
+      <c r="F322">
+        <v>5</v>
+      </c>
+      <c r="G322" t="s">
+        <v>50</v>
+      </c>
+      <c r="H322" t="s">
+        <v>21</v>
+      </c>
+      <c r="I322" t="s">
+        <v>47</v>
+      </c>
+      <c r="J322">
+        <v>1032</v>
+      </c>
+      <c r="K322">
+        <v>0</v>
+      </c>
+      <c r="L322" s="2">
+        <v>1</v>
+      </c>
+      <c r="M322" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N322">
+        <v>1</v>
+      </c>
+      <c r="O322">
+        <v>0.5</v>
+      </c>
+      <c r="P322">
+        <v>16</v>
+      </c>
+      <c r="Q322">
+        <v>3</v>
+      </c>
+      <c r="S322">
+        <v>5</v>
+      </c>
+      <c r="T322">
+        <v>2.5</v>
+      </c>
+      <c r="V322">
+        <v>25</v>
+      </c>
+      <c r="W322">
+        <v>8</v>
+      </c>
+      <c r="Z322">
+        <v>3</v>
+      </c>
+      <c r="AA322">
+        <v>2</v>
+      </c>
+      <c r="AB322">
+        <v>23</v>
+      </c>
+      <c r="AC322">
         <v>11</v>
       </c>
     </row>
-    <row r="321" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L321" s="2"/>
-      <c r="M321" s="2"/>
-    </row>
-    <row r="322" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L322" s="2"/>
-      <c r="M322" s="2"/>
-    </row>
-    <row r="323" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L323" s="2"/>
-      <c r="M323" s="2"/>
-    </row>
-    <row r="324" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L324" s="2"/>
-      <c r="M324" s="2"/>
-    </row>
-    <row r="325" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L325" s="2"/>
-      <c r="M325" s="2"/>
-    </row>
-    <row r="326" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L326" s="2"/>
-      <c r="M326" s="2"/>
-    </row>
-    <row r="327" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A323">
+        <v>221</v>
+      </c>
+      <c r="B323">
+        <v>2022</v>
+      </c>
+      <c r="C323">
+        <v>4</v>
+      </c>
+      <c r="D323">
+        <v>4</v>
+      </c>
+      <c r="E323">
+        <v>4</v>
+      </c>
+      <c r="F323">
+        <v>5</v>
+      </c>
+      <c r="G323" t="s">
+        <v>33</v>
+      </c>
+      <c r="H323" t="s">
+        <v>21</v>
+      </c>
+      <c r="I323" t="s">
+        <v>47</v>
+      </c>
+      <c r="J323">
+        <v>888</v>
+      </c>
+      <c r="K323">
+        <v>0</v>
+      </c>
+      <c r="L323" s="2">
+        <v>1</v>
+      </c>
+      <c r="M323" s="2">
+        <v>1</v>
+      </c>
+      <c r="N323">
+        <v>1</v>
+      </c>
+      <c r="O323" t="s">
+        <v>31</v>
+      </c>
+      <c r="P323">
+        <v>15</v>
+      </c>
+      <c r="Q323">
+        <v>3</v>
+      </c>
+      <c r="S323">
+        <v>6</v>
+      </c>
+      <c r="T323">
+        <v>2</v>
+      </c>
+      <c r="V323">
+        <v>27</v>
+      </c>
+      <c r="W323">
+        <v>9</v>
+      </c>
+      <c r="Z323">
+        <v>3</v>
+      </c>
+      <c r="AA323">
+        <v>2</v>
+      </c>
+      <c r="AB323">
+        <v>23</v>
+      </c>
+      <c r="AC323">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="324" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A324">
+        <v>222</v>
+      </c>
+      <c r="B324">
+        <v>2022</v>
+      </c>
+      <c r="C324">
+        <v>4</v>
+      </c>
+      <c r="D324">
+        <v>2</v>
+      </c>
+      <c r="E324">
+        <v>4</v>
+      </c>
+      <c r="F324">
+        <v>6</v>
+      </c>
+      <c r="G324" t="s">
+        <v>33</v>
+      </c>
+      <c r="H324" t="s">
+        <v>21</v>
+      </c>
+      <c r="I324" t="s">
+        <v>38</v>
+      </c>
+      <c r="J324">
+        <v>1280</v>
+      </c>
+      <c r="K324">
+        <v>1</v>
+      </c>
+      <c r="L324" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M324" s="2">
+        <v>1</v>
+      </c>
+      <c r="N324">
+        <v>1</v>
+      </c>
+      <c r="O324" t="s">
+        <v>31</v>
+      </c>
+      <c r="P324">
+        <v>16</v>
+      </c>
+      <c r="Q324">
+        <v>3</v>
+      </c>
+      <c r="S324">
+        <v>5</v>
+      </c>
+      <c r="T324">
+        <v>2</v>
+      </c>
+      <c r="V324">
+        <v>27</v>
+      </c>
+      <c r="W324">
+        <v>9</v>
+      </c>
+      <c r="Z324">
+        <v>3</v>
+      </c>
+      <c r="AA324">
+        <v>2</v>
+      </c>
+      <c r="AB324">
+        <v>23</v>
+      </c>
+      <c r="AC324">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="325" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A325">
+        <v>223</v>
+      </c>
+      <c r="B325">
+        <v>2022</v>
+      </c>
+      <c r="C325">
+        <v>4</v>
+      </c>
+      <c r="D325">
+        <v>2</v>
+      </c>
+      <c r="E325">
+        <v>4</v>
+      </c>
+      <c r="F325">
+        <v>6</v>
+      </c>
+      <c r="G325" t="s">
+        <v>29</v>
+      </c>
+      <c r="H325" t="s">
+        <v>22</v>
+      </c>
+      <c r="I325" t="s">
+        <v>38</v>
+      </c>
+      <c r="J325">
+        <v>2293</v>
+      </c>
+      <c r="K325">
+        <v>1</v>
+      </c>
+      <c r="L325" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M325" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N325">
+        <v>0.5</v>
+      </c>
+      <c r="O325">
+        <v>0.5</v>
+      </c>
+      <c r="P325">
+        <v>17.5</v>
+      </c>
+      <c r="Q325">
+        <v>2.5</v>
+      </c>
+      <c r="S325">
+        <v>4.5</v>
+      </c>
+      <c r="T325">
+        <v>2</v>
+      </c>
+      <c r="V325">
+        <v>27</v>
+      </c>
+      <c r="W325">
+        <v>9</v>
+      </c>
+      <c r="Z325">
+        <v>2</v>
+      </c>
+      <c r="AA325">
+        <v>2</v>
+      </c>
+      <c r="AB325">
+        <v>23.5</v>
+      </c>
+      <c r="AC325">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="326" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A326">
+        <v>224</v>
+      </c>
+      <c r="B326">
+        <v>2022</v>
+      </c>
+      <c r="C326">
+        <v>4</v>
+      </c>
+      <c r="D326">
+        <v>4</v>
+      </c>
+      <c r="E326">
+        <v>4</v>
+      </c>
+      <c r="F326">
+        <v>6</v>
+      </c>
+      <c r="G326" t="s">
+        <v>1</v>
+      </c>
+      <c r="H326" t="s">
+        <v>2</v>
+      </c>
+      <c r="I326" t="s">
+        <v>38</v>
+      </c>
+      <c r="J326">
+        <v>980</v>
+      </c>
+      <c r="K326">
+        <v>0</v>
+      </c>
+      <c r="L326" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M326" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N326">
+        <v>1</v>
+      </c>
+      <c r="O326">
+        <v>0.5</v>
+      </c>
+      <c r="P326">
+        <v>17</v>
+      </c>
+      <c r="Q326">
+        <v>3.5</v>
+      </c>
+      <c r="S326">
+        <v>6</v>
+      </c>
+      <c r="T326">
+        <v>2</v>
+      </c>
+      <c r="V326">
+        <v>27</v>
+      </c>
+      <c r="W326">
+        <v>8</v>
+      </c>
+      <c r="Z326">
+        <v>2.5</v>
+      </c>
+      <c r="AA326">
+        <v>2</v>
+      </c>
+      <c r="AB326">
+        <v>22</v>
+      </c>
+      <c r="AC326">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="327" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L327" s="2"/>
       <c r="M327" s="2"/>
     </row>
-    <row r="328" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L328" s="2"/>
       <c r="M328" s="2"/>
     </row>
-    <row r="329" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L329" s="2"/>
       <c r="M329" s="2"/>
     </row>
-    <row r="330" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L330" s="2"/>
       <c r="M330" s="2"/>
     </row>
-    <row r="331" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L331" s="2"/>
       <c r="M331" s="2"/>
     </row>
-    <row r="332" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L332" s="2"/>
       <c r="M332" s="2"/>
     </row>
-    <row r="333" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L333" s="2"/>
       <c r="M333" s="2"/>
     </row>
-    <row r="334" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L334" s="2"/>
       <c r="M334" s="2"/>
     </row>
-    <row r="335" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L335" s="2"/>
       <c r="M335" s="2"/>
     </row>
-    <row r="336" spans="12:13" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L336" s="2"/>
       <c r="M336" s="2"/>
     </row>
@@ -27176,6 +27614,22 @@
     <row r="462" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L462" s="2"/>
       <c r="M462" s="2"/>
+    </row>
+    <row r="463" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L463" s="2"/>
+      <c r="M463" s="2"/>
+    </row>
+    <row r="464" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L464" s="2"/>
+      <c r="M464" s="2"/>
+    </row>
+    <row r="465" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L465" s="2"/>
+      <c r="M465" s="2"/>
+    </row>
+    <row r="466" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L466" s="2"/>
+      <c r="M466" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>

<commit_message>
update w/ rollings + ow poll (4/7)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7438ED62-2EF5-7F42-87E6-BEFA933CF599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB71FEFE-F065-9E4D-B61D-5F0A8B911E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21800" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="52">
   <si>
     <t>year</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>kantar</t>
+  </si>
+  <si>
+    <t>yougov</t>
   </si>
 </sst>
 </file>
@@ -556,9 +559,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
   <dimension ref="A1:AH466"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A301" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AC323" sqref="AC323"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AC326" sqref="AC326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25397,16 +25400,16 @@
         <v>31</v>
       </c>
       <c r="G305" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="H305" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I305" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J305">
-        <v>1083</v>
+        <v>1434</v>
       </c>
       <c r="K305">
         <v>0</v>
@@ -25420,26 +25423,26 @@
       <c r="N305">
         <v>1</v>
       </c>
-      <c r="O305">
-        <v>1</v>
+      <c r="O305" t="s">
+        <v>31</v>
       </c>
       <c r="P305">
         <v>15</v>
       </c>
       <c r="Q305">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S305">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T305">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V305">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W305">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Z305">
         <v>3</v>
@@ -25448,10 +25451,10 @@
         <v>2</v>
       </c>
       <c r="AB305">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="AC305">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="306" spans="1:29" x14ac:dyDescent="0.2">
@@ -25474,16 +25477,16 @@
         <v>31</v>
       </c>
       <c r="G306" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H306" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I306" t="s">
         <v>38</v>
       </c>
       <c r="J306">
-        <v>2256</v>
+        <v>1083</v>
       </c>
       <c r="K306">
         <v>0</v>
@@ -25492,25 +25495,25 @@
         <v>1</v>
       </c>
       <c r="M306" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N306">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O306">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P306">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="Q306">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S306">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T306">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V306">
         <v>28</v>
@@ -25519,16 +25522,16 @@
         <v>10</v>
       </c>
       <c r="Z306">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA306">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB306">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC306">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="307" spans="1:29" x14ac:dyDescent="0.2">
@@ -25542,7 +25545,7 @@
         <v>3</v>
       </c>
       <c r="D307">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E307">
         <v>3</v>
@@ -25551,16 +25554,16 @@
         <v>31</v>
       </c>
       <c r="G307" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H307" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I307" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J307">
-        <v>2515</v>
+        <v>2256</v>
       </c>
       <c r="K307">
         <v>0</v>
@@ -25572,40 +25575,40 @@
         <v>0.5</v>
       </c>
       <c r="N307">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O307">
         <v>0.5</v>
       </c>
       <c r="P307">
-        <v>16</v>
+        <v>15.5</v>
       </c>
       <c r="Q307">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S307">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="T307">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V307">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W307">
         <v>10</v>
       </c>
       <c r="Z307">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AA307">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="AB307">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="AC307">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="308" spans="1:29" x14ac:dyDescent="0.2">
@@ -25619,7 +25622,7 @@
         <v>3</v>
       </c>
       <c r="D308">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E308">
         <v>3</v>
@@ -25628,7 +25631,7 @@
         <v>31</v>
       </c>
       <c r="G308" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H308" t="s">
         <v>21</v>
@@ -25637,7 +25640,7 @@
         <v>47</v>
       </c>
       <c r="J308">
-        <v>743</v>
+        <v>2515</v>
       </c>
       <c r="K308">
         <v>0</v>
@@ -25646,19 +25649,19 @@
         <v>1</v>
       </c>
       <c r="M308" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N308">
         <v>1</v>
       </c>
-      <c r="O308" t="s">
-        <v>31</v>
+      <c r="O308">
+        <v>0.5</v>
       </c>
       <c r="P308">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q308">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S308">
         <v>5</v>
@@ -25673,16 +25676,16 @@
         <v>10</v>
       </c>
       <c r="Z308">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AA308">
         <v>3</v>
       </c>
       <c r="AB308">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AC308">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="309" spans="1:29" x14ac:dyDescent="0.2">
@@ -25705,7 +25708,7 @@
         <v>31</v>
       </c>
       <c r="G309" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H309" t="s">
         <v>21</v>
@@ -25714,7 +25717,7 @@
         <v>47</v>
       </c>
       <c r="J309">
-        <v>992</v>
+        <v>743</v>
       </c>
       <c r="K309">
         <v>0</v>
@@ -25723,19 +25726,19 @@
         <v>1</v>
       </c>
       <c r="M309" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N309">
         <v>1</v>
       </c>
-      <c r="O309">
-        <v>1</v>
+      <c r="O309" t="s">
+        <v>31</v>
       </c>
       <c r="P309">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="Q309">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S309">
         <v>5</v>
@@ -25747,19 +25750,19 @@
         <v>27</v>
       </c>
       <c r="W309">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="Z309">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AA309">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AB309">
         <v>21</v>
       </c>
       <c r="AC309">
-        <v>9.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="310" spans="1:29" x14ac:dyDescent="0.2">
@@ -25773,25 +25776,25 @@
         <v>3</v>
       </c>
       <c r="D310">
+        <v>30</v>
+      </c>
+      <c r="E310">
+        <v>3</v>
+      </c>
+      <c r="F310">
         <v>31</v>
       </c>
-      <c r="E310">
-        <v>4</v>
-      </c>
-      <c r="F310">
-        <v>1</v>
-      </c>
       <c r="G310" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H310" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I310" t="s">
         <v>47</v>
       </c>
       <c r="J310">
-        <v>1052</v>
+        <v>992</v>
       </c>
       <c r="K310">
         <v>0</v>
@@ -25806,10 +25809,10 @@
         <v>1</v>
       </c>
       <c r="O310">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P310">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="Q310">
         <v>3.5</v>
@@ -25824,19 +25827,19 @@
         <v>27</v>
       </c>
       <c r="W310">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="Z310">
         <v>2.5</v>
       </c>
       <c r="AA310">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB310">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AC310">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="311" spans="1:29" x14ac:dyDescent="0.2">
@@ -25850,25 +25853,25 @@
         <v>3</v>
       </c>
       <c r="D311">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E311">
         <v>4</v>
       </c>
       <c r="F311">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G311" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="H311" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I311" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J311">
-        <v>1066</v>
+        <v>1052</v>
       </c>
       <c r="K311">
         <v>0</v>
@@ -25880,40 +25883,40 @@
         <v>0.5</v>
       </c>
       <c r="N311">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O311">
         <v>0.5</v>
       </c>
       <c r="P311">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="Q311">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="S311">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T311">
         <v>2</v>
       </c>
       <c r="V311">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W311">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="Z311">
         <v>2.5</v>
       </c>
       <c r="AA311">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB311">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AC311">
-        <v>11</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="312" spans="1:29" x14ac:dyDescent="0.2">
@@ -25927,7 +25930,7 @@
         <v>3</v>
       </c>
       <c r="D312">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E312">
         <v>4</v>
@@ -25936,16 +25939,16 @@
         <v>2</v>
       </c>
       <c r="G312" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H312" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I312" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J312">
-        <v>999</v>
+        <v>1066</v>
       </c>
       <c r="K312">
         <v>0</v>
@@ -25963,34 +25966,34 @@
         <v>0.5</v>
       </c>
       <c r="P312">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="Q312">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S312">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="T312">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V312">
-        <v>28.5</v>
+        <v>26</v>
       </c>
       <c r="W312">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="Z312">
         <v>2.5</v>
       </c>
       <c r="AA312">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AB312">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AC312">
-        <v>9.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="313" spans="1:29" x14ac:dyDescent="0.2">
@@ -26001,19 +26004,19 @@
         <v>2022</v>
       </c>
       <c r="C313">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D313">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="E313">
         <v>4</v>
       </c>
       <c r="F313">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G313" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H313" t="s">
         <v>21</v>
@@ -26022,52 +26025,52 @@
         <v>47</v>
       </c>
       <c r="J313">
-        <v>700</v>
+        <v>999</v>
       </c>
       <c r="K313">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L313" s="2">
         <v>1</v>
       </c>
       <c r="M313" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N313">
-        <v>1</v>
-      </c>
-      <c r="O313" t="s">
-        <v>31</v>
+        <v>1.5</v>
+      </c>
+      <c r="O313">
+        <v>0.5</v>
       </c>
       <c r="P313">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q313">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S313">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="T313">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V313">
-        <v>27</v>
+        <v>28.5</v>
       </c>
       <c r="W313">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="Z313">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AA313">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB313">
         <v>22</v>
       </c>
       <c r="AC313">
-        <v>9</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="314" spans="1:29" x14ac:dyDescent="0.2">
@@ -26081,70 +26084,70 @@
         <v>4</v>
       </c>
       <c r="D314">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E314">
         <v>4</v>
       </c>
       <c r="F314">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G314" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="H314" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I314" t="s">
         <v>47</v>
       </c>
       <c r="J314">
-        <v>1892</v>
+        <v>700</v>
       </c>
       <c r="K314">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L314" s="2">
         <v>1</v>
       </c>
       <c r="M314" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N314">
         <v>1</v>
       </c>
-      <c r="O314">
-        <v>0.5</v>
+      <c r="O314" t="s">
+        <v>31</v>
       </c>
       <c r="P314">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="Q314">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="S314">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T314">
         <v>2</v>
       </c>
       <c r="V314">
-        <v>26.5</v>
+        <v>27</v>
       </c>
       <c r="W314">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="Z314">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA314">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB314">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AC314">
-        <v>9.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="315" spans="1:29" x14ac:dyDescent="0.2">
@@ -26158,7 +26161,7 @@
         <v>4</v>
       </c>
       <c r="D315">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E315">
         <v>4</v>
@@ -26167,16 +26170,16 @@
         <v>4</v>
       </c>
       <c r="G315" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="H315" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I315" t="s">
         <v>47</v>
       </c>
       <c r="J315">
-        <v>2793</v>
+        <v>1892</v>
       </c>
       <c r="K315">
         <v>0</v>
@@ -26200,28 +26203,28 @@
         <v>2.5</v>
       </c>
       <c r="S315">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T315">
         <v>2</v>
       </c>
       <c r="V315">
-        <v>26</v>
+        <v>26.5</v>
       </c>
       <c r="W315">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="Z315">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA315">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="AB315">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="AC315">
-        <v>11</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="316" spans="1:29" x14ac:dyDescent="0.2">
@@ -26244,16 +26247,16 @@
         <v>4</v>
       </c>
       <c r="G316" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="H316" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I316" t="s">
         <v>47</v>
       </c>
       <c r="J316">
-        <v>7037</v>
+        <v>2793</v>
       </c>
       <c r="K316">
         <v>0</v>
@@ -26271,34 +26274,34 @@
         <v>0.5</v>
       </c>
       <c r="P316">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q316">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="S316">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T316">
         <v>2</v>
       </c>
       <c r="V316">
-        <v>26.5</v>
+        <v>26</v>
       </c>
       <c r="W316">
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="Z316">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AA316">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB316">
-        <v>21.5</v>
+        <v>20</v>
       </c>
       <c r="AC316">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="317" spans="1:29" x14ac:dyDescent="0.2">
@@ -26312,7 +26315,7 @@
         <v>4</v>
       </c>
       <c r="D317">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E317">
         <v>4</v>
@@ -26321,16 +26324,16 @@
         <v>4</v>
       </c>
       <c r="G317" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="H317" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I317" t="s">
         <v>47</v>
       </c>
       <c r="J317">
-        <v>801</v>
+        <v>7037</v>
       </c>
       <c r="K317">
         <v>0</v>
@@ -26339,40 +26342,40 @@
         <v>1</v>
       </c>
       <c r="M317" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N317">
         <v>1</v>
       </c>
       <c r="O317">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P317">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Q317">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="S317">
         <v>6</v>
       </c>
       <c r="T317">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V317">
-        <v>26</v>
+        <v>26.5</v>
       </c>
       <c r="W317">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="Z317">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AA317">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB317">
-        <v>23</v>
+        <v>21.5</v>
       </c>
       <c r="AC317">
         <v>10</v>
@@ -26389,13 +26392,13 @@
         <v>4</v>
       </c>
       <c r="D318">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E318">
         <v>4</v>
       </c>
       <c r="F318">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G318" t="s">
         <v>33</v>
@@ -26404,10 +26407,10 @@
         <v>21</v>
       </c>
       <c r="I318" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J318">
-        <v>1280</v>
+        <v>801</v>
       </c>
       <c r="K318">
         <v>0</v>
@@ -26421,11 +26424,11 @@
       <c r="N318">
         <v>1</v>
       </c>
-      <c r="O318" t="s">
-        <v>31</v>
+      <c r="O318">
+        <v>1</v>
       </c>
       <c r="P318">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q318">
         <v>3</v>
@@ -26434,16 +26437,16 @@
         <v>6</v>
       </c>
       <c r="T318">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V318">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W318">
         <v>9</v>
       </c>
       <c r="Z318">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA318">
         <v>3</v>
@@ -26452,7 +26455,7 @@
         <v>23</v>
       </c>
       <c r="AC318">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="319" spans="1:29" x14ac:dyDescent="0.2">
@@ -26466,7 +26469,7 @@
         <v>4</v>
       </c>
       <c r="D319">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E319">
         <v>4</v>
@@ -26475,16 +26478,16 @@
         <v>5</v>
       </c>
       <c r="G319" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H319" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I319" t="s">
         <v>38</v>
       </c>
       <c r="J319">
-        <v>2293</v>
+        <v>1280</v>
       </c>
       <c r="K319">
         <v>0</v>
@@ -26493,43 +26496,43 @@
         <v>1</v>
       </c>
       <c r="M319" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N319">
-        <v>0.5</v>
-      </c>
-      <c r="O319">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="O319" t="s">
+        <v>31</v>
       </c>
       <c r="P319">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="Q319">
         <v>3</v>
       </c>
       <c r="S319">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="T319">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V319">
         <v>27</v>
       </c>
       <c r="W319">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="Z319">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA319">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AB319">
         <v>23</v>
       </c>
       <c r="AC319">
-        <v>9.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="320" spans="1:29" x14ac:dyDescent="0.2">
@@ -26543,7 +26546,7 @@
         <v>4</v>
       </c>
       <c r="D320">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E320">
         <v>4</v>
@@ -26552,16 +26555,16 @@
         <v>5</v>
       </c>
       <c r="G320" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="H320" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I320" t="s">
         <v>38</v>
       </c>
       <c r="J320">
-        <v>949</v>
+        <v>2293</v>
       </c>
       <c r="K320">
         <v>0</v>
@@ -26573,7 +26576,7 @@
         <v>0.5</v>
       </c>
       <c r="N320">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O320">
         <v>0.5</v>
@@ -26582,31 +26585,31 @@
         <v>16.5</v>
       </c>
       <c r="Q320">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S320">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="T320">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V320">
         <v>27</v>
       </c>
       <c r="W320">
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="Z320">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA320">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="AB320">
-        <v>20.5</v>
+        <v>23</v>
       </c>
       <c r="AC320">
-        <v>10</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="321" spans="1:29" x14ac:dyDescent="0.2">
@@ -26620,7 +26623,7 @@
         <v>4</v>
       </c>
       <c r="D321">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E321">
         <v>4</v>
@@ -26629,16 +26632,16 @@
         <v>5</v>
       </c>
       <c r="G321" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H321" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I321" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J321">
-        <v>993</v>
+        <v>949</v>
       </c>
       <c r="K321">
         <v>0</v>
@@ -26650,25 +26653,25 @@
         <v>0.5</v>
       </c>
       <c r="N321">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O321">
         <v>0.5</v>
       </c>
       <c r="P321">
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
       <c r="Q321">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="S321">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="T321">
         <v>2</v>
       </c>
       <c r="V321">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W321">
         <v>8</v>
@@ -26677,13 +26680,13 @@
         <v>3</v>
       </c>
       <c r="AA321">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB321">
-        <v>23</v>
+        <v>20.5</v>
       </c>
       <c r="AC321">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="322" spans="1:29" x14ac:dyDescent="0.2">
@@ -26706,7 +26709,7 @@
         <v>5</v>
       </c>
       <c r="G322" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H322" t="s">
         <v>21</v>
@@ -26715,7 +26718,7 @@
         <v>47</v>
       </c>
       <c r="J322">
-        <v>1032</v>
+        <v>993</v>
       </c>
       <c r="K322">
         <v>0</v>
@@ -26727,25 +26730,25 @@
         <v>0.5</v>
       </c>
       <c r="N322">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O322">
         <v>0.5</v>
       </c>
       <c r="P322">
-        <v>16</v>
+        <v>15.5</v>
       </c>
       <c r="Q322">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="S322">
         <v>5</v>
       </c>
       <c r="T322">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V322">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="W322">
         <v>8</v>
@@ -26760,7 +26763,7 @@
         <v>23</v>
       </c>
       <c r="AC322">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="323" spans="1:29" x14ac:dyDescent="0.2">
@@ -26783,7 +26786,7 @@
         <v>5</v>
       </c>
       <c r="G323" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H323" t="s">
         <v>21</v>
@@ -26792,7 +26795,7 @@
         <v>47</v>
       </c>
       <c r="J323">
-        <v>888</v>
+        <v>1032</v>
       </c>
       <c r="K323">
         <v>0</v>
@@ -26801,31 +26804,31 @@
         <v>1</v>
       </c>
       <c r="M323" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N323">
         <v>1</v>
       </c>
-      <c r="O323" t="s">
-        <v>31</v>
+      <c r="O323">
+        <v>0.5</v>
       </c>
       <c r="P323">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q323">
         <v>3</v>
       </c>
       <c r="S323">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T323">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V323">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="W323">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Z323">
         <v>3</v>
@@ -26837,7 +26840,7 @@
         <v>23</v>
       </c>
       <c r="AC323">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="324" spans="1:29" x14ac:dyDescent="0.2">
@@ -26851,13 +26854,13 @@
         <v>4</v>
       </c>
       <c r="D324">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E324">
         <v>4</v>
       </c>
       <c r="F324">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G324" t="s">
         <v>33</v>
@@ -26866,16 +26869,16 @@
         <v>21</v>
       </c>
       <c r="I324" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J324">
-        <v>1280</v>
+        <v>888</v>
       </c>
       <c r="K324">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L324" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M324" s="2">
         <v>1</v>
@@ -26887,13 +26890,13 @@
         <v>31</v>
       </c>
       <c r="P324">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q324">
         <v>3</v>
       </c>
       <c r="S324">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T324">
         <v>2</v>
@@ -26928,7 +26931,7 @@
         <v>4</v>
       </c>
       <c r="D325">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E325">
         <v>4</v>
@@ -26937,61 +26940,61 @@
         <v>6</v>
       </c>
       <c r="G325" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H325" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I325" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J325">
-        <v>2293</v>
+        <v>1499</v>
       </c>
       <c r="K325">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L325" s="2">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M325" s="2">
         <v>0.5</v>
       </c>
       <c r="N325">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O325">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P325">
-        <v>17.5</v>
+        <v>16</v>
       </c>
       <c r="Q325">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="S325">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T325">
         <v>2</v>
       </c>
       <c r="V325">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W325">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z325">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA325">
         <v>2</v>
       </c>
       <c r="AB325">
-        <v>23.5</v>
+        <v>24</v>
       </c>
       <c r="AC325">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="326" spans="1:29" x14ac:dyDescent="0.2">
@@ -27005,7 +27008,7 @@
         <v>4</v>
       </c>
       <c r="D326">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E326">
         <v>4</v>
@@ -27014,74 +27017,293 @@
         <v>6</v>
       </c>
       <c r="G326" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="H326" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I326" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J326">
-        <v>980</v>
+        <v>888</v>
       </c>
       <c r="K326">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L326" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M326" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N326">
         <v>1</v>
       </c>
       <c r="O326">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P326">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q326">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="S326">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T326">
         <v>2</v>
       </c>
       <c r="V326">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W326">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Z326">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AA326">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB326">
         <v>22</v>
       </c>
       <c r="AC326">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="327" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A327">
+        <v>225</v>
+      </c>
+      <c r="B327">
+        <v>2022</v>
+      </c>
+      <c r="C327">
+        <v>4</v>
+      </c>
+      <c r="D327">
+        <v>4</v>
+      </c>
+      <c r="E327">
+        <v>4</v>
+      </c>
+      <c r="F327">
+        <v>7</v>
+      </c>
+      <c r="G327" t="s">
+        <v>29</v>
+      </c>
+      <c r="H327" t="s">
+        <v>22</v>
+      </c>
+      <c r="I327" t="s">
+        <v>38</v>
+      </c>
+      <c r="J327">
+        <v>2293</v>
+      </c>
+      <c r="K327">
+        <v>1</v>
+      </c>
+      <c r="L327" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M327" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N327">
+        <v>1</v>
+      </c>
+      <c r="O327">
+        <v>0.5</v>
+      </c>
+      <c r="P327">
+        <v>17.5</v>
+      </c>
+      <c r="Q327">
+        <v>2.5</v>
+      </c>
+      <c r="S327">
+        <v>4.5</v>
+      </c>
+      <c r="T327">
+        <v>2</v>
+      </c>
+      <c r="V327">
+        <v>26.5</v>
+      </c>
+      <c r="W327">
+        <v>9</v>
+      </c>
+      <c r="Z327">
+        <v>2.5</v>
+      </c>
+      <c r="AA327">
+        <v>1.5</v>
+      </c>
+      <c r="AB327">
+        <v>24</v>
+      </c>
+      <c r="AC327">
         <v>8.5</v>
       </c>
     </row>
-    <row r="327" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L327" s="2"/>
-      <c r="M327" s="2"/>
-    </row>
     <row r="328" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L328" s="2"/>
-      <c r="M328" s="2"/>
+      <c r="A328">
+        <v>226</v>
+      </c>
+      <c r="B328">
+        <v>2022</v>
+      </c>
+      <c r="C328">
+        <v>4</v>
+      </c>
+      <c r="D328">
+        <v>4</v>
+      </c>
+      <c r="E328">
+        <v>4</v>
+      </c>
+      <c r="F328">
+        <v>7</v>
+      </c>
+      <c r="G328" t="s">
+        <v>33</v>
+      </c>
+      <c r="H328" t="s">
+        <v>21</v>
+      </c>
+      <c r="I328" t="s">
+        <v>38</v>
+      </c>
+      <c r="J328">
+        <v>1280</v>
+      </c>
+      <c r="K328">
+        <v>1</v>
+      </c>
+      <c r="L328" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M328" s="2">
+        <v>1</v>
+      </c>
+      <c r="N328">
+        <v>1</v>
+      </c>
+      <c r="O328">
+        <v>1</v>
+      </c>
+      <c r="P328">
+        <v>17</v>
+      </c>
+      <c r="Q328">
+        <v>3</v>
+      </c>
+      <c r="S328">
+        <v>5</v>
+      </c>
+      <c r="T328">
+        <v>2</v>
+      </c>
+      <c r="V328">
+        <v>26</v>
+      </c>
+      <c r="W328">
+        <v>9</v>
+      </c>
+      <c r="Z328">
+        <v>3</v>
+      </c>
+      <c r="AA328">
+        <v>2</v>
+      </c>
+      <c r="AB328">
+        <v>22</v>
+      </c>
+      <c r="AC328">
+        <v>9</v>
+      </c>
     </row>
     <row r="329" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L329" s="2"/>
-      <c r="M329" s="2"/>
+      <c r="A329">
+        <v>227</v>
+      </c>
+      <c r="B329">
+        <v>2022</v>
+      </c>
+      <c r="C329">
+        <v>4</v>
+      </c>
+      <c r="D329">
+        <v>5</v>
+      </c>
+      <c r="E329">
+        <v>4</v>
+      </c>
+      <c r="F329">
+        <v>7</v>
+      </c>
+      <c r="G329" t="s">
+        <v>1</v>
+      </c>
+      <c r="H329" t="s">
+        <v>2</v>
+      </c>
+      <c r="I329" t="s">
+        <v>38</v>
+      </c>
+      <c r="J329">
+        <v>981</v>
+      </c>
+      <c r="K329">
+        <v>0</v>
+      </c>
+      <c r="L329" s="2">
+        <v>1</v>
+      </c>
+      <c r="M329" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N329">
+        <v>1</v>
+      </c>
+      <c r="O329">
+        <v>0.5</v>
+      </c>
+      <c r="P329">
+        <v>16.5</v>
+      </c>
+      <c r="Q329">
+        <v>3.5</v>
+      </c>
+      <c r="S329">
+        <v>5.5</v>
+      </c>
+      <c r="T329">
+        <v>2</v>
+      </c>
+      <c r="V329">
+        <v>26.5</v>
+      </c>
+      <c r="W329">
+        <v>8.5</v>
+      </c>
+      <c r="Z329">
+        <v>2.5</v>
+      </c>
+      <c r="AA329">
+        <v>2</v>
+      </c>
+      <c r="AB329">
+        <v>23</v>
+      </c>
+      <c r="AC329">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="330" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L330" s="2"/>

</xml_diff>

<commit_message>
update w/ rollings + ow, cluster17, elabe, bva , harris polls (4/8)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB71FEFE-F065-9E4D-B61D-5F0A8B911E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EF936B-E8D3-F14C-B51A-1A22BA598801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21800" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="52">
   <si>
     <t>year</t>
   </si>
@@ -560,8 +560,8 @@
   <dimension ref="A1:AH466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AC326" sqref="AC326"/>
+      <pane ySplit="1" topLeftCell="A304" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="K328" sqref="K328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27085,7 +27085,7 @@
         <v>4</v>
       </c>
       <c r="D327">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E327">
         <v>4</v>
@@ -27094,22 +27094,22 @@
         <v>7</v>
       </c>
       <c r="G327" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H327" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I327" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J327">
-        <v>2293</v>
+        <v>1010</v>
       </c>
       <c r="K327">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L327" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M327" s="2">
         <v>0.5</v>
@@ -27130,25 +27130,25 @@
         <v>4.5</v>
       </c>
       <c r="T327">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V327">
-        <v>26.5</v>
+        <v>26</v>
       </c>
       <c r="W327">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="Z327">
         <v>2.5</v>
       </c>
       <c r="AA327">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AB327">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AC327">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="328" spans="1:29" x14ac:dyDescent="0.2">
@@ -27162,7 +27162,7 @@
         <v>4</v>
       </c>
       <c r="D328">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E328">
         <v>4</v>
@@ -27177,16 +27177,16 @@
         <v>21</v>
       </c>
       <c r="I328" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J328">
-        <v>1280</v>
+        <v>700</v>
       </c>
       <c r="K328">
         <v>1</v>
       </c>
       <c r="L328" s="2">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M328" s="2">
         <v>1</v>
@@ -27194,8 +27194,8 @@
       <c r="N328">
         <v>1</v>
       </c>
-      <c r="O328">
-        <v>1</v>
+      <c r="O328" t="s">
+        <v>31</v>
       </c>
       <c r="P328">
         <v>17</v>
@@ -27204,13 +27204,13 @@
         <v>3</v>
       </c>
       <c r="S328">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T328">
         <v>2</v>
       </c>
       <c r="V328">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="W328">
         <v>9</v>
@@ -27219,7 +27219,7 @@
         <v>3</v>
       </c>
       <c r="AA328">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB328">
         <v>22</v>
@@ -27245,22 +27245,22 @@
         <v>4</v>
       </c>
       <c r="F329">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G329" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="H329" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I329" t="s">
         <v>38</v>
       </c>
       <c r="J329">
-        <v>981</v>
+        <v>2293</v>
       </c>
       <c r="K329">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L329" s="2">
         <v>1</v>
@@ -27275,55 +27275,420 @@
         <v>0.5</v>
       </c>
       <c r="P329">
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="Q329">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="S329">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="T329">
         <v>2</v>
       </c>
       <c r="V329">
-        <v>26.5</v>
+        <v>26</v>
       </c>
       <c r="W329">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="Z329">
         <v>2.5</v>
       </c>
       <c r="AA329">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB329">
+        <v>24</v>
+      </c>
+      <c r="AC329">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="330" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A330">
+        <v>228</v>
+      </c>
+      <c r="B330">
+        <v>2022</v>
+      </c>
+      <c r="C330">
+        <v>4</v>
+      </c>
+      <c r="D330">
+        <v>5</v>
+      </c>
+      <c r="E330">
+        <v>4</v>
+      </c>
+      <c r="F330">
+        <v>8</v>
+      </c>
+      <c r="G330" t="s">
+        <v>33</v>
+      </c>
+      <c r="H330" t="s">
+        <v>21</v>
+      </c>
+      <c r="I330" t="s">
+        <v>38</v>
+      </c>
+      <c r="J330">
+        <v>1280</v>
+      </c>
+      <c r="K330">
+        <v>1</v>
+      </c>
+      <c r="L330" s="2">
+        <v>1</v>
+      </c>
+      <c r="M330" s="2">
+        <v>1</v>
+      </c>
+      <c r="N330">
+        <v>1</v>
+      </c>
+      <c r="O330">
+        <v>1</v>
+      </c>
+      <c r="P330">
+        <v>17</v>
+      </c>
+      <c r="Q330">
+        <v>3</v>
+      </c>
+      <c r="S330">
+        <v>5</v>
+      </c>
+      <c r="T330">
+        <v>2</v>
+      </c>
+      <c r="V330">
+        <v>26</v>
+      </c>
+      <c r="W330">
+        <v>9</v>
+      </c>
+      <c r="Z330">
+        <v>3</v>
+      </c>
+      <c r="AA330">
+        <v>2</v>
+      </c>
+      <c r="AB330">
+        <v>22</v>
+      </c>
+      <c r="AC330">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="331" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A331">
+        <v>229</v>
+      </c>
+      <c r="B331">
+        <v>2022</v>
+      </c>
+      <c r="C331">
+        <v>4</v>
+      </c>
+      <c r="D331">
+        <v>6</v>
+      </c>
+      <c r="E331">
+        <v>4</v>
+      </c>
+      <c r="F331">
+        <v>8</v>
+      </c>
+      <c r="G331" t="s">
+        <v>35</v>
+      </c>
+      <c r="H331" t="s">
+        <v>21</v>
+      </c>
+      <c r="I331" t="s">
+        <v>47</v>
+      </c>
+      <c r="J331">
+        <v>3097</v>
+      </c>
+      <c r="K331">
+        <v>0</v>
+      </c>
+      <c r="L331" s="2">
+        <v>1</v>
+      </c>
+      <c r="M331" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N331">
+        <v>1</v>
+      </c>
+      <c r="O331">
+        <v>0.5</v>
+      </c>
+      <c r="P331">
+        <v>18</v>
+      </c>
+      <c r="Q331">
+        <v>2.5</v>
+      </c>
+      <c r="S331">
+        <v>4</v>
+      </c>
+      <c r="T331">
+        <v>2</v>
+      </c>
+      <c r="V331">
+        <v>26</v>
+      </c>
+      <c r="W331">
+        <v>9.5</v>
+      </c>
+      <c r="Z331">
+        <v>3</v>
+      </c>
+      <c r="AA331">
+        <v>3</v>
+      </c>
+      <c r="AB331">
+        <v>21</v>
+      </c>
+      <c r="AC331">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="332" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A332">
+        <v>230</v>
+      </c>
+      <c r="B332">
+        <v>2022</v>
+      </c>
+      <c r="C332">
+        <v>4</v>
+      </c>
+      <c r="D332">
+        <v>6</v>
+      </c>
+      <c r="E332">
+        <v>4</v>
+      </c>
+      <c r="F332">
+        <v>8</v>
+      </c>
+      <c r="G332" t="s">
+        <v>1</v>
+      </c>
+      <c r="H332" t="s">
+        <v>2</v>
+      </c>
+      <c r="I332" t="s">
+        <v>38</v>
+      </c>
+      <c r="J332">
+        <v>985</v>
+      </c>
+      <c r="K332">
+        <v>0</v>
+      </c>
+      <c r="L332" s="2">
+        <v>1</v>
+      </c>
+      <c r="M332" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N332">
+        <v>1</v>
+      </c>
+      <c r="O332">
+        <v>0.5</v>
+      </c>
+      <c r="P332">
+        <v>16.5</v>
+      </c>
+      <c r="Q332">
+        <v>3</v>
+      </c>
+      <c r="S332">
+        <v>5</v>
+      </c>
+      <c r="T332">
+        <v>2.5</v>
+      </c>
+      <c r="V332">
+        <v>26.5</v>
+      </c>
+      <c r="W332">
+        <v>8.5</v>
+      </c>
+      <c r="Z332">
+        <v>2</v>
+      </c>
+      <c r="AA332">
+        <v>2.5</v>
+      </c>
+      <c r="AB332">
         <v>23</v>
       </c>
-      <c r="AC329">
+      <c r="AC332">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="333" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A333">
+        <v>231</v>
+      </c>
+      <c r="B333">
+        <v>2022</v>
+      </c>
+      <c r="C333">
+        <v>4</v>
+      </c>
+      <c r="D333">
+        <v>7</v>
+      </c>
+      <c r="E333">
+        <v>4</v>
+      </c>
+      <c r="F333">
+        <v>8</v>
+      </c>
+      <c r="G333" t="s">
+        <v>30</v>
+      </c>
+      <c r="H333" t="s">
+        <v>21</v>
+      </c>
+      <c r="I333" t="s">
+        <v>47</v>
+      </c>
+      <c r="J333">
+        <v>1200</v>
+      </c>
+      <c r="K333">
+        <v>0</v>
+      </c>
+      <c r="L333" s="2">
+        <v>1</v>
+      </c>
+      <c r="M333" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N333">
+        <v>1</v>
+      </c>
+      <c r="O333">
+        <v>0.5</v>
+      </c>
+      <c r="P333">
+        <v>17.5</v>
+      </c>
+      <c r="Q333">
+        <v>2.5</v>
+      </c>
+      <c r="S333">
+        <v>4</v>
+      </c>
+      <c r="T333">
+        <v>2</v>
+      </c>
+      <c r="V333">
+        <v>26</v>
+      </c>
+      <c r="W333">
+        <v>8</v>
+      </c>
+      <c r="Z333">
+        <v>2.5</v>
+      </c>
+      <c r="AA333">
+        <v>2.5</v>
+      </c>
+      <c r="AB333">
+        <v>25</v>
+      </c>
+      <c r="AC333">
         <v>8.5</v>
       </c>
     </row>
-    <row r="330" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L330" s="2"/>
-      <c r="M330" s="2"/>
-    </row>
-    <row r="331" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L331" s="2"/>
-      <c r="M331" s="2"/>
-    </row>
-    <row r="332" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L332" s="2"/>
-      <c r="M332" s="2"/>
-    </row>
-    <row r="333" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L333" s="2"/>
-      <c r="M333" s="2"/>
-    </row>
     <row r="334" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L334" s="2"/>
-      <c r="M334" s="2"/>
+      <c r="A334">
+        <v>232</v>
+      </c>
+      <c r="B334">
+        <v>2022</v>
+      </c>
+      <c r="C334">
+        <v>4</v>
+      </c>
+      <c r="D334">
+        <v>7</v>
+      </c>
+      <c r="E334">
+        <v>4</v>
+      </c>
+      <c r="F334">
+        <v>8</v>
+      </c>
+      <c r="G334" t="s">
+        <v>20</v>
+      </c>
+      <c r="H334" t="s">
+        <v>22</v>
+      </c>
+      <c r="I334" t="s">
+        <v>47</v>
+      </c>
+      <c r="J334">
+        <v>1890</v>
+      </c>
+      <c r="K334">
+        <v>1</v>
+      </c>
+      <c r="L334" s="2">
+        <v>1</v>
+      </c>
+      <c r="M334" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N334">
+        <v>1</v>
+      </c>
+      <c r="O334">
+        <v>0.5</v>
+      </c>
+      <c r="P334">
+        <v>18</v>
+      </c>
+      <c r="Q334">
+        <v>2.5</v>
+      </c>
+      <c r="S334">
+        <v>4.5</v>
+      </c>
+      <c r="T334">
+        <v>2</v>
+      </c>
+      <c r="V334">
+        <v>27</v>
+      </c>
+      <c r="W334">
+        <v>8</v>
+      </c>
+      <c r="Z334">
+        <v>2</v>
+      </c>
+      <c r="AA334">
+        <v>2</v>
+      </c>
+      <c r="AB334">
+        <v>24</v>
+      </c>
+      <c r="AC334">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="335" spans="1:29" x14ac:dyDescent="0.2">
       <c r="L335" s="2"/>

</xml_diff>

<commit_message>
update w/ ipsos and yougov polls (4/8)
</commit_message>
<xml_diff>
--- a/PollsData.xlsx
+++ b/PollsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flavienganter/Dropbox/PollsFrance2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EF936B-E8D3-F14C-B51A-1A22BA598801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A88C52-C4D8-B841-8391-04FECC9FE609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21800" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{675AE3D8-A0E6-044C-9B12-638CF7A22D98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="52">
   <si>
     <t>year</t>
   </si>
@@ -557,11 +557,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">
-  <dimension ref="A1:AH466"/>
+  <dimension ref="A1:AH467"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A304" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K328" sqref="K328"/>
+      <pane ySplit="1" topLeftCell="A305" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD327" sqref="AD327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27085,7 +27085,7 @@
         <v>4</v>
       </c>
       <c r="D327">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E327">
         <v>4</v>
@@ -27094,16 +27094,16 @@
         <v>7</v>
       </c>
       <c r="G327" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="H327" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I327" t="s">
         <v>47</v>
       </c>
       <c r="J327">
-        <v>1010</v>
+        <v>1948</v>
       </c>
       <c r="K327">
         <v>0</v>
@@ -27112,34 +27112,34 @@
         <v>1</v>
       </c>
       <c r="M327" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N327">
         <v>1</v>
       </c>
       <c r="O327">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P327">
-        <v>17.5</v>
+        <v>16</v>
       </c>
       <c r="Q327">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S327">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T327">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="V327">
         <v>26</v>
       </c>
       <c r="W327">
-        <v>8.5</v>
+        <v>6</v>
       </c>
       <c r="Z327">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AA327">
         <v>2</v>
@@ -27148,7 +27148,7 @@
         <v>23</v>
       </c>
       <c r="AC327">
-        <v>9.5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="328" spans="1:29" x14ac:dyDescent="0.2">
@@ -27171,7 +27171,7 @@
         <v>7</v>
       </c>
       <c r="G328" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H328" t="s">
         <v>21</v>
@@ -27180,52 +27180,52 @@
         <v>47</v>
       </c>
       <c r="J328">
-        <v>700</v>
+        <v>1010</v>
       </c>
       <c r="K328">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L328" s="2">
         <v>1</v>
       </c>
       <c r="M328" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N328">
         <v>1</v>
       </c>
-      <c r="O328" t="s">
-        <v>31</v>
+      <c r="O328">
+        <v>0.5</v>
       </c>
       <c r="P328">
-        <v>17</v>
+        <v>17.5</v>
       </c>
       <c r="Q328">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="S328">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="T328">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V328">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W328">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="Z328">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AA328">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB328">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AC328">
-        <v>9</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="329" spans="1:29" x14ac:dyDescent="0.2">
@@ -27239,25 +27239,25 @@
         <v>4</v>
       </c>
       <c r="D329">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E329">
         <v>4</v>
       </c>
       <c r="F329">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G329" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H329" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I329" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J329">
-        <v>2293</v>
+        <v>700</v>
       </c>
       <c r="K329">
         <v>1</v>
@@ -27266,40 +27266,40 @@
         <v>1</v>
       </c>
       <c r="M329" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N329">
         <v>1</v>
       </c>
-      <c r="O329">
-        <v>0.5</v>
+      <c r="O329" t="s">
+        <v>31</v>
       </c>
       <c r="P329">
         <v>17</v>
       </c>
       <c r="Q329">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="S329">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T329">
         <v>2</v>
       </c>
       <c r="V329">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="W329">
         <v>9</v>
       </c>
       <c r="Z329">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AA329">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AB329">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AC329">
         <v>9</v>
@@ -27325,37 +27325,37 @@
         <v>8</v>
       </c>
       <c r="G330" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H330" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I330" t="s">
         <v>38</v>
       </c>
       <c r="J330">
-        <v>1280</v>
+        <v>2349</v>
       </c>
       <c r="K330">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L330" s="2">
         <v>1</v>
       </c>
       <c r="M330" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N330">
         <v>1</v>
       </c>
       <c r="O330">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P330">
         <v>17</v>
       </c>
       <c r="Q330">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="S330">
         <v>5</v>
@@ -27370,13 +27370,13 @@
         <v>9</v>
       </c>
       <c r="Z330">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AA330">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="AB330">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="AC330">
         <v>9</v>
@@ -27393,7 +27393,7 @@
         <v>4</v>
       </c>
       <c r="D331">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E331">
         <v>4</v>
@@ -27402,40 +27402,40 @@
         <v>8</v>
       </c>
       <c r="G331" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H331" t="s">
         <v>21</v>
       </c>
       <c r="I331" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J331">
-        <v>3097</v>
+        <v>1280</v>
       </c>
       <c r="K331">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L331" s="2">
         <v>1</v>
       </c>
       <c r="M331" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N331">
         <v>1</v>
       </c>
       <c r="O331">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P331">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q331">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="S331">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T331">
         <v>2</v>
@@ -27444,19 +27444,19 @@
         <v>26</v>
       </c>
       <c r="W331">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="Z331">
         <v>3</v>
       </c>
       <c r="AA331">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB331">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AC331">
-        <v>9.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="332" spans="1:29" x14ac:dyDescent="0.2">
@@ -27479,16 +27479,16 @@
         <v>8</v>
       </c>
       <c r="G332" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="H332" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I332" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="J332">
-        <v>985</v>
+        <v>3097</v>
       </c>
       <c r="K332">
         <v>0</v>
@@ -27506,34 +27506,34 @@
         <v>0.5</v>
       </c>
       <c r="P332">
-        <v>16.5</v>
+        <v>18</v>
       </c>
       <c r="Q332">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="S332">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T332">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V332">
-        <v>26.5</v>
+        <v>26</v>
       </c>
       <c r="W332">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="Z332">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA332">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AB332">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AC332">
-        <v>9</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="333" spans="1:29" x14ac:dyDescent="0.2">
@@ -27547,7 +27547,7 @@
         <v>4</v>
       </c>
       <c r="D333">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E333">
         <v>4</v>
@@ -27556,16 +27556,16 @@
         <v>8</v>
       </c>
       <c r="G333" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H333" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I333" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J333">
-        <v>1200</v>
+        <v>985</v>
       </c>
       <c r="K333">
         <v>0</v>
@@ -27583,34 +27583,34 @@
         <v>0.5</v>
       </c>
       <c r="P333">
-        <v>17.5</v>
+        <v>16.5</v>
       </c>
       <c r="Q333">
+        <v>3</v>
+      </c>
+      <c r="S333">
+        <v>5</v>
+      </c>
+      <c r="T333">
         <v>2.5</v>
       </c>
-      <c r="S333">
-        <v>4</v>
-      </c>
-      <c r="T333">
-        <v>2</v>
-      </c>
       <c r="V333">
-        <v>26</v>
+        <v>26.5</v>
       </c>
       <c r="W333">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="Z333">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="AA333">
         <v>2.5</v>
       </c>
       <c r="AB333">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AC333">
-        <v>8.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="334" spans="1:29" x14ac:dyDescent="0.2">
@@ -27633,19 +27633,19 @@
         <v>8</v>
       </c>
       <c r="G334" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H334" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I334" t="s">
         <v>47</v>
       </c>
       <c r="J334">
-        <v>1890</v>
+        <v>1200</v>
       </c>
       <c r="K334">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L334" s="2">
         <v>1</v>
@@ -27660,43 +27660,189 @@
         <v>0.5</v>
       </c>
       <c r="P334">
-        <v>18</v>
+        <v>17.5</v>
       </c>
       <c r="Q334">
         <v>2.5</v>
       </c>
       <c r="S334">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="T334">
         <v>2</v>
       </c>
       <c r="V334">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W334">
         <v>8</v>
       </c>
       <c r="Z334">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AA334">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AB334">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AC334">
         <v>8.5</v>
       </c>
     </row>
     <row r="335" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L335" s="2"/>
-      <c r="M335" s="2"/>
+      <c r="A335">
+        <v>233</v>
+      </c>
+      <c r="B335">
+        <v>2022</v>
+      </c>
+      <c r="C335">
+        <v>4</v>
+      </c>
+      <c r="D335">
+        <v>7</v>
+      </c>
+      <c r="E335">
+        <v>4</v>
+      </c>
+      <c r="F335">
+        <v>8</v>
+      </c>
+      <c r="G335" t="s">
+        <v>20</v>
+      </c>
+      <c r="H335" t="s">
+        <v>22</v>
+      </c>
+      <c r="I335" t="s">
+        <v>47</v>
+      </c>
+      <c r="J335">
+        <v>1681</v>
+      </c>
+      <c r="K335">
+        <v>0</v>
+      </c>
+      <c r="L335" s="2">
+        <v>1</v>
+      </c>
+      <c r="M335" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N335">
+        <v>1</v>
+      </c>
+      <c r="O335">
+        <v>0.5</v>
+      </c>
+      <c r="P335">
+        <v>18</v>
+      </c>
+      <c r="Q335">
+        <v>2.5</v>
+      </c>
+      <c r="S335">
+        <v>4.5</v>
+      </c>
+      <c r="T335">
+        <v>2</v>
+      </c>
+      <c r="V335">
+        <v>27</v>
+      </c>
+      <c r="W335">
+        <v>8</v>
+      </c>
+      <c r="Z335">
+        <v>2</v>
+      </c>
+      <c r="AA335">
+        <v>2</v>
+      </c>
+      <c r="AB335">
+        <v>24</v>
+      </c>
+      <c r="AC335">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="336" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="L336" s="2"/>
-      <c r="M336" s="2"/>
+      <c r="A336">
+        <v>234</v>
+      </c>
+      <c r="B336">
+        <v>2022</v>
+      </c>
+      <c r="C336">
+        <v>4</v>
+      </c>
+      <c r="D336">
+        <v>8</v>
+      </c>
+      <c r="E336">
+        <v>4</v>
+      </c>
+      <c r="F336">
+        <v>8</v>
+      </c>
+      <c r="G336" t="s">
+        <v>1</v>
+      </c>
+      <c r="H336" t="s">
+        <v>2</v>
+      </c>
+      <c r="I336" t="s">
+        <v>47</v>
+      </c>
+      <c r="J336">
+        <v>7321</v>
+      </c>
+      <c r="K336">
+        <v>0</v>
+      </c>
+      <c r="L336" s="2">
+        <v>1</v>
+      </c>
+      <c r="M336" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N336">
+        <v>1</v>
+      </c>
+      <c r="O336">
+        <v>0.5</v>
+      </c>
+      <c r="P336">
+        <v>17.5</v>
+      </c>
+      <c r="Q336">
+        <v>3</v>
+      </c>
+      <c r="S336">
+        <v>5</v>
+      </c>
+      <c r="T336">
+        <v>2</v>
+      </c>
+      <c r="V336">
+        <v>26.5</v>
+      </c>
+      <c r="W336">
+        <v>8.5</v>
+      </c>
+      <c r="Z336">
+        <v>2</v>
+      </c>
+      <c r="AA336">
+        <v>2.5</v>
+      </c>
+      <c r="AB336">
+        <v>22.5</v>
+      </c>
+      <c r="AC336">
+        <v>9</v>
+      </c>
     </row>
     <row r="337" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L337" s="2"/>
@@ -28217,6 +28363,10 @@
     <row r="466" spans="12:13" x14ac:dyDescent="0.2">
       <c r="L466" s="2"/>
       <c r="M466" s="2"/>
+    </row>
+    <row r="467" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L467" s="2"/>
+      <c r="M467" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG128" xr:uid="{7057F566-E0FC-7B48-AE13-1D4B793F99D4}">

</xml_diff>